<commit_message>
Correcion del pequeña del GANTT
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\ProyectoFinal2019-\Actividades\Proy0100\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3DC063-A93A-4BA8-9BE9-2BB642215EC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE0ADB4-2DB1-4915-9FFB-AF57D17BEF62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0447A3F1-1398-4D39-88F7-8434CE3DAECB}"/>
   </bookViews>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30076E1-59D8-4123-BE7D-68CF91B16748}">
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1586,7 @@
         <v>226</v>
       </c>
       <c r="D5" s="16">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modificacion en la tabla de actiidades, y se añadio a la misma los estados de cada una
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\ProyectoFinal2019-\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\proyectofinal2019\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE0ADB4-2DB1-4915-9FFB-AF57D17BEF62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1094BAB0-8CED-4DA3-8D3D-E2AD4AEC32D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0447A3F1-1398-4D39-88F7-8434CE3DAECB}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="261">
   <si>
     <t>Nombre</t>
   </si>
@@ -713,9 +713,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Casos de uso (grafico y extendido)</t>
-  </si>
-  <si>
     <t>BD01001</t>
   </si>
   <si>
@@ -755,17 +752,74 @@
     <t>Consultas SQL 1º Version</t>
   </si>
   <si>
-    <t xml:space="preserve">Si la duracion tiene este color significa que no conocemos su duracio real </t>
-  </si>
-  <si>
     <t>Taller01006/Talelr01001/tTaller01002</t>
+  </si>
+  <si>
+    <t>ADA01006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelo de dominio </t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recursos </t>
+  </si>
+  <si>
+    <t>Casos de uso Grafico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casos de uso extendido </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin Asignar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asignado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asisgnado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asisgado </t>
+  </si>
+  <si>
+    <t>Realizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin asignar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizado constantemente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">realizado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">realizado constantemente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asigando </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asigado  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sin asisgnar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin asisgnar </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,8 +868,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -825,12 +885,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1114,12 +1168,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1130,6 +1178,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1506,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30076E1-59D8-4123-BE7D-68CF91B16748}">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,17 +1577,18 @@
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="70" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:6" ht="114" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
-    </row>
-    <row r="2" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="27"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>128</v>
       </c>
@@ -1542,11 +1601,14 @@
       <c r="D2" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E2" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>108</v>
       </c>
@@ -1559,9 +1621,11 @@
       <c r="D3" s="14">
         <v>2</v>
       </c>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E3" s="30" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>109</v>
       </c>
@@ -1574,8 +1638,11 @@
       <c r="D4" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E4" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>110</v>
       </c>
@@ -1588,8 +1655,11 @@
       <c r="D5" s="16">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E5" s="31" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>111</v>
       </c>
@@ -1602,629 +1672,694 @@
       <c r="D6" s="16">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E6" s="31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="16">
+        <v>2</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="16">
+        <v>5</v>
+      </c>
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="16">
+        <v>3</v>
+      </c>
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D10" s="17">
+        <v>2</v>
+      </c>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D11" s="17">
+        <v>2</v>
+      </c>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D12" s="17">
+        <v>2</v>
+      </c>
+      <c r="E12" s="31"/>
+    </row>
+    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D13" s="17">
+        <v>2</v>
+      </c>
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D14" s="17">
+        <v>2</v>
+      </c>
+      <c r="E14" s="31"/>
+    </row>
+    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D15" s="17">
+        <v>2</v>
+      </c>
+      <c r="E15" s="31"/>
+    </row>
+    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D16" s="17">
+        <v>2</v>
+      </c>
+      <c r="E16" s="31"/>
+    </row>
+    <row r="17" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D17" s="17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="31"/>
+    </row>
+    <row r="18" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D18" s="17">
+        <v>2</v>
+      </c>
+      <c r="E18" s="31"/>
+    </row>
+    <row r="19" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D19" s="17">
+        <v>2</v>
+      </c>
+      <c r="E19" s="31"/>
+    </row>
+    <row r="20" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D20" s="17">
+        <v>2</v>
+      </c>
+      <c r="E20" s="31"/>
+    </row>
+    <row r="21" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D21" s="17">
+        <v>2</v>
+      </c>
+      <c r="E21" s="31"/>
+    </row>
+    <row r="22" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D22" s="17">
+        <v>2</v>
+      </c>
+      <c r="E22" s="31"/>
+    </row>
+    <row r="23" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D23" s="17">
+        <v>2</v>
+      </c>
+      <c r="E23" s="31"/>
+    </row>
+    <row r="24" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D24" s="17">
+        <v>2</v>
+      </c>
+      <c r="E24" s="31"/>
+    </row>
+    <row r="25" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D8" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D9" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D10" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D11" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D12" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D13" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D14" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D15" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D16" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D17" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D18" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D19" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D20" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D21" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D22" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="B25" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="C25" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D25" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="E25" s="31" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="D24" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="D25" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="C26" s="15" t="s">
-        <v>113</v>
+        <v>227</v>
       </c>
       <c r="D26" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E26" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D27" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E27" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D28" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E28" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" s="16">
+        <v>1</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="16">
+        <v>1</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D29" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="C31" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D31" s="17">
+        <v>2</v>
+      </c>
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D30" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="C32" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D32" s="17">
+        <v>2</v>
+      </c>
+      <c r="E32" s="31"/>
+    </row>
+    <row r="33" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D31" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="C33" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D33" s="17">
+        <v>2</v>
+      </c>
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D32" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="C34" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D34" s="17">
+        <v>2</v>
+      </c>
+      <c r="E34" s="31"/>
+    </row>
+    <row r="35" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D33" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="C35" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D35" s="17">
+        <v>2</v>
+      </c>
+      <c r="E35" s="31"/>
+    </row>
+    <row r="36" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D34" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="C36" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D36" s="17">
+        <v>2</v>
+      </c>
+      <c r="E36" s="31"/>
+    </row>
+    <row r="37" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C35" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D35" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="B37" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D37" s="17">
+        <v>2</v>
+      </c>
+      <c r="E37" s="31"/>
+    </row>
+    <row r="38" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D36" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="C38" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D38" s="17">
+        <v>2</v>
+      </c>
+      <c r="E38" s="31"/>
+    </row>
+    <row r="39" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D37" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="C39" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D39" s="17">
+        <v>2</v>
+      </c>
+      <c r="E39" s="31"/>
+    </row>
+    <row r="40" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D38" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="B39" s="4" t="s">
+      <c r="C40" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D40" s="17">
+        <v>2</v>
+      </c>
+      <c r="E40" s="31"/>
+    </row>
+    <row r="41" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D39" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="C41" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D41" s="17">
+        <v>2</v>
+      </c>
+      <c r="E41" s="31"/>
+    </row>
+    <row r="42" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C42" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="D40" s="18">
+      <c r="D42" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="E42" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="D41" s="16">
+      <c r="D43" s="16">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="E43" s="31" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D42" s="16">
+      <c r="C44" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D44" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="E44" s="31"/>
+    </row>
+    <row r="45" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D43" s="16">
+      <c r="C45" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D45" s="16">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="E45" s="31"/>
+    </row>
+    <row r="46" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D44" s="16">
+      <c r="C46" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D46" s="16">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="E46" s="31"/>
+    </row>
+    <row r="47" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D45" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="C47" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D47" s="17">
+        <v>2</v>
+      </c>
+      <c r="E47" s="31"/>
+    </row>
+    <row r="48" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D46" s="16">
+      <c r="C48" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D48" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="E48" s="31"/>
+    </row>
+    <row r="49" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D47" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="C49" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D49" s="17">
+        <v>2</v>
+      </c>
+      <c r="E49" s="31"/>
+    </row>
+    <row r="50" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D48" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="C50" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D50" s="17">
+        <v>2</v>
+      </c>
+      <c r="E50" s="31"/>
+    </row>
+    <row r="51" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D49" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D50" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>226</v>
@@ -2232,27 +2367,33 @@
       <c r="D51" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E51" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E52" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>226</v>
@@ -2260,265 +2401,296 @@
       <c r="D53" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E53" s="31" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C54" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="D54" s="16">
+      <c r="D54" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E54" s="31" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>124</v>
+        <v>226</v>
       </c>
       <c r="D55" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E55" s="31" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D56" s="16">
+        <v>1</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="16">
+        <v>1</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C58" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D56" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="B57" s="4" t="s">
+      <c r="D58" s="16">
+        <v>2</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D57" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="C59" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D59" s="17">
+        <v>2</v>
+      </c>
+      <c r="E59" s="31"/>
+    </row>
+    <row r="60" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D58" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="C60" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D60" s="17">
+        <v>2</v>
+      </c>
+      <c r="E60" s="31"/>
+    </row>
+    <row r="61" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C59" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D59" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="C61" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D61" s="17">
+        <v>2</v>
+      </c>
+      <c r="E61" s="31"/>
+    </row>
+    <row r="62" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D60" s="18">
+      <c r="C62" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D62" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="E62" s="31"/>
+    </row>
+    <row r="63" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D61" s="17">
+      <c r="C63" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D63" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="E63" s="31"/>
+    </row>
+    <row r="64" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C64" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D62" s="18">
+      <c r="D64" s="18">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+      <c r="E64" s="31"/>
+    </row>
+    <row r="65" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C65" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D63" s="18">
+      <c r="D65" s="18">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="B64" s="4" t="s">
+      <c r="E65" s="31"/>
+    </row>
+    <row r="66" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C64" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D64" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C65" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D65" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>233</v>
+      <c r="C66" s="21">
+        <v>43712</v>
       </c>
       <c r="D66" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E66" s="31"/>
+    </row>
+    <row r="67" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D67" s="17">
+        <v>1</v>
+      </c>
+      <c r="E67" s="31"/>
+    </row>
+    <row r="68" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D68" s="16">
+        <v>1</v>
+      </c>
+      <c r="E68" s="31"/>
+    </row>
+    <row r="69" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="D67" s="16">
+      <c r="C69" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D69" s="16">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="E69" s="31"/>
+    </row>
+    <row r="70" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C68" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D68" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+      <c r="C70" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D70" s="17">
+        <v>2</v>
+      </c>
+      <c r="E70" s="31"/>
+    </row>
+    <row r="71" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C69" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D69" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
+      <c r="C71" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D71" s="17">
+        <v>2</v>
+      </c>
+      <c r="E71" s="31"/>
+    </row>
+    <row r="72" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D70" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D71" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>226</v>
@@ -2526,41 +2698,50 @@
       <c r="D72" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E72" s="31" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>226</v>
+        <v>129</v>
       </c>
       <c r="D73" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E73" s="31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>226</v>
       </c>
       <c r="D74" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E74" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>226</v>
@@ -2568,349 +2749,382 @@
       <c r="D75" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E75" s="31" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D76" s="16">
+        <v>2</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D77" s="16">
+        <v>1</v>
+      </c>
+      <c r="E77" s="31" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D78" s="18">
+        <v>1</v>
+      </c>
+      <c r="E78" s="31"/>
+    </row>
+    <row r="79" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D79" s="17">
+        <v>2</v>
+      </c>
+      <c r="E79" s="31"/>
+    </row>
+    <row r="80" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D80" s="17">
+        <v>2</v>
+      </c>
+      <c r="E80" s="31"/>
+    </row>
+    <row r="81" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C81" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D81" s="17">
+        <v>2</v>
+      </c>
+      <c r="E81" s="31"/>
+    </row>
+    <row r="82" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D82" s="17">
+        <v>2</v>
+      </c>
+      <c r="E82" s="31"/>
+    </row>
+    <row r="83" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D83" s="17">
+        <v>2</v>
+      </c>
+      <c r="E83" s="31"/>
+    </row>
+    <row r="84" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C76" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D76" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C77" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D77" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C78" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D78" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C79" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D79" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C80" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D80" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C81" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D81" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="B82" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C82" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D82" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+      <c r="C84" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D84" s="17">
+        <v>2</v>
+      </c>
+      <c r="E84" s="31"/>
+    </row>
+    <row r="85" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C83" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D83" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+      <c r="C85" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D85" s="17">
+        <v>2</v>
+      </c>
+      <c r="E85" s="31"/>
+    </row>
+    <row r="86" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C84" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D84" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
+      <c r="C86" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D86" s="17">
+        <v>2</v>
+      </c>
+      <c r="E86" s="31"/>
+    </row>
+    <row r="87" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C85" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D85" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
+      <c r="C87" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D87" s="17">
+        <v>2</v>
+      </c>
+      <c r="E87" s="31"/>
+    </row>
+    <row r="88" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D86" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D87" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>226</v>
       </c>
       <c r="D88" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E88" s="31"/>
+    </row>
+    <row r="89" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>226</v>
       </c>
       <c r="D89" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E89" s="31"/>
+    </row>
+    <row r="90" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D90" s="16">
+        <v>3</v>
+      </c>
+      <c r="E90" s="31"/>
+    </row>
+    <row r="91" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D91" s="16">
+        <v>2</v>
+      </c>
+      <c r="E91" s="31"/>
+    </row>
+    <row r="92" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C90" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D90" s="16">
+      <c r="C92" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D92" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A91" s="11" t="s">
+      <c r="E92" s="31"/>
+    </row>
+    <row r="93" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C91" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D91" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D92" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>176</v>
+      <c r="C93" s="21">
+        <v>43641</v>
       </c>
       <c r="D93" s="16">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E93" s="31"/>
+    </row>
+    <row r="94" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D94" s="16">
+        <v>2</v>
+      </c>
+      <c r="E94" s="31"/>
+    </row>
+    <row r="95" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A95" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D95" s="16">
+        <v>3</v>
+      </c>
+      <c r="E95" s="31"/>
+    </row>
+    <row r="96" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C94" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D94" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="11" t="s">
+      <c r="C96" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D96" s="20">
+        <v>2</v>
+      </c>
+      <c r="E96" s="31"/>
+    </row>
+    <row r="97" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C95" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D95" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
+      <c r="C97" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D97" s="20">
+        <v>2</v>
+      </c>
+      <c r="E97" s="31"/>
+    </row>
+    <row r="98" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A98" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C96" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D96" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
+      <c r="C98" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D98" s="20">
+        <v>2</v>
+      </c>
+      <c r="E98" s="31"/>
+    </row>
+    <row r="99" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C97" s="15" t="s">
+      <c r="C99" s="15" t="s">
         <v>226</v>
-      </c>
-      <c r="D97" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A98" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D98" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>141</v>
       </c>
       <c r="D99" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E99" s="31" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>237</v>
+        <v>30</v>
       </c>
       <c r="C100" s="15" t="s">
         <v>226</v>
@@ -2918,181 +3132,208 @@
       <c r="D100" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E100" s="31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>238</v>
+        <v>31</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>226</v>
+        <v>141</v>
       </c>
       <c r="D101" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E101" s="31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D102" s="16">
+        <v>1</v>
+      </c>
+      <c r="E102" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D103" s="16">
+        <v>1</v>
+      </c>
+      <c r="E103" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="15" t="s">
+      <c r="C104" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="D102" s="16">
+      <c r="D104" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
+      <c r="E104" s="31" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A105" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C103" s="15" t="s">
+      <c r="C105" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="D103" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A104" s="11" t="s">
+      <c r="D105" s="16">
+        <v>2</v>
+      </c>
+      <c r="E105" s="31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A106" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C104" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="D104" s="16">
+      <c r="C106" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D106" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A105" s="11" t="s">
+      <c r="E106" s="31" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A107" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C105" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D105" s="16">
+      <c r="C107" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D107" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A106" s="11" t="s">
+      <c r="E107" s="31"/>
+    </row>
+    <row r="108" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A108" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C106" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D106" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A107" s="11" t="s">
+      <c r="C108" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D108" s="17">
+        <v>2</v>
+      </c>
+      <c r="E108" s="31"/>
+    </row>
+    <row r="109" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A109" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C107" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D107" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A108" s="11" t="s">
+      <c r="C109" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D109" s="17">
+        <v>2</v>
+      </c>
+      <c r="E109" s="31"/>
+    </row>
+    <row r="110" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A110" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C108" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D108" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
+      <c r="C110" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D110" s="17">
+        <v>2</v>
+      </c>
+      <c r="E110" s="31"/>
+    </row>
+    <row r="111" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A111" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C109" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D109" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A110" s="11" t="s">
+      <c r="C111" s="21">
+        <v>43641</v>
+      </c>
+      <c r="D111" s="17">
+        <v>2</v>
+      </c>
+      <c r="E111" s="31"/>
+    </row>
+    <row r="112" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A112" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C110" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D110" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C111" s="21">
-        <v>43641</v>
-      </c>
-      <c r="D111" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A112" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="C112" s="21">
         <v>43641</v>
       </c>
       <c r="D112" s="17">
         <v>2</v>
       </c>
+      <c r="E112" s="31"/>
     </row>
     <row r="113" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C113" s="21">
         <v>43641</v>
@@ -3100,41 +3341,44 @@
       <c r="D113" s="17">
         <v>2</v>
       </c>
+      <c r="E113" s="31"/>
     </row>
     <row r="114" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="C114" s="21">
-        <v>43712</v>
+        <v>43641</v>
       </c>
       <c r="D114" s="17">
         <v>2</v>
       </c>
+      <c r="E114" s="31"/>
     </row>
     <row r="115" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="C115" s="21">
-        <v>43712</v>
+        <v>43641</v>
       </c>
       <c r="D115" s="17">
         <v>2</v>
       </c>
+      <c r="E115" s="31"/>
     </row>
     <row r="116" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C116" s="21">
         <v>43712</v>
@@ -3142,13 +3386,14 @@
       <c r="D116" s="17">
         <v>2</v>
       </c>
+      <c r="E116" s="31"/>
     </row>
     <row r="117" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C117" s="21">
         <v>43712</v>
@@ -3156,13 +3401,14 @@
       <c r="D117" s="17">
         <v>2</v>
       </c>
+      <c r="E117" s="31"/>
     </row>
     <row r="118" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C118" s="21">
         <v>43712</v>
@@ -3170,13 +3416,14 @@
       <c r="D118" s="17">
         <v>2</v>
       </c>
+      <c r="E118" s="31"/>
     </row>
     <row r="119" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C119" s="21">
         <v>43712</v>
@@ -3184,13 +3431,14 @@
       <c r="D119" s="17">
         <v>2</v>
       </c>
+      <c r="E119" s="31"/>
     </row>
     <row r="120" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C120" s="21">
         <v>43712</v>
@@ -3198,55 +3446,86 @@
       <c r="D120" s="17">
         <v>2</v>
       </c>
+      <c r="E120" s="31"/>
     </row>
     <row r="121" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C121" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D121" s="17">
+        <v>2</v>
+      </c>
+      <c r="E121" s="31"/>
+    </row>
+    <row r="122" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A122" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C122" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D122" s="17">
+        <v>2</v>
+      </c>
+      <c r="E122" s="31"/>
+    </row>
+    <row r="123" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A123" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C121" s="21">
-        <v>43712</v>
-      </c>
-      <c r="D121" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="23" t="s">
+      <c r="C123" s="21">
+        <v>43712</v>
+      </c>
+      <c r="D123" s="17">
+        <v>2</v>
+      </c>
+      <c r="E123" s="31"/>
+    </row>
+    <row r="124" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B124" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C122" s="22">
-        <v>43712</v>
-      </c>
-      <c r="D122" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="7"/>
-      <c r="B123" s="8"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="9"/>
-      <c r="B124" s="9"/>
-      <c r="C124" s="9"/>
-      <c r="D124" s="9"/>
+      <c r="C124" s="22">
+        <v>43712</v>
+      </c>
+      <c r="D124" s="17">
+        <v>2</v>
+      </c>
+      <c r="E124" s="31"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="9"/>
-      <c r="B125" s="9"/>
-      <c r="C125" s="9"/>
-      <c r="D125" s="9"/>
+      <c r="A125" s="7"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="8"/>
+      <c r="D125" s="8"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="9"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
       <c r="E126" s="12"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="9"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
     </row>
     <row r="128" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="130" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Recursos asignados al gantt, cambios en la tabla de actividades y tabla de recursos. Gantt sin holgura agregada
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\proyectofinal2019\Actividades\Proy01005\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02EF76-890C-4D7F-963E-3388C7F08868}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="17115" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{0447A3F1-1398-4D39-88F7-8434CE3DAECB}"/>
+    <workbookView xWindow="17115" yWindow="1275" windowWidth="19440" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="268">
   <si>
     <t>Nombre</t>
   </si>
@@ -476,9 +470,6 @@
     <t>Taller01008</t>
   </si>
   <si>
-    <t>ADA02007</t>
-  </si>
-  <si>
     <t>ADA02008</t>
   </si>
   <si>
@@ -593,9 +584,6 @@
     <t>Taller02017</t>
   </si>
   <si>
-    <t>ADA03012</t>
-  </si>
-  <si>
     <t>ADA03013</t>
   </si>
   <si>
@@ -779,33 +767,12 @@
     <t xml:space="preserve">Asignado </t>
   </si>
   <si>
-    <t xml:space="preserve">Asisgnado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asisgado </t>
-  </si>
-  <si>
-    <t>Realizado</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sin asignar </t>
   </si>
   <si>
     <t xml:space="preserve">Realizado constantemente </t>
   </si>
   <si>
-    <t xml:space="preserve">realizado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">realizado constantemente </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asigando </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asigado  </t>
-  </si>
-  <si>
     <t xml:space="preserve">sin asisgnar </t>
   </si>
   <si>
@@ -816,12 +783,57 @@
   </si>
   <si>
     <t>P[02],S[02],T[04],E[05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asignado  </t>
+  </si>
+  <si>
+    <t>Asignado</t>
+  </si>
+  <si>
+    <t>P[03],S[01],T[03],E[03]</t>
+  </si>
+  <si>
+    <t>P[03],S[01],T[03],E[02]</t>
+  </si>
+  <si>
+    <t>P[02],S[01],T[04],E[05]</t>
+  </si>
+  <si>
+    <t>P[01],S[02],T[02],E[04]</t>
+  </si>
+  <si>
+    <t>P[04],S[05],T[01],E[02]</t>
+  </si>
+  <si>
+    <t>P[01],S[11],T[02],E[04]</t>
+  </si>
+  <si>
+    <t>P[01],S[13],T[02],E[04]</t>
+  </si>
+  <si>
+    <t>ADA01007</t>
+  </si>
+  <si>
+    <t>ADA02012</t>
+  </si>
+  <si>
+    <t>ADA03021</t>
+  </si>
+  <si>
+    <t>ADA03022</t>
+  </si>
+  <si>
+    <t>P[04],S[09],T[01],E[02]</t>
+  </si>
+  <si>
+    <t>P[04],S[06],T[01],E[02]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -1173,15 +1185,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1209,9 +1212,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,7 +1266,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1332,7 +1344,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1384,7 +1396,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1578,18 +1590,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30076E1-59D8-4123-BE7D-68CF91B16748}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1603,71 +1615,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="114" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
+      <c r="A2" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A2" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>243</v>
+      <c r="E2" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="26">
         <v>4</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="F3" s="31"/>
+      <c r="E3" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>260</v>
+        <v>245</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75">
@@ -1678,16 +1690,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D5" s="6">
         <v>6</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>261</v>
+        <v>246</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75">
@@ -1704,16 +1716,18 @@
         <v>15</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="F6" s="23"/>
+        <v>246</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="18.75">
       <c r="A7" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>111</v>
@@ -1722,16 +1736,18 @@
         <v>2</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="1:6" ht="26.25" customHeight="1">
+        <v>246</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>111</v>
@@ -1740,16 +1756,16 @@
         <v>5</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F8" s="23"/>
+        <v>244</v>
+      </c>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="4" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>111</v>
@@ -1758,9 +1774,9 @@
         <v>3</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F9" s="23"/>
+        <v>244</v>
+      </c>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="4" t="s">
@@ -1776,11 +1792,11 @@
         <v>2</v>
       </c>
       <c r="E10" s="15"/>
-      <c r="F10" s="23"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>36</v>
@@ -1792,11 +1808,11 @@
         <v>2</v>
       </c>
       <c r="E11" s="15"/>
-      <c r="F11" s="23"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
@@ -1808,11 +1824,11 @@
         <v>2</v>
       </c>
       <c r="E12" s="15"/>
-      <c r="F12" s="23"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="18.75">
       <c r="A13" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>38</v>
@@ -1824,11 +1840,11 @@
         <v>2</v>
       </c>
       <c r="E13" s="15"/>
-      <c r="F13" s="23"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" ht="18.75">
       <c r="A14" s="4" t="s">
-        <v>151</v>
+        <v>263</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
@@ -1840,11 +1856,11 @@
         <v>2</v>
       </c>
       <c r="E14" s="15"/>
-      <c r="F14" s="23"/>
+      <c r="F14" s="20"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="A15" s="4" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>40</v>
@@ -1856,7 +1872,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="15"/>
-      <c r="F15" s="23"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" ht="18.75">
       <c r="A16" s="4" t="s">
@@ -1872,7 +1888,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="15"/>
-      <c r="F16" s="23"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6" ht="18.75">
       <c r="A17" s="4" t="s">
@@ -1888,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="15"/>
-      <c r="F17" s="23"/>
+      <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:6" ht="18.75">
       <c r="A18" s="4" t="s">
@@ -1904,7 +1920,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="15"/>
-      <c r="F18" s="23"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" ht="18.75">
       <c r="A19" s="4" t="s">
@@ -1920,7 +1936,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="15"/>
-      <c r="F19" s="23"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" ht="18.75">
       <c r="A20" s="4" t="s">
@@ -1936,7 +1952,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="15"/>
-      <c r="F20" s="23"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:6" ht="18.75">
       <c r="A21" s="4" t="s">
@@ -1952,7 +1968,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="15"/>
-      <c r="F21" s="23"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="4" t="s">
@@ -1968,11 +1984,11 @@
         <v>2</v>
       </c>
       <c r="E22" s="15"/>
-      <c r="F22" s="23"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>194</v>
+        <v>264</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>79</v>
@@ -1984,11 +2000,11 @@
         <v>2</v>
       </c>
       <c r="E23" s="15"/>
-      <c r="F23" s="23"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:6" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>195</v>
+        <v>265</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>80</v>
@@ -2000,14 +2016,14 @@
         <v>2</v>
       </c>
       <c r="E24" s="15"/>
-      <c r="F24" s="23"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>111</v>
@@ -2016,9 +2032,11 @@
         <v>8</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="F25" s="23"/>
+        <v>246</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="18.75">
       <c r="A26" s="4" t="s">
@@ -2028,15 +2046,15 @@
         <v>4</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D26" s="6">
         <v>3</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F26" s="23"/>
+        <v>244</v>
+      </c>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" ht="18.75">
       <c r="A27" s="4" t="s">
@@ -2046,15 +2064,15 @@
         <v>5</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F27" s="23"/>
+        <v>244</v>
+      </c>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" ht="18.75">
       <c r="A28" s="4" t="s">
@@ -2070,9 +2088,9 @@
         <v>1</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F28" s="23"/>
+        <v>244</v>
+      </c>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" ht="18.75">
       <c r="A29" s="4" t="s">
@@ -2082,15 +2100,15 @@
         <v>7</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D29" s="6">
         <v>2</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F29" s="23"/>
+        <v>244</v>
+      </c>
+      <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" ht="18.75">
       <c r="A30" s="4" t="s">
@@ -2106,13 +2124,13 @@
         <v>1</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F30" s="23"/>
+        <v>244</v>
+      </c>
+      <c r="F30" s="20"/>
     </row>
     <row r="31" spans="1:6" ht="18.75">
       <c r="A31" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>41</v>
@@ -2124,11 +2142,11 @@
         <v>2</v>
       </c>
       <c r="E31" s="15"/>
-      <c r="F31" s="23"/>
+      <c r="F31" s="20"/>
     </row>
     <row r="32" spans="1:6" ht="18.75">
       <c r="A32" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>42</v>
@@ -2140,11 +2158,11 @@
         <v>2</v>
       </c>
       <c r="E32" s="15"/>
-      <c r="F32" s="23"/>
+      <c r="F32" s="20"/>
     </row>
     <row r="33" spans="1:6" ht="18.75">
       <c r="A33" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>43</v>
@@ -2156,11 +2174,11 @@
         <v>2</v>
       </c>
       <c r="E33" s="15"/>
-      <c r="F33" s="23"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="1:6" ht="18.75">
       <c r="A34" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>44</v>
@@ -2172,11 +2190,11 @@
         <v>2</v>
       </c>
       <c r="E34" s="15"/>
-      <c r="F34" s="23"/>
+      <c r="F34" s="20"/>
     </row>
     <row r="35" spans="1:6" ht="18.75">
       <c r="A35" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>45</v>
@@ -2188,11 +2206,11 @@
         <v>2</v>
       </c>
       <c r="E35" s="15"/>
-      <c r="F35" s="23"/>
+      <c r="F35" s="20"/>
     </row>
     <row r="36" spans="1:6" ht="18.75">
       <c r="A36" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>46</v>
@@ -2204,14 +2222,14 @@
         <v>2</v>
       </c>
       <c r="E36" s="15"/>
-      <c r="F36" s="23"/>
+      <c r="F36" s="20"/>
     </row>
     <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C37" s="8">
         <v>43641</v>
@@ -2220,11 +2238,11 @@
         <v>2</v>
       </c>
       <c r="E37" s="15"/>
-      <c r="F37" s="23"/>
+      <c r="F37" s="20"/>
     </row>
     <row r="38" spans="1:6" ht="18.75">
       <c r="A38" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>81</v>
@@ -2236,11 +2254,11 @@
         <v>2</v>
       </c>
       <c r="E38" s="15"/>
-      <c r="F38" s="23"/>
+      <c r="F38" s="20"/>
     </row>
     <row r="39" spans="1:6" ht="18.75">
       <c r="A39" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>82</v>
@@ -2252,11 +2270,11 @@
         <v>2</v>
       </c>
       <c r="E39" s="15"/>
-      <c r="F39" s="23"/>
+      <c r="F39" s="20"/>
     </row>
     <row r="40" spans="1:6" ht="18.75">
       <c r="A40" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>83</v>
@@ -2268,11 +2286,11 @@
         <v>2</v>
       </c>
       <c r="E40" s="15"/>
-      <c r="F40" s="23"/>
+      <c r="F40" s="20"/>
     </row>
     <row r="41" spans="1:6" ht="18.75">
       <c r="A41" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>84</v>
@@ -2284,7 +2302,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="15"/>
-      <c r="F41" s="23"/>
+      <c r="F41" s="20"/>
     </row>
     <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="4" t="s">
@@ -2294,15 +2312,17 @@
         <v>9</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D42" s="16">
         <v>1</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F42" s="23"/>
+        <v>245</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="18.75">
       <c r="A43" s="4" t="s">
@@ -2312,19 +2332,19 @@
         <v>10</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D43" s="6">
         <v>13</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F43" s="23"/>
+        <v>244</v>
+      </c>
+      <c r="F43" s="20"/>
     </row>
     <row r="44" spans="1:6" ht="18.75">
       <c r="A44" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>47</v>
@@ -2336,11 +2356,11 @@
         <v>4</v>
       </c>
       <c r="E44" s="15"/>
-      <c r="F44" s="23"/>
+      <c r="F44" s="20"/>
     </row>
     <row r="45" spans="1:6" ht="18.75">
       <c r="A45" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>48</v>
@@ -2352,11 +2372,11 @@
         <v>8</v>
       </c>
       <c r="E45" s="15"/>
-      <c r="F45" s="23"/>
+      <c r="F45" s="20"/>
     </row>
     <row r="46" spans="1:6" ht="18.75">
       <c r="A46" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>49</v>
@@ -2368,11 +2388,11 @@
         <v>8</v>
       </c>
       <c r="E46" s="15"/>
-      <c r="F46" s="23"/>
+      <c r="F46" s="20"/>
     </row>
     <row r="47" spans="1:6" ht="18.75">
       <c r="A47" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>50</v>
@@ -2384,11 +2404,11 @@
         <v>2</v>
       </c>
       <c r="E47" s="15"/>
-      <c r="F47" s="23"/>
+      <c r="F47" s="20"/>
     </row>
     <row r="48" spans="1:6" ht="18.75">
       <c r="A48" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>85</v>
@@ -2400,11 +2420,11 @@
         <v>4</v>
       </c>
       <c r="E48" s="15"/>
-      <c r="F48" s="23"/>
+      <c r="F48" s="20"/>
     </row>
     <row r="49" spans="1:6" ht="18.75">
       <c r="A49" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>86</v>
@@ -2416,11 +2436,11 @@
         <v>2</v>
       </c>
       <c r="E49" s="15"/>
-      <c r="F49" s="23"/>
+      <c r="F49" s="20"/>
     </row>
     <row r="50" spans="1:6" ht="18.75">
       <c r="A50" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>87</v>
@@ -2432,7 +2452,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="15"/>
-      <c r="F50" s="23"/>
+      <c r="F50" s="20"/>
     </row>
     <row r="51" spans="1:6" ht="18.75">
       <c r="A51" s="4" t="s">
@@ -2442,15 +2462,17 @@
         <v>11</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D51" s="6">
         <v>1</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F51" s="23"/>
+        <v>245</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="18.75">
       <c r="A52" s="4" t="s">
@@ -2460,15 +2482,17 @@
         <v>12</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D52" s="6">
         <v>1</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F52" s="23"/>
+        <v>245</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="18.75">
       <c r="A53" s="4" t="s">
@@ -2478,15 +2502,15 @@
         <v>13</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D53" s="6">
         <v>4</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="F53" s="23"/>
+        <v>247</v>
+      </c>
+      <c r="F53" s="20"/>
     </row>
     <row r="54" spans="1:6" ht="18.75">
       <c r="A54" s="4" t="s">
@@ -2496,15 +2520,17 @@
         <v>15</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D54" s="7">
         <v>1</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="F54" s="23"/>
+        <v>248</v>
+      </c>
+      <c r="F54" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="18.75">
       <c r="A55" s="4" t="s">
@@ -2514,15 +2540,17 @@
         <v>14</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D55" s="6">
         <v>1</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="F55" s="23"/>
+        <v>248</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="18.75">
       <c r="A56" s="4" t="s">
@@ -2532,15 +2560,17 @@
         <v>16</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D56" s="6">
         <v>1</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="F56" s="23"/>
+        <v>246</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="18.75">
       <c r="A57" s="4" t="s">
@@ -2556,9 +2586,11 @@
         <v>1</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="F57" s="23"/>
+        <v>248</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="18.75">
       <c r="A58" s="4" t="s">
@@ -2574,13 +2606,15 @@
         <v>2</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="F58" s="23"/>
+        <v>253</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="18.75">
       <c r="A59" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>51</v>
@@ -2592,11 +2626,11 @@
         <v>2</v>
       </c>
       <c r="E59" s="15"/>
-      <c r="F59" s="23"/>
+      <c r="F59" s="20"/>
     </row>
     <row r="60" spans="1:6" ht="18.75">
       <c r="A60" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>52</v>
@@ -2608,11 +2642,11 @@
         <v>2</v>
       </c>
       <c r="E60" s="15"/>
-      <c r="F60" s="23"/>
+      <c r="F60" s="20"/>
     </row>
     <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>53</v>
@@ -2624,11 +2658,11 @@
         <v>2</v>
       </c>
       <c r="E61" s="15"/>
-      <c r="F61" s="23"/>
+      <c r="F61" s="20"/>
     </row>
     <row r="62" spans="1:6" ht="18.75">
       <c r="A62" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>14</v>
@@ -2640,11 +2674,11 @@
         <v>1</v>
       </c>
       <c r="E62" s="15"/>
-      <c r="F62" s="23"/>
+      <c r="F62" s="20"/>
     </row>
     <row r="63" spans="1:6" ht="18.75">
       <c r="A63" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>16</v>
@@ -2656,43 +2690,43 @@
         <v>1</v>
       </c>
       <c r="E63" s="15"/>
-      <c r="F63" s="23"/>
+      <c r="F63" s="20"/>
     </row>
     <row r="64" spans="1:6" ht="18.75">
       <c r="A64" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D64" s="16">
         <v>3</v>
       </c>
       <c r="E64" s="15"/>
-      <c r="F64" s="23"/>
+      <c r="F64" s="20"/>
     </row>
     <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D65" s="16">
         <v>1</v>
       </c>
       <c r="E65" s="15"/>
-      <c r="F65" s="23"/>
+      <c r="F65" s="20"/>
     </row>
     <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>14</v>
@@ -2704,11 +2738,11 @@
         <v>1</v>
       </c>
       <c r="E66" s="15"/>
-      <c r="F66" s="23"/>
+      <c r="F66" s="20"/>
     </row>
     <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>16</v>
@@ -2720,43 +2754,43 @@
         <v>1</v>
       </c>
       <c r="E67" s="15"/>
-      <c r="F67" s="23"/>
+      <c r="F67" s="20"/>
     </row>
     <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D68" s="6">
         <v>1</v>
       </c>
       <c r="E68" s="15"/>
-      <c r="F68" s="23"/>
+      <c r="F68" s="20"/>
     </row>
     <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D69" s="6">
         <v>3</v>
       </c>
       <c r="E69" s="15"/>
-      <c r="F69" s="23"/>
+      <c r="F69" s="20"/>
     </row>
     <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>90</v>
@@ -2768,11 +2802,11 @@
         <v>2</v>
       </c>
       <c r="E70" s="15"/>
-      <c r="F70" s="23"/>
+      <c r="F70" s="20"/>
     </row>
     <row r="71" spans="1:6" ht="18.75">
       <c r="A71" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>91</v>
@@ -2784,7 +2818,7 @@
         <v>2</v>
       </c>
       <c r="E71" s="15"/>
-      <c r="F71" s="23"/>
+      <c r="F71" s="20"/>
     </row>
     <row r="72" spans="1:6" ht="18.75">
       <c r="A72" s="4" t="s">
@@ -2794,15 +2828,17 @@
         <v>19</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D72" s="6">
         <v>1</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="F72" s="23"/>
+        <v>245</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="73" spans="1:6" ht="18.75">
       <c r="A73" s="4" t="s">
@@ -2818,9 +2854,11 @@
         <v>6</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="F73" s="23"/>
+        <v>254</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="74" spans="1:6" ht="18.75">
       <c r="A74" s="4" t="s">
@@ -2830,15 +2868,17 @@
         <v>21</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D74" s="6">
         <v>1</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F74" s="23"/>
+        <v>245</v>
+      </c>
+      <c r="F74" s="20" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="18.75">
       <c r="A75" s="4" t="s">
@@ -2848,15 +2888,17 @@
         <v>23</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D75" s="6">
         <v>1</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="F75" s="23"/>
+        <v>245</v>
+      </c>
+      <c r="F75" s="20" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="76" spans="1:6" ht="18.75">
       <c r="A76" s="4" t="s">
@@ -2866,15 +2908,17 @@
         <v>22</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D76" s="6">
         <v>4</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="F76" s="23"/>
+        <v>254</v>
+      </c>
+      <c r="F76" s="20" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="77" spans="1:6" ht="18.75">
       <c r="A77" s="4" t="s">
@@ -2884,19 +2928,19 @@
         <v>24</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D77" s="6">
         <v>1</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="F77" s="23"/>
+        <v>249</v>
+      </c>
+      <c r="F77" s="20"/>
     </row>
     <row r="78" spans="1:6" ht="18.75">
       <c r="A78" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>54</v>
@@ -2908,11 +2952,11 @@
         <v>1</v>
       </c>
       <c r="E78" s="15"/>
-      <c r="F78" s="23"/>
+      <c r="F78" s="20"/>
     </row>
     <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>55</v>
@@ -2924,11 +2968,11 @@
         <v>2</v>
       </c>
       <c r="E79" s="15"/>
-      <c r="F79" s="23"/>
+      <c r="F79" s="20"/>
     </row>
     <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>56</v>
@@ -2940,11 +2984,11 @@
         <v>2</v>
       </c>
       <c r="E80" s="15"/>
-      <c r="F80" s="23"/>
+      <c r="F80" s="20"/>
     </row>
     <row r="81" spans="1:6" ht="18.75">
       <c r="A81" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>57</v>
@@ -2956,11 +3000,11 @@
         <v>2</v>
       </c>
       <c r="E81" s="15"/>
-      <c r="F81" s="23"/>
+      <c r="F81" s="20"/>
     </row>
     <row r="82" spans="1:6" ht="18.75">
       <c r="A82" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>58</v>
@@ -2972,11 +3016,11 @@
         <v>2</v>
       </c>
       <c r="E82" s="15"/>
-      <c r="F82" s="23"/>
+      <c r="F82" s="20"/>
     </row>
     <row r="83" spans="1:6" ht="18.75">
       <c r="A83" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>92</v>
@@ -2988,11 +3032,11 @@
         <v>2</v>
       </c>
       <c r="E83" s="15"/>
-      <c r="F83" s="23"/>
+      <c r="F83" s="20"/>
     </row>
     <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>93</v>
@@ -3004,11 +3048,11 @@
         <v>2</v>
       </c>
       <c r="E84" s="15"/>
-      <c r="F84" s="23"/>
+      <c r="F84" s="20"/>
     </row>
     <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>94</v>
@@ -3020,11 +3064,11 @@
         <v>2</v>
       </c>
       <c r="E85" s="15"/>
-      <c r="F85" s="23"/>
+      <c r="F85" s="20"/>
     </row>
     <row r="86" spans="1:6" ht="18.75">
       <c r="A86" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>95</v>
@@ -3036,11 +3080,11 @@
         <v>2</v>
       </c>
       <c r="E86" s="15"/>
-      <c r="F86" s="23"/>
+      <c r="F86" s="20"/>
     </row>
     <row r="87" spans="1:6" ht="18.75">
       <c r="A87" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>96</v>
@@ -3052,7 +3096,7 @@
         <v>2</v>
       </c>
       <c r="E87" s="15"/>
-      <c r="F87" s="23"/>
+      <c r="F87" s="20"/>
     </row>
     <row r="88" spans="1:6" ht="18.75">
       <c r="A88" s="4" t="s">
@@ -3062,13 +3106,13 @@
         <v>25</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D88" s="6">
         <v>1</v>
       </c>
       <c r="E88" s="15"/>
-      <c r="F88" s="23"/>
+      <c r="F88" s="20"/>
     </row>
     <row r="89" spans="1:6" ht="18.75">
       <c r="A89" s="4" t="s">
@@ -3078,13 +3122,13 @@
         <v>26</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D89" s="6">
         <v>1</v>
       </c>
       <c r="E89" s="15"/>
-      <c r="F89" s="23"/>
+      <c r="F89" s="20"/>
     </row>
     <row r="90" spans="1:6" ht="18.75">
       <c r="A90" s="4" t="s">
@@ -3094,13 +3138,13 @@
         <v>27</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D90" s="6">
         <v>3</v>
       </c>
       <c r="E90" s="15"/>
-      <c r="F90" s="23"/>
+      <c r="F90" s="20"/>
     </row>
     <row r="91" spans="1:6" ht="18.75">
       <c r="A91" s="4" t="s">
@@ -3110,17 +3154,17 @@
         <v>28</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D91" s="6">
         <v>2</v>
       </c>
       <c r="E91" s="15"/>
-      <c r="F91" s="23"/>
+      <c r="F91" s="20"/>
     </row>
     <row r="92" spans="1:6" ht="18.75">
       <c r="A92" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>59</v>
@@ -3132,11 +3176,11 @@
         <v>1</v>
       </c>
       <c r="E92" s="15"/>
-      <c r="F92" s="23"/>
+      <c r="F92" s="20"/>
     </row>
     <row r="93" spans="1:6" ht="18.75">
       <c r="A93" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>60</v>
@@ -3148,43 +3192,43 @@
         <v>3</v>
       </c>
       <c r="E93" s="15"/>
-      <c r="F93" s="23"/>
+      <c r="F93" s="20"/>
     </row>
     <row r="94" spans="1:6" ht="18.75">
       <c r="A94" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D94" s="6">
         <v>2</v>
       </c>
       <c r="E94" s="15"/>
-      <c r="F94" s="23"/>
+      <c r="F94" s="20"/>
     </row>
     <row r="95" spans="1:6" ht="18.75">
       <c r="A95" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D95" s="6">
         <v>3</v>
       </c>
       <c r="E95" s="15"/>
-      <c r="F95" s="23"/>
+      <c r="F95" s="20"/>
     </row>
     <row r="96" spans="1:6" ht="18.75">
       <c r="A96" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>97</v>
@@ -3196,11 +3240,11 @@
         <v>2</v>
       </c>
       <c r="E96" s="15"/>
-      <c r="F96" s="23"/>
+      <c r="F96" s="20"/>
     </row>
     <row r="97" spans="1:6" ht="18.75">
       <c r="A97" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>98</v>
@@ -3212,11 +3256,11 @@
         <v>2</v>
       </c>
       <c r="E97" s="15"/>
-      <c r="F97" s="23"/>
+      <c r="F97" s="20"/>
     </row>
     <row r="98" spans="1:6" ht="18.75">
       <c r="A98" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>139</v>
@@ -3228,7 +3272,7 @@
         <v>2</v>
       </c>
       <c r="E98" s="15"/>
-      <c r="F98" s="23"/>
+      <c r="F98" s="20"/>
     </row>
     <row r="99" spans="1:6" ht="18.75">
       <c r="A99" s="4" t="s">
@@ -3238,15 +3282,17 @@
         <v>29</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D99" s="6">
         <v>5</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="F99" s="23"/>
+        <v>246</v>
+      </c>
+      <c r="F99" s="20" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="100" spans="1:6" ht="18.75">
       <c r="A100" s="4" t="s">
@@ -3256,15 +3302,17 @@
         <v>30</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D100" s="6">
         <v>5</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="F100" s="23"/>
+        <v>254</v>
+      </c>
+      <c r="F100" s="20" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="101" spans="1:6" ht="18.75">
       <c r="A101" s="4" t="s">
@@ -3280,45 +3328,51 @@
         <v>5</v>
       </c>
       <c r="E101" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="F101" s="23"/>
+        <v>254</v>
+      </c>
+      <c r="F101" s="20" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="102" spans="1:6" ht="18.75">
       <c r="A102" s="4" t="s">
         <v>143</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D102" s="6">
         <v>1</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F102" s="23"/>
+        <v>245</v>
+      </c>
+      <c r="F102" s="20" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="103" spans="1:6" ht="18.75">
       <c r="A103" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D103" s="6">
         <v>1</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F103" s="23"/>
+        <v>245</v>
+      </c>
+      <c r="F103" s="20" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="104" spans="1:6" ht="18.75">
       <c r="A104" s="4" t="s">
@@ -3334,9 +3388,11 @@
         <v>6</v>
       </c>
       <c r="E104" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="F104" s="23"/>
+        <v>254</v>
+      </c>
+      <c r="F104" s="20" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="105" spans="1:6" ht="18.75">
       <c r="A105" s="4" t="s">
@@ -3352,9 +3408,11 @@
         <v>2</v>
       </c>
       <c r="E105" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="F105" s="23"/>
+        <v>254</v>
+      </c>
+      <c r="F105" s="20" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="18.75">
       <c r="A106" s="4" t="s">
@@ -3364,19 +3422,19 @@
         <v>34</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D106" s="6">
         <v>2</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="F106" s="23"/>
+        <v>250</v>
+      </c>
+      <c r="F106" s="20"/>
     </row>
     <row r="107" spans="1:6" ht="18.75">
       <c r="A107" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>63</v>
@@ -3388,11 +3446,11 @@
         <v>4</v>
       </c>
       <c r="E107" s="15"/>
-      <c r="F107" s="23"/>
+      <c r="F107" s="20"/>
     </row>
     <row r="108" spans="1:6" ht="18.75">
       <c r="A108" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>64</v>
@@ -3404,11 +3462,11 @@
         <v>2</v>
       </c>
       <c r="E108" s="15"/>
-      <c r="F108" s="23"/>
+      <c r="F108" s="20"/>
     </row>
     <row r="109" spans="1:6" ht="18.75">
       <c r="A109" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>65</v>
@@ -3420,11 +3478,11 @@
         <v>2</v>
       </c>
       <c r="E109" s="15"/>
-      <c r="F109" s="23"/>
+      <c r="F109" s="20"/>
     </row>
     <row r="110" spans="1:6" ht="18.75">
       <c r="A110" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>66</v>
@@ -3436,11 +3494,11 @@
         <v>2</v>
       </c>
       <c r="E110" s="15"/>
-      <c r="F110" s="23"/>
+      <c r="F110" s="20"/>
     </row>
     <row r="111" spans="1:6" ht="18.75">
       <c r="A111" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>67</v>
@@ -3452,11 +3510,11 @@
         <v>2</v>
       </c>
       <c r="E111" s="15"/>
-      <c r="F111" s="23"/>
+      <c r="F111" s="20"/>
     </row>
     <row r="112" spans="1:6" ht="18.75">
       <c r="A112" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>68</v>
@@ -3468,11 +3526,11 @@
         <v>2</v>
       </c>
       <c r="E112" s="15"/>
-      <c r="F112" s="23"/>
+      <c r="F112" s="20"/>
     </row>
     <row r="113" spans="1:6" ht="18.75">
       <c r="A113" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>69</v>
@@ -3484,11 +3542,11 @@
         <v>2</v>
       </c>
       <c r="E113" s="15"/>
-      <c r="F113" s="23"/>
+      <c r="F113" s="20"/>
     </row>
     <row r="114" spans="1:6" ht="18.75">
       <c r="A114" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>70</v>
@@ -3500,11 +3558,11 @@
         <v>2</v>
       </c>
       <c r="E114" s="15"/>
-      <c r="F114" s="23"/>
+      <c r="F114" s="20"/>
     </row>
     <row r="115" spans="1:6" ht="18.75">
       <c r="A115" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>71</v>
@@ -3516,11 +3574,11 @@
         <v>2</v>
       </c>
       <c r="E115" s="15"/>
-      <c r="F115" s="23"/>
+      <c r="F115" s="20"/>
     </row>
     <row r="116" spans="1:6" ht="18.75">
       <c r="A116" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>99</v>
@@ -3532,11 +3590,11 @@
         <v>2</v>
       </c>
       <c r="E116" s="15"/>
-      <c r="F116" s="23"/>
+      <c r="F116" s="20"/>
     </row>
     <row r="117" spans="1:6" ht="18.75">
       <c r="A117" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>100</v>
@@ -3548,11 +3606,11 @@
         <v>2</v>
       </c>
       <c r="E117" s="15"/>
-      <c r="F117" s="23"/>
+      <c r="F117" s="20"/>
     </row>
     <row r="118" spans="1:6" ht="18.75">
       <c r="A118" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>101</v>
@@ -3564,11 +3622,11 @@
         <v>2</v>
       </c>
       <c r="E118" s="15"/>
-      <c r="F118" s="23"/>
+      <c r="F118" s="20"/>
     </row>
     <row r="119" spans="1:6" ht="18.75">
       <c r="A119" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>102</v>
@@ -3580,11 +3638,11 @@
         <v>2</v>
       </c>
       <c r="E119" s="15"/>
-      <c r="F119" s="23"/>
+      <c r="F119" s="20"/>
     </row>
     <row r="120" spans="1:6" ht="18.75">
       <c r="A120" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>103</v>
@@ -3596,11 +3654,11 @@
         <v>2</v>
       </c>
       <c r="E120" s="15"/>
-      <c r="F120" s="23"/>
+      <c r="F120" s="20"/>
     </row>
     <row r="121" spans="1:6" ht="18.75">
       <c r="A121" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>104</v>
@@ -3612,11 +3670,11 @@
         <v>2</v>
       </c>
       <c r="E121" s="15"/>
-      <c r="F121" s="23"/>
+      <c r="F121" s="20"/>
     </row>
     <row r="122" spans="1:6" ht="18.75">
       <c r="A122" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>105</v>
@@ -3628,11 +3686,11 @@
         <v>2</v>
       </c>
       <c r="E122" s="15"/>
-      <c r="F122" s="23"/>
+      <c r="F122" s="20"/>
     </row>
     <row r="123" spans="1:6" ht="18.75">
       <c r="A123" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>106</v>
@@ -3644,11 +3702,11 @@
         <v>2</v>
       </c>
       <c r="E123" s="15"/>
-      <c r="F123" s="23"/>
+      <c r="F123" s="20"/>
     </row>
     <row r="124" spans="1:6" ht="19.5" thickBot="1">
       <c r="A124" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>107</v>
@@ -3656,11 +3714,11 @@
       <c r="C124" s="9">
         <v>43712</v>
       </c>
-      <c r="D124" s="24">
-        <v>2</v>
-      </c>
-      <c r="E124" s="25"/>
-      <c r="F124" s="26"/>
+      <c r="D124" s="21">
+        <v>2</v>
+      </c>
+      <c r="E124" s="22"/>
+      <c r="F124" s="23"/>
     </row>
     <row r="125" spans="1:6">
       <c r="A125" s="11"/>

</xml_diff>

<commit_message>
Actualizacion en la tabla de actividades y correcion en el PERT
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\proyectofinal2019\Actividades\Proy01005\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032CAC6C-1BEF-495E-9F6B-14E21C82C6B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17115" yWindow="1275" windowWidth="19440" windowHeight="11325"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -785,9 +786,6 @@
     <t>P[02],S[02],T[04],E[05]</t>
   </si>
   <si>
-    <t xml:space="preserve">Asignado  </t>
-  </si>
-  <si>
     <t>Asignado</t>
   </si>
   <si>
@@ -828,13 +826,16 @@
   </si>
   <si>
     <t>P[04],S[06],T[01],E[02]</t>
+  </si>
+  <si>
+    <t>Realizado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1223,7 +1224,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,7 +1267,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1590,21 +1591,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
@@ -1614,7 +1615,7 @@
     <col min="6" max="6" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="114" customHeight="1">
+    <row r="1" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>219</v>
       </c>
@@ -1624,7 +1625,7 @@
       <c r="E1" s="18"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>128</v>
       </c>
@@ -1644,7 +1645,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
+    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>108</v>
       </c>
@@ -1662,7 +1663,7 @@
       </c>
       <c r="F3" s="28"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>109</v>
       </c>
@@ -1682,7 +1683,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
+    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>110</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>111</v>
       </c>
@@ -1715,14 +1716,14 @@
       <c r="D6" s="6">
         <v>15</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>246</v>
+      <c r="E6" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
+    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>112</v>
       </c>
@@ -1739,10 +1740,10 @@
         <v>246</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>238</v>
       </c>
@@ -1760,9 +1761,9 @@
       </c>
       <c r="F8" s="20"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
+    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>239</v>
@@ -1778,7 +1779,7 @@
       </c>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
+    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>148</v>
       </c>
@@ -1794,7 +1795,7 @@
       <c r="E10" s="15"/>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75">
+    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>149</v>
       </c>
@@ -1810,7 +1811,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="20"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75">
+    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>150</v>
       </c>
@@ -1826,7 +1827,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75">
+    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>151</v>
       </c>
@@ -1842,9 +1843,9 @@
       <c r="E13" s="15"/>
       <c r="F13" s="20"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75">
+    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
@@ -1858,7 +1859,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75">
+    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>186</v>
       </c>
@@ -1874,7 +1875,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="20"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75">
+    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>187</v>
       </c>
@@ -1890,7 +1891,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="20"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75">
+    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>188</v>
       </c>
@@ -1906,7 +1907,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="20"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75">
+    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>189</v>
       </c>
@@ -1922,7 +1923,7 @@
       <c r="E18" s="15"/>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75">
+    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>190</v>
       </c>
@@ -1938,7 +1939,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>191</v>
       </c>
@@ -1954,7 +1955,7 @@
       <c r="E20" s="15"/>
       <c r="F20" s="20"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75">
+    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>192</v>
       </c>
@@ -1970,7 +1971,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="20"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75">
+    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>193</v>
       </c>
@@ -1986,9 +1987,9 @@
       <c r="E22" s="15"/>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75">
+    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>79</v>
@@ -2002,9 +2003,9 @@
       <c r="E23" s="15"/>
       <c r="F23" s="20"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75">
+    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>80</v>
@@ -2018,7 +2019,7 @@
       <c r="E24" s="15"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75">
+    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>224</v>
       </c>
@@ -2035,10 +2036,10 @@
         <v>246</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="18.75">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>113</v>
       </c>
@@ -2056,7 +2057,7 @@
       </c>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75">
+    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>114</v>
       </c>
@@ -2074,7 +2075,7 @@
       </c>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75">
+    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>115</v>
       </c>
@@ -2092,7 +2093,7 @@
       </c>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75">
+    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>116</v>
       </c>
@@ -2110,7 +2111,7 @@
       </c>
       <c r="F29" s="20"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75">
+    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>117</v>
       </c>
@@ -2128,7 +2129,7 @@
       </c>
       <c r="F30" s="20"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75">
+    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>152</v>
       </c>
@@ -2144,7 +2145,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="20"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75">
+    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>153</v>
       </c>
@@ -2160,7 +2161,7 @@
       <c r="E32" s="15"/>
       <c r="F32" s="20"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75">
+    <row r="33" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>154</v>
       </c>
@@ -2176,7 +2177,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75">
+    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>155</v>
       </c>
@@ -2192,7 +2193,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75">
+    <row r="35" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>156</v>
       </c>
@@ -2208,7 +2209,7 @@
       <c r="E35" s="15"/>
       <c r="F35" s="20"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75">
+    <row r="36" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>157</v>
       </c>
@@ -2224,7 +2225,7 @@
       <c r="E36" s="15"/>
       <c r="F36" s="20"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75">
+    <row r="37" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>158</v>
       </c>
@@ -2240,7 +2241,7 @@
       <c r="E37" s="15"/>
       <c r="F37" s="20"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75">
+    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>194</v>
       </c>
@@ -2256,7 +2257,7 @@
       <c r="E38" s="15"/>
       <c r="F38" s="20"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75">
+    <row r="39" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>195</v>
       </c>
@@ -2272,7 +2273,7 @@
       <c r="E39" s="15"/>
       <c r="F39" s="20"/>
     </row>
-    <row r="40" spans="1:6" ht="18.75">
+    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>196</v>
       </c>
@@ -2288,7 +2289,7 @@
       <c r="E40" s="15"/>
       <c r="F40" s="20"/>
     </row>
-    <row r="41" spans="1:6" ht="18.75">
+    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>235</v>
       </c>
@@ -2304,7 +2305,7 @@
       <c r="E41" s="15"/>
       <c r="F41" s="20"/>
     </row>
-    <row r="42" spans="1:6" ht="18.75">
+    <row r="42" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>118</v>
       </c>
@@ -2321,10 +2322,10 @@
         <v>245</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>119</v>
       </c>
@@ -2342,7 +2343,7 @@
       </c>
       <c r="F43" s="20"/>
     </row>
-    <row r="44" spans="1:6" ht="18.75">
+    <row r="44" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>159</v>
       </c>
@@ -2358,7 +2359,7 @@
       <c r="E44" s="15"/>
       <c r="F44" s="20"/>
     </row>
-    <row r="45" spans="1:6" ht="18.75">
+    <row r="45" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>160</v>
       </c>
@@ -2374,7 +2375,7 @@
       <c r="E45" s="15"/>
       <c r="F45" s="20"/>
     </row>
-    <row r="46" spans="1:6" ht="18.75">
+    <row r="46" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>161</v>
       </c>
@@ -2390,7 +2391,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="20"/>
     </row>
-    <row r="47" spans="1:6" ht="18.75">
+    <row r="47" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>162</v>
       </c>
@@ -2406,7 +2407,7 @@
       <c r="E47" s="15"/>
       <c r="F47" s="20"/>
     </row>
-    <row r="48" spans="1:6" ht="18.75">
+    <row r="48" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>197</v>
       </c>
@@ -2422,7 +2423,7 @@
       <c r="E48" s="15"/>
       <c r="F48" s="20"/>
     </row>
-    <row r="49" spans="1:6" ht="18.75">
+    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>198</v>
       </c>
@@ -2438,7 +2439,7 @@
       <c r="E49" s="15"/>
       <c r="F49" s="20"/>
     </row>
-    <row r="50" spans="1:6" ht="18.75">
+    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>199</v>
       </c>
@@ -2454,7 +2455,7 @@
       <c r="E50" s="15"/>
       <c r="F50" s="20"/>
     </row>
-    <row r="51" spans="1:6" ht="18.75">
+    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>120</v>
       </c>
@@ -2474,7 +2475,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18.75">
+    <row r="52" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>121</v>
       </c>
@@ -2494,7 +2495,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18.75">
+    <row r="53" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>122</v>
       </c>
@@ -2512,7 +2513,7 @@
       </c>
       <c r="F53" s="20"/>
     </row>
-    <row r="54" spans="1:6" ht="18.75">
+    <row r="54" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>123</v>
       </c>
@@ -2529,10 +2530,10 @@
         <v>248</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="18.75">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>124</v>
       </c>
@@ -2549,10 +2550,10 @@
         <v>248</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="18.75">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>125</v>
       </c>
@@ -2565,14 +2566,14 @@
       <c r="D56" s="6">
         <v>1</v>
       </c>
-      <c r="E56" s="14" t="s">
-        <v>246</v>
+      <c r="E56" s="13" t="s">
+        <v>245</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="18.75">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>126</v>
       </c>
@@ -2589,10 +2590,10 @@
         <v>248</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="18.75">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>127</v>
       </c>
@@ -2605,14 +2606,14 @@
       <c r="D58" s="6">
         <v>2</v>
       </c>
-      <c r="E58" s="14" t="s">
-        <v>253</v>
+      <c r="E58" s="13" t="s">
+        <v>245</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="18.75">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>227</v>
       </c>
@@ -2628,7 +2629,7 @@
       <c r="E59" s="15"/>
       <c r="F59" s="20"/>
     </row>
-    <row r="60" spans="1:6" ht="18.75">
+    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>163</v>
       </c>
@@ -2644,7 +2645,7 @@
       <c r="E60" s="15"/>
       <c r="F60" s="20"/>
     </row>
-    <row r="61" spans="1:6" ht="18.75">
+    <row r="61" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>164</v>
       </c>
@@ -2660,7 +2661,7 @@
       <c r="E61" s="15"/>
       <c r="F61" s="20"/>
     </row>
-    <row r="62" spans="1:6" ht="18.75">
+    <row r="62" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>165</v>
       </c>
@@ -2676,7 +2677,7 @@
       <c r="E62" s="15"/>
       <c r="F62" s="20"/>
     </row>
-    <row r="63" spans="1:6" ht="18.75">
+    <row r="63" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>166</v>
       </c>
@@ -2692,7 +2693,7 @@
       <c r="E63" s="15"/>
       <c r="F63" s="20"/>
     </row>
-    <row r="64" spans="1:6" ht="18.75">
+    <row r="64" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>167</v>
       </c>
@@ -2708,7 +2709,7 @@
       <c r="E64" s="15"/>
       <c r="F64" s="20"/>
     </row>
-    <row r="65" spans="1:6" ht="18.75">
+    <row r="65" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>168</v>
       </c>
@@ -2724,7 +2725,7 @@
       <c r="E65" s="15"/>
       <c r="F65" s="20"/>
     </row>
-    <row r="66" spans="1:6" ht="18.75">
+    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>229</v>
       </c>
@@ -2740,7 +2741,7 @@
       <c r="E66" s="15"/>
       <c r="F66" s="20"/>
     </row>
-    <row r="67" spans="1:6" ht="18.75">
+    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>228</v>
       </c>
@@ -2756,7 +2757,7 @@
       <c r="E67" s="15"/>
       <c r="F67" s="20"/>
     </row>
-    <row r="68" spans="1:6" ht="18.75">
+    <row r="68" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>200</v>
       </c>
@@ -2772,7 +2773,7 @@
       <c r="E68" s="15"/>
       <c r="F68" s="20"/>
     </row>
-    <row r="69" spans="1:6" ht="18.75">
+    <row r="69" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>201</v>
       </c>
@@ -2788,7 +2789,7 @@
       <c r="E69" s="15"/>
       <c r="F69" s="20"/>
     </row>
-    <row r="70" spans="1:6" ht="18.75">
+    <row r="70" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>202</v>
       </c>
@@ -2804,7 +2805,7 @@
       <c r="E70" s="15"/>
       <c r="F70" s="20"/>
     </row>
-    <row r="71" spans="1:6" ht="18.75">
+    <row r="71" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>203</v>
       </c>
@@ -2820,7 +2821,7 @@
       <c r="E71" s="15"/>
       <c r="F71" s="20"/>
     </row>
-    <row r="72" spans="1:6" ht="18.75">
+    <row r="72" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>129</v>
       </c>
@@ -2837,10 +2838,10 @@
         <v>245</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="18.75">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>130</v>
       </c>
@@ -2854,13 +2855,13 @@
         <v>6</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="18.75">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>131</v>
       </c>
@@ -2877,10 +2878,10 @@
         <v>245</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="18.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>132</v>
       </c>
@@ -2897,10 +2898,10 @@
         <v>245</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="18.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>133</v>
       </c>
@@ -2914,13 +2915,13 @@
         <v>4</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F76" s="20" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="18.75">
+    <row r="77" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>134</v>
       </c>
@@ -2938,7 +2939,7 @@
       </c>
       <c r="F77" s="20"/>
     </row>
-    <row r="78" spans="1:6" ht="18.75">
+    <row r="78" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>230</v>
       </c>
@@ -2954,7 +2955,7 @@
       <c r="E78" s="15"/>
       <c r="F78" s="20"/>
     </row>
-    <row r="79" spans="1:6" ht="18.75">
+    <row r="79" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>169</v>
       </c>
@@ -2970,7 +2971,7 @@
       <c r="E79" s="15"/>
       <c r="F79" s="20"/>
     </row>
-    <row r="80" spans="1:6" ht="18.75">
+    <row r="80" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>170</v>
       </c>
@@ -2986,7 +2987,7 @@
       <c r="E80" s="15"/>
       <c r="F80" s="20"/>
     </row>
-    <row r="81" spans="1:6" ht="18.75">
+    <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>171</v>
       </c>
@@ -3002,7 +3003,7 @@
       <c r="E81" s="15"/>
       <c r="F81" s="20"/>
     </row>
-    <row r="82" spans="1:6" ht="18.75">
+    <row r="82" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>172</v>
       </c>
@@ -3018,7 +3019,7 @@
       <c r="E82" s="15"/>
       <c r="F82" s="20"/>
     </row>
-    <row r="83" spans="1:6" ht="18.75">
+    <row r="83" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>232</v>
       </c>
@@ -3034,7 +3035,7 @@
       <c r="E83" s="15"/>
       <c r="F83" s="20"/>
     </row>
-    <row r="84" spans="1:6" ht="18.75">
+    <row r="84" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>231</v>
       </c>
@@ -3050,7 +3051,7 @@
       <c r="E84" s="15"/>
       <c r="F84" s="20"/>
     </row>
-    <row r="85" spans="1:6" ht="18.75">
+    <row r="85" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>204</v>
       </c>
@@ -3066,7 +3067,7 @@
       <c r="E85" s="15"/>
       <c r="F85" s="20"/>
     </row>
-    <row r="86" spans="1:6" ht="18.75">
+    <row r="86" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>205</v>
       </c>
@@ -3082,7 +3083,7 @@
       <c r="E86" s="15"/>
       <c r="F86" s="20"/>
     </row>
-    <row r="87" spans="1:6" ht="18.75">
+    <row r="87" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>206</v>
       </c>
@@ -3098,7 +3099,7 @@
       <c r="E87" s="15"/>
       <c r="F87" s="20"/>
     </row>
-    <row r="88" spans="1:6" ht="18.75">
+    <row r="88" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>135</v>
       </c>
@@ -3114,7 +3115,7 @@
       <c r="E88" s="15"/>
       <c r="F88" s="20"/>
     </row>
-    <row r="89" spans="1:6" ht="18.75">
+    <row r="89" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>136</v>
       </c>
@@ -3130,7 +3131,7 @@
       <c r="E89" s="15"/>
       <c r="F89" s="20"/>
     </row>
-    <row r="90" spans="1:6" ht="18.75">
+    <row r="90" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>137</v>
       </c>
@@ -3146,7 +3147,7 @@
       <c r="E90" s="15"/>
       <c r="F90" s="20"/>
     </row>
-    <row r="91" spans="1:6" ht="18.75">
+    <row r="91" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>138</v>
       </c>
@@ -3162,7 +3163,7 @@
       <c r="E91" s="15"/>
       <c r="F91" s="20"/>
     </row>
-    <row r="92" spans="1:6" ht="18.75">
+    <row r="92" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>173</v>
       </c>
@@ -3178,7 +3179,7 @@
       <c r="E92" s="15"/>
       <c r="F92" s="20"/>
     </row>
-    <row r="93" spans="1:6" ht="18.75">
+    <row r="93" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>174</v>
       </c>
@@ -3194,7 +3195,7 @@
       <c r="E93" s="15"/>
       <c r="F93" s="20"/>
     </row>
-    <row r="94" spans="1:6" ht="18.75">
+    <row r="94" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>175</v>
       </c>
@@ -3210,7 +3211,7 @@
       <c r="E94" s="15"/>
       <c r="F94" s="20"/>
     </row>
-    <row r="95" spans="1:6" ht="18.75">
+    <row r="95" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>176</v>
       </c>
@@ -3226,7 +3227,7 @@
       <c r="E95" s="15"/>
       <c r="F95" s="20"/>
     </row>
-    <row r="96" spans="1:6" ht="18.75">
+    <row r="96" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>207</v>
       </c>
@@ -3242,7 +3243,7 @@
       <c r="E96" s="15"/>
       <c r="F96" s="20"/>
     </row>
-    <row r="97" spans="1:6" ht="18.75">
+    <row r="97" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>208</v>
       </c>
@@ -3258,7 +3259,7 @@
       <c r="E97" s="15"/>
       <c r="F97" s="20"/>
     </row>
-    <row r="98" spans="1:6" ht="18.75">
+    <row r="98" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>209</v>
       </c>
@@ -3274,7 +3275,7 @@
       <c r="E98" s="15"/>
       <c r="F98" s="20"/>
     </row>
-    <row r="99" spans="1:6" ht="18.75">
+    <row r="99" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>140</v>
       </c>
@@ -3291,10 +3292,10 @@
         <v>246</v>
       </c>
       <c r="F99" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="18.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>141</v>
       </c>
@@ -3308,13 +3309,13 @@
         <v>5</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F100" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="18.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>142</v>
       </c>
@@ -3328,13 +3329,13 @@
         <v>5</v>
       </c>
       <c r="E101" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="18.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>143</v>
       </c>
@@ -3351,10 +3352,10 @@
         <v>245</v>
       </c>
       <c r="F102" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="18.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>144</v>
       </c>
@@ -3371,10 +3372,10 @@
         <v>245</v>
       </c>
       <c r="F103" s="20" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="18.75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>145</v>
       </c>
@@ -3388,13 +3389,13 @@
         <v>6</v>
       </c>
       <c r="E104" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="18.75">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>146</v>
       </c>
@@ -3408,13 +3409,13 @@
         <v>2</v>
       </c>
       <c r="E105" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="18.75">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>147</v>
       </c>
@@ -3432,7 +3433,7 @@
       </c>
       <c r="F106" s="20"/>
     </row>
-    <row r="107" spans="1:6" ht="18.75">
+    <row r="107" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>177</v>
       </c>
@@ -3448,7 +3449,7 @@
       <c r="E107" s="15"/>
       <c r="F107" s="20"/>
     </row>
-    <row r="108" spans="1:6" ht="18.75">
+    <row r="108" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>178</v>
       </c>
@@ -3464,7 +3465,7 @@
       <c r="E108" s="15"/>
       <c r="F108" s="20"/>
     </row>
-    <row r="109" spans="1:6" ht="18.75">
+    <row r="109" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>179</v>
       </c>
@@ -3480,7 +3481,7 @@
       <c r="E109" s="15"/>
       <c r="F109" s="20"/>
     </row>
-    <row r="110" spans="1:6" ht="18.75">
+    <row r="110" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>180</v>
       </c>
@@ -3496,7 +3497,7 @@
       <c r="E110" s="15"/>
       <c r="F110" s="20"/>
     </row>
-    <row r="111" spans="1:6" ht="18.75">
+    <row r="111" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>181</v>
       </c>
@@ -3512,7 +3513,7 @@
       <c r="E111" s="15"/>
       <c r="F111" s="20"/>
     </row>
-    <row r="112" spans="1:6" ht="18.75">
+    <row r="112" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>182</v>
       </c>
@@ -3528,7 +3529,7 @@
       <c r="E112" s="15"/>
       <c r="F112" s="20"/>
     </row>
-    <row r="113" spans="1:6" ht="18.75">
+    <row r="113" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>183</v>
       </c>
@@ -3544,7 +3545,7 @@
       <c r="E113" s="15"/>
       <c r="F113" s="20"/>
     </row>
-    <row r="114" spans="1:6" ht="18.75">
+    <row r="114" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>184</v>
       </c>
@@ -3560,7 +3561,7 @@
       <c r="E114" s="15"/>
       <c r="F114" s="20"/>
     </row>
-    <row r="115" spans="1:6" ht="18.75">
+    <row r="115" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>185</v>
       </c>
@@ -3576,7 +3577,7 @@
       <c r="E115" s="15"/>
       <c r="F115" s="20"/>
     </row>
-    <row r="116" spans="1:6" ht="18.75">
+    <row r="116" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>210</v>
       </c>
@@ -3592,7 +3593,7 @@
       <c r="E116" s="15"/>
       <c r="F116" s="20"/>
     </row>
-    <row r="117" spans="1:6" ht="18.75">
+    <row r="117" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>211</v>
       </c>
@@ -3608,7 +3609,7 @@
       <c r="E117" s="15"/>
       <c r="F117" s="20"/>
     </row>
-    <row r="118" spans="1:6" ht="18.75">
+    <row r="118" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>212</v>
       </c>
@@ -3624,7 +3625,7 @@
       <c r="E118" s="15"/>
       <c r="F118" s="20"/>
     </row>
-    <row r="119" spans="1:6" ht="18.75">
+    <row r="119" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>213</v>
       </c>
@@ -3640,7 +3641,7 @@
       <c r="E119" s="15"/>
       <c r="F119" s="20"/>
     </row>
-    <row r="120" spans="1:6" ht="18.75">
+    <row r="120" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>214</v>
       </c>
@@ -3656,7 +3657,7 @@
       <c r="E120" s="15"/>
       <c r="F120" s="20"/>
     </row>
-    <row r="121" spans="1:6" ht="18.75">
+    <row r="121" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>215</v>
       </c>
@@ -3672,7 +3673,7 @@
       <c r="E121" s="15"/>
       <c r="F121" s="20"/>
     </row>
-    <row r="122" spans="1:6" ht="18.75">
+    <row r="122" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>216</v>
       </c>
@@ -3688,7 +3689,7 @@
       <c r="E122" s="15"/>
       <c r="F122" s="20"/>
     </row>
-    <row r="123" spans="1:6" ht="18.75">
+    <row r="123" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>217</v>
       </c>
@@ -3704,7 +3705,7 @@
       <c r="E123" s="15"/>
       <c r="F123" s="20"/>
     </row>
-    <row r="124" spans="1:6" ht="19.5" thickBot="1">
+    <row r="124" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="10" t="s">
         <v>218</v>
       </c>
@@ -3720,28 +3721,28 @@
       <c r="E124" s="22"/>
       <c r="F124" s="23"/>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="11"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="5"/>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="20.25" customHeight="1"/>
-    <row r="130" ht="26.25" customHeight="1"/>
-    <row r="131" ht="27.75" customHeight="1"/>
+    <row r="128" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
Se agregan las encuestas en primera vercion, Se agregaron las planificaciones y por ultimo se modifico el formato del reglamento interno
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\proyectofinal2019\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\proyectofinal2019\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032CAC6C-1BEF-495E-9F6B-14E21C82C6B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308C6786-2885-4718-B30E-C8975639C384}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -835,7 +835,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1345,7 +1345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1397,7 +1397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1601,11 +1601,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
@@ -1615,7 +1615,7 @@
     <col min="6" max="6" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="114" customHeight="1">
       <c r="A1" s="34" t="s">
         <v>219</v>
       </c>
@@ -1625,7 +1625,7 @@
       <c r="E1" s="18"/>
       <c r="F1" s="19"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
       <c r="A2" s="29" t="s">
         <v>128</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="26.25">
       <c r="A3" s="24" t="s">
         <v>108</v>
       </c>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="F3" s="28"/>
     </row>
-    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="26.25">
       <c r="A4" s="4" t="s">
         <v>109</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="18.75">
       <c r="A5" s="4" t="s">
         <v>110</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="26.25">
       <c r="A6" s="4" t="s">
         <v>111</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="26.25">
       <c r="A7" s="4" t="s">
         <v>112</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>238</v>
       </c>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="F8" s="20"/>
     </row>
-    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="26.25">
       <c r="A9" s="4" t="s">
         <v>261</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="4" t="s">
         <v>148</v>
       </c>
@@ -1795,7 +1795,7 @@
       <c r="E10" s="15"/>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="4" t="s">
         <v>149</v>
       </c>
@@ -1811,7 +1811,7 @@
       <c r="E11" s="15"/>
       <c r="F11" s="20"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="4" t="s">
         <v>150</v>
       </c>
@@ -1827,7 +1827,7 @@
       <c r="E12" s="15"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="26.25">
       <c r="A13" s="4" t="s">
         <v>151</v>
       </c>
@@ -1843,7 +1843,7 @@
       <c r="E13" s="15"/>
       <c r="F13" s="20"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="26.25">
       <c r="A14" s="4" t="s">
         <v>262</v>
       </c>
@@ -1859,7 +1859,7 @@
       <c r="E14" s="15"/>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="18.75">
       <c r="A15" s="4" t="s">
         <v>186</v>
       </c>
@@ -1875,7 +1875,7 @@
       <c r="E15" s="15"/>
       <c r="F15" s="20"/>
     </row>
-    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="18.75">
       <c r="A16" s="4" t="s">
         <v>187</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="E16" s="15"/>
       <c r="F16" s="20"/>
     </row>
-    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="26.25">
       <c r="A17" s="4" t="s">
         <v>188</v>
       </c>
@@ -1907,7 +1907,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="20"/>
     </row>
-    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="26.25">
       <c r="A18" s="4" t="s">
         <v>189</v>
       </c>
@@ -1923,7 +1923,7 @@
       <c r="E18" s="15"/>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75">
       <c r="A19" s="4" t="s">
         <v>190</v>
       </c>
@@ -1939,7 +1939,7 @@
       <c r="E19" s="15"/>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75">
       <c r="A20" s="4" t="s">
         <v>191</v>
       </c>
@@ -1955,7 +1955,7 @@
       <c r="E20" s="15"/>
       <c r="F20" s="20"/>
     </row>
-    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75">
       <c r="A21" s="4" t="s">
         <v>192</v>
       </c>
@@ -1971,7 +1971,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="20"/>
     </row>
-    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="4" t="s">
         <v>193</v>
       </c>
@@ -1987,7 +1987,7 @@
       <c r="E22" s="15"/>
       <c r="F22" s="20"/>
     </row>
-    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="26.25">
       <c r="A23" s="4" t="s">
         <v>263</v>
       </c>
@@ -2003,7 +2003,7 @@
       <c r="E23" s="15"/>
       <c r="F23" s="20"/>
     </row>
-    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.25">
       <c r="A24" s="4" t="s">
         <v>264</v>
       </c>
@@ -2019,7 +2019,7 @@
       <c r="E24" s="15"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="4" t="s">
         <v>224</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="18.75">
       <c r="A26" s="4" t="s">
         <v>113</v>
       </c>
@@ -2052,12 +2052,12 @@
       <c r="D26" s="6">
         <v>3</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>244</v>
+      <c r="E26" s="14" t="s">
+        <v>253</v>
       </c>
       <c r="F26" s="20"/>
     </row>
-    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="26.25">
       <c r="A27" s="4" t="s">
         <v>114</v>
       </c>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="F27" s="20"/>
     </row>
-    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="26.25">
       <c r="A28" s="4" t="s">
         <v>115</v>
       </c>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="26.25">
       <c r="A29" s="4" t="s">
         <v>116</v>
       </c>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="F29" s="20"/>
     </row>
-    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="26.25">
       <c r="A30" s="4" t="s">
         <v>117</v>
       </c>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="F30" s="20"/>
     </row>
-    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="18.75">
       <c r="A31" s="4" t="s">
         <v>152</v>
       </c>
@@ -2145,7 +2145,7 @@
       <c r="E31" s="15"/>
       <c r="F31" s="20"/>
     </row>
-    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75">
       <c r="A32" s="4" t="s">
         <v>153</v>
       </c>
@@ -2161,7 +2161,7 @@
       <c r="E32" s="15"/>
       <c r="F32" s="20"/>
     </row>
-    <row r="33" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="26.25">
       <c r="A33" s="4" t="s">
         <v>154</v>
       </c>
@@ -2177,7 +2177,7 @@
       <c r="E33" s="15"/>
       <c r="F33" s="20"/>
     </row>
-    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="26.25">
       <c r="A34" s="4" t="s">
         <v>155</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="26.25">
       <c r="A35" s="4" t="s">
         <v>156</v>
       </c>
@@ -2209,7 +2209,7 @@
       <c r="E35" s="15"/>
       <c r="F35" s="20"/>
     </row>
-    <row r="36" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="26.25">
       <c r="A36" s="4" t="s">
         <v>157</v>
       </c>
@@ -2225,7 +2225,7 @@
       <c r="E36" s="15"/>
       <c r="F36" s="20"/>
     </row>
-    <row r="37" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="4" t="s">
         <v>158</v>
       </c>
@@ -2241,7 +2241,7 @@
       <c r="E37" s="15"/>
       <c r="F37" s="20"/>
     </row>
-    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18.75">
       <c r="A38" s="4" t="s">
         <v>194</v>
       </c>
@@ -2257,7 +2257,7 @@
       <c r="E38" s="15"/>
       <c r="F38" s="20"/>
     </row>
-    <row r="39" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="18.75">
       <c r="A39" s="4" t="s">
         <v>195</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="E39" s="15"/>
       <c r="F39" s="20"/>
     </row>
-    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="26.25">
       <c r="A40" s="4" t="s">
         <v>196</v>
       </c>
@@ -2289,7 +2289,7 @@
       <c r="E40" s="15"/>
       <c r="F40" s="20"/>
     </row>
-    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="26.25">
       <c r="A41" s="4" t="s">
         <v>235</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="E41" s="15"/>
       <c r="F41" s="20"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="4" t="s">
         <v>118</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="18.75">
       <c r="A43" s="4" t="s">
         <v>119</v>
       </c>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="F43" s="20"/>
     </row>
-    <row r="44" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="18.75">
       <c r="A44" s="4" t="s">
         <v>159</v>
       </c>
@@ -2359,7 +2359,7 @@
       <c r="E44" s="15"/>
       <c r="F44" s="20"/>
     </row>
-    <row r="45" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="26.25">
       <c r="A45" s="4" t="s">
         <v>160</v>
       </c>
@@ -2375,7 +2375,7 @@
       <c r="E45" s="15"/>
       <c r="F45" s="20"/>
     </row>
-    <row r="46" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="26.25">
       <c r="A46" s="4" t="s">
         <v>161</v>
       </c>
@@ -2391,7 +2391,7 @@
       <c r="E46" s="15"/>
       <c r="F46" s="20"/>
     </row>
-    <row r="47" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="18.75">
       <c r="A47" s="4" t="s">
         <v>162</v>
       </c>
@@ -2407,7 +2407,7 @@
       <c r="E47" s="15"/>
       <c r="F47" s="20"/>
     </row>
-    <row r="48" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="18.75">
       <c r="A48" s="4" t="s">
         <v>197</v>
       </c>
@@ -2423,7 +2423,7 @@
       <c r="E48" s="15"/>
       <c r="F48" s="20"/>
     </row>
-    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="26.25">
       <c r="A49" s="4" t="s">
         <v>198</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="E49" s="15"/>
       <c r="F49" s="20"/>
     </row>
-    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="18.75">
       <c r="A50" s="4" t="s">
         <v>199</v>
       </c>
@@ -2455,7 +2455,7 @@
       <c r="E50" s="15"/>
       <c r="F50" s="20"/>
     </row>
-    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="26.25">
       <c r="A51" s="4" t="s">
         <v>120</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="26.25">
       <c r="A52" s="4" t="s">
         <v>121</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="26.25">
       <c r="A53" s="4" t="s">
         <v>122</v>
       </c>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="F53" s="20"/>
     </row>
-    <row r="54" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="26.25">
       <c r="A54" s="4" t="s">
         <v>123</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="26.25">
       <c r="A55" s="4" t="s">
         <v>124</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="26.25">
       <c r="A56" s="4" t="s">
         <v>125</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="26.25">
       <c r="A57" s="4" t="s">
         <v>126</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="26.25">
       <c r="A58" s="4" t="s">
         <v>127</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="18.75">
       <c r="A59" s="4" t="s">
         <v>227</v>
       </c>
@@ -2629,7 +2629,7 @@
       <c r="E59" s="15"/>
       <c r="F59" s="20"/>
     </row>
-    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="18.75">
       <c r="A60" s="4" t="s">
         <v>163</v>
       </c>
@@ -2645,7 +2645,7 @@
       <c r="E60" s="15"/>
       <c r="F60" s="20"/>
     </row>
-    <row r="61" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="4" t="s">
         <v>164</v>
       </c>
@@ -2661,7 +2661,7 @@
       <c r="E61" s="15"/>
       <c r="F61" s="20"/>
     </row>
-    <row r="62" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="26.25">
       <c r="A62" s="4" t="s">
         <v>165</v>
       </c>
@@ -2677,7 +2677,7 @@
       <c r="E62" s="15"/>
       <c r="F62" s="20"/>
     </row>
-    <row r="63" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="26.25">
       <c r="A63" s="4" t="s">
         <v>166</v>
       </c>
@@ -2693,7 +2693,7 @@
       <c r="E63" s="15"/>
       <c r="F63" s="20"/>
     </row>
-    <row r="64" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="26.25">
       <c r="A64" s="4" t="s">
         <v>167</v>
       </c>
@@ -2709,7 +2709,7 @@
       <c r="E64" s="15"/>
       <c r="F64" s="20"/>
     </row>
-    <row r="65" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="4" t="s">
         <v>168</v>
       </c>
@@ -2725,7 +2725,7 @@
       <c r="E65" s="15"/>
       <c r="F65" s="20"/>
     </row>
-    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="4" t="s">
         <v>229</v>
       </c>
@@ -2741,7 +2741,7 @@
       <c r="E66" s="15"/>
       <c r="F66" s="20"/>
     </row>
-    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="4" t="s">
         <v>228</v>
       </c>
@@ -2757,7 +2757,7 @@
       <c r="E67" s="15"/>
       <c r="F67" s="20"/>
     </row>
-    <row r="68" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="4" t="s">
         <v>200</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="E68" s="15"/>
       <c r="F68" s="20"/>
     </row>
-    <row r="69" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="4" t="s">
         <v>201</v>
       </c>
@@ -2789,7 +2789,7 @@
       <c r="E69" s="15"/>
       <c r="F69" s="20"/>
     </row>
-    <row r="70" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="4" t="s">
         <v>202</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="E70" s="15"/>
       <c r="F70" s="20"/>
     </row>
-    <row r="71" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="18.75">
       <c r="A71" s="4" t="s">
         <v>203</v>
       </c>
@@ -2821,7 +2821,7 @@
       <c r="E71" s="15"/>
       <c r="F71" s="20"/>
     </row>
-    <row r="72" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="18.75">
       <c r="A72" s="4" t="s">
         <v>129</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="18.75">
       <c r="A73" s="4" t="s">
         <v>130</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="18.75">
       <c r="A74" s="4" t="s">
         <v>131</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="18.75">
       <c r="A75" s="4" t="s">
         <v>132</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="18.75">
       <c r="A76" s="4" t="s">
         <v>133</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="18.75">
       <c r="A77" s="4" t="s">
         <v>134</v>
       </c>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="F77" s="20"/>
     </row>
-    <row r="78" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="18.75">
       <c r="A78" s="4" t="s">
         <v>230</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="E78" s="15"/>
       <c r="F78" s="20"/>
     </row>
-    <row r="79" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="4" t="s">
         <v>169</v>
       </c>
@@ -2971,7 +2971,7 @@
       <c r="E79" s="15"/>
       <c r="F79" s="20"/>
     </row>
-    <row r="80" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="4" t="s">
         <v>170</v>
       </c>
@@ -2987,7 +2987,7 @@
       <c r="E80" s="15"/>
       <c r="F80" s="20"/>
     </row>
-    <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="18.75">
       <c r="A81" s="4" t="s">
         <v>171</v>
       </c>
@@ -3003,7 +3003,7 @@
       <c r="E81" s="15"/>
       <c r="F81" s="20"/>
     </row>
-    <row r="82" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="18.75">
       <c r="A82" s="4" t="s">
         <v>172</v>
       </c>
@@ -3019,7 +3019,7 @@
       <c r="E82" s="15"/>
       <c r="F82" s="20"/>
     </row>
-    <row r="83" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="18.75">
       <c r="A83" s="4" t="s">
         <v>232</v>
       </c>
@@ -3035,7 +3035,7 @@
       <c r="E83" s="15"/>
       <c r="F83" s="20"/>
     </row>
-    <row r="84" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="4" t="s">
         <v>231</v>
       </c>
@@ -3051,7 +3051,7 @@
       <c r="E84" s="15"/>
       <c r="F84" s="20"/>
     </row>
-    <row r="85" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="4" t="s">
         <v>204</v>
       </c>
@@ -3067,7 +3067,7 @@
       <c r="E85" s="15"/>
       <c r="F85" s="20"/>
     </row>
-    <row r="86" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="18.75">
       <c r="A86" s="4" t="s">
         <v>205</v>
       </c>
@@ -3083,7 +3083,7 @@
       <c r="E86" s="15"/>
       <c r="F86" s="20"/>
     </row>
-    <row r="87" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="18.75">
       <c r="A87" s="4" t="s">
         <v>206</v>
       </c>
@@ -3099,7 +3099,7 @@
       <c r="E87" s="15"/>
       <c r="F87" s="20"/>
     </row>
-    <row r="88" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="18.75">
       <c r="A88" s="4" t="s">
         <v>135</v>
       </c>
@@ -3115,7 +3115,7 @@
       <c r="E88" s="15"/>
       <c r="F88" s="20"/>
     </row>
-    <row r="89" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="18.75">
       <c r="A89" s="4" t="s">
         <v>136</v>
       </c>
@@ -3131,7 +3131,7 @@
       <c r="E89" s="15"/>
       <c r="F89" s="20"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="18.75">
       <c r="A90" s="4" t="s">
         <v>137</v>
       </c>
@@ -3147,7 +3147,7 @@
       <c r="E90" s="15"/>
       <c r="F90" s="20"/>
     </row>
-    <row r="91" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="18.75">
       <c r="A91" s="4" t="s">
         <v>138</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="E91" s="15"/>
       <c r="F91" s="20"/>
     </row>
-    <row r="92" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="18.75">
       <c r="A92" s="4" t="s">
         <v>173</v>
       </c>
@@ -3179,7 +3179,7 @@
       <c r="E92" s="15"/>
       <c r="F92" s="20"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="18.75">
       <c r="A93" s="4" t="s">
         <v>174</v>
       </c>
@@ -3195,7 +3195,7 @@
       <c r="E93" s="15"/>
       <c r="F93" s="20"/>
     </row>
-    <row r="94" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="18.75">
       <c r="A94" s="4" t="s">
         <v>175</v>
       </c>
@@ -3211,7 +3211,7 @@
       <c r="E94" s="15"/>
       <c r="F94" s="20"/>
     </row>
-    <row r="95" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="18.75">
       <c r="A95" s="4" t="s">
         <v>176</v>
       </c>
@@ -3227,7 +3227,7 @@
       <c r="E95" s="15"/>
       <c r="F95" s="20"/>
     </row>
-    <row r="96" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="18.75">
       <c r="A96" s="4" t="s">
         <v>207</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="E96" s="15"/>
       <c r="F96" s="20"/>
     </row>
-    <row r="97" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="18.75">
       <c r="A97" s="4" t="s">
         <v>208</v>
       </c>
@@ -3259,7 +3259,7 @@
       <c r="E97" s="15"/>
       <c r="F97" s="20"/>
     </row>
-    <row r="98" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="18.75">
       <c r="A98" s="4" t="s">
         <v>209</v>
       </c>
@@ -3275,7 +3275,7 @@
       <c r="E98" s="15"/>
       <c r="F98" s="20"/>
     </row>
-    <row r="99" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="18.75">
       <c r="A99" s="4" t="s">
         <v>140</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="18.75">
       <c r="A100" s="4" t="s">
         <v>141</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="18.75">
       <c r="A101" s="4" t="s">
         <v>142</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="18.75">
       <c r="A102" s="4" t="s">
         <v>143</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="18.75">
       <c r="A103" s="4" t="s">
         <v>144</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="18.75">
       <c r="A104" s="4" t="s">
         <v>145</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="18.75">
       <c r="A105" s="4" t="s">
         <v>146</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="18.75">
       <c r="A106" s="4" t="s">
         <v>147</v>
       </c>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="F106" s="20"/>
     </row>
-    <row r="107" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="18.75">
       <c r="A107" s="4" t="s">
         <v>177</v>
       </c>
@@ -3449,7 +3449,7 @@
       <c r="E107" s="15"/>
       <c r="F107" s="20"/>
     </row>
-    <row r="108" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="18.75">
       <c r="A108" s="4" t="s">
         <v>178</v>
       </c>
@@ -3465,7 +3465,7 @@
       <c r="E108" s="15"/>
       <c r="F108" s="20"/>
     </row>
-    <row r="109" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="18.75">
       <c r="A109" s="4" t="s">
         <v>179</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="E109" s="15"/>
       <c r="F109" s="20"/>
     </row>
-    <row r="110" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="18.75">
       <c r="A110" s="4" t="s">
         <v>180</v>
       </c>
@@ -3497,7 +3497,7 @@
       <c r="E110" s="15"/>
       <c r="F110" s="20"/>
     </row>
-    <row r="111" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="18.75">
       <c r="A111" s="4" t="s">
         <v>181</v>
       </c>
@@ -3513,7 +3513,7 @@
       <c r="E111" s="15"/>
       <c r="F111" s="20"/>
     </row>
-    <row r="112" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="18.75">
       <c r="A112" s="4" t="s">
         <v>182</v>
       </c>
@@ -3529,7 +3529,7 @@
       <c r="E112" s="15"/>
       <c r="F112" s="20"/>
     </row>
-    <row r="113" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="18.75">
       <c r="A113" s="4" t="s">
         <v>183</v>
       </c>
@@ -3545,7 +3545,7 @@
       <c r="E113" s="15"/>
       <c r="F113" s="20"/>
     </row>
-    <row r="114" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="18.75">
       <c r="A114" s="4" t="s">
         <v>184</v>
       </c>
@@ -3561,7 +3561,7 @@
       <c r="E114" s="15"/>
       <c r="F114" s="20"/>
     </row>
-    <row r="115" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="18.75">
       <c r="A115" s="4" t="s">
         <v>185</v>
       </c>
@@ -3577,7 +3577,7 @@
       <c r="E115" s="15"/>
       <c r="F115" s="20"/>
     </row>
-    <row r="116" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="18.75">
       <c r="A116" s="4" t="s">
         <v>210</v>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="E116" s="15"/>
       <c r="F116" s="20"/>
     </row>
-    <row r="117" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="18.75">
       <c r="A117" s="4" t="s">
         <v>211</v>
       </c>
@@ -3609,7 +3609,7 @@
       <c r="E117" s="15"/>
       <c r="F117" s="20"/>
     </row>
-    <row r="118" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="18.75">
       <c r="A118" s="4" t="s">
         <v>212</v>
       </c>
@@ -3625,7 +3625,7 @@
       <c r="E118" s="15"/>
       <c r="F118" s="20"/>
     </row>
-    <row r="119" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="18.75">
       <c r="A119" s="4" t="s">
         <v>213</v>
       </c>
@@ -3641,7 +3641,7 @@
       <c r="E119" s="15"/>
       <c r="F119" s="20"/>
     </row>
-    <row r="120" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="18.75">
       <c r="A120" s="4" t="s">
         <v>214</v>
       </c>
@@ -3657,7 +3657,7 @@
       <c r="E120" s="15"/>
       <c r="F120" s="20"/>
     </row>
-    <row r="121" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="18.75">
       <c r="A121" s="4" t="s">
         <v>215</v>
       </c>
@@ -3673,7 +3673,7 @@
       <c r="E121" s="15"/>
       <c r="F121" s="20"/>
     </row>
-    <row r="122" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="18.75">
       <c r="A122" s="4" t="s">
         <v>216</v>
       </c>
@@ -3689,7 +3689,7 @@
       <c r="E122" s="15"/>
       <c r="F122" s="20"/>
     </row>
-    <row r="123" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="18.75">
       <c r="A123" s="4" t="s">
         <v>217</v>
       </c>
@@ -3705,7 +3705,7 @@
       <c r="E123" s="15"/>
       <c r="F123" s="20"/>
     </row>
-    <row r="124" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="19.5" thickBot="1">
       <c r="A124" s="10" t="s">
         <v>218</v>
       </c>
@@ -3721,28 +3721,28 @@
       <c r="E124" s="22"/>
       <c r="F124" s="23"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6">
       <c r="A125" s="11"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="5"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="130" ht="26.25" customHeight="1"/>
+    <row r="131" ht="27.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
Modificacion en el GANTT, tabla de actividades y recurso
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\proyectofinal2019\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROYECTO 2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308C6786-2885-4718-B30E-C8975639C384}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA065991-BE37-4A4B-A19C-B47CE7C19343}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6255" yWindow="1140" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="273">
   <si>
     <t>Nombre</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Tabla de recursos</t>
   </si>
   <si>
-    <t>GANTT</t>
-  </si>
-  <si>
     <t>PERT</t>
   </si>
   <si>
@@ -294,9 +291,6 @@
     <t>Diagrama PERT</t>
   </si>
   <si>
-    <t>Diagrama GANTT (con replanificación)</t>
-  </si>
-  <si>
     <t>Documentación de gestión y avance de proyecto</t>
   </si>
   <si>
@@ -465,12 +459,6 @@
     <t>Taller01006</t>
   </si>
   <si>
-    <t>Taller01007</t>
-  </si>
-  <si>
-    <t>Taller01008</t>
-  </si>
-  <si>
     <t>ADA02008</t>
   </si>
   <si>
@@ -579,12 +567,6 @@
     <t>Taller02015</t>
   </si>
   <si>
-    <t>Taller02016</t>
-  </si>
-  <si>
-    <t>Taller02017</t>
-  </si>
-  <si>
     <t>ADA03013</t>
   </si>
   <si>
@@ -636,9 +618,6 @@
     <t>Proy03020</t>
   </si>
   <si>
-    <t>Proy03021</t>
-  </si>
-  <si>
     <t>SO03014</t>
   </si>
   <si>
@@ -678,12 +657,6 @@
     <t>Taller03024</t>
   </si>
   <si>
-    <t>Taller03025</t>
-  </si>
-  <si>
-    <t>Taller03026</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tabla de actividades </t>
   </si>
   <si>
@@ -708,9 +681,6 @@
     <t>BD01002/BD01003</t>
   </si>
   <si>
-    <t>Proy02009</t>
-  </si>
-  <si>
     <t>Proy03017</t>
   </si>
   <si>
@@ -726,12 +696,6 @@
     <t>SO03012</t>
   </si>
   <si>
-    <t xml:space="preserve">Justificativo del S.O. del servidor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justificativo del S.O. de la terminal </t>
-  </si>
-  <si>
     <t>BD03017</t>
   </si>
   <si>
@@ -768,48 +732,12 @@
     <t xml:space="preserve">Asignado </t>
   </si>
   <si>
-    <t xml:space="preserve">Sin asignar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realizado constantemente </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sin asisgnar </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sin asisgnar </t>
   </si>
   <si>
-    <t>P[04],S[02],T[01],E[02]</t>
-  </si>
-  <si>
-    <t>P[02],S[02],T[04],E[05]</t>
-  </si>
-  <si>
     <t>Asignado</t>
   </si>
   <si>
-    <t>P[03],S[01],T[03],E[03]</t>
-  </si>
-  <si>
-    <t>P[03],S[01],T[03],E[02]</t>
-  </si>
-  <si>
-    <t>P[02],S[01],T[04],E[05]</t>
-  </si>
-  <si>
-    <t>P[01],S[02],T[02],E[04]</t>
-  </si>
-  <si>
-    <t>P[04],S[05],T[01],E[02]</t>
-  </si>
-  <si>
-    <t>P[01],S[11],T[02],E[04]</t>
-  </si>
-  <si>
-    <t>P[01],S[13],T[02],E[04]</t>
-  </si>
-  <si>
     <t>ADA01007</t>
   </si>
   <si>
@@ -822,13 +750,100 @@
     <t>ADA03022</t>
   </si>
   <si>
-    <t>P[04],S[09],T[01],E[02]</t>
-  </si>
-  <si>
-    <t>P[04],S[06],T[01],E[02]</t>
-  </si>
-  <si>
     <t>Realizado</t>
+  </si>
+  <si>
+    <t>P[04], P[03]</t>
+  </si>
+  <si>
+    <t>P[01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asignado  </t>
+  </si>
+  <si>
+    <t>P[01],P[02]</t>
+  </si>
+  <si>
+    <t>P[04],S[02],T[01]</t>
+  </si>
+  <si>
+    <t>P[02],S[02],T[04]</t>
+  </si>
+  <si>
+    <t>P[02],S[01],T[04]</t>
+  </si>
+  <si>
+    <t>P[03],S[01],T[03]</t>
+  </si>
+  <si>
+    <t>P[01],S[02],T[02]</t>
+  </si>
+  <si>
+    <t>P[04],S[05],T[01]</t>
+  </si>
+  <si>
+    <t>P[04],S[09],T[01]</t>
+  </si>
+  <si>
+    <t>P[04],S[06],T[01]</t>
+  </si>
+  <si>
+    <t>P[01],S[11],T[02]</t>
+  </si>
+  <si>
+    <t>P[01],S[13],T[02]</t>
+  </si>
+  <si>
+    <t>P[03]</t>
+  </si>
+  <si>
+    <t>P[01], P[02], P[03], P[04]</t>
+  </si>
+  <si>
+    <t>P[02]</t>
+  </si>
+  <si>
+    <t>P[04]</t>
+  </si>
+  <si>
+    <t>GANTT Primera Vercion</t>
+  </si>
+  <si>
+    <t>Proy01009</t>
+  </si>
+  <si>
+    <t>Mantenimiento del GANTT</t>
+  </si>
+  <si>
+    <t>Duracion del proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizado  </t>
+  </si>
+  <si>
+    <t>En proseso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En proseso </t>
+  </si>
+  <si>
+    <t>P[03],S[02],T[02]</t>
+  </si>
+  <si>
+    <t>Taller02007</t>
+  </si>
+  <si>
+    <t>Taller02008</t>
+  </si>
+  <si>
+    <t>Taller03016</t>
+  </si>
+  <si>
+    <t>Taller03017</t>
+  </si>
+  <si>
+    <t>Proy01005 -Proy01006</t>
   </si>
 </sst>
 </file>
@@ -941,7 +956,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -995,21 +1010,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1127,6 +1127,43 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1139,14 +1176,14 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1159,13 +1196,10 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -1186,41 +1220,45 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1252,15 +1290,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:rowOff>188383</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1666245</xdr:colOff>
+      <xdr:colOff>1856745</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1323975</xdr:rowOff>
+      <xdr:rowOff>1302808</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1289,7 +1327,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6105525" y="209550"/>
+          <a:off x="6427258" y="188383"/>
           <a:ext cx="1504320" cy="1114425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1601,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1610,181 +1648,187 @@
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="114" customHeight="1">
-      <c r="A1" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="33"/>
+      <c r="A1" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="33"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A2" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>222</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>241</v>
+      <c r="C2" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="26.25">
-      <c r="A3" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="26">
+      <c r="C3" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="23">
         <v>4</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="24" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="26.25">
       <c r="A4" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>251</v>
+      <c r="E4" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75">
       <c r="A5" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D5" s="6">
         <v>6</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>252</v>
+      <c r="E5" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="26.25">
       <c r="A6" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D6" s="6">
         <v>15</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>251</v>
+      <c r="E6" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="26.25">
       <c r="A7" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>256</v>
+      <c r="E7" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="6">
         <v>5</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F8" s="20"/>
+      <c r="E8" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="26.25">
       <c r="A9" s="4" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F9" s="20"/>
+      <c r="E9" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="8">
         <v>43641</v>
@@ -1792,15 +1836,15 @@
       <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="20"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="8">
         <v>43641</v>
@@ -1808,15 +1852,15 @@
       <c r="D11" s="7">
         <v>2</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="20"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="8">
         <v>43641</v>
@@ -1824,15 +1868,15 @@
       <c r="D12" s="7">
         <v>2</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6" ht="26.25">
       <c r="A13" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="8">
         <v>43641</v>
@@ -1840,15 +1884,15 @@
       <c r="D13" s="7">
         <v>2</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="26.25">
       <c r="A14" s="4" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="8">
         <v>43641</v>
@@ -1856,15 +1900,15 @@
       <c r="D14" s="7">
         <v>2</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="A15" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="8">
         <v>43641</v>
@@ -1872,15 +1916,15 @@
       <c r="D15" s="7">
         <v>2</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="20"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:6" ht="18.75">
       <c r="A16" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="8">
         <v>43712</v>
@@ -1888,15 +1932,15 @@
       <c r="D16" s="7">
         <v>2</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="20"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" ht="26.25">
       <c r="A17" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="8">
         <v>43712</v>
@@ -1904,15 +1948,15 @@
       <c r="D17" s="7">
         <v>2</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="20"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6" ht="26.25">
       <c r="A18" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="8">
         <v>43712</v>
@@ -1920,15 +1964,15 @@
       <c r="D18" s="7">
         <v>2</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="20"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" spans="1:6" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="8">
         <v>43712</v>
@@ -1936,15 +1980,15 @@
       <c r="D19" s="7">
         <v>2</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="20"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="8">
         <v>43712</v>
@@ -1952,15 +1996,15 @@
       <c r="D20" s="7">
         <v>2</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="20"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="8">
         <v>43712</v>
@@ -1968,15 +2012,15 @@
       <c r="D21" s="7">
         <v>2</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="20"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="8">
         <v>43712</v>
@@ -1984,15 +2028,15 @@
       <c r="D22" s="7">
         <v>2</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="20"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" ht="26.25">
       <c r="A23" s="4" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="8">
         <v>43712</v>
@@ -2000,15 +2044,15 @@
       <c r="D23" s="7">
         <v>2</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="20"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6" ht="26.25">
       <c r="A24" s="4" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="8">
         <v>43712</v>
@@ -2016,125 +2060,133 @@
       <c r="D24" s="7">
         <v>2</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="20"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="4" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="16">
+        <v>109</v>
+      </c>
+      <c r="D25" s="15">
         <v>8</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>255</v>
+      <c r="E25" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18.75">
       <c r="A26" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D26" s="6">
         <v>3</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="F26" s="20"/>
-    </row>
-    <row r="27" spans="1:6" ht="26.25">
+      <c r="E26" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18.75">
       <c r="A27" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F27" s="20"/>
-    </row>
-    <row r="28" spans="1:6" ht="26.25">
+      <c r="E27" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="18.75">
       <c r="A28" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F28" s="20"/>
-    </row>
-    <row r="29" spans="1:6" ht="26.25">
+      <c r="E28" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="18.75">
       <c r="A29" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D29" s="6">
         <v>2</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F29" s="20"/>
+      <c r="E29" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="26.25">
       <c r="A30" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D30" s="6">
         <v>1</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F30" s="20"/>
+      <c r="E30" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F30" s="17"/>
     </row>
     <row r="31" spans="1:6" ht="18.75">
       <c r="A31" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="8">
         <v>43641</v>
@@ -2142,15 +2194,15 @@
       <c r="D31" s="7">
         <v>2</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="20"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="17"/>
     </row>
     <row r="32" spans="1:6" ht="18.75">
       <c r="A32" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="8">
         <v>43641</v>
@@ -2158,15 +2210,15 @@
       <c r="D32" s="7">
         <v>2</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="20"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="17"/>
     </row>
     <row r="33" spans="1:6" ht="26.25">
       <c r="A33" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="8">
         <v>43641</v>
@@ -2174,15 +2226,15 @@
       <c r="D33" s="7">
         <v>2</v>
       </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="20"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" ht="26.25">
       <c r="A34" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="8">
         <v>43641</v>
@@ -2190,15 +2242,15 @@
       <c r="D34" s="7">
         <v>2</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="20"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="17"/>
     </row>
     <row r="35" spans="1:6" ht="26.25">
       <c r="A35" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="8">
         <v>43641</v>
@@ -2206,15 +2258,15 @@
       <c r="D35" s="7">
         <v>2</v>
       </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="20"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="1:6" ht="26.25">
       <c r="A36" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="8">
         <v>43641</v>
@@ -2222,15 +2274,15 @@
       <c r="D36" s="7">
         <v>2</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="20"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="17"/>
     </row>
     <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C37" s="8">
         <v>43641</v>
@@ -2238,15 +2290,15 @@
       <c r="D37" s="7">
         <v>2</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="20"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:6" ht="18.75">
       <c r="A38" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="8">
         <v>43712</v>
@@ -2254,15 +2306,15 @@
       <c r="D38" s="7">
         <v>2</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="20"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="17"/>
     </row>
     <row r="39" spans="1:6" ht="18.75">
       <c r="A39" s="4" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="8">
         <v>43712</v>
@@ -2270,15 +2322,15 @@
       <c r="D39" s="7">
         <v>2</v>
       </c>
-      <c r="E39" s="15"/>
-      <c r="F39" s="20"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:6" ht="26.25">
       <c r="A40" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="8">
         <v>43712</v>
@@ -2286,15 +2338,15 @@
       <c r="D40" s="7">
         <v>2</v>
       </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="20"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="17"/>
     </row>
     <row r="41" spans="1:6" ht="26.25">
       <c r="A41" s="4" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C41" s="8">
         <v>43712</v>
@@ -2302,53 +2354,55 @@
       <c r="D41" s="7">
         <v>2</v>
       </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="20"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="17"/>
     </row>
     <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D42" s="16">
-        <v>1</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>257</v>
+        <v>214</v>
+      </c>
+      <c r="D42" s="15">
+        <v>2</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18.75">
       <c r="A43" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D43" s="6">
         <v>13</v>
       </c>
-      <c r="E43" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F43" s="20"/>
+      <c r="E43" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="18.75">
       <c r="A44" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" s="8">
         <v>43641</v>
@@ -2356,15 +2410,15 @@
       <c r="D44" s="6">
         <v>4</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="20"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="17"/>
     </row>
     <row r="45" spans="1:6" ht="26.25">
       <c r="A45" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" s="8">
         <v>43641</v>
@@ -2372,15 +2426,15 @@
       <c r="D45" s="6">
         <v>8</v>
       </c>
-      <c r="E45" s="15"/>
-      <c r="F45" s="20"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="17"/>
     </row>
     <row r="46" spans="1:6" ht="26.25">
       <c r="A46" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" s="8">
         <v>43641</v>
@@ -2388,15 +2442,15 @@
       <c r="D46" s="6">
         <v>8</v>
       </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="20"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="17"/>
     </row>
     <row r="47" spans="1:6" ht="18.75">
       <c r="A47" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="8">
         <v>43641</v>
@@ -2404,15 +2458,15 @@
       <c r="D47" s="7">
         <v>2</v>
       </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="20"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="17"/>
     </row>
     <row r="48" spans="1:6" ht="18.75">
       <c r="A48" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="8">
         <v>43712</v>
@@ -2420,15 +2474,15 @@
       <c r="D48" s="6">
         <v>4</v>
       </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="20"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="17"/>
     </row>
     <row r="49" spans="1:6" ht="26.25">
       <c r="A49" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C49" s="8">
         <v>43712</v>
@@ -2436,15 +2490,15 @@
       <c r="D49" s="7">
         <v>2</v>
       </c>
-      <c r="E49" s="15"/>
-      <c r="F49" s="20"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="17"/>
     </row>
     <row r="50" spans="1:6" ht="18.75">
       <c r="A50" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="8">
         <v>43712</v>
@@ -2452,189 +2506,193 @@
       <c r="D50" s="7">
         <v>2</v>
       </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="20"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="17"/>
     </row>
     <row r="51" spans="1:6" ht="26.25">
       <c r="A51" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D51" s="6">
-        <v>1</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>252</v>
+        <v>2</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="26.25">
       <c r="A52" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D52" s="6">
         <v>1</v>
       </c>
-      <c r="E52" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F52" s="20" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="26.25">
+      <c r="E52" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="18.75">
       <c r="A53" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D53" s="6">
         <v>4</v>
       </c>
-      <c r="E53" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="F53" s="20"/>
-    </row>
-    <row r="54" spans="1:6" ht="26.25">
+      <c r="E53" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="18.75">
       <c r="A54" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D54" s="7">
-        <v>1</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>258</v>
+        <v>214</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="26.25">
       <c r="A55" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D55" s="6">
         <v>1</v>
       </c>
-      <c r="E55" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>258</v>
+      <c r="E55" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="26.25">
       <c r="A56" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D56" s="6">
         <v>1</v>
       </c>
-      <c r="E56" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="26.25">
+      <c r="E56" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="18.75">
       <c r="A57" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>17</v>
+        <v>260</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>124</v>
+        <v>272</v>
       </c>
       <c r="D57" s="6">
         <v>1</v>
       </c>
-      <c r="E57" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="26.25">
+      <c r="E57" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="18.75">
       <c r="A58" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D58" s="6">
         <v>2</v>
       </c>
-      <c r="E58" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F58" s="20" t="s">
-        <v>254</v>
+      <c r="E58" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="18.75">
       <c r="A59" s="4" t="s">
-        <v>227</v>
+        <v>261</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C59" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D59" s="7">
-        <v>2</v>
-      </c>
-      <c r="E59" s="15"/>
-      <c r="F59" s="20"/>
+        <v>262</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="F59" s="17"/>
     </row>
     <row r="60" spans="1:6" ht="18.75">
       <c r="A60" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C60" s="8">
         <v>43641</v>
@@ -2642,15 +2700,15 @@
       <c r="D60" s="7">
         <v>2</v>
       </c>
-      <c r="E60" s="15"/>
-      <c r="F60" s="20"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="17"/>
     </row>
     <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C61" s="8">
         <v>43641</v>
@@ -2658,76 +2716,76 @@
       <c r="D61" s="7">
         <v>2</v>
       </c>
-      <c r="E61" s="15"/>
-      <c r="F61" s="20"/>
-    </row>
-    <row r="62" spans="1:6" ht="26.25">
+      <c r="E61" s="14"/>
+      <c r="F61" s="17"/>
+    </row>
+    <row r="62" spans="1:6" ht="18.75">
       <c r="A62" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C62" s="8">
         <v>43641</v>
       </c>
-      <c r="D62" s="16">
-        <v>1</v>
-      </c>
-      <c r="E62" s="15"/>
-      <c r="F62" s="20"/>
-    </row>
-    <row r="63" spans="1:6" ht="26.25">
+      <c r="D62" s="7">
+        <v>2</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="17"/>
+    </row>
+    <row r="63" spans="1:6" ht="18.75">
       <c r="A63" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C63" s="8">
         <v>43641</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="15">
         <v>1</v>
       </c>
-      <c r="E63" s="15"/>
-      <c r="F63" s="20"/>
-    </row>
-    <row r="64" spans="1:6" ht="26.25">
+      <c r="E63" s="14"/>
+      <c r="F63" s="17"/>
+    </row>
+    <row r="64" spans="1:6" ht="18.75">
       <c r="A64" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D64" s="16">
-        <v>3</v>
-      </c>
-      <c r="E64" s="15"/>
-      <c r="F64" s="20"/>
+        <v>16</v>
+      </c>
+      <c r="C64" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1</v>
+      </c>
+      <c r="E64" s="14"/>
+      <c r="F64" s="17"/>
     </row>
     <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D65" s="16">
-        <v>1</v>
-      </c>
-      <c r="E65" s="15"/>
-      <c r="F65" s="20"/>
+        <v>161</v>
+      </c>
+      <c r="D65" s="15">
+        <v>3</v>
+      </c>
+      <c r="E65" s="14"/>
+      <c r="F65" s="17"/>
     </row>
     <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="4" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>14</v>
@@ -2738,12 +2796,12 @@
       <c r="D66" s="6">
         <v>1</v>
       </c>
-      <c r="E66" s="15"/>
-      <c r="F66" s="20"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="17"/>
     </row>
     <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="4" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>16</v>
@@ -2754,47 +2812,47 @@
       <c r="D67" s="7">
         <v>1</v>
       </c>
-      <c r="E67" s="15"/>
-      <c r="F67" s="20"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="17"/>
     </row>
     <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D68" s="6">
-        <v>1</v>
-      </c>
-      <c r="E68" s="15"/>
-      <c r="F68" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="E68" s="14"/>
+      <c r="F68" s="17"/>
     </row>
     <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D69" s="6">
-        <v>3</v>
-      </c>
-      <c r="E69" s="15"/>
-      <c r="F69" s="20"/>
+      <c r="C69" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D69" s="7">
+        <v>2</v>
+      </c>
+      <c r="E69" s="14"/>
+      <c r="F69" s="17"/>
     </row>
     <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C70" s="8">
         <v>43712</v>
@@ -2802,146 +2860,148 @@
       <c r="D70" s="7">
         <v>2</v>
       </c>
-      <c r="E70" s="15"/>
-      <c r="F70" s="20"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="17"/>
     </row>
     <row r="71" spans="1:6" ht="18.75">
       <c r="A71" s="4" t="s">
-        <v>203</v>
+        <v>127</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C71" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D71" s="7">
-        <v>2</v>
-      </c>
-      <c r="E71" s="15"/>
-      <c r="F71" s="20"/>
+        <v>18</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D71" s="6">
+        <v>1</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="72" spans="1:6" ht="18.75">
       <c r="A72" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>223</v>
+        <v>127</v>
       </c>
       <c r="D72" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F72" s="20" t="s">
-        <v>259</v>
+        <v>236</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="18.75">
       <c r="A73" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>129</v>
+        <v>214</v>
       </c>
       <c r="D73" s="6">
-        <v>6</v>
-      </c>
-      <c r="E73" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="F73" s="20" t="s">
-        <v>259</v>
+        <v>3</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="18.75">
       <c r="A74" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D74" s="6">
-        <v>1</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F74" s="20" t="s">
-        <v>257</v>
+        <v>3</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="18.75">
       <c r="A75" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D75" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F75" s="20" t="s">
-        <v>257</v>
+        <v>236</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="18.75">
       <c r="A76" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D76" s="6">
-        <v>4</v>
-      </c>
-      <c r="E76" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="F76" s="20" t="s">
-        <v>251</v>
+        <v>1</v>
+      </c>
+      <c r="E76" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="18.75">
       <c r="A77" s="4" t="s">
-        <v>134</v>
+        <v>220</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D77" s="6">
+        <v>53</v>
+      </c>
+      <c r="C77" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D77" s="15">
         <v>1</v>
       </c>
-      <c r="E77" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="F77" s="20"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="17"/>
     </row>
     <row r="78" spans="1:6" ht="18.75">
       <c r="A78" s="4" t="s">
-        <v>230</v>
+        <v>165</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>54</v>
@@ -2949,15 +3009,15 @@
       <c r="C78" s="8">
         <v>43641</v>
       </c>
-      <c r="D78" s="16">
-        <v>1</v>
-      </c>
-      <c r="E78" s="15"/>
-      <c r="F78" s="20"/>
+      <c r="D78" s="7">
+        <v>2</v>
+      </c>
+      <c r="E78" s="14"/>
+      <c r="F78" s="17"/>
     </row>
     <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>55</v>
@@ -2968,12 +3028,12 @@
       <c r="D79" s="7">
         <v>2</v>
       </c>
-      <c r="E79" s="15"/>
-      <c r="F79" s="20"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="17"/>
     </row>
     <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>56</v>
@@ -2984,12 +3044,12 @@
       <c r="D80" s="7">
         <v>2</v>
       </c>
-      <c r="E80" s="15"/>
-      <c r="F80" s="20"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="17"/>
     </row>
     <row r="81" spans="1:6" ht="18.75">
       <c r="A81" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>57</v>
@@ -3000,31 +3060,31 @@
       <c r="D81" s="7">
         <v>2</v>
       </c>
-      <c r="E81" s="15"/>
-      <c r="F81" s="20"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="17"/>
     </row>
     <row r="82" spans="1:6" ht="18.75">
       <c r="A82" s="4" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="C82" s="8">
-        <v>43641</v>
+        <v>43712</v>
       </c>
       <c r="D82" s="7">
         <v>2</v>
       </c>
-      <c r="E82" s="15"/>
-      <c r="F82" s="20"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="17"/>
     </row>
     <row r="83" spans="1:6" ht="18.75">
       <c r="A83" s="4" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C83" s="8">
         <v>43712</v>
@@ -3032,15 +3092,15 @@
       <c r="D83" s="7">
         <v>2</v>
       </c>
-      <c r="E83" s="15"/>
-      <c r="F83" s="20"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="17"/>
     </row>
     <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="4" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C84" s="8">
         <v>43712</v>
@@ -3048,15 +3108,15 @@
       <c r="D84" s="7">
         <v>2</v>
       </c>
-      <c r="E84" s="15"/>
-      <c r="F84" s="20"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="17"/>
     </row>
     <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C85" s="8">
         <v>43712</v>
@@ -3064,15 +3124,15 @@
       <c r="D85" s="7">
         <v>2</v>
       </c>
-      <c r="E85" s="15"/>
-      <c r="F85" s="20"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="17"/>
     </row>
     <row r="86" spans="1:6" ht="18.75">
       <c r="A86" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C86" s="8">
         <v>43712</v>
@@ -3080,92 +3140,92 @@
       <c r="D86" s="7">
         <v>2</v>
       </c>
-      <c r="E86" s="15"/>
-      <c r="F86" s="20"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="17"/>
     </row>
     <row r="87" spans="1:6" ht="18.75">
       <c r="A87" s="4" t="s">
-        <v>206</v>
+        <v>133</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C87" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D87" s="7">
-        <v>2</v>
-      </c>
-      <c r="E87" s="15"/>
-      <c r="F87" s="20"/>
+        <v>24</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D87" s="6">
+        <v>1</v>
+      </c>
+      <c r="E87" s="14"/>
+      <c r="F87" s="17"/>
     </row>
     <row r="88" spans="1:6" ht="18.75">
       <c r="A88" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D88" s="6">
         <v>1</v>
       </c>
-      <c r="E88" s="15"/>
-      <c r="F88" s="20"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="17"/>
     </row>
     <row r="89" spans="1:6" ht="18.75">
       <c r="A89" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D89" s="6">
-        <v>1</v>
-      </c>
-      <c r="E89" s="15"/>
-      <c r="F89" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="E89" s="14"/>
+      <c r="F89" s="17"/>
     </row>
     <row r="90" spans="1:6" ht="18.75">
       <c r="A90" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D90" s="6">
-        <v>3</v>
-      </c>
-      <c r="E90" s="15"/>
-      <c r="F90" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="E90" s="14"/>
+      <c r="F90" s="17"/>
     </row>
     <row r="91" spans="1:6" ht="18.75">
       <c r="A91" s="4" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>223</v>
+        <v>58</v>
+      </c>
+      <c r="C91" s="8">
+        <v>43641</v>
       </c>
       <c r="D91" s="6">
-        <v>2</v>
-      </c>
-      <c r="E91" s="15"/>
-      <c r="F91" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="E91" s="14"/>
+      <c r="F91" s="17"/>
     </row>
     <row r="92" spans="1:6" ht="18.75">
       <c r="A92" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>59</v>
@@ -3174,287 +3234,279 @@
         <v>43641</v>
       </c>
       <c r="D92" s="6">
-        <v>1</v>
-      </c>
-      <c r="E92" s="15"/>
-      <c r="F92" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="E92" s="14"/>
+      <c r="F92" s="17"/>
     </row>
     <row r="93" spans="1:6" ht="18.75">
       <c r="A93" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C93" s="8">
-        <v>43641</v>
+      <c r="C93" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="D93" s="6">
-        <v>3</v>
-      </c>
-      <c r="E93" s="15"/>
-      <c r="F93" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="E93" s="14"/>
+      <c r="F93" s="17"/>
     </row>
     <row r="94" spans="1:6" ht="18.75">
       <c r="A94" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D94" s="6">
-        <v>2</v>
-      </c>
-      <c r="E94" s="15"/>
-      <c r="F94" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="E94" s="14"/>
+      <c r="F94" s="17"/>
     </row>
     <row r="95" spans="1:6" ht="18.75">
       <c r="A95" s="4" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D95" s="6">
-        <v>3</v>
-      </c>
-      <c r="E95" s="15"/>
-      <c r="F95" s="20"/>
+        <v>95</v>
+      </c>
+      <c r="C95" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D95" s="16">
+        <v>2</v>
+      </c>
+      <c r="E95" s="14"/>
+      <c r="F95" s="17"/>
     </row>
     <row r="96" spans="1:6" ht="18.75">
       <c r="A96" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C96" s="8">
         <v>43712</v>
       </c>
-      <c r="D96" s="17">
-        <v>2</v>
-      </c>
-      <c r="E96" s="15"/>
-      <c r="F96" s="20"/>
+      <c r="D96" s="16">
+        <v>2</v>
+      </c>
+      <c r="E96" s="14"/>
+      <c r="F96" s="17"/>
     </row>
     <row r="97" spans="1:6" ht="18.75">
       <c r="A97" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="C97" s="8">
         <v>43712</v>
       </c>
-      <c r="D97" s="17">
-        <v>2</v>
-      </c>
-      <c r="E97" s="15"/>
-      <c r="F97" s="20"/>
+      <c r="D97" s="16">
+        <v>2</v>
+      </c>
+      <c r="E97" s="14"/>
+      <c r="F97" s="17"/>
     </row>
     <row r="98" spans="1:6" ht="18.75">
       <c r="A98" s="4" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C98" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D98" s="17">
-        <v>2</v>
-      </c>
-      <c r="E98" s="15"/>
-      <c r="F98" s="20"/>
+        <v>28</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D98" s="6">
+        <v>5</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="F98" s="17" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="99" spans="1:6" ht="18.75">
       <c r="A99" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D99" s="6">
         <v>5</v>
       </c>
-      <c r="E99" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="F99" s="20" t="s">
-        <v>257</v>
+      <c r="E99" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F99" s="17" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="18.75">
       <c r="A100" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>223</v>
+        <v>139</v>
       </c>
       <c r="D100" s="6">
         <v>5</v>
       </c>
-      <c r="E100" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="F100" s="20" t="s">
-        <v>257</v>
+      <c r="E100" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F100" s="17" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="18.75">
       <c r="A101" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D101" s="6">
-        <v>5</v>
-      </c>
-      <c r="E101" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="F101" s="20" t="s">
-        <v>257</v>
+        <v>6</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F101" s="17" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="18.75">
       <c r="A102" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C102" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="D102" s="6">
         <v>1</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F102" s="20" t="s">
-        <v>257</v>
+        <v>236</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="18.75">
       <c r="A103" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D103" s="6">
-        <v>1</v>
-      </c>
-      <c r="E103" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F103" s="20" t="s">
-        <v>257</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F103" s="17"/>
     </row>
     <row r="104" spans="1:6" ht="18.75">
       <c r="A104" s="4" t="s">
-        <v>145</v>
+        <v>268</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>142</v>
+        <v>62</v>
+      </c>
+      <c r="C104" s="8">
+        <v>43641</v>
       </c>
       <c r="D104" s="6">
-        <v>6</v>
-      </c>
-      <c r="E104" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="F104" s="20" t="s">
-        <v>260</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E104" s="14"/>
+      <c r="F104" s="17"/>
     </row>
     <row r="105" spans="1:6" ht="18.75">
       <c r="A105" s="4" t="s">
-        <v>146</v>
+        <v>269</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D105" s="6">
-        <v>2</v>
-      </c>
-      <c r="E105" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="F105" s="20" t="s">
-        <v>260</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C105" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D105" s="7">
+        <v>2</v>
+      </c>
+      <c r="E105" s="14"/>
+      <c r="F105" s="17"/>
     </row>
     <row r="106" spans="1:6" ht="18.75">
       <c r="A106" s="4" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="D106" s="6">
-        <v>2</v>
-      </c>
-      <c r="E106" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="F106" s="20"/>
+        <v>64</v>
+      </c>
+      <c r="C106" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D106" s="7">
+        <v>2</v>
+      </c>
+      <c r="E106" s="14"/>
+      <c r="F106" s="17"/>
     </row>
     <row r="107" spans="1:6" ht="18.75">
       <c r="A107" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C107" s="8">
         <v>43641</v>
       </c>
-      <c r="D107" s="6">
-        <v>4</v>
-      </c>
-      <c r="E107" s="15"/>
-      <c r="F107" s="20"/>
+      <c r="D107" s="7">
+        <v>2</v>
+      </c>
+      <c r="E107" s="14"/>
+      <c r="F107" s="17"/>
     </row>
     <row r="108" spans="1:6" ht="18.75">
       <c r="A108" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C108" s="8">
         <v>43641</v>
@@ -3462,15 +3514,15 @@
       <c r="D108" s="7">
         <v>2</v>
       </c>
-      <c r="E108" s="15"/>
-      <c r="F108" s="20"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="17"/>
     </row>
     <row r="109" spans="1:6" ht="18.75">
       <c r="A109" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C109" s="8">
         <v>43641</v>
@@ -3478,15 +3530,15 @@
       <c r="D109" s="7">
         <v>2</v>
       </c>
-      <c r="E109" s="15"/>
-      <c r="F109" s="20"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="17"/>
     </row>
     <row r="110" spans="1:6" ht="18.75">
       <c r="A110" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C110" s="8">
         <v>43641</v>
@@ -3494,15 +3546,15 @@
       <c r="D110" s="7">
         <v>2</v>
       </c>
-      <c r="E110" s="15"/>
-      <c r="F110" s="20"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="17"/>
     </row>
     <row r="111" spans="1:6" ht="18.75">
       <c r="A111" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C111" s="8">
         <v>43641</v>
@@ -3510,15 +3562,15 @@
       <c r="D111" s="7">
         <v>2</v>
       </c>
-      <c r="E111" s="15"/>
-      <c r="F111" s="20"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="17"/>
     </row>
     <row r="112" spans="1:6" ht="18.75">
       <c r="A112" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C112" s="8">
         <v>43641</v>
@@ -3526,63 +3578,63 @@
       <c r="D112" s="7">
         <v>2</v>
       </c>
-      <c r="E112" s="15"/>
-      <c r="F112" s="20"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="17"/>
     </row>
     <row r="113" spans="1:6" ht="18.75">
       <c r="A113" s="4" t="s">
-        <v>183</v>
+        <v>270</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="C113" s="8">
-        <v>43641</v>
+        <v>43712</v>
       </c>
       <c r="D113" s="7">
         <v>2</v>
       </c>
-      <c r="E113" s="15"/>
-      <c r="F113" s="20"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="17"/>
     </row>
     <row r="114" spans="1:6" ht="18.75">
       <c r="A114" s="4" t="s">
-        <v>184</v>
+        <v>271</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="C114" s="8">
-        <v>43641</v>
+        <v>43712</v>
       </c>
       <c r="D114" s="7">
         <v>2</v>
       </c>
-      <c r="E114" s="15"/>
-      <c r="F114" s="20"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="17"/>
     </row>
     <row r="115" spans="1:6" ht="18.75">
       <c r="A115" s="4" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="C115" s="8">
-        <v>43641</v>
+        <v>43712</v>
       </c>
       <c r="D115" s="7">
         <v>2</v>
       </c>
-      <c r="E115" s="15"/>
-      <c r="F115" s="20"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="17"/>
     </row>
     <row r="116" spans="1:6" ht="18.75">
       <c r="A116" s="4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C116" s="8">
         <v>43712</v>
@@ -3590,15 +3642,15 @@
       <c r="D116" s="7">
         <v>2</v>
       </c>
-      <c r="E116" s="15"/>
-      <c r="F116" s="20"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="17"/>
     </row>
     <row r="117" spans="1:6" ht="18.75">
       <c r="A117" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C117" s="8">
         <v>43712</v>
@@ -3606,15 +3658,15 @@
       <c r="D117" s="7">
         <v>2</v>
       </c>
-      <c r="E117" s="15"/>
-      <c r="F117" s="20"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="17"/>
     </row>
     <row r="118" spans="1:6" ht="18.75">
       <c r="A118" s="4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C118" s="8">
         <v>43712</v>
@@ -3622,15 +3674,15 @@
       <c r="D118" s="7">
         <v>2</v>
       </c>
-      <c r="E118" s="15"/>
-      <c r="F118" s="20"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="17"/>
     </row>
     <row r="119" spans="1:6" ht="18.75">
       <c r="A119" s="4" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C119" s="8">
         <v>43712</v>
@@ -3638,15 +3690,15 @@
       <c r="D119" s="7">
         <v>2</v>
       </c>
-      <c r="E119" s="15"/>
-      <c r="F119" s="20"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="17"/>
     </row>
     <row r="120" spans="1:6" ht="18.75">
       <c r="A120" s="4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C120" s="8">
         <v>43712</v>
@@ -3654,99 +3706,51 @@
       <c r="D120" s="7">
         <v>2</v>
       </c>
-      <c r="E120" s="15"/>
-      <c r="F120" s="20"/>
-    </row>
-    <row r="121" spans="1:6" ht="18.75">
+      <c r="E120" s="14"/>
+      <c r="F120" s="17"/>
+    </row>
+    <row r="121" spans="1:6" ht="19.5" thickBot="1">
       <c r="A121" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C121" s="8">
+        <v>209</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C121" s="9">
         <v>43712</v>
       </c>
-      <c r="D121" s="7">
-        <v>2</v>
-      </c>
-      <c r="E121" s="15"/>
+      <c r="D121" s="18">
+        <v>2</v>
+      </c>
+      <c r="E121" s="19"/>
       <c r="F121" s="20"/>
     </row>
-    <row r="122" spans="1:6" ht="18.75">
-      <c r="A122" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C122" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D122" s="7">
-        <v>2</v>
-      </c>
-      <c r="E122" s="15"/>
-      <c r="F122" s="20"/>
-    </row>
-    <row r="123" spans="1:6" ht="18.75">
-      <c r="A123" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C123" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D123" s="7">
-        <v>2</v>
-      </c>
-      <c r="E123" s="15"/>
-      <c r="F123" s="20"/>
-    </row>
-    <row r="124" spans="1:6" ht="19.5" thickBot="1">
-      <c r="A124" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C124" s="9">
-        <v>43712</v>
-      </c>
-      <c r="D124" s="21">
-        <v>2</v>
-      </c>
-      <c r="E124" s="22"/>
-      <c r="F124" s="23"/>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" s="11"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="3"/>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
-      <c r="E126" s="5"/>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" s="3"/>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
+    <row r="122" spans="1:6">
+      <c r="A122" s="10"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="3"/>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="5"/>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="3"/>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
     </row>
     <row r="128" spans="1:6" ht="20.25" customHeight="1"/>
     <row r="130" ht="26.25" customHeight="1"/>
     <row r="131" ht="27.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modificacion de gantt y asignacion de recursos en gantt
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\proyectofinal2019\Actividades\Proy01005\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEAC007-49D7-4C1F-83ED-FCD6B0C23D27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-600" yWindow="1995" windowWidth="19440" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="274">
   <si>
     <t>Nombre</t>
   </si>
@@ -753,18 +747,9 @@
     <t>Realizado</t>
   </si>
   <si>
-    <t>P[04], P[03]</t>
-  </si>
-  <si>
-    <t>P[01]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Asignado  </t>
   </si>
   <si>
-    <t>P[01],P[02]</t>
-  </si>
-  <si>
     <t>P[04],S[02],T[01]</t>
   </si>
   <si>
@@ -795,18 +780,9 @@
     <t>P[01],S[13],T[02]</t>
   </si>
   <si>
-    <t>P[03]</t>
-  </si>
-  <si>
     <t>P[01], P[02], P[03], P[04]</t>
   </si>
   <si>
-    <t>P[02]</t>
-  </si>
-  <si>
-    <t>P[04]</t>
-  </si>
-  <si>
     <t>GANTT Primera Vercion</t>
   </si>
   <si>
@@ -850,13 +826,28 @@
   </si>
   <si>
     <t>P[03],S[05],T[01]</t>
+  </si>
+  <si>
+    <t>P[04],P[03],S[02],T[03],T[01]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],S[01],T[02],T[04]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>P[03],S[01],T[03],</t>
+  </si>
+  <si>
+    <t>P[03],S[11],T[03]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1268,7 +1259,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,7 +1302,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1389,7 +1380,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1441,7 +1432,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1635,21 +1626,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
@@ -1659,7 +1650,7 @@
     <col min="6" max="6" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="114" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>210</v>
       </c>
@@ -1669,7 +1660,7 @@
       <c r="E1" s="33"/>
       <c r="F1" s="34"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>126</v>
       </c>
@@ -1689,7 +1680,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18.75">
       <c r="A3" s="21" t="s">
         <v>106</v>
       </c>
@@ -1703,13 +1694,13 @@
         <v>4</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
@@ -1726,10 +1717,10 @@
         <v>233</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
       <c r="A5" s="4" t="s">
         <v>108</v>
       </c>
@@ -1746,10 +1737,10 @@
         <v>234</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75">
       <c r="A6" s="4" t="s">
         <v>109</v>
       </c>
@@ -1766,10 +1757,10 @@
         <v>241</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75">
       <c r="A7" s="4" t="s">
         <v>110</v>
       </c>
@@ -1786,10 +1777,10 @@
         <v>234</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>226</v>
       </c>
@@ -1806,10 +1797,10 @@
         <v>234</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="4" t="s">
         <v>237</v>
       </c>
@@ -1826,10 +1817,10 @@
         <v>234</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="4" t="s">
         <v>144</v>
       </c>
@@ -1845,7 +1836,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="4" t="s">
         <v>145</v>
       </c>
@@ -1861,7 +1852,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="4" t="s">
         <v>146</v>
       </c>
@@ -1877,7 +1868,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="18.75">
       <c r="A13" s="4" t="s">
         <v>147</v>
       </c>
@@ -1893,7 +1884,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="18.75">
       <c r="A14" s="4" t="s">
         <v>238</v>
       </c>
@@ -1909,7 +1900,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="18.75">
       <c r="A15" s="4" t="s">
         <v>180</v>
       </c>
@@ -1925,7 +1916,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="18.75">
       <c r="A16" s="4" t="s">
         <v>181</v>
       </c>
@@ -1941,7 +1932,7 @@
       <c r="E16" s="14"/>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="18.75">
       <c r="A17" s="4" t="s">
         <v>182</v>
       </c>
@@ -1957,7 +1948,7 @@
       <c r="E17" s="14"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75">
       <c r="A18" s="4" t="s">
         <v>183</v>
       </c>
@@ -1973,7 +1964,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75">
       <c r="A19" s="4" t="s">
         <v>184</v>
       </c>
@@ -1989,7 +1980,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75">
       <c r="A20" s="4" t="s">
         <v>185</v>
       </c>
@@ -2005,7 +1996,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75">
       <c r="A21" s="4" t="s">
         <v>186</v>
       </c>
@@ -2021,7 +2012,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="4" t="s">
         <v>187</v>
       </c>
@@ -2037,7 +2028,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75">
       <c r="A23" s="4" t="s">
         <v>239</v>
       </c>
@@ -2053,7 +2044,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75">
       <c r="A24" s="4" t="s">
         <v>240</v>
       </c>
@@ -2069,7 +2060,7 @@
       <c r="E24" s="14"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="4" t="s">
         <v>215</v>
       </c>
@@ -2086,10 +2077,10 @@
         <v>234</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="18.75">
       <c r="A26" s="4" t="s">
         <v>111</v>
       </c>
@@ -2106,10 +2097,10 @@
         <v>236</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18.75">
       <c r="A27" s="4" t="s">
         <v>112</v>
       </c>
@@ -2126,10 +2117,10 @@
         <v>236</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="18.75">
       <c r="A28" s="4" t="s">
         <v>113</v>
       </c>
@@ -2146,10 +2137,10 @@
         <v>236</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="18.75">
       <c r="A29" s="4" t="s">
         <v>114</v>
       </c>
@@ -2166,10 +2157,10 @@
         <v>236</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="18.75">
       <c r="A30" s="4" t="s">
         <v>115</v>
       </c>
@@ -2187,7 +2178,7 @@
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="18.75">
       <c r="A31" s="4" t="s">
         <v>148</v>
       </c>
@@ -2203,7 +2194,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75">
       <c r="A32" s="4" t="s">
         <v>149</v>
       </c>
@@ -2219,7 +2210,7 @@
       <c r="E32" s="14"/>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18.75">
       <c r="A33" s="4" t="s">
         <v>150</v>
       </c>
@@ -2235,7 +2226,7 @@
       <c r="E33" s="14"/>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75">
       <c r="A34" s="4" t="s">
         <v>151</v>
       </c>
@@ -2251,7 +2242,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75">
       <c r="A35" s="4" t="s">
         <v>152</v>
       </c>
@@ -2267,7 +2258,7 @@
       <c r="E35" s="14"/>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75">
       <c r="A36" s="4" t="s">
         <v>153</v>
       </c>
@@ -2283,7 +2274,7 @@
       <c r="E36" s="14"/>
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="4" t="s">
         <v>154</v>
       </c>
@@ -2299,7 +2290,7 @@
       <c r="E37" s="14"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18.75">
       <c r="A38" s="4" t="s">
         <v>188</v>
       </c>
@@ -2315,7 +2306,7 @@
       <c r="E38" s="14"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="18.75">
       <c r="A39" s="4" t="s">
         <v>189</v>
       </c>
@@ -2331,7 +2322,7 @@
       <c r="E39" s="14"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="18.75">
       <c r="A40" s="4" t="s">
         <v>190</v>
       </c>
@@ -2347,7 +2338,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="18.75">
       <c r="A41" s="4" t="s">
         <v>223</v>
       </c>
@@ -2363,7 +2354,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="4" t="s">
         <v>116</v>
       </c>
@@ -2380,10 +2371,10 @@
         <v>233</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="18.75">
       <c r="A43" s="4" t="s">
         <v>117</v>
       </c>
@@ -2400,10 +2391,10 @@
         <v>232</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="18.75">
       <c r="A44" s="4" t="s">
         <v>155</v>
       </c>
@@ -2419,7 +2410,7 @@
       <c r="E44" s="14"/>
       <c r="F44" s="17"/>
     </row>
-    <row r="45" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="18.75">
       <c r="A45" s="4" t="s">
         <v>156</v>
       </c>
@@ -2435,7 +2426,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="18.75">
       <c r="A46" s="4" t="s">
         <v>157</v>
       </c>
@@ -2451,7 +2442,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="17"/>
     </row>
-    <row r="47" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="18.75">
       <c r="A47" s="4" t="s">
         <v>158</v>
       </c>
@@ -2467,7 +2458,7 @@
       <c r="E47" s="14"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="18.75">
       <c r="A48" s="4" t="s">
         <v>191</v>
       </c>
@@ -2483,7 +2474,7 @@
       <c r="E48" s="14"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="18.75">
       <c r="A49" s="4" t="s">
         <v>192</v>
       </c>
@@ -2499,7 +2490,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="17"/>
     </row>
-    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="18.75">
       <c r="A50" s="4" t="s">
         <v>193</v>
       </c>
@@ -2515,7 +2506,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="18.75">
       <c r="A51" s="4" t="s">
         <v>118</v>
       </c>
@@ -2532,10 +2523,10 @@
         <v>233</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="18.75">
       <c r="A52" s="4" t="s">
         <v>119</v>
       </c>
@@ -2552,10 +2543,10 @@
         <v>233</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="18.75">
       <c r="A53" s="4" t="s">
         <v>120</v>
       </c>
@@ -2572,10 +2563,10 @@
         <v>236</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="18.75">
       <c r="A54" s="4" t="s">
         <v>121</v>
       </c>
@@ -2586,16 +2577,16 @@
         <v>214</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="18.75">
       <c r="A55" s="4" t="s">
         <v>122</v>
       </c>
@@ -2612,10 +2603,10 @@
         <v>241</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="18.75">
       <c r="A56" s="4" t="s">
         <v>123</v>
       </c>
@@ -2632,30 +2623,30 @@
         <v>233</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="18.75">
       <c r="A57" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D57" s="6">
         <v>1</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="18.75">
       <c r="A58" s="4" t="s">
         <v>125</v>
       </c>
@@ -2672,28 +2663,28 @@
         <v>233</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="18.75">
       <c r="A59" s="4" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>124</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F59" s="17"/>
     </row>
-    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="18.75">
       <c r="A60" s="4" t="s">
         <v>159</v>
       </c>
@@ -2709,7 +2700,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="17"/>
     </row>
-    <row r="61" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="4" t="s">
         <v>160</v>
       </c>
@@ -2725,7 +2716,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="17"/>
     </row>
-    <row r="62" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="18.75">
       <c r="A62" s="4" t="s">
         <v>161</v>
       </c>
@@ -2741,7 +2732,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="17"/>
     </row>
-    <row r="63" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="18.75">
       <c r="A63" s="4" t="s">
         <v>162</v>
       </c>
@@ -2757,7 +2748,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="17"/>
     </row>
-    <row r="64" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="18.75">
       <c r="A64" s="4" t="s">
         <v>163</v>
       </c>
@@ -2773,7 +2764,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="17"/>
     </row>
-    <row r="65" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="4" t="s">
         <v>164</v>
       </c>
@@ -2789,7 +2780,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="17"/>
     </row>
-    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="4" t="s">
         <v>219</v>
       </c>
@@ -2805,7 +2796,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="17"/>
     </row>
-    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="4" t="s">
         <v>218</v>
       </c>
@@ -2821,7 +2812,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="17"/>
     </row>
-    <row r="68" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="4" t="s">
         <v>194</v>
       </c>
@@ -2837,7 +2828,7 @@
       <c r="E68" s="14"/>
       <c r="F68" s="17"/>
     </row>
-    <row r="69" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="4" t="s">
         <v>195</v>
       </c>
@@ -2853,7 +2844,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="17"/>
     </row>
-    <row r="70" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="4" t="s">
         <v>196</v>
       </c>
@@ -2869,7 +2860,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="17"/>
     </row>
-    <row r="71" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="18.75">
       <c r="A71" s="4" t="s">
         <v>127</v>
       </c>
@@ -2886,10 +2877,10 @@
         <v>233</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="18.75">
       <c r="A72" s="4" t="s">
         <v>128</v>
       </c>
@@ -2906,10 +2897,10 @@
         <v>236</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="18.75">
       <c r="A73" s="4" t="s">
         <v>129</v>
       </c>
@@ -2926,10 +2917,10 @@
         <v>233</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="18.75">
       <c r="A74" s="4" t="s">
         <v>130</v>
       </c>
@@ -2946,10 +2937,10 @@
         <v>233</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="18.75">
       <c r="A75" s="4" t="s">
         <v>131</v>
       </c>
@@ -2966,10 +2957,10 @@
         <v>236</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="18.75">
       <c r="A76" s="4" t="s">
         <v>132</v>
       </c>
@@ -2986,10 +2977,10 @@
         <v>236</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="18.75">
       <c r="A77" s="4" t="s">
         <v>220</v>
       </c>
@@ -3005,7 +2996,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="17"/>
     </row>
-    <row r="78" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="18.75">
       <c r="A78" s="4" t="s">
         <v>165</v>
       </c>
@@ -3021,7 +3012,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="17"/>
     </row>
-    <row r="79" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="4" t="s">
         <v>166</v>
       </c>
@@ -3037,7 +3028,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="17"/>
     </row>
-    <row r="80" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="4" t="s">
         <v>167</v>
       </c>
@@ -3053,7 +3044,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="17"/>
     </row>
-    <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="18.75">
       <c r="A81" s="4" t="s">
         <v>168</v>
       </c>
@@ -3069,7 +3060,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="17"/>
     </row>
-    <row r="82" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="18.75">
       <c r="A82" s="4" t="s">
         <v>222</v>
       </c>
@@ -3085,7 +3076,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="17"/>
     </row>
-    <row r="83" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="18.75">
       <c r="A83" s="4" t="s">
         <v>221</v>
       </c>
@@ -3101,7 +3092,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="17"/>
     </row>
-    <row r="84" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="4" t="s">
         <v>197</v>
       </c>
@@ -3117,7 +3108,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="4" t="s">
         <v>198</v>
       </c>
@@ -3133,7 +3124,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="17"/>
     </row>
-    <row r="86" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="18.75">
       <c r="A86" s="4" t="s">
         <v>199</v>
       </c>
@@ -3149,7 +3140,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="17"/>
     </row>
-    <row r="87" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="18.75">
       <c r="A87" s="4" t="s">
         <v>133</v>
       </c>
@@ -3165,7 +3156,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="17"/>
     </row>
-    <row r="88" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="18.75">
       <c r="A88" s="4" t="s">
         <v>134</v>
       </c>
@@ -3181,7 +3172,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="17"/>
     </row>
-    <row r="89" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="18.75">
       <c r="A89" s="4" t="s">
         <v>135</v>
       </c>
@@ -3197,7 +3188,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="17"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="18.75">
       <c r="A90" s="4" t="s">
         <v>136</v>
       </c>
@@ -3213,7 +3204,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="17"/>
     </row>
-    <row r="91" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="18.75">
       <c r="A91" s="4" t="s">
         <v>169</v>
       </c>
@@ -3229,7 +3220,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="17"/>
     </row>
-    <row r="92" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="18.75">
       <c r="A92" s="4" t="s">
         <v>170</v>
       </c>
@@ -3245,7 +3236,7 @@
       <c r="E92" s="14"/>
       <c r="F92" s="17"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="18.75">
       <c r="A93" s="4" t="s">
         <v>171</v>
       </c>
@@ -3261,7 +3252,7 @@
       <c r="E93" s="14"/>
       <c r="F93" s="17"/>
     </row>
-    <row r="94" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="18.75">
       <c r="A94" s="4" t="s">
         <v>172</v>
       </c>
@@ -3277,7 +3268,7 @@
       <c r="E94" s="14"/>
       <c r="F94" s="17"/>
     </row>
-    <row r="95" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="18.75">
       <c r="A95" s="4" t="s">
         <v>200</v>
       </c>
@@ -3293,7 +3284,7 @@
       <c r="E95" s="14"/>
       <c r="F95" s="17"/>
     </row>
-    <row r="96" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="18.75">
       <c r="A96" s="4" t="s">
         <v>201</v>
       </c>
@@ -3309,7 +3300,7 @@
       <c r="E96" s="14"/>
       <c r="F96" s="17"/>
     </row>
-    <row r="97" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="18.75">
       <c r="A97" s="4" t="s">
         <v>202</v>
       </c>
@@ -3325,7 +3316,7 @@
       <c r="E97" s="14"/>
       <c r="F97" s="17"/>
     </row>
-    <row r="98" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="18.75">
       <c r="A98" s="4" t="s">
         <v>138</v>
       </c>
@@ -3342,10 +3333,10 @@
         <v>234</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="18.75">
       <c r="A99" s="4" t="s">
         <v>139</v>
       </c>
@@ -3362,10 +3353,10 @@
         <v>236</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="18.75">
       <c r="A100" s="4" t="s">
         <v>140</v>
       </c>
@@ -3382,10 +3373,10 @@
         <v>236</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="18.75">
       <c r="A101" s="4" t="s">
         <v>141</v>
       </c>
@@ -3402,10 +3393,10 @@
         <v>236</v>
       </c>
       <c r="F101" s="17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="18.75">
       <c r="A102" s="4" t="s">
         <v>142</v>
       </c>
@@ -3422,10 +3413,10 @@
         <v>236</v>
       </c>
       <c r="F102" s="17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="18.75">
       <c r="A103" s="4" t="s">
         <v>143</v>
       </c>
@@ -3443,9 +3434,9 @@
       </c>
       <c r="F103" s="17"/>
     </row>
-    <row r="104" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="18.75">
       <c r="A104" s="4" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>62</v>
@@ -3459,9 +3450,9 @@
       <c r="E104" s="14"/>
       <c r="F104" s="17"/>
     </row>
-    <row r="105" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="18.75">
       <c r="A105" s="4" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>63</v>
@@ -3475,7 +3466,7 @@
       <c r="E105" s="14"/>
       <c r="F105" s="17"/>
     </row>
-    <row r="106" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="18.75">
       <c r="A106" s="4" t="s">
         <v>173</v>
       </c>
@@ -3491,7 +3482,7 @@
       <c r="E106" s="14"/>
       <c r="F106" s="17"/>
     </row>
-    <row r="107" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="18.75">
       <c r="A107" s="4" t="s">
         <v>174</v>
       </c>
@@ -3507,7 +3498,7 @@
       <c r="E107" s="14"/>
       <c r="F107" s="17"/>
     </row>
-    <row r="108" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="18.75">
       <c r="A108" s="4" t="s">
         <v>175</v>
       </c>
@@ -3523,7 +3514,7 @@
       <c r="E108" s="14"/>
       <c r="F108" s="17"/>
     </row>
-    <row r="109" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="18.75">
       <c r="A109" s="4" t="s">
         <v>176</v>
       </c>
@@ -3539,7 +3530,7 @@
       <c r="E109" s="14"/>
       <c r="F109" s="17"/>
     </row>
-    <row r="110" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="18.75">
       <c r="A110" s="4" t="s">
         <v>177</v>
       </c>
@@ -3555,7 +3546,7 @@
       <c r="E110" s="14"/>
       <c r="F110" s="17"/>
     </row>
-    <row r="111" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="18.75">
       <c r="A111" s="4" t="s">
         <v>178</v>
       </c>
@@ -3571,7 +3562,7 @@
       <c r="E111" s="14"/>
       <c r="F111" s="17"/>
     </row>
-    <row r="112" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="18.75">
       <c r="A112" s="4" t="s">
         <v>179</v>
       </c>
@@ -3587,9 +3578,9 @@
       <c r="E112" s="14"/>
       <c r="F112" s="17"/>
     </row>
-    <row r="113" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="18.75">
       <c r="A113" s="4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>97</v>
@@ -3603,9 +3594,9 @@
       <c r="E113" s="14"/>
       <c r="F113" s="17"/>
     </row>
-    <row r="114" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="18.75">
       <c r="A114" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>98</v>
@@ -3619,7 +3610,7 @@
       <c r="E114" s="14"/>
       <c r="F114" s="17"/>
     </row>
-    <row r="115" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="18.75">
       <c r="A115" s="4" t="s">
         <v>203</v>
       </c>
@@ -3635,7 +3626,7 @@
       <c r="E115" s="14"/>
       <c r="F115" s="17"/>
     </row>
-    <row r="116" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="18.75">
       <c r="A116" s="4" t="s">
         <v>204</v>
       </c>
@@ -3651,7 +3642,7 @@
       <c r="E116" s="14"/>
       <c r="F116" s="17"/>
     </row>
-    <row r="117" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="18.75">
       <c r="A117" s="4" t="s">
         <v>205</v>
       </c>
@@ -3667,7 +3658,7 @@
       <c r="E117" s="14"/>
       <c r="F117" s="17"/>
     </row>
-    <row r="118" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="18.75">
       <c r="A118" s="4" t="s">
         <v>206</v>
       </c>
@@ -3683,7 +3674,7 @@
       <c r="E118" s="14"/>
       <c r="F118" s="17"/>
     </row>
-    <row r="119" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="18.75">
       <c r="A119" s="4" t="s">
         <v>207</v>
       </c>
@@ -3699,7 +3690,7 @@
       <c r="E119" s="14"/>
       <c r="F119" s="17"/>
     </row>
-    <row r="120" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="18.75">
       <c r="A120" s="4" t="s">
         <v>208</v>
       </c>
@@ -3715,7 +3706,7 @@
       <c r="E120" s="14"/>
       <c r="F120" s="17"/>
     </row>
-    <row r="121" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="19.5" thickBot="1">
       <c r="A121" s="4" t="s">
         <v>209</v>
       </c>
@@ -3731,28 +3722,28 @@
       <c r="E121" s="19"/>
       <c r="F121" s="20"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6">
       <c r="A122" s="10"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="5"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="130" ht="26.25" customHeight="1"/>
+    <row r="131" ht="27.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Se agrega la F[004], se modifico el GANTT para lo que hablamos hoy
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\proyectofinal2019\Actividades\Proy01005\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4079A64-F820-4556-8A39-1BAB7624CFBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-600" yWindow="1995" windowWidth="19440" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -822,15 +828,9 @@
     <t>Proy01005 -Proy01006</t>
   </si>
   <si>
-    <t>P[01], P[03,] S[11],T[02]</t>
-  </si>
-  <si>
     <t>P[03],S[05],T[01]</t>
   </si>
   <si>
-    <t>P[04],P[03],S[02],T[03],T[01]</t>
-  </si>
-  <si>
     <t>P[01],P[02],S[01],T[02],T[04]</t>
   </si>
   <si>
@@ -841,12 +841,18 @@
   </si>
   <si>
     <t>P[03],S[11],T[03]</t>
+  </si>
+  <si>
+    <t>P[04] S[11],T[01]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],P[03],S[02],T[03],T[04],T[02]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -1259,7 +1265,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1302,7 +1308,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1626,18 +1632,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1647,7 +1653,7 @@
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="114" customHeight="1">
@@ -1797,7 +1803,7 @@
         <v>234</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75">
@@ -1817,7 +1823,7 @@
         <v>234</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.75">
@@ -2371,7 +2377,7 @@
         <v>233</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18.75">
@@ -2523,7 +2529,7 @@
         <v>233</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="18.75">
@@ -2603,7 +2609,7 @@
         <v>241</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18.75">
@@ -2897,7 +2903,7 @@
         <v>236</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="18.75">
@@ -2977,7 +2983,7 @@
         <v>236</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="18.75">

</xml_diff>

<commit_message>
Cambios en el GANTT, falta areglar la tabla de actividades con eso
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\proyectofinal2019\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\proyectofinal2019\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4079A64-F820-4556-8A39-1BAB7624CFBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2D64A6-82BB-4C06-8E7C-81BB9FFF36DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -853,7 +853,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1386,7 +1386,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1438,7 +1438,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1642,11 +1642,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
@@ -1656,7 +1656,7 @@
     <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="114" customHeight="1">
+    <row r="1" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>210</v>
       </c>
@@ -1666,7 +1666,7 @@
       <c r="E1" s="33"/>
       <c r="F1" s="34"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>126</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
+    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>106</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>107</v>
       </c>
       <c r="D3" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>242</v>
@@ -1706,7 +1706,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
+    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>108</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>109</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
+    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>110</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>226</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
+    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>237</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>109</v>
       </c>
       <c r="D9" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>234</v>
@@ -1826,7 +1826,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
+    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>144</v>
       </c>
@@ -1842,7 +1842,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75">
+    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>145</v>
       </c>
@@ -1858,7 +1858,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75">
+    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>146</v>
       </c>
@@ -1874,7 +1874,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75">
+    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>147</v>
       </c>
@@ -1890,7 +1890,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75">
+    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>238</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75">
+    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>180</v>
       </c>
@@ -1922,7 +1922,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75">
+    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>181</v>
       </c>
@@ -1938,7 +1938,7 @@
       <c r="E16" s="14"/>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75">
+    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>182</v>
       </c>
@@ -1954,7 +1954,7 @@
       <c r="E17" s="14"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75">
+    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>183</v>
       </c>
@@ -1970,7 +1970,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75">
+    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>184</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>185</v>
       </c>
@@ -2002,7 +2002,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75">
+    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>186</v>
       </c>
@@ -2018,7 +2018,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75">
+    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>187</v>
       </c>
@@ -2034,7 +2034,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75">
+    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>239</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75">
+    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>240</v>
       </c>
@@ -2066,7 +2066,7 @@
       <c r="E24" s="14"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75">
+    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>215</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18.75">
+    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>111</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18.75">
+    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>112</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="18.75">
+    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>113</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="18.75">
+    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>114</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="18.75">
+    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>115</v>
       </c>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75">
+    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>148</v>
       </c>
@@ -2200,7 +2200,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75">
+    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>149</v>
       </c>
@@ -2216,7 +2216,7 @@
       <c r="E32" s="14"/>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75">
+    <row r="33" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>150</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="E33" s="14"/>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75">
+    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>151</v>
       </c>
@@ -2248,7 +2248,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75">
+    <row r="35" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>152</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="E35" s="14"/>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75">
+    <row r="36" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>153</v>
       </c>
@@ -2280,7 +2280,7 @@
       <c r="E36" s="14"/>
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75">
+    <row r="37" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>154</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="E37" s="14"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75">
+    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>188</v>
       </c>
@@ -2312,7 +2312,7 @@
       <c r="E38" s="14"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75">
+    <row r="39" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>189</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="E39" s="14"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" ht="18.75">
+    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>190</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" ht="18.75">
+    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>223</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" ht="18.75">
+    <row r="42" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>116</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18.75">
+    <row r="43" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>117</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18.75">
+    <row r="44" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>155</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="E44" s="14"/>
       <c r="F44" s="17"/>
     </row>
-    <row r="45" spans="1:6" ht="18.75">
+    <row r="45" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>156</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" ht="18.75">
+    <row r="46" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>157</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="17"/>
     </row>
-    <row r="47" spans="1:6" ht="18.75">
+    <row r="47" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>158</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="E47" s="14"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" ht="18.75">
+    <row r="48" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>191</v>
       </c>
@@ -2480,7 +2480,7 @@
       <c r="E48" s="14"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" ht="18.75">
+    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>192</v>
       </c>
@@ -2496,7 +2496,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="17"/>
     </row>
-    <row r="50" spans="1:6" ht="18.75">
+    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>193</v>
       </c>
@@ -2512,7 +2512,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:6" ht="18.75">
+    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>118</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18.75">
+    <row r="52" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>119</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18.75">
+    <row r="53" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>120</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="18.75">
+    <row r="54" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>121</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18.75">
+    <row r="55" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>122</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18.75">
+    <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>123</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="18.75">
+    <row r="57" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>124</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="18.75">
+    <row r="58" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>125</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="18.75">
+    <row r="59" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>255</v>
       </c>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="F59" s="17"/>
     </row>
-    <row r="60" spans="1:6" ht="18.75">
+    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>159</v>
       </c>
@@ -2706,7 +2706,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="17"/>
     </row>
-    <row r="61" spans="1:6" ht="18.75">
+    <row r="61" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>160</v>
       </c>
@@ -2722,7 +2722,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="17"/>
     </row>
-    <row r="62" spans="1:6" ht="18.75">
+    <row r="62" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>161</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="17"/>
     </row>
-    <row r="63" spans="1:6" ht="18.75">
+    <row r="63" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>162</v>
       </c>
@@ -2754,7 +2754,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="17"/>
     </row>
-    <row r="64" spans="1:6" ht="18.75">
+    <row r="64" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>163</v>
       </c>
@@ -2770,7 +2770,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="17"/>
     </row>
-    <row r="65" spans="1:6" ht="18.75">
+    <row r="65" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>164</v>
       </c>
@@ -2786,7 +2786,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="17"/>
     </row>
-    <row r="66" spans="1:6" ht="18.75">
+    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>219</v>
       </c>
@@ -2802,7 +2802,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="17"/>
     </row>
-    <row r="67" spans="1:6" ht="18.75">
+    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>218</v>
       </c>
@@ -2818,7 +2818,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="17"/>
     </row>
-    <row r="68" spans="1:6" ht="18.75">
+    <row r="68" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>194</v>
       </c>
@@ -2834,7 +2834,7 @@
       <c r="E68" s="14"/>
       <c r="F68" s="17"/>
     </row>
-    <row r="69" spans="1:6" ht="18.75">
+    <row r="69" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>195</v>
       </c>
@@ -2850,7 +2850,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="17"/>
     </row>
-    <row r="70" spans="1:6" ht="18.75">
+    <row r="70" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>196</v>
       </c>
@@ -2866,7 +2866,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="17"/>
     </row>
-    <row r="71" spans="1:6" ht="18.75">
+    <row r="71" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>127</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="18.75">
+    <row r="72" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>128</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>127</v>
       </c>
       <c r="D72" s="6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E72" s="13" t="s">
         <v>236</v>
@@ -2906,7 +2906,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="18.75">
+    <row r="73" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>129</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="18.75">
+    <row r="74" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>130</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="18.75">
+    <row r="75" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>131</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="18.75">
+    <row r="76" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>132</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="18.75">
+    <row r="77" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>220</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="17"/>
     </row>
-    <row r="78" spans="1:6" ht="18.75">
+    <row r="78" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>165</v>
       </c>
@@ -3018,7 +3018,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="17"/>
     </row>
-    <row r="79" spans="1:6" ht="18.75">
+    <row r="79" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>166</v>
       </c>
@@ -3034,7 +3034,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="17"/>
     </row>
-    <row r="80" spans="1:6" ht="18.75">
+    <row r="80" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>167</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="17"/>
     </row>
-    <row r="81" spans="1:6" ht="18.75">
+    <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>168</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="17"/>
     </row>
-    <row r="82" spans="1:6" ht="18.75">
+    <row r="82" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>222</v>
       </c>
@@ -3082,7 +3082,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="17"/>
     </row>
-    <row r="83" spans="1:6" ht="18.75">
+    <row r="83" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>221</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="17"/>
     </row>
-    <row r="84" spans="1:6" ht="18.75">
+    <row r="84" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>197</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="1:6" ht="18.75">
+    <row r="85" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>198</v>
       </c>
@@ -3130,7 +3130,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="17"/>
     </row>
-    <row r="86" spans="1:6" ht="18.75">
+    <row r="86" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>199</v>
       </c>
@@ -3146,7 +3146,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="17"/>
     </row>
-    <row r="87" spans="1:6" ht="18.75">
+    <row r="87" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>133</v>
       </c>
@@ -3162,7 +3162,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="17"/>
     </row>
-    <row r="88" spans="1:6" ht="18.75">
+    <row r="88" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>134</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="17"/>
     </row>
-    <row r="89" spans="1:6" ht="18.75">
+    <row r="89" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>135</v>
       </c>
@@ -3194,7 +3194,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="17"/>
     </row>
-    <row r="90" spans="1:6" ht="18.75">
+    <row r="90" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>136</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="17"/>
     </row>
-    <row r="91" spans="1:6" ht="18.75">
+    <row r="91" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>169</v>
       </c>
@@ -3226,7 +3226,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="17"/>
     </row>
-    <row r="92" spans="1:6" ht="18.75">
+    <row r="92" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>170</v>
       </c>
@@ -3242,7 +3242,7 @@
       <c r="E92" s="14"/>
       <c r="F92" s="17"/>
     </row>
-    <row r="93" spans="1:6" ht="18.75">
+    <row r="93" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>171</v>
       </c>
@@ -3258,7 +3258,7 @@
       <c r="E93" s="14"/>
       <c r="F93" s="17"/>
     </row>
-    <row r="94" spans="1:6" ht="18.75">
+    <row r="94" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>172</v>
       </c>
@@ -3274,7 +3274,7 @@
       <c r="E94" s="14"/>
       <c r="F94" s="17"/>
     </row>
-    <row r="95" spans="1:6" ht="18.75">
+    <row r="95" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>200</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="E95" s="14"/>
       <c r="F95" s="17"/>
     </row>
-    <row r="96" spans="1:6" ht="18.75">
+    <row r="96" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>201</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="E96" s="14"/>
       <c r="F96" s="17"/>
     </row>
-    <row r="97" spans="1:6" ht="18.75">
+    <row r="97" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>202</v>
       </c>
@@ -3322,7 +3322,7 @@
       <c r="E97" s="14"/>
       <c r="F97" s="17"/>
     </row>
-    <row r="98" spans="1:6" ht="18.75">
+    <row r="98" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>138</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="18.75">
+    <row r="99" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>139</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="18.75">
+    <row r="100" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>140</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="18.75">
+    <row r="101" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>141</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="18.75">
+    <row r="102" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>142</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="18.75">
+    <row r="103" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>143</v>
       </c>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="F103" s="17"/>
     </row>
-    <row r="104" spans="1:6" ht="18.75">
+    <row r="104" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>262</v>
       </c>
@@ -3456,7 +3456,7 @@
       <c r="E104" s="14"/>
       <c r="F104" s="17"/>
     </row>
-    <row r="105" spans="1:6" ht="18.75">
+    <row r="105" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>263</v>
       </c>
@@ -3472,7 +3472,7 @@
       <c r="E105" s="14"/>
       <c r="F105" s="17"/>
     </row>
-    <row r="106" spans="1:6" ht="18.75">
+    <row r="106" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>173</v>
       </c>
@@ -3488,7 +3488,7 @@
       <c r="E106" s="14"/>
       <c r="F106" s="17"/>
     </row>
-    <row r="107" spans="1:6" ht="18.75">
+    <row r="107" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>174</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="E107" s="14"/>
       <c r="F107" s="17"/>
     </row>
-    <row r="108" spans="1:6" ht="18.75">
+    <row r="108" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>175</v>
       </c>
@@ -3520,7 +3520,7 @@
       <c r="E108" s="14"/>
       <c r="F108" s="17"/>
     </row>
-    <row r="109" spans="1:6" ht="18.75">
+    <row r="109" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>176</v>
       </c>
@@ -3536,7 +3536,7 @@
       <c r="E109" s="14"/>
       <c r="F109" s="17"/>
     </row>
-    <row r="110" spans="1:6" ht="18.75">
+    <row r="110" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>177</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="E110" s="14"/>
       <c r="F110" s="17"/>
     </row>
-    <row r="111" spans="1:6" ht="18.75">
+    <row r="111" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>178</v>
       </c>
@@ -3568,7 +3568,7 @@
       <c r="E111" s="14"/>
       <c r="F111" s="17"/>
     </row>
-    <row r="112" spans="1:6" ht="18.75">
+    <row r="112" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>179</v>
       </c>
@@ -3584,7 +3584,7 @@
       <c r="E112" s="14"/>
       <c r="F112" s="17"/>
     </row>
-    <row r="113" spans="1:6" ht="18.75">
+    <row r="113" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>264</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="E113" s="14"/>
       <c r="F113" s="17"/>
     </row>
-    <row r="114" spans="1:6" ht="18.75">
+    <row r="114" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>265</v>
       </c>
@@ -3616,7 +3616,7 @@
       <c r="E114" s="14"/>
       <c r="F114" s="17"/>
     </row>
-    <row r="115" spans="1:6" ht="18.75">
+    <row r="115" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>203</v>
       </c>
@@ -3632,7 +3632,7 @@
       <c r="E115" s="14"/>
       <c r="F115" s="17"/>
     </row>
-    <row r="116" spans="1:6" ht="18.75">
+    <row r="116" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>204</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="E116" s="14"/>
       <c r="F116" s="17"/>
     </row>
-    <row r="117" spans="1:6" ht="18.75">
+    <row r="117" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>205</v>
       </c>
@@ -3664,7 +3664,7 @@
       <c r="E117" s="14"/>
       <c r="F117" s="17"/>
     </row>
-    <row r="118" spans="1:6" ht="18.75">
+    <row r="118" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>206</v>
       </c>
@@ -3680,7 +3680,7 @@
       <c r="E118" s="14"/>
       <c r="F118" s="17"/>
     </row>
-    <row r="119" spans="1:6" ht="18.75">
+    <row r="119" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>207</v>
       </c>
@@ -3696,7 +3696,7 @@
       <c r="E119" s="14"/>
       <c r="F119" s="17"/>
     </row>
-    <row r="120" spans="1:6" ht="18.75">
+    <row r="120" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>208</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="E120" s="14"/>
       <c r="F120" s="17"/>
     </row>
-    <row r="121" spans="1:6" ht="19.5" thickBot="1">
+    <row r="121" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>209</v>
       </c>
@@ -3728,28 +3728,28 @@
       <c r="E121" s="19"/>
       <c r="F121" s="20"/>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="5"/>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="20.25" customHeight="1"/>
-    <row r="130" ht="26.25" customHeight="1"/>
-    <row r="131" ht="27.75" customHeight="1"/>
+    <row r="128" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Correcion en los repositorios
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\proyectofinal2019\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\proyectofinal2019\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4079A64-F820-4556-8A39-1BAB7624CFBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2D64A6-82BB-4C06-8E7C-81BB9FFF36DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -853,7 +853,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1386,7 +1386,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1438,7 +1438,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1642,11 +1642,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
@@ -1656,7 +1656,7 @@
     <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="114" customHeight="1">
+    <row r="1" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>210</v>
       </c>
@@ -1666,7 +1666,7 @@
       <c r="E1" s="33"/>
       <c r="F1" s="34"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>126</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
+    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>106</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>107</v>
       </c>
       <c r="D3" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>242</v>
@@ -1706,7 +1706,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
+    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>108</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>109</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
+    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>110</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>226</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
+    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>237</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>109</v>
       </c>
       <c r="D9" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>234</v>
@@ -1826,7 +1826,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
+    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>144</v>
       </c>
@@ -1842,7 +1842,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75">
+    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>145</v>
       </c>
@@ -1858,7 +1858,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75">
+    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>146</v>
       </c>
@@ -1874,7 +1874,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75">
+    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>147</v>
       </c>
@@ -1890,7 +1890,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75">
+    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>238</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75">
+    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>180</v>
       </c>
@@ -1922,7 +1922,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75">
+    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>181</v>
       </c>
@@ -1938,7 +1938,7 @@
       <c r="E16" s="14"/>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75">
+    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>182</v>
       </c>
@@ -1954,7 +1954,7 @@
       <c r="E17" s="14"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75">
+    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>183</v>
       </c>
@@ -1970,7 +1970,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75">
+    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>184</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>185</v>
       </c>
@@ -2002,7 +2002,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75">
+    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>186</v>
       </c>
@@ -2018,7 +2018,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75">
+    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>187</v>
       </c>
@@ -2034,7 +2034,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75">
+    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>239</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75">
+    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>240</v>
       </c>
@@ -2066,7 +2066,7 @@
       <c r="E24" s="14"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75">
+    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>215</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18.75">
+    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>111</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18.75">
+    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>112</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="18.75">
+    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>113</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="18.75">
+    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>114</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="18.75">
+    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>115</v>
       </c>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75">
+    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>148</v>
       </c>
@@ -2200,7 +2200,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75">
+    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>149</v>
       </c>
@@ -2216,7 +2216,7 @@
       <c r="E32" s="14"/>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75">
+    <row r="33" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>150</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="E33" s="14"/>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75">
+    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>151</v>
       </c>
@@ -2248,7 +2248,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75">
+    <row r="35" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>152</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="E35" s="14"/>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75">
+    <row r="36" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>153</v>
       </c>
@@ -2280,7 +2280,7 @@
       <c r="E36" s="14"/>
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75">
+    <row r="37" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>154</v>
       </c>
@@ -2296,7 +2296,7 @@
       <c r="E37" s="14"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75">
+    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>188</v>
       </c>
@@ -2312,7 +2312,7 @@
       <c r="E38" s="14"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75">
+    <row r="39" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>189</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="E39" s="14"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" ht="18.75">
+    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>190</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" ht="18.75">
+    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>223</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" ht="18.75">
+    <row r="42" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>116</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18.75">
+    <row r="43" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>117</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18.75">
+    <row r="44" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>155</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="E44" s="14"/>
       <c r="F44" s="17"/>
     </row>
-    <row r="45" spans="1:6" ht="18.75">
+    <row r="45" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>156</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" ht="18.75">
+    <row r="46" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>157</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="17"/>
     </row>
-    <row r="47" spans="1:6" ht="18.75">
+    <row r="47" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>158</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="E47" s="14"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" ht="18.75">
+    <row r="48" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>191</v>
       </c>
@@ -2480,7 +2480,7 @@
       <c r="E48" s="14"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" ht="18.75">
+    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>192</v>
       </c>
@@ -2496,7 +2496,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="17"/>
     </row>
-    <row r="50" spans="1:6" ht="18.75">
+    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>193</v>
       </c>
@@ -2512,7 +2512,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:6" ht="18.75">
+    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>118</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18.75">
+    <row r="52" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>119</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18.75">
+    <row r="53" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>120</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="18.75">
+    <row r="54" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>121</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18.75">
+    <row r="55" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>122</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18.75">
+    <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>123</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="18.75">
+    <row r="57" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>124</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="18.75">
+    <row r="58" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>125</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="18.75">
+    <row r="59" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>255</v>
       </c>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="F59" s="17"/>
     </row>
-    <row r="60" spans="1:6" ht="18.75">
+    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>159</v>
       </c>
@@ -2706,7 +2706,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="17"/>
     </row>
-    <row r="61" spans="1:6" ht="18.75">
+    <row r="61" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>160</v>
       </c>
@@ -2722,7 +2722,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="17"/>
     </row>
-    <row r="62" spans="1:6" ht="18.75">
+    <row r="62" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>161</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="17"/>
     </row>
-    <row r="63" spans="1:6" ht="18.75">
+    <row r="63" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>162</v>
       </c>
@@ -2754,7 +2754,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="17"/>
     </row>
-    <row r="64" spans="1:6" ht="18.75">
+    <row r="64" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>163</v>
       </c>
@@ -2770,7 +2770,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="17"/>
     </row>
-    <row r="65" spans="1:6" ht="18.75">
+    <row r="65" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>164</v>
       </c>
@@ -2786,7 +2786,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="17"/>
     </row>
-    <row r="66" spans="1:6" ht="18.75">
+    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>219</v>
       </c>
@@ -2802,7 +2802,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="17"/>
     </row>
-    <row r="67" spans="1:6" ht="18.75">
+    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>218</v>
       </c>
@@ -2818,7 +2818,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="17"/>
     </row>
-    <row r="68" spans="1:6" ht="18.75">
+    <row r="68" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>194</v>
       </c>
@@ -2834,7 +2834,7 @@
       <c r="E68" s="14"/>
       <c r="F68" s="17"/>
     </row>
-    <row r="69" spans="1:6" ht="18.75">
+    <row r="69" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>195</v>
       </c>
@@ -2850,7 +2850,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="17"/>
     </row>
-    <row r="70" spans="1:6" ht="18.75">
+    <row r="70" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>196</v>
       </c>
@@ -2866,7 +2866,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="17"/>
     </row>
-    <row r="71" spans="1:6" ht="18.75">
+    <row r="71" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>127</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="18.75">
+    <row r="72" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>128</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>127</v>
       </c>
       <c r="D72" s="6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E72" s="13" t="s">
         <v>236</v>
@@ -2906,7 +2906,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="18.75">
+    <row r="73" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>129</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="18.75">
+    <row r="74" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>130</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="18.75">
+    <row r="75" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>131</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="18.75">
+    <row r="76" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>132</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="18.75">
+    <row r="77" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>220</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="17"/>
     </row>
-    <row r="78" spans="1:6" ht="18.75">
+    <row r="78" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>165</v>
       </c>
@@ -3018,7 +3018,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="17"/>
     </row>
-    <row r="79" spans="1:6" ht="18.75">
+    <row r="79" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>166</v>
       </c>
@@ -3034,7 +3034,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="17"/>
     </row>
-    <row r="80" spans="1:6" ht="18.75">
+    <row r="80" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>167</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="17"/>
     </row>
-    <row r="81" spans="1:6" ht="18.75">
+    <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>168</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="17"/>
     </row>
-    <row r="82" spans="1:6" ht="18.75">
+    <row r="82" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>222</v>
       </c>
@@ -3082,7 +3082,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="17"/>
     </row>
-    <row r="83" spans="1:6" ht="18.75">
+    <row r="83" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>221</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="17"/>
     </row>
-    <row r="84" spans="1:6" ht="18.75">
+    <row r="84" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>197</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="1:6" ht="18.75">
+    <row r="85" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>198</v>
       </c>
@@ -3130,7 +3130,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="17"/>
     </row>
-    <row r="86" spans="1:6" ht="18.75">
+    <row r="86" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>199</v>
       </c>
@@ -3146,7 +3146,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="17"/>
     </row>
-    <row r="87" spans="1:6" ht="18.75">
+    <row r="87" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>133</v>
       </c>
@@ -3162,7 +3162,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="17"/>
     </row>
-    <row r="88" spans="1:6" ht="18.75">
+    <row r="88" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>134</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="17"/>
     </row>
-    <row r="89" spans="1:6" ht="18.75">
+    <row r="89" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>135</v>
       </c>
@@ -3194,7 +3194,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="17"/>
     </row>
-    <row r="90" spans="1:6" ht="18.75">
+    <row r="90" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>136</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="17"/>
     </row>
-    <row r="91" spans="1:6" ht="18.75">
+    <row r="91" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>169</v>
       </c>
@@ -3226,7 +3226,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="17"/>
     </row>
-    <row r="92" spans="1:6" ht="18.75">
+    <row r="92" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>170</v>
       </c>
@@ -3242,7 +3242,7 @@
       <c r="E92" s="14"/>
       <c r="F92" s="17"/>
     </row>
-    <row r="93" spans="1:6" ht="18.75">
+    <row r="93" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>171</v>
       </c>
@@ -3258,7 +3258,7 @@
       <c r="E93" s="14"/>
       <c r="F93" s="17"/>
     </row>
-    <row r="94" spans="1:6" ht="18.75">
+    <row r="94" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>172</v>
       </c>
@@ -3274,7 +3274,7 @@
       <c r="E94" s="14"/>
       <c r="F94" s="17"/>
     </row>
-    <row r="95" spans="1:6" ht="18.75">
+    <row r="95" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>200</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="E95" s="14"/>
       <c r="F95" s="17"/>
     </row>
-    <row r="96" spans="1:6" ht="18.75">
+    <row r="96" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>201</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="E96" s="14"/>
       <c r="F96" s="17"/>
     </row>
-    <row r="97" spans="1:6" ht="18.75">
+    <row r="97" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>202</v>
       </c>
@@ -3322,7 +3322,7 @@
       <c r="E97" s="14"/>
       <c r="F97" s="17"/>
     </row>
-    <row r="98" spans="1:6" ht="18.75">
+    <row r="98" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>138</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="18.75">
+    <row r="99" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>139</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="18.75">
+    <row r="100" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>140</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="18.75">
+    <row r="101" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>141</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="18.75">
+    <row r="102" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>142</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="18.75">
+    <row r="103" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>143</v>
       </c>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="F103" s="17"/>
     </row>
-    <row r="104" spans="1:6" ht="18.75">
+    <row r="104" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>262</v>
       </c>
@@ -3456,7 +3456,7 @@
       <c r="E104" s="14"/>
       <c r="F104" s="17"/>
     </row>
-    <row r="105" spans="1:6" ht="18.75">
+    <row r="105" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>263</v>
       </c>
@@ -3472,7 +3472,7 @@
       <c r="E105" s="14"/>
       <c r="F105" s="17"/>
     </row>
-    <row r="106" spans="1:6" ht="18.75">
+    <row r="106" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>173</v>
       </c>
@@ -3488,7 +3488,7 @@
       <c r="E106" s="14"/>
       <c r="F106" s="17"/>
     </row>
-    <row r="107" spans="1:6" ht="18.75">
+    <row r="107" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>174</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="E107" s="14"/>
       <c r="F107" s="17"/>
     </row>
-    <row r="108" spans="1:6" ht="18.75">
+    <row r="108" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>175</v>
       </c>
@@ -3520,7 +3520,7 @@
       <c r="E108" s="14"/>
       <c r="F108" s="17"/>
     </row>
-    <row r="109" spans="1:6" ht="18.75">
+    <row r="109" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>176</v>
       </c>
@@ -3536,7 +3536,7 @@
       <c r="E109" s="14"/>
       <c r="F109" s="17"/>
     </row>
-    <row r="110" spans="1:6" ht="18.75">
+    <row r="110" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>177</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="E110" s="14"/>
       <c r="F110" s="17"/>
     </row>
-    <row r="111" spans="1:6" ht="18.75">
+    <row r="111" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>178</v>
       </c>
@@ -3568,7 +3568,7 @@
       <c r="E111" s="14"/>
       <c r="F111" s="17"/>
     </row>
-    <row r="112" spans="1:6" ht="18.75">
+    <row r="112" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>179</v>
       </c>
@@ -3584,7 +3584,7 @@
       <c r="E112" s="14"/>
       <c r="F112" s="17"/>
     </row>
-    <row r="113" spans="1:6" ht="18.75">
+    <row r="113" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>264</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="E113" s="14"/>
       <c r="F113" s="17"/>
     </row>
-    <row r="114" spans="1:6" ht="18.75">
+    <row r="114" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>265</v>
       </c>
@@ -3616,7 +3616,7 @@
       <c r="E114" s="14"/>
       <c r="F114" s="17"/>
     </row>
-    <row r="115" spans="1:6" ht="18.75">
+    <row r="115" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>203</v>
       </c>
@@ -3632,7 +3632,7 @@
       <c r="E115" s="14"/>
       <c r="F115" s="17"/>
     </row>
-    <row r="116" spans="1:6" ht="18.75">
+    <row r="116" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>204</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="E116" s="14"/>
       <c r="F116" s="17"/>
     </row>
-    <row r="117" spans="1:6" ht="18.75">
+    <row r="117" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>205</v>
       </c>
@@ -3664,7 +3664,7 @@
       <c r="E117" s="14"/>
       <c r="F117" s="17"/>
     </row>
-    <row r="118" spans="1:6" ht="18.75">
+    <row r="118" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>206</v>
       </c>
@@ -3680,7 +3680,7 @@
       <c r="E118" s="14"/>
       <c r="F118" s="17"/>
     </row>
-    <row r="119" spans="1:6" ht="18.75">
+    <row r="119" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>207</v>
       </c>
@@ -3696,7 +3696,7 @@
       <c r="E119" s="14"/>
       <c r="F119" s="17"/>
     </row>
-    <row r="120" spans="1:6" ht="18.75">
+    <row r="120" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>208</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="E120" s="14"/>
       <c r="F120" s="17"/>
     </row>
-    <row r="121" spans="1:6" ht="19.5" thickBot="1">
+    <row r="121" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>209</v>
       </c>
@@ -3728,28 +3728,28 @@
       <c r="E121" s="19"/>
       <c r="F121" s="20"/>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="5"/>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
     </row>
-    <row r="128" spans="1:6" ht="20.25" customHeight="1"/>
-    <row r="130" ht="26.25" customHeight="1"/>
-    <row r="131" ht="27.75" customHeight="1"/>
+    <row r="128" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Modificacion en la tabla de actividades, tabla de recursos y gantt
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\utu de informatica avansada\tercer año\proyectofinal2019\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2D64A6-82BB-4C06-8E7C-81BB9FFF36DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39E1687-2167-4C0A-86A6-3D9EA2CA9839}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28905" yWindow="90" windowWidth="16770" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="277">
   <si>
     <t>Nombre</t>
   </si>
@@ -786,9 +786,6 @@
     <t>P[01],S[13],T[02]</t>
   </si>
   <si>
-    <t>P[01], P[02], P[03], P[04]</t>
-  </si>
-  <si>
     <t>GANTT Primera Vercion</t>
   </si>
   <si>
@@ -828,25 +825,37 @@
     <t>Proy01005 -Proy01006</t>
   </si>
   <si>
-    <t>P[03],S[05],T[01]</t>
-  </si>
-  <si>
     <t>P[01],P[02],S[01],T[02],T[04]</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>P[03],S[01],T[03],</t>
   </si>
   <si>
-    <t>P[03],S[11],T[03]</t>
-  </si>
-  <si>
     <t>P[04] S[11],T[01]</t>
   </si>
   <si>
-    <t>P[01],P[02],P[03],S[02],T[03],T[04],T[02]</t>
+    <t>P[02], P[01,T[02],]S[01],T[04]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],S[02],T[04],T[02]</t>
+  </si>
+  <si>
+    <t>P[03],P[04]S[01],T[03],T[01]</t>
+  </si>
+  <si>
+    <t>P[03],S[02],T[04]</t>
+  </si>
+  <si>
+    <t>P[03],S[02],S[14],T[03]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P[01], S[02], T[02]</t>
+  </si>
+  <si>
+    <t>P[03], P[04], S[08], T[01], T[03]</t>
+  </si>
+  <si>
+    <t>P[04],S[11],T[01]</t>
   </si>
 </sst>
 </file>
@@ -959,7 +968,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1169,6 +1178,21 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1179,7 +1203,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1262,6 +1286,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1642,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,8 +1766,8 @@
       <c r="D5" s="6">
         <v>8</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>234</v>
+      <c r="E5" s="12" t="s">
+        <v>233</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>244</v>
@@ -1783,7 +1810,7 @@
         <v>234</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1803,7 +1830,7 @@
         <v>234</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -1823,7 +1850,7 @@
         <v>234</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2079,11 +2106,11 @@
       <c r="D25" s="15">
         <v>10</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>234</v>
+      <c r="E25" s="12" t="s">
+        <v>233</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2099,8 +2126,8 @@
       <c r="D26" s="6">
         <v>3</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>236</v>
+      <c r="E26" s="12" t="s">
+        <v>233</v>
       </c>
       <c r="F26" s="17" t="s">
         <v>246</v>
@@ -2123,7 +2150,7 @@
         <v>236</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2143,7 +2170,7 @@
         <v>236</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2159,11 +2186,11 @@
       <c r="D29" s="6">
         <v>2</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>236</v>
+      <c r="E29" s="12" t="s">
+        <v>233</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2179,10 +2206,12 @@
       <c r="D30" s="6">
         <v>1</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="F30" s="17"/>
+      <c r="E30" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -2377,7 +2406,7 @@
         <v>233</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2397,7 +2426,7 @@
         <v>232</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2529,7 +2558,7 @@
         <v>233</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2565,8 +2594,8 @@
       <c r="D53" s="6">
         <v>4</v>
       </c>
-      <c r="E53" s="13" t="s">
-        <v>236</v>
+      <c r="E53" s="12" t="s">
+        <v>233</v>
       </c>
       <c r="F53" s="17" t="s">
         <v>247</v>
@@ -2583,10 +2612,10 @@
         <v>214</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F54" s="17" t="s">
         <v>248</v>
@@ -2609,7 +2638,7 @@
         <v>241</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2637,16 +2666,16 @@
         <v>124</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D57" s="6">
         <v>1</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F57" s="17" t="s">
         <v>250</v>
@@ -2674,19 +2703,19 @@
     </row>
     <row r="59" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>124</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F59" s="17"/>
     </row>
@@ -2903,7 +2932,7 @@
         <v>236</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2923,7 +2952,7 @@
         <v>233</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2943,7 +2972,7 @@
         <v>233</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -2983,7 +3012,7 @@
         <v>236</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
@@ -3306,7 +3335,7 @@
       <c r="E96" s="14"/>
       <c r="F96" s="17"/>
     </row>
-    <row r="97" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>202</v>
       </c>
@@ -3322,7 +3351,7 @@
       <c r="E97" s="14"/>
       <c r="F97" s="17"/>
     </row>
-    <row r="98" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>138</v>
       </c>
@@ -3335,14 +3364,14 @@
       <c r="D98" s="6">
         <v>5</v>
       </c>
-      <c r="E98" s="13" t="s">
-        <v>234</v>
+      <c r="E98" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="F98" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>139</v>
       </c>
@@ -3355,14 +3384,14 @@
       <c r="D99" s="6">
         <v>5</v>
       </c>
-      <c r="E99" s="13" t="s">
-        <v>236</v>
+      <c r="E99" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="F99" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>140</v>
       </c>
@@ -3375,14 +3404,14 @@
       <c r="D100" s="6">
         <v>5</v>
       </c>
-      <c r="E100" s="13" t="s">
-        <v>236</v>
+      <c r="E100" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="F100" s="17" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>141</v>
       </c>
@@ -3442,7 +3471,7 @@
     </row>
     <row r="104" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>62</v>
@@ -3458,7 +3487,7 @@
     </row>
     <row r="105" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>63</v>
@@ -3586,7 +3615,7 @@
     </row>
     <row r="113" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>97</v>
@@ -3602,7 +3631,7 @@
     </row>
     <row r="114" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
arreglos en gantt y tabla de acctividades, se sube tambien el acta f[008]
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\ProyectoFinal2019-\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3B63AD-B2E2-4D60-BBE5-BC70E88B2F5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3296993-0294-4B9E-9331-3C1D61C41FC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="283">
   <si>
     <t>Nombre</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Tabla de actividades</t>
   </si>
   <si>
-    <t>Pizarra colaborativa del Dia</t>
-  </si>
-  <si>
     <t>Tabla de recursos</t>
   </si>
   <si>
@@ -750,60 +747,21 @@
     <t>Realizado</t>
   </si>
   <si>
-    <t>P[04],S[02],T[01]</t>
-  </si>
-  <si>
-    <t>P[02],S[02],T[04]</t>
-  </si>
-  <si>
-    <t>P[02],S[01],T[04]</t>
-  </si>
-  <si>
-    <t>P[03],S[01],T[03]</t>
-  </si>
-  <si>
-    <t>P[01],S[02],T[02]</t>
-  </si>
-  <si>
     <t>P[04],S[05],T[01]</t>
   </si>
   <si>
-    <t>P[04],S[09],T[01]</t>
-  </si>
-  <si>
-    <t>P[04],S[06],T[01]</t>
-  </si>
-  <si>
-    <t>P[01],S[11],T[02]</t>
-  </si>
-  <si>
-    <t>P[01],S[13],T[02]</t>
-  </si>
-  <si>
     <t>GANTT Primera Vercion</t>
   </si>
   <si>
-    <t>Proy01009</t>
-  </si>
-  <si>
-    <t>Mantenimiento del GANTT</t>
-  </si>
-  <si>
     <t>Duracion del proyecto</t>
   </si>
   <si>
     <t xml:space="preserve">Realizado  </t>
   </si>
   <si>
-    <t>En proseso</t>
-  </si>
-  <si>
     <t xml:space="preserve">En proseso </t>
   </si>
   <si>
-    <t>P[03],S[02],T[02]</t>
-  </si>
-  <si>
     <t>Taller02007</t>
   </si>
   <si>
@@ -819,44 +777,110 @@
     <t>Proy01005 -Proy01006</t>
   </si>
   <si>
-    <t>P[01],P[02],S[01],T[02],T[04]</t>
-  </si>
-  <si>
-    <t>P[03],S[01],T[03],</t>
-  </si>
-  <si>
-    <t>P[04] S[11],T[01]</t>
-  </si>
-  <si>
-    <t>P[02], P[01,T[02],]S[01],T[04]</t>
-  </si>
-  <si>
-    <t>P[01],P[02],S[02],T[04],T[02]</t>
-  </si>
-  <si>
-    <t>P[03],P[04]S[01],T[03],T[01]</t>
-  </si>
-  <si>
-    <t>P[03],S[02],T[04]</t>
-  </si>
-  <si>
-    <t>P[03],S[02],S[14],T[03]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> P[01], S[02], T[02]</t>
-  </si>
-  <si>
-    <t>P[03], P[04], S[08], T[01], T[03]</t>
-  </si>
-  <si>
-    <t>P[04],S[11],T[01]</t>
+    <t>Replanificacion</t>
+  </si>
+  <si>
+    <t>P[01],S[02],P[02],T[02],T[04],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],S[02],T[01],P[01];T[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[02],S[02],T[04],P[03],T[03],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],S[02],T[01],P[02],T[04],S[07]</t>
+  </si>
+  <si>
+    <t>P[02], P[04],T[01],]S[01],T[04],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],P[03],P[04],S[02],T[02],T[03],T[04],T[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],S[01],T[02],T[04],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[03],P[04]S[01],T[03],T[01],T[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],T[04],T[02],S[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],T[04],T[02],S[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],T[02],T[04],S[02],S[14],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],T[02],S[14],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],P[04],T[01],T[02],T[04],S[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[03], P[04], S[08], T[01], T[03],S[07]</t>
+  </si>
+  <si>
+    <t>P[03],S[01],T[03],S[07]</t>
+  </si>
+  <si>
+    <t>P[03],S[02],T[03],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],S[02],T[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],S[11],T[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],P[01],S[02],T[02],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],S[02],T[04],T[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],P[03],S[09],T[03],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[03],S[09],T[02],T[03],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],P[01],S[06],T[02],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],P[03],S[11],T[03],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],P[02],S[03],T[04],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[03],S[02],T[03],T[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],P[03],S[02],T[03],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[04],P[02],S[11],T[04],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],P[04],S[02],T[01],T[04],T[02],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[04],S[09],T[02],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[02],S[13],T[02],T[04],S[07]</t>
+  </si>
+  <si>
+    <t>P[01],P[04],S[13],T[02],T[01],S[07]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1641,25 +1665,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L99" sqref="L99"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="114" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="31"/>
@@ -1667,172 +1691,172 @@
       <c r="E1" s="32"/>
       <c r="F1" s="33"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
       <c r="A2" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E2" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="18.75">
       <c r="A3" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="22">
         <v>3</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="26.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
       <c r="A5" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" s="6">
         <v>8</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75">
       <c r="A6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="6">
         <v>20</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75">
       <c r="A7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="6">
-        <v>2</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="C8" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="6">
         <v>6</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8">
         <v>43641</v>
@@ -1843,12 +1867,12 @@
       <c r="E10" s="13"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="8">
         <v>43641</v>
@@ -1859,12 +1883,12 @@
       <c r="E11" s="13"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="8">
         <v>43641</v>
@@ -1875,12 +1899,12 @@
       <c r="E12" s="13"/>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="18.75">
       <c r="A13" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="8">
         <v>43641</v>
@@ -1891,12 +1915,12 @@
       <c r="E13" s="13"/>
       <c r="F13" s="16"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="18.75">
       <c r="A14" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="8">
         <v>43641</v>
@@ -1907,12 +1931,12 @@
       <c r="E14" s="13"/>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="18.75">
       <c r="A15" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="8">
         <v>43641</v>
@@ -1923,12 +1947,12 @@
       <c r="E15" s="13"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="18.75">
       <c r="A16" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="8">
         <v>43712</v>
@@ -1939,12 +1963,12 @@
       <c r="E16" s="13"/>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="18.75">
       <c r="A17" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="8">
         <v>43712</v>
@@ -1955,12 +1979,12 @@
       <c r="E17" s="13"/>
       <c r="F17" s="16"/>
     </row>
-    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75">
       <c r="A18" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="8">
         <v>43712</v>
@@ -1971,12 +1995,12 @@
       <c r="E18" s="13"/>
       <c r="F18" s="16"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="8">
         <v>43712</v>
@@ -1987,12 +2011,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="8">
         <v>43712</v>
@@ -2003,12 +2027,12 @@
       <c r="E20" s="13"/>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="8">
         <v>43712</v>
@@ -2019,12 +2043,12 @@
       <c r="E21" s="13"/>
       <c r="F21" s="16"/>
     </row>
-    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="8">
         <v>43712</v>
@@ -2035,12 +2059,12 @@
       <c r="E22" s="13"/>
       <c r="F22" s="16"/>
     </row>
-    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="8">
         <v>43712</v>
@@ -2051,12 +2075,12 @@
       <c r="E23" s="13"/>
       <c r="F23" s="16"/>
     </row>
-    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="8">
         <v>43712</v>
@@ -2067,132 +2091,132 @@
       <c r="E24" s="13"/>
       <c r="F24" s="16"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="C25" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D25" s="14">
         <v>10</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="18.75">
       <c r="A26" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D26" s="6">
         <v>3</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18.75">
       <c r="A27" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26.25" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="18.75">
       <c r="A29" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D29" s="6">
         <v>2</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="18.75">
       <c r="A30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="6">
         <v>1</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="18.75">
       <c r="A31" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="8">
         <v>43641</v>
@@ -2203,12 +2227,12 @@
       <c r="E31" s="13"/>
       <c r="F31" s="16"/>
     </row>
-    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75">
       <c r="A32" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="8">
         <v>43641</v>
@@ -2219,12 +2243,12 @@
       <c r="E32" s="13"/>
       <c r="F32" s="16"/>
     </row>
-    <row r="33" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18.75">
       <c r="A33" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="8">
         <v>43641</v>
@@ -2235,12 +2259,12 @@
       <c r="E33" s="13"/>
       <c r="F33" s="16"/>
     </row>
-    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75">
       <c r="A34" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="8">
         <v>43641</v>
@@ -2251,12 +2275,12 @@
       <c r="E34" s="13"/>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75">
       <c r="A35" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="8">
         <v>43641</v>
@@ -2267,12 +2291,12 @@
       <c r="E35" s="13"/>
       <c r="F35" s="16"/>
     </row>
-    <row r="36" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75">
       <c r="A36" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="8">
         <v>43641</v>
@@ -2283,12 +2307,12 @@
       <c r="E36" s="13"/>
       <c r="F36" s="16"/>
     </row>
-    <row r="37" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C37" s="8">
         <v>43641</v>
@@ -2299,12 +2323,12 @@
       <c r="E37" s="13"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18.75">
       <c r="A38" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="8">
         <v>43712</v>
@@ -2315,12 +2339,12 @@
       <c r="E38" s="13"/>
       <c r="F38" s="16"/>
     </row>
-    <row r="39" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="18.75">
       <c r="A39" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" s="8">
         <v>43712</v>
@@ -2331,12 +2355,12 @@
       <c r="E39" s="13"/>
       <c r="F39" s="16"/>
     </row>
-    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="18.75">
       <c r="A40" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C40" s="8">
         <v>43712</v>
@@ -2347,12 +2371,12 @@
       <c r="E40" s="13"/>
       <c r="F40" s="16"/>
     </row>
-    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="18.75">
       <c r="A41" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="8">
         <v>43712</v>
@@ -2363,52 +2387,52 @@
       <c r="E41" s="13"/>
       <c r="F41" s="16"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D42" s="14">
         <v>2</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="18.75">
       <c r="A43" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D43" s="6">
         <v>13</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="18.75">
       <c r="A44" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="8">
         <v>43641</v>
@@ -2419,12 +2443,12 @@
       <c r="E44" s="13"/>
       <c r="F44" s="16"/>
     </row>
-    <row r="45" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="18.75">
       <c r="A45" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="8">
         <v>43641</v>
@@ -2435,12 +2459,12 @@
       <c r="E45" s="13"/>
       <c r="F45" s="16"/>
     </row>
-    <row r="46" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="18.75">
       <c r="A46" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="8">
         <v>43641</v>
@@ -2451,12 +2475,12 @@
       <c r="E46" s="13"/>
       <c r="F46" s="16"/>
     </row>
-    <row r="47" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="18.75">
       <c r="A47" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="8">
         <v>43641</v>
@@ -2467,12 +2491,12 @@
       <c r="E47" s="13"/>
       <c r="F47" s="16"/>
     </row>
-    <row r="48" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="18.75">
       <c r="A48" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" s="8">
         <v>43712</v>
@@ -2483,12 +2507,12 @@
       <c r="E48" s="13"/>
       <c r="F48" s="16"/>
     </row>
-    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="18.75">
       <c r="A49" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="8">
         <v>43712</v>
@@ -2499,12 +2523,12 @@
       <c r="E49" s="13"/>
       <c r="F49" s="16"/>
     </row>
-    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="18.75">
       <c r="A50" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C50" s="8">
         <v>43712</v>
@@ -2515,185 +2539,183 @@
       <c r="E50" s="13"/>
       <c r="F50" s="16"/>
     </row>
-    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="18.75">
       <c r="A51" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D51" s="6">
         <v>3</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="18.75">
       <c r="A52" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D52" s="6">
         <v>1</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="18.75">
       <c r="A53" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D53" s="6">
         <v>4</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="18.75">
       <c r="A54" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="18.75">
+      <c r="A55" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D55" s="6">
         <v>1</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="18.75">
       <c r="A56" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D56" s="6">
         <v>1</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="18.75">
       <c r="A57" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="D57" s="6">
         <v>1</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="18.75">
       <c r="A58" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D58" s="6">
         <v>2</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="18.75">
       <c r="A59" s="4" t="s">
-        <v>252</v>
+        <v>158</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>256</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C59" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D59" s="7">
+        <v>2</v>
+      </c>
+      <c r="E59" s="13"/>
       <c r="F59" s="16"/>
     </row>
-    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="18.75">
       <c r="A60" s="4" t="s">
         <v>159</v>
       </c>
@@ -2709,7 +2731,7 @@
       <c r="E60" s="13"/>
       <c r="F60" s="16"/>
     </row>
-    <row r="61" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="4" t="s">
         <v>160</v>
       </c>
@@ -2725,119 +2747,119 @@
       <c r="E61" s="13"/>
       <c r="F61" s="16"/>
     </row>
-    <row r="62" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="18.75">
       <c r="A62" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="C62" s="8">
         <v>43641</v>
       </c>
-      <c r="D62" s="7">
-        <v>2</v>
+      <c r="D62" s="14">
+        <v>1</v>
       </c>
       <c r="E62" s="13"/>
       <c r="F62" s="16"/>
     </row>
-    <row r="63" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="18.75">
       <c r="A63" s="4" t="s">
         <v>162</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C63" s="8">
         <v>43641</v>
       </c>
-      <c r="D63" s="14">
+      <c r="D63" s="7">
         <v>1</v>
       </c>
       <c r="E63" s="13"/>
       <c r="F63" s="16"/>
     </row>
-    <row r="64" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="18.75">
       <c r="A64" s="4" t="s">
         <v>163</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D64" s="7">
-        <v>1</v>
+      <c r="C64" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" s="14">
+        <v>3</v>
       </c>
       <c r="E64" s="13"/>
       <c r="F64" s="16"/>
     </row>
-    <row r="65" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="4" t="s">
-        <v>164</v>
+        <v>218</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D65" s="14">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="C65" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D65" s="6">
+        <v>1</v>
       </c>
       <c r="E65" s="13"/>
       <c r="F65" s="16"/>
     </row>
-    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C66" s="8">
         <v>43712</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66" s="7">
         <v>1</v>
       </c>
       <c r="E66" s="13"/>
       <c r="F66" s="16"/>
     </row>
-    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D67" s="7">
-        <v>1</v>
+      <c r="D67" s="6">
+        <v>3</v>
       </c>
       <c r="E67" s="13"/>
       <c r="F67" s="16"/>
     </row>
-    <row r="68" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="4" t="s">
         <v>194</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C68" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D68" s="6">
-        <v>3</v>
+      <c r="C68" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D68" s="7">
+        <v>2</v>
       </c>
       <c r="E68" s="13"/>
       <c r="F68" s="16"/>
     </row>
-    <row r="69" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="4" t="s">
         <v>195</v>
       </c>
@@ -2853,23 +2875,27 @@
       <c r="E69" s="13"/>
       <c r="F69" s="16"/>
     </row>
-    <row r="70" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="4" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C70" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D70" s="7">
-        <v>2</v>
-      </c>
-      <c r="E70" s="13"/>
-      <c r="F70" s="16"/>
-    </row>
-    <row r="71" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D70" s="6">
+        <v>1</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="18.75">
       <c r="A71" s="4" t="s">
         <v>127</v>
       </c>
@@ -2877,19 +2903,19 @@
         <v>18</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>214</v>
+        <v>126</v>
       </c>
       <c r="D71" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="18.75">
       <c r="A72" s="4" t="s">
         <v>128</v>
       </c>
@@ -2897,101 +2923,97 @@
         <v>19</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>127</v>
+        <v>213</v>
       </c>
       <c r="D72" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F72" s="16" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="18.75">
       <c r="A73" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D73" s="6">
         <v>3</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="18.75">
       <c r="A74" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D74" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="18.75">
       <c r="A75" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D75" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="18.75">
       <c r="A76" s="4" t="s">
-        <v>132</v>
+        <v>219</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D76" s="6">
+        <v>52</v>
+      </c>
+      <c r="C76" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D76" s="14">
         <v>1</v>
       </c>
-      <c r="E76" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E76" s="13"/>
+      <c r="F76" s="16"/>
+    </row>
+    <row r="77" spans="1:6" ht="18.75">
       <c r="A77" s="4" t="s">
-        <v>220</v>
+        <v>164</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>53</v>
@@ -2999,13 +3021,13 @@
       <c r="C77" s="8">
         <v>43641</v>
       </c>
-      <c r="D77" s="14">
-        <v>1</v>
+      <c r="D77" s="7">
+        <v>2</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="16"/>
     </row>
-    <row r="78" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="18.75">
       <c r="A78" s="4" t="s">
         <v>165</v>
       </c>
@@ -3021,7 +3043,7 @@
       <c r="E78" s="13"/>
       <c r="F78" s="16"/>
     </row>
-    <row r="79" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="4" t="s">
         <v>166</v>
       </c>
@@ -3037,7 +3059,7 @@
       <c r="E79" s="13"/>
       <c r="F79" s="16"/>
     </row>
-    <row r="80" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="4" t="s">
         <v>167</v>
       </c>
@@ -3053,15 +3075,15 @@
       <c r="E80" s="13"/>
       <c r="F80" s="16"/>
     </row>
-    <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="18.75">
       <c r="A81" s="4" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="C81" s="8">
-        <v>43641</v>
+        <v>43712</v>
       </c>
       <c r="D81" s="7">
         <v>2</v>
@@ -3069,9 +3091,9 @@
       <c r="E81" s="13"/>
       <c r="F81" s="16"/>
     </row>
-    <row r="82" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="18.75">
       <c r="A82" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>90</v>
@@ -3085,9 +3107,9 @@
       <c r="E82" s="13"/>
       <c r="F82" s="16"/>
     </row>
-    <row r="83" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="18.75">
       <c r="A83" s="4" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>91</v>
@@ -3101,7 +3123,7 @@
       <c r="E83" s="13"/>
       <c r="F83" s="16"/>
     </row>
-    <row r="84" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="4" t="s">
         <v>197</v>
       </c>
@@ -3117,7 +3139,7 @@
       <c r="E84" s="13"/>
       <c r="F84" s="16"/>
     </row>
-    <row r="85" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="4" t="s">
         <v>198</v>
       </c>
@@ -3133,23 +3155,23 @@
       <c r="E85" s="13"/>
       <c r="F85" s="16"/>
     </row>
-    <row r="86" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="18.75">
       <c r="A86" s="4" t="s">
-        <v>199</v>
+        <v>132</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C86" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D86" s="7">
-        <v>2</v>
+        <v>23</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D86" s="6">
+        <v>1</v>
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="16"/>
     </row>
-    <row r="87" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="18.75">
       <c r="A87" s="4" t="s">
         <v>133</v>
       </c>
@@ -3157,7 +3179,7 @@
         <v>24</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D87" s="6">
         <v>1</v>
@@ -3165,7 +3187,7 @@
       <c r="E87" s="13"/>
       <c r="F87" s="16"/>
     </row>
-    <row r="88" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="18.75">
       <c r="A88" s="4" t="s">
         <v>134</v>
       </c>
@@ -3173,15 +3195,15 @@
         <v>25</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D88" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E88" s="13"/>
       <c r="F88" s="16"/>
     </row>
-    <row r="89" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="18.75">
       <c r="A89" s="4" t="s">
         <v>135</v>
       </c>
@@ -3189,31 +3211,31 @@
         <v>26</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D89" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E89" s="13"/>
       <c r="F89" s="16"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="18.75">
       <c r="A90" s="4" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>214</v>
+        <v>57</v>
+      </c>
+      <c r="C90" s="8">
+        <v>43641</v>
       </c>
       <c r="D90" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90" s="13"/>
       <c r="F90" s="16"/>
     </row>
-    <row r="91" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="18.75">
       <c r="A91" s="4" t="s">
         <v>169</v>
       </c>
@@ -3224,28 +3246,28 @@
         <v>43641</v>
       </c>
       <c r="D91" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E91" s="13"/>
       <c r="F91" s="16"/>
     </row>
-    <row r="92" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="18.75">
       <c r="A92" s="4" t="s">
         <v>170</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C92" s="8">
-        <v>43641</v>
+      <c r="C92" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="D92" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E92" s="13"/>
       <c r="F92" s="16"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="18.75">
       <c r="A93" s="4" t="s">
         <v>171</v>
       </c>
@@ -3253,31 +3275,31 @@
         <v>60</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D93" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E93" s="13"/>
       <c r="F93" s="16"/>
     </row>
-    <row r="94" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="18.75">
       <c r="A94" s="4" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D94" s="6">
-        <v>3</v>
+        <v>94</v>
+      </c>
+      <c r="C94" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D94" s="15">
+        <v>2</v>
       </c>
       <c r="E94" s="13"/>
       <c r="F94" s="16"/>
     </row>
-    <row r="95" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="18.75">
       <c r="A95" s="4" t="s">
         <v>200</v>
       </c>
@@ -3293,12 +3315,12 @@
       <c r="E95" s="13"/>
       <c r="F95" s="16"/>
     </row>
-    <row r="96" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="19.5" thickBot="1">
       <c r="A96" s="4" t="s">
         <v>201</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="C96" s="8">
         <v>43712</v>
@@ -3309,23 +3331,27 @@
       <c r="E96" s="13"/>
       <c r="F96" s="16"/>
     </row>
-    <row r="97" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
       <c r="A97" s="4" t="s">
-        <v>202</v>
+        <v>137</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C97" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D97" s="15">
-        <v>2</v>
-      </c>
-      <c r="E97" s="13"/>
-      <c r="F97" s="16"/>
-    </row>
-    <row r="98" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D97" s="6">
+        <v>5</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="F97" s="16" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
       <c r="A98" s="4" t="s">
         <v>138</v>
       </c>
@@ -3333,19 +3359,19 @@
         <v>28</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D98" s="6">
         <v>5</v>
       </c>
       <c r="E98" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F98" s="16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
       <c r="A99" s="4" t="s">
         <v>139</v>
       </c>
@@ -3353,19 +3379,19 @@
         <v>29</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>214</v>
+        <v>138</v>
       </c>
       <c r="D99" s="6">
         <v>5</v>
       </c>
       <c r="E99" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F99" s="16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="19.5" thickTop="1">
       <c r="A100" s="4" t="s">
         <v>140</v>
       </c>
@@ -3378,14 +3404,14 @@
       <c r="D100" s="6">
         <v>5</v>
       </c>
-      <c r="E100" s="28" t="s">
-        <v>233</v>
+      <c r="E100" s="11" t="s">
+        <v>232</v>
       </c>
       <c r="F100" s="16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="18.75">
       <c r="A101" s="4" t="s">
         <v>141</v>
       </c>
@@ -3393,19 +3419,19 @@
         <v>31</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D101" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F101" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="18.75">
       <c r="A102" s="4" t="s">
         <v>142</v>
       </c>
@@ -3413,39 +3439,37 @@
         <v>32</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>143</v>
+        <v>224</v>
       </c>
       <c r="D102" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F102" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="18.75">
       <c r="A103" s="4" t="s">
-        <v>143</v>
+        <v>245</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>225</v>
+        <v>61</v>
+      </c>
+      <c r="C103" s="8">
+        <v>43641</v>
       </c>
       <c r="D103" s="6">
-        <v>2</v>
-      </c>
-      <c r="E103" s="11" t="s">
-        <v>233</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E103" s="13"/>
       <c r="F103" s="16"/>
     </row>
-    <row r="104" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="18.75">
       <c r="A104" s="4" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>62</v>
@@ -3453,15 +3477,15 @@
       <c r="C104" s="8">
         <v>43641</v>
       </c>
-      <c r="D104" s="6">
-        <v>4</v>
+      <c r="D104" s="7">
+        <v>2</v>
       </c>
       <c r="E104" s="13"/>
       <c r="F104" s="16"/>
     </row>
-    <row r="105" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="18.75">
       <c r="A105" s="4" t="s">
-        <v>260</v>
+        <v>172</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>63</v>
@@ -3475,7 +3499,7 @@
       <c r="E105" s="13"/>
       <c r="F105" s="16"/>
     </row>
-    <row r="106" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="18.75">
       <c r="A106" s="4" t="s">
         <v>173</v>
       </c>
@@ -3491,7 +3515,7 @@
       <c r="E106" s="13"/>
       <c r="F106" s="16"/>
     </row>
-    <row r="107" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="18.75">
       <c r="A107" s="4" t="s">
         <v>174</v>
       </c>
@@ -3507,7 +3531,7 @@
       <c r="E107" s="13"/>
       <c r="F107" s="16"/>
     </row>
-    <row r="108" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="18.75">
       <c r="A108" s="4" t="s">
         <v>175</v>
       </c>
@@ -3523,7 +3547,7 @@
       <c r="E108" s="13"/>
       <c r="F108" s="16"/>
     </row>
-    <row r="109" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="18.75">
       <c r="A109" s="4" t="s">
         <v>176</v>
       </c>
@@ -3539,7 +3563,7 @@
       <c r="E109" s="13"/>
       <c r="F109" s="16"/>
     </row>
-    <row r="110" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="18.75">
       <c r="A110" s="4" t="s">
         <v>177</v>
       </c>
@@ -3555,7 +3579,7 @@
       <c r="E110" s="13"/>
       <c r="F110" s="16"/>
     </row>
-    <row r="111" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="18.75">
       <c r="A111" s="4" t="s">
         <v>178</v>
       </c>
@@ -3571,15 +3595,15 @@
       <c r="E111" s="13"/>
       <c r="F111" s="16"/>
     </row>
-    <row r="112" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="18.75">
       <c r="A112" s="4" t="s">
-        <v>179</v>
+        <v>247</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C112" s="8">
-        <v>43641</v>
+        <v>43712</v>
       </c>
       <c r="D112" s="7">
         <v>2</v>
@@ -3587,9 +3611,9 @@
       <c r="E112" s="13"/>
       <c r="F112" s="16"/>
     </row>
-    <row r="113" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="18.75">
       <c r="A113" s="4" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>97</v>
@@ -3603,9 +3627,9 @@
       <c r="E113" s="13"/>
       <c r="F113" s="16"/>
     </row>
-    <row r="114" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="18.75">
       <c r="A114" s="4" t="s">
-        <v>262</v>
+        <v>202</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>98</v>
@@ -3619,7 +3643,7 @@
       <c r="E114" s="13"/>
       <c r="F114" s="16"/>
     </row>
-    <row r="115" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="18.75">
       <c r="A115" s="4" t="s">
         <v>203</v>
       </c>
@@ -3635,7 +3659,7 @@
       <c r="E115" s="13"/>
       <c r="F115" s="16"/>
     </row>
-    <row r="116" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="18.75">
       <c r="A116" s="4" t="s">
         <v>204</v>
       </c>
@@ -3651,7 +3675,7 @@
       <c r="E116" s="13"/>
       <c r="F116" s="16"/>
     </row>
-    <row r="117" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="18.75">
       <c r="A117" s="4" t="s">
         <v>205</v>
       </c>
@@ -3667,7 +3691,7 @@
       <c r="E117" s="13"/>
       <c r="F117" s="16"/>
     </row>
-    <row r="118" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="18.75">
       <c r="A118" s="4" t="s">
         <v>206</v>
       </c>
@@ -3683,7 +3707,7 @@
       <c r="E118" s="13"/>
       <c r="F118" s="16"/>
     </row>
-    <row r="119" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="18.75">
       <c r="A119" s="4" t="s">
         <v>207</v>
       </c>
@@ -3699,60 +3723,44 @@
       <c r="E119" s="13"/>
       <c r="F119" s="16"/>
     </row>
-    <row r="120" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="19.5" thickBot="1">
       <c r="A120" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C120" s="8">
+      <c r="C120" s="9">
         <v>43712</v>
       </c>
-      <c r="D120" s="7">
-        <v>2</v>
-      </c>
-      <c r="E120" s="13"/>
-      <c r="F120" s="16"/>
-    </row>
-    <row r="121" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C121" s="9">
-        <v>43712</v>
-      </c>
-      <c r="D121" s="17">
-        <v>2</v>
-      </c>
-      <c r="E121" s="18"/>
-      <c r="F121" s="19"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="10"/>
+      <c r="D120" s="17">
+        <v>2</v>
+      </c>
+      <c r="E120" s="18"/>
+      <c r="F120" s="19"/>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="10"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E122" s="5"/>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
-      <c r="E123" s="5"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-    </row>
-    <row r="128" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="127" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="129" ht="26.25" customHeight="1"/>
+    <row r="130" ht="27.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Micro correcion en el MER y MR de cliente
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudios\ProyectoFinal2019-\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\estudios\utu de informatica avansada\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FCE5A3-981D-40DD-9A2F-F64AB7809083}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC4DE3A-4CA2-45EB-B7DA-C0119D46E992}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="286">
   <si>
     <t>Nombre</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Estudio de factibilidades</t>
   </si>
   <si>
-    <t>Diagrama de clases, secuencia y estados</t>
-  </si>
-  <si>
     <t>Especificación de procesos</t>
   </si>
   <si>
@@ -564,12 +561,6 @@
     <t>Taller02015</t>
   </si>
   <si>
-    <t>ADA03013</t>
-  </si>
-  <si>
-    <t>ADA03014</t>
-  </si>
-  <si>
     <t>ADA03015</t>
   </si>
   <si>
@@ -865,13 +856,40 @@
   </si>
   <si>
     <t>P[01],P[04],S[13],T[02],T[01],S[07]</t>
+  </si>
+  <si>
+    <t>ADA02013</t>
+  </si>
+  <si>
+    <t>ADA02014</t>
+  </si>
+  <si>
+    <t>ADA03023</t>
+  </si>
+  <si>
+    <t>ADA03024</t>
+  </si>
+  <si>
+    <t>Diagrama de clases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digrama secuencial </t>
+  </si>
+  <si>
+    <t>Diagrama de Estados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin asignar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin comenzar </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -933,8 +951,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -952,8 +990,18 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1181,12 +1229,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1264,9 +1329,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Entrada" xfId="3" builtinId="20"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1642,10 +1715,10 @@
   <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
@@ -1655,9 +1728,9 @@
     <col min="6" max="6" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="114" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="30"/>
@@ -1665,169 +1738,169 @@
       <c r="E1" s="31"/>
       <c r="F1" s="32"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
       <c r="A2" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75">
       <c r="A3" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="21">
         <v>3</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="26.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
       <c r="A5" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D5" s="6">
         <v>8</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.75">
       <c r="A6" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="6">
         <v>20</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.75">
       <c r="A7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="6">
         <v>2</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="6">
         <v>6</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>33</v>
@@ -1835,15 +1908,15 @@
       <c r="C10" s="8">
         <v>43641</v>
       </c>
-      <c r="D10" s="7">
-        <v>2</v>
-      </c>
-      <c r="E10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="33" t="s">
+        <v>284</v>
+      </c>
       <c r="F10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>34</v>
@@ -1851,15 +1924,15 @@
       <c r="C11" s="8">
         <v>43641</v>
       </c>
-      <c r="D11" s="7">
-        <v>2</v>
-      </c>
-      <c r="E11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="33" t="s">
+        <v>284</v>
+      </c>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>35</v>
@@ -1867,15 +1940,15 @@
       <c r="C12" s="8">
         <v>43641</v>
       </c>
-      <c r="D12" s="7">
-        <v>2</v>
-      </c>
-      <c r="E12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="33" t="s">
+        <v>284</v>
+      </c>
       <c r="F12" s="15"/>
     </row>
-    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="18.75">
       <c r="A13" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>36</v>
@@ -1883,69 +1956,69 @@
       <c r="C13" s="8">
         <v>43641</v>
       </c>
-      <c r="D13" s="7">
-        <v>2</v>
-      </c>
-      <c r="E13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="33" t="s">
+        <v>284</v>
+      </c>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="18.75">
       <c r="A14" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C14" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75">
+      <c r="A15" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C15" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75">
+      <c r="A16" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C16" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75">
+      <c r="A17" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D14" s="7">
-        <v>2</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D15" s="7">
-        <v>2</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D16" s="7">
-        <v>2</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C17" s="8">
-        <v>43712</v>
+        <v>43641</v>
       </c>
       <c r="D17" s="7">
         <v>2</v>
@@ -1953,12 +2026,12 @@
       <c r="E17" s="12"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75">
       <c r="A18" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C18" s="8">
         <v>43712</v>
@@ -1969,12 +2042,12 @@
       <c r="E18" s="12"/>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75">
       <c r="A19" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C19" s="8">
         <v>43712</v>
@@ -1985,12 +2058,12 @@
       <c r="E19" s="12"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75">
       <c r="A20" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" s="8">
         <v>43712</v>
@@ -2001,12 +2074,12 @@
       <c r="E20" s="12"/>
       <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75">
       <c r="A21" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C21" s="8">
         <v>43712</v>
@@ -2017,12 +2090,12 @@
       <c r="E21" s="12"/>
       <c r="F21" s="15"/>
     </row>
-    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C22" s="8">
         <v>43712</v>
@@ -2033,12 +2106,12 @@
       <c r="E22" s="12"/>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C23" s="8">
         <v>43712</v>
@@ -2049,12 +2122,12 @@
       <c r="E23" s="12"/>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C24" s="8">
         <v>43712</v>
@@ -2065,263 +2138,253 @@
       <c r="E24" s="12"/>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="4" t="s">
-        <v>214</v>
+        <v>279</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="13">
+        <v>76</v>
+      </c>
+      <c r="C25" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D25" s="7">
+        <v>2</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.75">
+      <c r="A26" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" spans="1:6" ht="18.75">
+      <c r="A27" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="13">
         <v>10</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="E27" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26.25" customHeight="1">
+      <c r="A28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" s="6">
+        <v>3</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="18.75">
+      <c r="A29" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D26" s="6">
-        <v>3</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="18.75">
+      <c r="A30" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="6">
-        <v>1</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D29" s="6">
-        <v>2</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C30" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D30" s="6">
         <v>1</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="18.75">
       <c r="A31" s="4" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D31" s="7">
-        <v>2</v>
-      </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="15"/>
-    </row>
-    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D31" s="6">
+        <v>2</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="18.75">
       <c r="A32" s="4" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D32" s="7">
-        <v>2</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="15"/>
-    </row>
-    <row r="33" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18.75">
       <c r="A33" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C33" s="8">
         <v>43641</v>
       </c>
-      <c r="D33" s="7">
-        <v>2</v>
+      <c r="D33" s="13">
+        <v>8</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="15"/>
     </row>
-    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75">
       <c r="A34" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C34" s="8">
         <v>43641</v>
       </c>
-      <c r="D34" s="7">
-        <v>2</v>
-      </c>
+      <c r="D34" s="13"/>
       <c r="E34" s="12"/>
       <c r="F34" s="15"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75">
       <c r="A35" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C35" s="8">
         <v>43641</v>
       </c>
-      <c r="D35" s="7">
-        <v>2</v>
-      </c>
+      <c r="D35" s="13"/>
       <c r="E35" s="12"/>
       <c r="F35" s="15"/>
     </row>
-    <row r="36" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75">
       <c r="A36" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C36" s="8">
         <v>43641</v>
       </c>
-      <c r="D36" s="7">
-        <v>2</v>
-      </c>
+      <c r="D36" s="13"/>
       <c r="E36" s="12"/>
       <c r="F36" s="15"/>
     </row>
-    <row r="37" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>223</v>
+        <v>42</v>
       </c>
       <c r="C37" s="8">
         <v>43641</v>
       </c>
-      <c r="D37" s="7">
-        <v>2</v>
-      </c>
+      <c r="D37" s="13"/>
       <c r="E37" s="12"/>
       <c r="F37" s="15"/>
     </row>
-    <row r="38" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18.75">
       <c r="A38" s="4" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C38" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D38" s="7">
-        <v>2</v>
-      </c>
+        <v>43641</v>
+      </c>
+      <c r="D38" s="13"/>
       <c r="E38" s="12"/>
       <c r="F38" s="15"/>
     </row>
-    <row r="39" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="18.75">
       <c r="A39" s="4" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>220</v>
       </c>
       <c r="C39" s="8">
-        <v>43712</v>
+        <v>43641</v>
       </c>
       <c r="D39" s="7">
         <v>2</v>
@@ -2329,12 +2392,12 @@
       <c r="E39" s="12"/>
       <c r="F39" s="15"/>
     </row>
-    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="18.75">
       <c r="A40" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C40" s="8">
         <v>43712</v>
@@ -2345,12 +2408,12 @@
       <c r="E40" s="12"/>
       <c r="F40" s="15"/>
     </row>
-    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="18.75">
       <c r="A41" s="4" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C41" s="8">
         <v>43712</v>
@@ -2361,732 +2424,714 @@
       <c r="E41" s="12"/>
       <c r="F41" s="15"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D42" s="7">
+        <v>2</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="15"/>
+    </row>
+    <row r="43" spans="1:6" ht="18.75">
+      <c r="A43" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D43" s="7">
+        <v>2</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="15"/>
+    </row>
+    <row r="44" spans="1:6" ht="18.75">
+      <c r="A44" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D44" s="13">
+        <v>2</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="18.75">
+      <c r="A45" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D42" s="13">
-        <v>2</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F42" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D43" s="6">
+      <c r="C45" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D45" s="6">
         <v>13</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D44" s="6">
-        <v>4</v>
-      </c>
-      <c r="E44" s="12"/>
-      <c r="F44" s="15"/>
-    </row>
-    <row r="45" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D45" s="6">
-        <v>8</v>
-      </c>
-      <c r="E45" s="12"/>
-      <c r="F45" s="15"/>
-    </row>
-    <row r="46" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="E45" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="18.75">
       <c r="A46" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C46" s="8">
         <v>43641</v>
       </c>
       <c r="D46" s="6">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="18.75">
       <c r="A47" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C47" s="8">
         <v>43641</v>
       </c>
-      <c r="D47" s="7">
-        <v>2</v>
+      <c r="D47" s="6">
+        <v>9</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="15"/>
     </row>
-    <row r="48" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="18.75">
       <c r="A48" s="4" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C48" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D48" s="6">
-        <v>4</v>
+        <v>43641</v>
+      </c>
+      <c r="D48" s="13">
+        <v>17</v>
       </c>
       <c r="E48" s="12"/>
       <c r="F48" s="15"/>
     </row>
-    <row r="49" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="18.75">
       <c r="A49" s="4" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="C49" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D49" s="7">
-        <v>2</v>
+        <v>43641</v>
+      </c>
+      <c r="D49" s="13">
+        <v>5</v>
       </c>
       <c r="E49" s="12"/>
       <c r="F49" s="15"/>
     </row>
-    <row r="50" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="18.75">
       <c r="A50" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C50" s="8">
         <v>43712</v>
       </c>
-      <c r="D50" s="7">
-        <v>2</v>
+      <c r="D50" s="6">
+        <v>4</v>
       </c>
       <c r="E50" s="12"/>
       <c r="F50" s="15"/>
     </row>
-    <row r="51" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="18.75">
       <c r="A51" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D51" s="7">
+        <v>2</v>
+      </c>
+      <c r="E51" s="12"/>
+      <c r="F51" s="15"/>
+    </row>
+    <row r="52" spans="1:6" ht="18.75">
+      <c r="A52" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D52" s="7">
+        <v>2</v>
+      </c>
+      <c r="E52" s="12"/>
+      <c r="F52" s="15"/>
+    </row>
+    <row r="53" spans="1:6" ht="18.75">
+      <c r="A53" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D53" s="6">
+        <v>3</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="18.75">
+      <c r="A54" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D51" s="6">
-        <v>3</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F51" s="15" t="s">
+      <c r="B54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D54" s="6">
+        <v>1</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F54" s="15" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+    <row r="55" spans="1:6" ht="18.75">
+      <c r="A55" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D52" s="6">
-        <v>1</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="B55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D55" s="6">
+        <v>4</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="18.75">
+      <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D53" s="6">
-        <v>4</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="B56" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="18.75">
+      <c r="A57" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D55" s="6">
-        <v>1</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D56" s="6">
-        <v>1</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F56" s="15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="C57" s="6" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="D57" s="6">
         <v>1</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="18.75">
       <c r="A58" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" s="6">
+        <v>1</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="18.75">
+      <c r="A59" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D59" s="6">
+        <v>1</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="18.75">
+      <c r="A60" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D58" s="6">
-        <v>2</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F58" s="15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C59" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D59" s="7">
-        <v>2</v>
-      </c>
-      <c r="E59" s="12"/>
-      <c r="F59" s="15"/>
-    </row>
-    <row r="60" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C60" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D60" s="7">
-        <v>2</v>
-      </c>
-      <c r="E60" s="12"/>
-      <c r="F60" s="15"/>
-    </row>
-    <row r="61" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="C60" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D60" s="6">
+        <v>2</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C61" s="8">
         <v>43641</v>
       </c>
-      <c r="D61" s="7">
-        <v>2</v>
-      </c>
+      <c r="D61" s="13"/>
       <c r="E61" s="12"/>
       <c r="F61" s="15"/>
     </row>
-    <row r="62" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="18.75">
       <c r="A62" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C62" s="8">
         <v>43641</v>
       </c>
-      <c r="D62" s="13">
-        <v>1</v>
-      </c>
+      <c r="D62" s="13"/>
       <c r="E62" s="12"/>
       <c r="F62" s="15"/>
     </row>
-    <row r="63" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="18.75">
       <c r="A63" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C63" s="8">
         <v>43641</v>
       </c>
-      <c r="D63" s="7">
-        <v>1</v>
+      <c r="D63" s="13">
+        <v>4</v>
       </c>
       <c r="E63" s="12"/>
       <c r="F63" s="15"/>
     </row>
-    <row r="64" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="18.75">
       <c r="A64" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D64" s="13">
-        <v>3</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C64" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D64" s="13"/>
       <c r="E64" s="12"/>
       <c r="F64" s="15"/>
     </row>
-    <row r="65" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="4" t="s">
-        <v>218</v>
+        <v>161</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C65" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D65" s="6">
-        <v>1</v>
-      </c>
+        <v>43641</v>
+      </c>
+      <c r="D65" s="13"/>
       <c r="E65" s="12"/>
       <c r="F65" s="15"/>
     </row>
-    <row r="66" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="4" t="s">
-        <v>217</v>
+        <v>162</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C66" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D66" s="7">
-        <v>1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D66" s="13"/>
       <c r="E66" s="12"/>
       <c r="F66" s="15"/>
     </row>
-    <row r="67" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="4" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>218</v>
+        <v>14</v>
+      </c>
+      <c r="C67" s="8">
+        <v>43712</v>
       </c>
       <c r="D67" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E67" s="12"/>
       <c r="F67" s="15"/>
     </row>
-    <row r="68" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="4" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="C68" s="8">
         <v>43712</v>
       </c>
       <c r="D68" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E68" s="12"/>
       <c r="F68" s="15"/>
     </row>
-    <row r="69" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C69" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D69" s="7">
-        <v>2</v>
+        <v>85</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D69" s="6">
+        <v>3</v>
       </c>
       <c r="E69" s="12"/>
       <c r="F69" s="15"/>
     </row>
-    <row r="70" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D70" s="7">
+        <v>2</v>
+      </c>
+      <c r="E70" s="12"/>
+      <c r="F70" s="15"/>
+    </row>
+    <row r="71" spans="1:6" ht="18.75">
+      <c r="A71" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D71" s="7">
+        <v>2</v>
+      </c>
+      <c r="E71" s="12"/>
+      <c r="F71" s="15"/>
+    </row>
+    <row r="72" spans="1:6" ht="18.75">
+      <c r="A72" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D72" s="6">
+        <v>1</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F72" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="18.75">
+      <c r="A73" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D70" s="6">
+      <c r="B73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D73" s="6">
+        <v>10</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="18.75">
+      <c r="A74" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D74" s="6">
+        <v>3</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F74" s="15" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="18.75">
+      <c r="A75" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D75" s="6">
+        <v>3</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F75" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="18.75">
+      <c r="A76" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D76" s="6">
+        <v>4</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="18.75">
+      <c r="A77" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D77" s="6">
         <v>1</v>
       </c>
-      <c r="E70" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F70" s="15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D71" s="6">
-        <v>10</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F71" s="15" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D72" s="6">
-        <v>3</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F72" s="15" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D73" s="6">
-        <v>3</v>
-      </c>
-      <c r="E73" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F73" s="15" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D74" s="6">
-        <v>4</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F74" s="15" t="s">
+      <c r="E77" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F77" s="15" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D75" s="6">
+    <row r="78" spans="1:6" ht="18.75">
+      <c r="A78" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D78" s="13">
         <v>1</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F75" s="15" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C76" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D76" s="13">
-        <v>1</v>
-      </c>
-      <c r="E76" s="12"/>
-      <c r="F76" s="15"/>
-    </row>
-    <row r="77" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C77" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D77" s="7">
-        <v>2</v>
-      </c>
-      <c r="E77" s="12"/>
-      <c r="F77" s="15"/>
-    </row>
-    <row r="78" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C78" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D78" s="7">
-        <v>2</v>
       </c>
       <c r="E78" s="12"/>
       <c r="F78" s="15"/>
     </row>
-    <row r="79" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C79" s="8">
         <v>43641</v>
       </c>
-      <c r="D79" s="7">
-        <v>2</v>
-      </c>
+      <c r="D79" s="7"/>
       <c r="E79" s="12"/>
       <c r="F79" s="15"/>
     </row>
-    <row r="80" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C80" s="8">
         <v>43641</v>
       </c>
-      <c r="D80" s="7">
-        <v>2</v>
-      </c>
+      <c r="D80" s="7"/>
       <c r="E80" s="12"/>
       <c r="F80" s="15"/>
     </row>
-    <row r="81" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="18.75">
       <c r="A81" s="4" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="C81" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D81" s="7">
-        <v>2</v>
-      </c>
+        <v>43641</v>
+      </c>
+      <c r="D81" s="7"/>
       <c r="E81" s="12"/>
       <c r="F81" s="15"/>
     </row>
-    <row r="82" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="18.75">
       <c r="A82" s="4" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="C82" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D82" s="7">
-        <v>2</v>
-      </c>
+        <v>43641</v>
+      </c>
+      <c r="D82" s="7"/>
       <c r="E82" s="12"/>
       <c r="F82" s="15"/>
     </row>
-    <row r="83" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="18.75">
       <c r="A83" s="4" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C83" s="8">
         <v>43712</v>
@@ -3097,12 +3142,12 @@
       <c r="E83" s="12"/>
       <c r="F83" s="15"/>
     </row>
-    <row r="84" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="4" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C84" s="8">
         <v>43712</v>
@@ -3113,12 +3158,12 @@
       <c r="E84" s="12"/>
       <c r="F84" s="15"/>
     </row>
-    <row r="85" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C85" s="8">
         <v>43712</v>
@@ -3129,172 +3174,172 @@
       <c r="E85" s="12"/>
       <c r="F85" s="15"/>
     </row>
-    <row r="86" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="18.75">
       <c r="A86" s="4" t="s">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D86" s="6">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="C86" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D86" s="7">
+        <v>2</v>
       </c>
       <c r="E86" s="12"/>
       <c r="F86" s="15"/>
     </row>
-    <row r="87" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="18.75">
       <c r="A87" s="4" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D87" s="6">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="C87" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D87" s="7">
+        <v>2</v>
       </c>
       <c r="E87" s="12"/>
       <c r="F87" s="15"/>
     </row>
-    <row r="88" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="18.75">
       <c r="A88" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D88" s="6">
-        <v>3</v>
+        <v>210</v>
+      </c>
+      <c r="D88" s="13">
+        <v>2</v>
       </c>
       <c r="E88" s="12"/>
       <c r="F88" s="15"/>
     </row>
-    <row r="89" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="18.75">
       <c r="A89" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D89" s="6">
-        <v>2</v>
+        <v>210</v>
+      </c>
+      <c r="D89" s="13">
+        <v>6</v>
       </c>
       <c r="E89" s="12"/>
       <c r="F89" s="15"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="18.75">
       <c r="A90" s="4" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C90" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D90" s="6">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D90" s="13">
+        <v>2</v>
       </c>
       <c r="E90" s="12"/>
       <c r="F90" s="15"/>
     </row>
-    <row r="91" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="18.75">
       <c r="A91" s="4" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C91" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D91" s="6">
+        <v>26</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D91" s="13">
         <v>3</v>
       </c>
       <c r="E91" s="12"/>
       <c r="F91" s="15"/>
     </row>
-    <row r="92" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="18.75">
       <c r="A92" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D92" s="6">
+        <v>56</v>
+      </c>
+      <c r="C92" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D92" s="13">
         <v>2</v>
       </c>
       <c r="E92" s="12"/>
       <c r="F92" s="15"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="18.75">
       <c r="A93" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D93" s="6">
-        <v>3</v>
+        <v>57</v>
+      </c>
+      <c r="C93" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D93" s="13">
+        <v>6</v>
       </c>
       <c r="E93" s="12"/>
       <c r="F93" s="15"/>
     </row>
-    <row r="94" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="18.75">
       <c r="A94" s="4" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C94" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D94" s="14">
-        <v>2</v>
+        <v>58</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D94" s="13">
+        <v>7</v>
       </c>
       <c r="E94" s="12"/>
       <c r="F94" s="15"/>
     </row>
-    <row r="95" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="18.75">
       <c r="A95" s="4" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C95" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D95" s="14">
-        <v>2</v>
+        <v>59</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D95" s="6">
+        <v>3</v>
       </c>
       <c r="E95" s="12"/>
       <c r="F95" s="15"/>
     </row>
-    <row r="96" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="18.75">
       <c r="A96" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="C96" s="8">
         <v>43712</v>
@@ -3305,308 +3350,292 @@
       <c r="E96" s="12"/>
       <c r="F96" s="15"/>
     </row>
-    <row r="97" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="18.75">
       <c r="A97" s="4" t="s">
-        <v>137</v>
+        <v>197</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D97" s="14">
+        <v>2</v>
+      </c>
+      <c r="E97" s="12"/>
+      <c r="F97" s="15"/>
+    </row>
+    <row r="98" spans="1:6" ht="19.5" thickBot="1">
+      <c r="A98" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C98" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D98" s="14">
+        <v>2</v>
+      </c>
+      <c r="E98" s="12"/>
+      <c r="F98" s="15"/>
+    </row>
+    <row r="99" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
+      <c r="A99" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C97" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D97" s="6">
-        <v>5</v>
-      </c>
-      <c r="E97" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="F97" s="15" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D98" s="6">
-        <v>5</v>
-      </c>
-      <c r="E98" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="F98" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C99" s="6" t="s">
-        <v>138</v>
+        <v>210</v>
       </c>
       <c r="D99" s="6">
         <v>5</v>
       </c>
       <c r="E99" s="27" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F99" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
       <c r="A100" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>139</v>
+        <v>210</v>
       </c>
       <c r="D100" s="6">
         <v>5</v>
       </c>
-      <c r="E100" s="11" t="s">
-        <v>231</v>
+      <c r="E100" s="27" t="s">
+        <v>228</v>
       </c>
       <c r="F100" s="15" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
       <c r="A101" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D101" s="6">
+        <v>5</v>
+      </c>
+      <c r="E101" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="F101" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="19.5" thickTop="1">
+      <c r="A102" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D102" s="6">
+        <v>5</v>
+      </c>
+      <c r="E102" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F102" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="18.75">
+      <c r="A103" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C103" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D101" s="6">
+      <c r="D103" s="6">
         <v>1</v>
       </c>
-      <c r="E101" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F101" s="15" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B102" s="1" t="s">
+      <c r="E103" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F103" s="15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="18.75">
+      <c r="A104" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D102" s="6">
-        <v>2</v>
-      </c>
-      <c r="E102" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F102" s="15" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C103" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D103" s="6">
-        <v>4</v>
-      </c>
-      <c r="E103" s="12"/>
-      <c r="F103" s="15"/>
-    </row>
-    <row r="104" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C104" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D104" s="7">
-        <v>2</v>
-      </c>
-      <c r="E104" s="12"/>
-      <c r="F104" s="15"/>
-    </row>
-    <row r="105" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="C104" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D104" s="6">
+        <v>2</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F104" s="15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="18.75">
       <c r="A105" s="4" t="s">
-        <v>172</v>
+        <v>239</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C105" s="8">
         <v>43641</v>
       </c>
-      <c r="D105" s="7">
-        <v>2</v>
+      <c r="D105" s="6">
+        <v>8</v>
       </c>
       <c r="E105" s="12"/>
       <c r="F105" s="15"/>
     </row>
-    <row r="106" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="18.75">
       <c r="A106" s="4" t="s">
-        <v>173</v>
+        <v>240</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C106" s="8">
         <v>43641</v>
       </c>
-      <c r="D106" s="7">
-        <v>2</v>
-      </c>
+      <c r="D106" s="7"/>
       <c r="E106" s="12"/>
       <c r="F106" s="15"/>
     </row>
-    <row r="107" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="18.75">
       <c r="A107" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C107" s="8">
         <v>43641</v>
       </c>
-      <c r="D107" s="7">
-        <v>2</v>
-      </c>
+      <c r="D107" s="7"/>
       <c r="E107" s="12"/>
       <c r="F107" s="15"/>
     </row>
-    <row r="108" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="18.75">
       <c r="A108" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C108" s="8">
         <v>43641</v>
       </c>
-      <c r="D108" s="7">
-        <v>2</v>
-      </c>
+      <c r="D108" s="7"/>
       <c r="E108" s="12"/>
       <c r="F108" s="15"/>
     </row>
-    <row r="109" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="18.75">
       <c r="A109" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C109" s="8">
         <v>43641</v>
       </c>
-      <c r="D109" s="7">
-        <v>2</v>
-      </c>
+      <c r="D109" s="7"/>
       <c r="E109" s="12"/>
       <c r="F109" s="15"/>
     </row>
-    <row r="110" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="18.75">
       <c r="A110" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C110" s="8">
         <v>43641</v>
       </c>
-      <c r="D110" s="7">
-        <v>2</v>
-      </c>
+      <c r="D110" s="7"/>
       <c r="E110" s="12"/>
       <c r="F110" s="15"/>
     </row>
-    <row r="111" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="18.75">
       <c r="A111" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C111" s="8">
         <v>43641</v>
       </c>
-      <c r="D111" s="7">
-        <v>2</v>
-      </c>
+      <c r="D111" s="7"/>
       <c r="E111" s="12"/>
       <c r="F111" s="15"/>
     </row>
-    <row r="112" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="18.75">
       <c r="A112" s="4" t="s">
-        <v>244</v>
+        <v>176</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C112" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D112" s="7">
-        <v>2</v>
-      </c>
+        <v>43641</v>
+      </c>
+      <c r="D112" s="7"/>
       <c r="E112" s="12"/>
       <c r="F112" s="15"/>
     </row>
-    <row r="113" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="18.75">
       <c r="A113" s="4" t="s">
-        <v>245</v>
+        <v>177</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="C113" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D113" s="7">
-        <v>2</v>
-      </c>
+        <v>43641</v>
+      </c>
+      <c r="D113" s="7"/>
       <c r="E113" s="12"/>
       <c r="F113" s="15"/>
     </row>
-    <row r="114" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="18.75">
       <c r="A114" s="4" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C114" s="8">
         <v>43712</v>
@@ -3617,12 +3646,12 @@
       <c r="E114" s="12"/>
       <c r="F114" s="15"/>
     </row>
-    <row r="115" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="18.75">
       <c r="A115" s="4" t="s">
-        <v>203</v>
+        <v>242</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C115" s="8">
         <v>43712</v>
@@ -3633,12 +3662,12 @@
       <c r="E115" s="12"/>
       <c r="F115" s="15"/>
     </row>
-    <row r="116" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="18.75">
       <c r="A116" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C116" s="8">
         <v>43712</v>
@@ -3649,12 +3678,12 @@
       <c r="E116" s="12"/>
       <c r="F116" s="15"/>
     </row>
-    <row r="117" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="18.75">
       <c r="A117" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C117" s="8">
         <v>43712</v>
@@ -3665,12 +3694,12 @@
       <c r="E117" s="12"/>
       <c r="F117" s="15"/>
     </row>
-    <row r="118" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="18.75">
       <c r="A118" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C118" s="8">
         <v>43712</v>
@@ -3681,12 +3710,12 @@
       <c r="E118" s="12"/>
       <c r="F118" s="15"/>
     </row>
-    <row r="119" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="18.75">
       <c r="A119" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C119" s="8">
         <v>43712</v>
@@ -3697,49 +3726,82 @@
       <c r="E119" s="12"/>
       <c r="F119" s="15"/>
     </row>
-    <row r="120" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="18.75">
       <c r="A120" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C120" s="9">
+        <v>203</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C120" s="8">
         <v>43712</v>
       </c>
-      <c r="D120" s="16">
-        <v>2</v>
-      </c>
-      <c r="E120" s="17"/>
-      <c r="F120" s="18"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="10"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="5"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="3"/>
+      <c r="D120" s="7">
+        <v>2</v>
+      </c>
+      <c r="E120" s="12"/>
+      <c r="F120" s="15"/>
+    </row>
+    <row r="121" spans="1:6" ht="18.75">
+      <c r="A121" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C121" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D121" s="7">
+        <v>2</v>
+      </c>
+      <c r="E121" s="12"/>
+      <c r="F121" s="15"/>
+    </row>
+    <row r="122" spans="1:6" ht="19.5" thickBot="1">
+      <c r="A122" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C122" s="9">
+        <v>43712</v>
+      </c>
+      <c r="D122" s="16">
+        <v>2</v>
+      </c>
+      <c r="E122" s="17"/>
+      <c r="F122" s="18"/>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="10"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
     </row>
-    <row r="127" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:6">
+      <c r="A124" s="3"/>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+      <c r="E124" s="5"/>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="3"/>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+    </row>
+    <row r="127" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="129" ht="26.25" customHeight="1"/>
+    <row r="130" ht="27.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Pongo las correciones, mañana van el resto de las cosas
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\estudios\utu de informatica avansada\ProyectoFinal2019-\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC4DE3A-4CA2-45EB-B7DA-C0119D46E992}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E16E3D1-208E-4E3F-A119-EDF0DC887DDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1314,6 +1314,12 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1328,12 +1334,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1714,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1729,14 +1729,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="114" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
       <c r="A2" s="23" t="s">
@@ -1909,7 +1909,7 @@
         <v>43641</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="28" t="s">
         <v>284</v>
       </c>
       <c r="F10" s="15"/>
@@ -1925,7 +1925,7 @@
         <v>43641</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="28" t="s">
         <v>284</v>
       </c>
       <c r="F11" s="15"/>
@@ -1941,7 +1941,7 @@
         <v>43641</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="28" t="s">
         <v>284</v>
       </c>
       <c r="F12" s="15"/>
@@ -1957,7 +1957,7 @@
         <v>43641</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="28" t="s">
         <v>284</v>
       </c>
       <c r="F13" s="15"/>
@@ -1973,7 +1973,7 @@
         <v>43641</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="29" t="s">
         <v>285</v>
       </c>
       <c r="F14" s="15"/>
@@ -1989,7 +1989,7 @@
         <v>43641</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="28" t="s">
         <v>284</v>
       </c>
       <c r="F15" s="15"/>
@@ -2005,7 +2005,7 @@
         <v>43641</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="28" t="s">
         <v>284</v>
       </c>
       <c r="F16" s="15"/>

</xml_diff>

<commit_message>
vercion v2 de tabla de actividades, GANTT INCOMPLETO
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E16E3D1-208E-4E3F-A119-EDF0DC887DDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE962C76-BB83-4C92-B9B0-329909E7981B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="313">
   <si>
     <t>Nombre</t>
   </si>
@@ -882,14 +887,95 @@
     <t xml:space="preserve">Sin asignar </t>
   </si>
   <si>
-    <t xml:space="preserve">Sin comenzar </t>
+    <t xml:space="preserve">ELIMINADO </t>
+  </si>
+  <si>
+    <t>No comenzado</t>
+  </si>
+  <si>
+    <t>Salvador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvador </t>
+  </si>
+  <si>
+    <t>Daniel y salvador</t>
+  </si>
+  <si>
+    <t>Couto y salvador</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvador, Daniel y couto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel y salvador </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel y Salvador </t>
+  </si>
+  <si>
+    <t>Prog02003,Prog02004,Prog02005</t>
+  </si>
+  <si>
+    <t>TODOS</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvador y Daniel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couto y tomas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomas y Couto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvador y couto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couto y Daniel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Couto y salvador </t>
+  </si>
+  <si>
+    <t>Proy02009</t>
+  </si>
+  <si>
+    <t>GANTT V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvador, tomas </t>
+  </si>
+  <si>
+    <t>Salvador , tomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel, tomas  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel , tomas </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -909,11 +995,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="36"/>
-      <color theme="1"/>
-      <name val="Montserrat Medium"/>
     </font>
     <font>
       <b/>
@@ -971,8 +1052,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Montserrat Medium"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1000,8 +1101,18 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1017,36 +1128,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -1139,58 +1220,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -1244,102 +1273,141 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Celda de comprobación" xfId="5" builtinId="23"/>
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1364,16 +1432,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1583533</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>188383</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1856745</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4007330</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1302808</xdr:rowOff>
+      <xdr:rowOff>2423797</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1396,14 +1464,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6427258" y="188383"/>
-          <a:ext cx="1504320" cy="1114425"/>
+          <a:off x="16204408" y="0"/>
+          <a:ext cx="2423797" cy="2423797"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1714,67 +1781,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.28515625" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="114" customHeight="1">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:6" ht="192.75" customHeight="1">
+      <c r="A1" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
-    </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" ht="24.75" customHeight="1">
+      <c r="A2" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="19" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="6">
         <v>3</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="13" t="s">
         <v>245</v>
       </c>
     </row>
@@ -1794,7 +1861,7 @@
       <c r="E4" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>246</v>
       </c>
     </row>
@@ -1814,7 +1881,7 @@
       <c r="E5" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="13" t="s">
         <v>247</v>
       </c>
     </row>
@@ -1834,7 +1901,7 @@
       <c r="E6" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="13" t="s">
         <v>248</v>
       </c>
     </row>
@@ -1854,7 +1921,7 @@
       <c r="E7" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>249</v>
       </c>
     </row>
@@ -1874,7 +1941,7 @@
       <c r="E8" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>250</v>
       </c>
     </row>
@@ -1894,7 +1961,7 @@
       <c r="E9" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>251</v>
       </c>
     </row>
@@ -1908,11 +1975,15 @@
       <c r="C10" s="8">
         <v>43641</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="F10" s="15"/>
+      <c r="D10" s="12">
+        <v>4</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="4" t="s">
@@ -1924,11 +1995,15 @@
       <c r="C11" s="8">
         <v>43641</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="F11" s="15"/>
+      <c r="D11" s="12">
+        <v>4</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="4" t="s">
@@ -1940,11 +2015,15 @@
       <c r="C12" s="8">
         <v>43641</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="F12" s="15"/>
+      <c r="D12" s="12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="18.75">
       <c r="A13" s="4" t="s">
@@ -1956,11 +2035,15 @@
       <c r="C13" s="8">
         <v>43641</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="F13" s="15"/>
+      <c r="D13" s="12">
+        <v>5</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="18.75">
       <c r="A14" s="4" t="s">
@@ -1972,11 +2055,15 @@
       <c r="C14" s="8">
         <v>43641</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="F14" s="15"/>
+      <c r="D14" s="12">
+        <v>3</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="A15" s="4" t="s">
@@ -1988,11 +2075,15 @@
       <c r="C15" s="8">
         <v>43641</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="F15" s="15"/>
+      <c r="D15" s="12">
+        <v>4</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="18.75">
       <c r="A16" s="4" t="s">
@@ -2004,11 +2095,15 @@
       <c r="C16" s="8">
         <v>43641</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="F16" s="15"/>
+      <c r="D16" s="12">
+        <v>4</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="18.75">
       <c r="A17" s="4" t="s">
@@ -2020,11 +2115,13 @@
       <c r="C17" s="8">
         <v>43641</v>
       </c>
-      <c r="D17" s="7">
-        <v>2</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="18.75">
       <c r="A18" s="4" t="s">
@@ -2036,11 +2133,11 @@
       <c r="C18" s="8">
         <v>43712</v>
       </c>
-      <c r="D18" s="7">
-        <v>2</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="18.75">
       <c r="A19" s="4" t="s">
@@ -2052,11 +2149,11 @@
       <c r="C19" s="8">
         <v>43712</v>
       </c>
-      <c r="D19" s="7">
-        <v>2</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" ht="18.75">
       <c r="A20" s="4" t="s">
@@ -2068,11 +2165,11 @@
       <c r="C20" s="8">
         <v>43712</v>
       </c>
-      <c r="D20" s="7">
-        <v>2</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" ht="18.75">
       <c r="A21" s="4" t="s">
@@ -2084,11 +2181,11 @@
       <c r="C21" s="8">
         <v>43712</v>
       </c>
-      <c r="D21" s="7">
-        <v>2</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="4" t="s">
@@ -2100,11 +2197,11 @@
       <c r="C22" s="8">
         <v>43712</v>
       </c>
-      <c r="D22" s="7">
-        <v>2</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" ht="18.75">
       <c r="A23" s="4" t="s">
@@ -2116,11 +2213,11 @@
       <c r="C23" s="8">
         <v>43712</v>
       </c>
-      <c r="D23" s="7">
-        <v>2</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" ht="18.75">
       <c r="A24" s="4" t="s">
@@ -2132,11 +2229,11 @@
       <c r="C24" s="8">
         <v>43712</v>
       </c>
-      <c r="D24" s="7">
-        <v>2</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="4" t="s">
@@ -2148,11 +2245,11 @@
       <c r="C25" s="8">
         <v>43712</v>
       </c>
-      <c r="D25" s="7">
-        <v>2</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" ht="18.75">
       <c r="A26" s="4" t="s">
@@ -2164,11 +2261,11 @@
       <c r="C26" s="8">
         <v>43712</v>
       </c>
-      <c r="D26" s="7">
-        <v>2</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:6" ht="18.75">
       <c r="A27" s="4" t="s">
@@ -2180,13 +2277,13 @@
       <c r="C27" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="12">
         <v>10</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="13" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2206,7 +2303,7 @@
       <c r="E28" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="13" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2226,7 +2323,7 @@
       <c r="E29" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="13" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2246,7 +2343,7 @@
       <c r="E30" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="13" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2266,7 +2363,7 @@
       <c r="E31" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="13" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2286,7 +2383,7 @@
       <c r="E32" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="13" t="s">
         <v>256</v>
       </c>
     </row>
@@ -2300,11 +2397,15 @@
       <c r="C33" s="8">
         <v>43641</v>
       </c>
-      <c r="D33" s="13">
-        <v>8</v>
-      </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="15"/>
+      <c r="D33" s="12">
+        <v>20</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="18.75">
       <c r="A34" s="4" t="s">
@@ -2313,12 +2414,16 @@
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="15"/>
+      <c r="C34" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" ht="18.75">
       <c r="A35" s="4" t="s">
@@ -2327,12 +2432,18 @@
       <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="15"/>
+      <c r="C35" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="12">
+        <v>3</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="18.75">
       <c r="A36" s="4" t="s">
@@ -2341,12 +2452,18 @@
       <c r="B36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="15"/>
+      <c r="C36" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="12">
+        <v>2</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="4" t="s">
@@ -2355,12 +2472,18 @@
       <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="15"/>
+      <c r="C37" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="12">
+        <v>5</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="18.75">
       <c r="A38" s="4" t="s">
@@ -2369,12 +2492,16 @@
       <c r="B38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="15"/>
+      <c r="C38" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:6" ht="18.75">
       <c r="A39" s="4" t="s">
@@ -2383,14 +2510,18 @@
       <c r="B39" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C39" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D39" s="7">
-        <v>2</v>
-      </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="15"/>
+      <c r="C39" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="12">
+        <v>5</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="18.75">
       <c r="A40" s="4" t="s">
@@ -2402,11 +2533,11 @@
       <c r="C40" s="8">
         <v>43712</v>
       </c>
-      <c r="D40" s="7">
-        <v>2</v>
-      </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" ht="18.75">
       <c r="A41" s="4" t="s">
@@ -2418,11 +2549,11 @@
       <c r="C41" s="8">
         <v>43712</v>
       </c>
-      <c r="D41" s="7">
-        <v>2</v>
-      </c>
-      <c r="E41" s="12"/>
-      <c r="F41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="4" t="s">
@@ -2434,11 +2565,11 @@
       <c r="C42" s="8">
         <v>43712</v>
       </c>
-      <c r="D42" s="7">
-        <v>2</v>
-      </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" ht="18.75">
       <c r="A43" s="4" t="s">
@@ -2450,11 +2581,11 @@
       <c r="C43" s="8">
         <v>43712</v>
       </c>
-      <c r="D43" s="7">
-        <v>2</v>
-      </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" ht="18.75">
       <c r="A44" s="4" t="s">
@@ -2466,13 +2597,13 @@
       <c r="C44" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="D44" s="13">
+      <c r="D44" s="12">
         <v>2</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="13" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2492,7 +2623,7 @@
       <c r="E45" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="13" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2503,14 +2634,18 @@
       <c r="B46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="8">
-        <v>43641</v>
+      <c r="C46" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="D46" s="6">
-        <v>12</v>
-      </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="15"/>
+        <v>10</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="18.75">
       <c r="A47" s="4" t="s">
@@ -2519,14 +2654,18 @@
       <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="8">
-        <v>43641</v>
+      <c r="C47" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="D47" s="6">
         <v>9</v>
       </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="15"/>
+      <c r="E47" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="18.75">
       <c r="A48" s="4" t="s">
@@ -2535,14 +2674,18 @@
       <c r="B48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D48" s="13">
-        <v>17</v>
-      </c>
-      <c r="E48" s="12"/>
-      <c r="F48" s="15"/>
+      <c r="C48" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="12">
+        <v>10</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="18.75">
       <c r="A49" s="4" t="s">
@@ -2551,14 +2694,18 @@
       <c r="B49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D49" s="13">
-        <v>5</v>
-      </c>
-      <c r="E49" s="12"/>
-      <c r="F49" s="15"/>
+      <c r="C49" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D49" s="12">
+        <v>2</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="18.75">
       <c r="A50" s="4" t="s">
@@ -2570,11 +2717,11 @@
       <c r="C50" s="8">
         <v>43712</v>
       </c>
-      <c r="D50" s="6">
-        <v>4</v>
-      </c>
-      <c r="E50" s="12"/>
-      <c r="F50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F50" s="13"/>
     </row>
     <row r="51" spans="1:6" ht="18.75">
       <c r="A51" s="4" t="s">
@@ -2586,11 +2733,11 @@
       <c r="C51" s="8">
         <v>43712</v>
       </c>
-      <c r="D51" s="7">
-        <v>2</v>
-      </c>
-      <c r="E51" s="12"/>
-      <c r="F51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F51" s="13"/>
     </row>
     <row r="52" spans="1:6" ht="18.75">
       <c r="A52" s="4" t="s">
@@ -2602,11 +2749,11 @@
       <c r="C52" s="8">
         <v>43712</v>
       </c>
-      <c r="D52" s="7">
-        <v>2</v>
-      </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F52" s="13"/>
     </row>
     <row r="53" spans="1:6" ht="18.75">
       <c r="A53" s="4" t="s">
@@ -2624,7 +2771,7 @@
       <c r="E53" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="13" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2644,7 +2791,7 @@
       <c r="E54" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="13" t="s">
         <v>263</v>
       </c>
     </row>
@@ -2664,7 +2811,7 @@
       <c r="E55" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F55" s="15" t="s">
+      <c r="F55" s="13" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2678,13 +2825,13 @@
       <c r="C56" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="D56" s="12" t="s">
         <v>236</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="13" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2704,7 +2851,7 @@
       <c r="E57" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="F57" s="15" t="s">
+      <c r="F57" s="13" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2724,7 +2871,7 @@
       <c r="E58" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F58" s="13" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2744,7 +2891,7 @@
       <c r="E59" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="F59" s="15" t="s">
+      <c r="F59" s="13" t="s">
         <v>267</v>
       </c>
     </row>
@@ -2764,242 +2911,274 @@
       <c r="E60" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F60" s="15" t="s">
+      <c r="F60" s="13" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="4" t="s">
-        <v>157</v>
+        <v>307</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C61" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D61" s="13"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="15"/>
+        <v>308</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" s="6">
+        <v>2</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="18.75">
       <c r="A62" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C62" s="8">
         <v>43641</v>
       </c>
-      <c r="D62" s="13"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="15"/>
+      <c r="D62" s="12">
+        <v>3</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F62" s="13"/>
     </row>
     <row r="63" spans="1:6" ht="18.75">
       <c r="A63" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C63" s="8">
         <v>43641</v>
       </c>
-      <c r="D63" s="13">
-        <v>4</v>
-      </c>
-      <c r="E63" s="12"/>
-      <c r="F63" s="15"/>
+      <c r="D63" s="12">
+        <v>3</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="18.75">
       <c r="A64" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C64" s="8">
         <v>43641</v>
       </c>
-      <c r="D64" s="13"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="15"/>
+      <c r="D64" s="12">
+        <v>4</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C65" s="8">
         <v>43641</v>
       </c>
-      <c r="D65" s="13"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="15"/>
+      <c r="D65" s="12">
+        <v>1</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D66" s="13"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="15"/>
+        <v>15</v>
+      </c>
+      <c r="C66" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D66" s="12">
+        <v>1</v>
+      </c>
+      <c r="E66" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="4" t="s">
-        <v>215</v>
+        <v>162</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C67" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D67" s="6">
-        <v>1</v>
-      </c>
-      <c r="E67" s="12"/>
-      <c r="F67" s="15"/>
+        <v>16</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D67" s="12">
+        <v>3</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C68" s="8">
         <v>43712</v>
       </c>
-      <c r="D68" s="7">
-        <v>1</v>
-      </c>
-      <c r="E68" s="12"/>
-      <c r="F68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F68" s="13"/>
     </row>
     <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D69" s="6">
-        <v>3</v>
-      </c>
-      <c r="E69" s="12"/>
-      <c r="F69" s="15"/>
+        <v>15</v>
+      </c>
+      <c r="C69" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F69" s="13"/>
     </row>
     <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C70" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D70" s="7">
-        <v>2</v>
-      </c>
-      <c r="E70" s="12"/>
-      <c r="F70" s="15"/>
+        <v>85</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F70" s="13"/>
     </row>
     <row r="71" spans="1:6" ht="18.75">
       <c r="A71" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C71" s="8">
         <v>43712</v>
       </c>
-      <c r="D71" s="7">
-        <v>2</v>
-      </c>
-      <c r="E71" s="12"/>
-      <c r="F71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F71" s="13"/>
     </row>
     <row r="72" spans="1:6" ht="18.75">
       <c r="A72" s="4" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D72" s="6">
-        <v>1</v>
-      </c>
-      <c r="E72" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="F72" s="15" t="s">
-        <v>262</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C72" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F72" s="13"/>
     </row>
     <row r="73" spans="1:6" ht="18.75">
       <c r="A73" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>125</v>
+        <v>210</v>
       </c>
       <c r="D73" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F73" s="15" t="s">
-        <v>268</v>
+      <c r="F73" s="13" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="18.75">
       <c r="A74" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
       <c r="D74" s="6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F74" s="15" t="s">
-        <v>271</v>
+      <c r="F74" s="13" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="18.75">
       <c r="A75" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>210</v>
@@ -3010,404 +3189,464 @@
       <c r="E75" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F75" s="15" t="s">
-        <v>270</v>
+      <c r="F75" s="13" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="18.75">
       <c r="A76" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>210</v>
       </c>
       <c r="D76" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F76" s="15" t="s">
-        <v>269</v>
+      <c r="F76" s="13" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="18.75">
       <c r="A77" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>210</v>
       </c>
       <c r="D77" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F77" s="15" t="s">
-        <v>272</v>
+      <c r="F77" s="13" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="18.75">
       <c r="A78" s="4" t="s">
-        <v>216</v>
+        <v>130</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D78" s="13">
+        <v>22</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D78" s="6">
         <v>1</v>
       </c>
-      <c r="E78" s="12"/>
-      <c r="F78" s="15"/>
+      <c r="E78" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="4" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C79" s="8">
         <v>43641</v>
       </c>
-      <c r="D79" s="7"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="15"/>
+      <c r="D79" s="12">
+        <v>2</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F79" s="13" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C80" s="8">
         <v>43641</v>
       </c>
-      <c r="D80" s="7"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="15"/>
+      <c r="D80" s="12">
+        <v>3</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="81" spans="1:6" ht="18.75">
       <c r="A81" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C81" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D81" s="7"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="15"/>
+        <v>53</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D81" s="12">
+        <v>1</v>
+      </c>
+      <c r="E81" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="82" spans="1:6" ht="18.75">
       <c r="A82" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C82" s="8">
         <v>43641</v>
       </c>
-      <c r="D82" s="7"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="15"/>
+      <c r="D82" s="12">
+        <v>10</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="83" spans="1:6" ht="18.75">
       <c r="A83" s="4" t="s">
-        <v>218</v>
+        <v>166</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C83" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D83" s="7">
-        <v>2</v>
-      </c>
-      <c r="E83" s="12"/>
-      <c r="F83" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D83" s="12">
+        <v>5</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C84" s="8">
         <v>43712</v>
       </c>
-      <c r="D84" s="7">
-        <v>2</v>
-      </c>
-      <c r="E84" s="12"/>
-      <c r="F84" s="15"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F84" s="13"/>
     </row>
     <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C85" s="8">
         <v>43712</v>
       </c>
-      <c r="D85" s="7">
-        <v>2</v>
-      </c>
-      <c r="E85" s="12"/>
-      <c r="F85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F85" s="13"/>
     </row>
     <row r="86" spans="1:6" ht="18.75">
       <c r="A86" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C86" s="8">
         <v>43712</v>
       </c>
-      <c r="D86" s="7">
-        <v>2</v>
-      </c>
-      <c r="E86" s="12"/>
-      <c r="F86" s="15"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F86" s="13"/>
     </row>
     <row r="87" spans="1:6" ht="18.75">
       <c r="A87" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C87" s="8">
         <v>43712</v>
       </c>
-      <c r="D87" s="7">
-        <v>2</v>
-      </c>
-      <c r="E87" s="12"/>
-      <c r="F87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F87" s="13"/>
     </row>
     <row r="88" spans="1:6" ht="18.75">
       <c r="A88" s="4" t="s">
-        <v>131</v>
+        <v>195</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D88" s="13">
-        <v>2</v>
-      </c>
-      <c r="E88" s="12"/>
-      <c r="F88" s="15"/>
+        <v>92</v>
+      </c>
+      <c r="C88" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D88" s="15"/>
+      <c r="E88" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F88" s="13"/>
     </row>
     <row r="89" spans="1:6" ht="18.75">
       <c r="A89" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="D89" s="13">
-        <v>6</v>
-      </c>
-      <c r="E89" s="12"/>
-      <c r="F89" s="15"/>
+      <c r="D89" s="12">
+        <v>2</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="90" spans="1:6" ht="18.75">
       <c r="A90" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="D90" s="13">
-        <v>2</v>
-      </c>
-      <c r="E90" s="12"/>
-      <c r="F90" s="15"/>
+      <c r="D90" s="12">
+        <v>5</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F90" s="13" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="91" spans="1:6" ht="18.75">
       <c r="A91" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="D91" s="13">
-        <v>3</v>
-      </c>
-      <c r="E91" s="12"/>
-      <c r="F91" s="15"/>
+      <c r="D91" s="12">
+        <v>2</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F91" s="13" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="92" spans="1:6" ht="18.75">
       <c r="A92" s="4" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C92" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D92" s="13">
-        <v>2</v>
-      </c>
-      <c r="E92" s="12"/>
-      <c r="F92" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D92" s="12">
+        <v>3</v>
+      </c>
+      <c r="E92" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="93" spans="1:6" ht="18.75">
       <c r="A93" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C93" s="8">
         <v>43641</v>
       </c>
-      <c r="D93" s="13">
-        <v>6</v>
-      </c>
-      <c r="E93" s="12"/>
-      <c r="F93" s="15"/>
+      <c r="D93" s="12">
+        <v>2</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="94" spans="1:6" ht="18.75">
       <c r="A94" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D94" s="13">
-        <v>7</v>
-      </c>
-      <c r="E94" s="12"/>
-      <c r="F94" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="C94" s="8">
+        <v>43641</v>
+      </c>
+      <c r="D94" s="12">
+        <v>5</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F94" s="13" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="95" spans="1:6" ht="18.75">
       <c r="A95" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D95" s="6">
-        <v>3</v>
-      </c>
-      <c r="E95" s="12"/>
-      <c r="F95" s="15"/>
+      <c r="D95" s="12">
+        <v>5</v>
+      </c>
+      <c r="E95" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F95" s="13" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="96" spans="1:6" ht="18.75">
       <c r="A96" s="4" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C96" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D96" s="14">
-        <v>2</v>
-      </c>
-      <c r="E96" s="12"/>
-      <c r="F96" s="15"/>
+        <v>59</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D96" s="6">
+        <v>3</v>
+      </c>
+      <c r="E96" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="97" spans="1:6" ht="18.75">
       <c r="A97" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C97" s="8">
         <v>43712</v>
       </c>
-      <c r="D97" s="14">
-        <v>2</v>
-      </c>
-      <c r="E97" s="12"/>
-      <c r="F97" s="15"/>
-    </row>
-    <row r="98" spans="1:6" ht="19.5" thickBot="1">
+      <c r="D97" s="15"/>
+      <c r="E97" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F97" s="13"/>
+    </row>
+    <row r="98" spans="1:6" ht="18.75">
       <c r="A98" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="C98" s="8">
         <v>43712</v>
       </c>
-      <c r="D98" s="14">
-        <v>2</v>
-      </c>
-      <c r="E98" s="12"/>
-      <c r="F98" s="15"/>
-    </row>
-    <row r="99" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
+      <c r="D98" s="15"/>
+      <c r="E98" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F98" s="13"/>
+    </row>
+    <row r="99" spans="1:6" ht="18.75">
       <c r="A99" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C99" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D99" s="15"/>
+      <c r="E99" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F99" s="13"/>
+    </row>
+    <row r="100" spans="1:6" ht="18.75">
+      <c r="A100" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D99" s="6">
-        <v>5</v>
-      </c>
-      <c r="E99" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="F99" s="15" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
-      <c r="A100" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>210</v>
@@ -3415,42 +3654,42 @@
       <c r="D100" s="6">
         <v>5</v>
       </c>
-      <c r="E100" s="27" t="s">
+      <c r="E100" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F100" s="15" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="20.25" thickTop="1" thickBot="1">
+      <c r="F100" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="18.75">
       <c r="A101" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>137</v>
+        <v>210</v>
       </c>
       <c r="D101" s="6">
         <v>5</v>
       </c>
-      <c r="E101" s="27" t="s">
+      <c r="E101" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F101" s="15" t="s">
+      <c r="F101" s="13" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="19.5" thickTop="1">
+    <row r="102" spans="1:6" ht="18.75">
       <c r="A102" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D102" s="6">
         <v>5</v>
@@ -3458,350 +3697,421 @@
       <c r="E102" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F102" s="15" t="s">
-        <v>275</v>
+      <c r="F102" s="13" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="18.75">
       <c r="A103" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D103" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E103" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F103" s="15" t="s">
-        <v>276</v>
+      <c r="F103" s="13" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="18.75">
       <c r="A104" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>221</v>
-      </c>
       <c r="D104" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E104" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F104" s="15" t="s">
-        <v>274</v>
+      <c r="F104" s="13" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="18.75">
       <c r="A105" s="4" t="s">
-        <v>239</v>
+        <v>141</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C105" s="8">
-        <v>43641</v>
+        <v>32</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>221</v>
       </c>
       <c r="D105" s="6">
-        <v>8</v>
-      </c>
-      <c r="E105" s="12"/>
-      <c r="F105" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F105" s="13" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="18.75">
       <c r="A106" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C106" s="8">
         <v>43641</v>
       </c>
-      <c r="D106" s="7"/>
-      <c r="E106" s="12"/>
-      <c r="F106" s="15"/>
+      <c r="D106" s="6">
+        <v>8</v>
+      </c>
+      <c r="E106" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F106" s="13" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="107" spans="1:6" ht="18.75">
       <c r="A107" s="4" t="s">
-        <v>171</v>
+        <v>240</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C107" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D107" s="7"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="15"/>
+        <v>61</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D107" s="12">
+        <v>2</v>
+      </c>
+      <c r="E107" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F107" s="13" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="108" spans="1:6" ht="18.75">
       <c r="A108" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C108" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D108" s="7"/>
-      <c r="E108" s="12"/>
-      <c r="F108" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D108" s="12">
+        <v>3</v>
+      </c>
+      <c r="E108" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F108" s="13" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="109" spans="1:6" ht="18.75">
       <c r="A109" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C109" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D109" s="7"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="15"/>
+        <v>63</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D109" s="12">
+        <v>2</v>
+      </c>
+      <c r="E109" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F109" s="13" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="110" spans="1:6" ht="18.75">
       <c r="A110" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C110" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D110" s="7"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D110" s="12">
+        <v>2</v>
+      </c>
+      <c r="E110" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F110" s="13" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="111" spans="1:6" ht="18.75">
       <c r="A111" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C111" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D111" s="7"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D111" s="12">
+        <v>1</v>
+      </c>
+      <c r="E111" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F111" s="13" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="112" spans="1:6" ht="18.75">
       <c r="A112" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C112" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D112" s="7"/>
-      <c r="E112" s="12"/>
-      <c r="F112" s="15"/>
+        <v>66</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D112" s="12">
+        <v>3</v>
+      </c>
+      <c r="E112" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F112" s="13" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="113" spans="1:6" ht="18.75">
       <c r="A113" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C113" s="8">
-        <v>43641</v>
-      </c>
-      <c r="D113" s="7"/>
-      <c r="E113" s="12"/>
-      <c r="F113" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D113" s="12">
+        <v>2</v>
+      </c>
+      <c r="E113" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F113" s="13" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="114" spans="1:6" ht="18.75">
       <c r="A114" s="4" t="s">
-        <v>241</v>
+        <v>177</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C114" s="8">
-        <v>43712</v>
-      </c>
-      <c r="D114" s="7">
-        <v>2</v>
-      </c>
-      <c r="E114" s="12"/>
-      <c r="F114" s="15"/>
+        <v>68</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D114" s="12">
+        <v>4</v>
+      </c>
+      <c r="E114" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="F114" s="13" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="115" spans="1:6" ht="18.75">
       <c r="A115" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C115" s="8">
         <v>43712</v>
       </c>
-      <c r="D115" s="7">
-        <v>2</v>
-      </c>
-      <c r="E115" s="12"/>
-      <c r="F115" s="15"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F115" s="13"/>
     </row>
     <row r="116" spans="1:6" ht="18.75">
       <c r="A116" s="4" t="s">
-        <v>199</v>
+        <v>242</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C116" s="8">
         <v>43712</v>
       </c>
-      <c r="D116" s="7">
-        <v>2</v>
-      </c>
-      <c r="E116" s="12"/>
-      <c r="F116" s="15"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F116" s="13"/>
     </row>
     <row r="117" spans="1:6" ht="18.75">
       <c r="A117" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C117" s="8">
         <v>43712</v>
       </c>
-      <c r="D117" s="7">
-        <v>2</v>
-      </c>
-      <c r="E117" s="12"/>
-      <c r="F117" s="15"/>
+      <c r="D117" s="15"/>
+      <c r="E117" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F117" s="13"/>
     </row>
     <row r="118" spans="1:6" ht="18.75">
       <c r="A118" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C118" s="8">
         <v>43712</v>
       </c>
-      <c r="D118" s="7">
-        <v>2</v>
-      </c>
-      <c r="E118" s="12"/>
-      <c r="F118" s="15"/>
+      <c r="D118" s="15"/>
+      <c r="E118" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F118" s="13"/>
     </row>
     <row r="119" spans="1:6" ht="18.75">
       <c r="A119" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C119" s="8">
         <v>43712</v>
       </c>
-      <c r="D119" s="7">
-        <v>2</v>
-      </c>
-      <c r="E119" s="12"/>
-      <c r="F119" s="15"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F119" s="13"/>
     </row>
     <row r="120" spans="1:6" ht="18.75">
       <c r="A120" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C120" s="8">
         <v>43712</v>
       </c>
-      <c r="D120" s="7">
-        <v>2</v>
-      </c>
-      <c r="E120" s="12"/>
-      <c r="F120" s="15"/>
+      <c r="D120" s="15"/>
+      <c r="E120" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F120" s="13"/>
     </row>
     <row r="121" spans="1:6" ht="18.75">
       <c r="A121" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C121" s="8">
         <v>43712</v>
       </c>
-      <c r="D121" s="7">
-        <v>2</v>
-      </c>
-      <c r="E121" s="12"/>
-      <c r="F121" s="15"/>
-    </row>
-    <row r="122" spans="1:6" ht="19.5" thickBot="1">
+      <c r="D121" s="15"/>
+      <c r="E121" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F121" s="13"/>
+    </row>
+    <row r="122" spans="1:6" ht="18.75">
       <c r="A122" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C122" s="8">
+        <v>43712</v>
+      </c>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F122" s="13"/>
+    </row>
+    <row r="123" spans="1:6" ht="19.5" thickBot="1">
+      <c r="A123" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C122" s="9">
+      <c r="C123" s="9">
         <v>43712</v>
       </c>
-      <c r="D122" s="16">
-        <v>2</v>
-      </c>
-      <c r="E122" s="17"/>
-      <c r="F122" s="18"/>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" s="10"/>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F123" s="14"/>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" s="3"/>
+      <c r="A124" s="10"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
-      <c r="E124" s="5"/>
     </row>
     <row r="125" spans="1:6">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
+      <c r="E125" s="5"/>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:6" ht="20.25" customHeight="1"/>
     <row r="129" ht="26.25" customHeight="1"/>
     <row r="130" ht="27.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Mejoras en informes y registros
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE962C76-BB83-4C92-B9B0-329909E7981B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C76CA7-25FC-42D7-9AC0-1D8BCB55C563}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="313">
   <si>
     <t>Nombre</t>
   </si>
@@ -1389,6 +1389,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1397,9 +1400,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1781,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1796,14 +1796,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="192.75" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:6" ht="24.75" customHeight="1">
       <c r="A2" s="16" t="s">
@@ -2116,12 +2116,10 @@
         <v>43641</v>
       </c>
       <c r="D17" s="15"/>
-      <c r="E17" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>287</v>
-      </c>
+      <c r="E17" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" ht="18.75">
       <c r="A18" s="4" t="s">
@@ -4079,7 +4077,7 @@
       <c r="C123" s="9">
         <v>43712</v>
       </c>
-      <c r="D123" s="27"/>
+      <c r="D123" s="24"/>
       <c r="E123" s="15" t="s">
         <v>284</v>
       </c>

</xml_diff>

<commit_message>
Aranque basico con la nueva arquitectura y BBDD, falta por subzona y lote
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C76CA7-25FC-42D7-9AC0-1D8BCB55C563}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50422D08-F934-4CF0-9782-C8EBCBFE15C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -650,9 +650,6 @@
     <t>Taller03024</t>
   </si>
   <si>
-    <t xml:space="preserve">Tabla de actividades </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fundamentacion del ciclo de vida </t>
   </si>
   <si>
@@ -969,6 +966,9 @@
   </si>
   <si>
     <t xml:space="preserve">Daniel , tomas </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tabla de actividades </t>
   </si>
 </sst>
 </file>
@@ -1781,8 +1781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1797,7 +1797,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="192.75" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>206</v>
+        <v>312</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1813,16 +1813,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>224</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75">
@@ -1839,10 +1839,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" customHeight="1">
@@ -1850,19 +1850,19 @@
         <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75">
@@ -1873,16 +1873,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D5" s="6">
         <v>8</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75">
@@ -1899,10 +1899,10 @@
         <v>20</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75">
@@ -1910,7 +1910,7 @@
         <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>107</v>
@@ -1919,18 +1919,18 @@
         <v>2</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>107</v>
@@ -1939,18 +1939,18 @@
         <v>6</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>107</v>
@@ -1959,10 +1959,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.75">
@@ -1978,11 +1978,11 @@
       <c r="D10" s="12">
         <v>4</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>286</v>
+      <c r="E10" s="20" t="s">
+        <v>237</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18.75">
@@ -1999,10 +1999,10 @@
         <v>4</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18.75">
@@ -2019,10 +2019,10 @@
         <v>3</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75">
@@ -2039,18 +2039,18 @@
         <v>5</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18.75">
       <c r="A14" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C14" s="8">
         <v>43641</v>
@@ -2059,18 +2059,18 @@
         <v>3</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18.75">
       <c r="A15" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C15" s="8">
         <v>43641</v>
@@ -2079,18 +2079,18 @@
         <v>4</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18.75">
       <c r="A16" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C16" s="8">
         <v>43641</v>
@@ -2099,10 +2099,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>286</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18.75">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F17" s="13"/>
     </row>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F18" s="13"/>
     </row>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F19" s="13"/>
     </row>
@@ -2165,7 +2165,7 @@
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F20" s="13"/>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F21" s="13"/>
     </row>
@@ -2197,13 +2197,13 @@
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" ht="18.75">
       <c r="A23" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>74</v>
@@ -2213,13 +2213,13 @@
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" ht="18.75">
       <c r="A24" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>75</v>
@@ -2229,13 +2229,13 @@
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>76</v>
@@ -2245,13 +2245,13 @@
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" ht="18.75">
       <c r="A26" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>77</v>
@@ -2261,16 +2261,16 @@
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:6" ht="18.75">
       <c r="A27" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>107</v>
@@ -2279,10 +2279,10 @@
         <v>10</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26.25" customHeight="1">
@@ -2293,16 +2293,16 @@
         <v>4</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D28" s="6">
         <v>3</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="18.75">
@@ -2313,16 +2313,16 @@
         <v>5</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D29" s="6">
         <v>1</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="18.75">
@@ -2339,10 +2339,10 @@
         <v>1</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18.75">
@@ -2353,16 +2353,16 @@
         <v>7</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D31" s="6">
         <v>2</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18.75">
@@ -2379,10 +2379,10 @@
         <v>1</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="18.75">
@@ -2399,10 +2399,10 @@
         <v>20</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18.75">
@@ -2416,10 +2416,10 @@
         <v>146</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F34" s="13"/>
     </row>
@@ -2437,10 +2437,10 @@
         <v>3</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="18.75">
@@ -2457,10 +2457,10 @@
         <v>2</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="18.75">
@@ -2477,10 +2477,10 @@
         <v>5</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18.75">
@@ -2494,10 +2494,10 @@
         <v>146</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F38" s="13"/>
     </row>
@@ -2506,7 +2506,7 @@
         <v>152</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>146</v>
@@ -2514,11 +2514,11 @@
       <c r="D39" s="12">
         <v>5</v>
       </c>
-      <c r="E39" s="22" t="s">
-        <v>286</v>
+      <c r="E39" s="20" t="s">
+        <v>237</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18.75">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F40" s="13"/>
     </row>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F41" s="13"/>
     </row>
@@ -2565,13 +2565,13 @@
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" ht="18.75">
       <c r="A43" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>81</v>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F43" s="13"/>
     </row>
@@ -2593,16 +2593,16 @@
         <v>9</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D44" s="12">
         <v>2</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18.75">
@@ -2613,16 +2613,16 @@
         <v>10</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D45" s="6">
         <v>13</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18.75">
@@ -2639,10 +2639,10 @@
         <v>10</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18.75">
@@ -2659,10 +2659,10 @@
         <v>9</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="18.75">
@@ -2679,10 +2679,10 @@
         <v>10</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18.75">
@@ -2693,16 +2693,16 @@
         <v>47</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D49" s="12">
         <v>2</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="18.75">
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F50" s="13"/>
     </row>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F51" s="13"/>
     </row>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F52" s="13"/>
     </row>
@@ -2761,16 +2761,16 @@
         <v>11</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D53" s="6">
         <v>3</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18.75">
@@ -2781,16 +2781,16 @@
         <v>12</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D54" s="6">
         <v>1</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="18.75">
@@ -2801,16 +2801,16 @@
         <v>13</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D55" s="6">
         <v>4</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18.75">
@@ -2818,19 +2818,19 @@
         <v>119</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="18.75">
@@ -2841,16 +2841,16 @@
         <v>14</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D57" s="6">
         <v>1</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18.75">
@@ -2861,16 +2861,16 @@
         <v>15</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D58" s="6">
         <v>1</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="18.75">
@@ -2878,19 +2878,19 @@
         <v>122</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D59" s="6">
         <v>1</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="18.75">
@@ -2907,18 +2907,18 @@
         <v>2</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>160</v>
@@ -2927,10 +2927,10 @@
         <v>2</v>
       </c>
       <c r="E61" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="18.75">
@@ -2947,7 +2947,7 @@
         <v>3</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F62" s="13"/>
     </row>
@@ -2965,10 +2965,10 @@
         <v>3</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="18.75">
@@ -2985,10 +2985,10 @@
         <v>4</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="18.75">
@@ -3005,10 +3005,10 @@
         <v>1</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="18.75">
@@ -3025,10 +3025,10 @@
         <v>1</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="18.75">
@@ -3045,15 +3045,15 @@
         <v>3</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>14</v>
@@ -3063,13 +3063,13 @@
       </c>
       <c r="D68" s="15"/>
       <c r="E68" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F68" s="13"/>
     </row>
     <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>15</v>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F69" s="13"/>
     </row>
@@ -3091,11 +3091,11 @@
         <v>85</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D70" s="15"/>
       <c r="E70" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F70" s="13"/>
     </row>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="D71" s="15"/>
       <c r="E71" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F71" s="13"/>
     </row>
@@ -3127,7 +3127,7 @@
       </c>
       <c r="D72" s="15"/>
       <c r="E72" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F72" s="13"/>
     </row>
@@ -3139,16 +3139,16 @@
         <v>17</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D73" s="6">
         <v>1</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="18.75">
@@ -3165,10 +3165,10 @@
         <v>10</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="18.75">
@@ -3179,16 +3179,16 @@
         <v>19</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D75" s="6">
         <v>3</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="18.75">
@@ -3199,16 +3199,16 @@
         <v>21</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D76" s="6">
         <v>3</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="18.75">
@@ -3219,16 +3219,16 @@
         <v>20</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D77" s="6">
         <v>4</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="18.75">
@@ -3239,21 +3239,21 @@
         <v>22</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D78" s="6">
         <v>1</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>51</v>
@@ -3264,11 +3264,11 @@
       <c r="D79" s="12">
         <v>2</v>
       </c>
-      <c r="E79" s="22" t="s">
-        <v>286</v>
+      <c r="E79" s="20" t="s">
+        <v>237</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="18.75">
@@ -3285,10 +3285,10 @@
         <v>3</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="18.75">
@@ -3305,10 +3305,10 @@
         <v>1</v>
       </c>
       <c r="E81" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="F81" s="13" t="s">
         <v>286</v>
-      </c>
-      <c r="F81" s="13" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="18.75">
@@ -3325,10 +3325,10 @@
         <v>10</v>
       </c>
       <c r="E82" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="F82" s="13" t="s">
         <v>286</v>
-      </c>
-      <c r="F82" s="13" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="18.75">
@@ -3345,15 +3345,15 @@
         <v>5</v>
       </c>
       <c r="E83" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="F83" s="13" t="s">
         <v>286</v>
-      </c>
-      <c r="F83" s="13" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="18.75">
       <c r="A84" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>88</v>
@@ -3363,13 +3363,13 @@
       </c>
       <c r="D84" s="15"/>
       <c r="E84" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F84" s="13"/>
     </row>
     <row r="85" spans="1:6" ht="18.75">
       <c r="A85" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>89</v>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="D85" s="15"/>
       <c r="E85" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F85" s="13"/>
     </row>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="D86" s="15"/>
       <c r="E86" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F86" s="13"/>
     </row>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="D87" s="15"/>
       <c r="E87" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F87" s="13"/>
     </row>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="D88" s="15"/>
       <c r="E88" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F88" s="13"/>
     </row>
@@ -3439,16 +3439,16 @@
         <v>23</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D89" s="12">
         <v>2</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="18.75">
@@ -3459,16 +3459,16 @@
         <v>24</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D90" s="12">
         <v>5</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="18.75">
@@ -3479,16 +3479,16 @@
         <v>25</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D91" s="12">
         <v>2</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="18.75">
@@ -3499,16 +3499,16 @@
         <v>26</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D92" s="12">
         <v>3</v>
       </c>
       <c r="E92" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="18.75">
@@ -3525,10 +3525,10 @@
         <v>2</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="18.75">
@@ -3545,10 +3545,10 @@
         <v>5</v>
       </c>
       <c r="E94" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="18.75">
@@ -3565,10 +3565,10 @@
         <v>5</v>
       </c>
       <c r="E95" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="18.75">
@@ -3585,10 +3585,10 @@
         <v>3</v>
       </c>
       <c r="E96" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="18.75">
@@ -3603,7 +3603,7 @@
       </c>
       <c r="D97" s="15"/>
       <c r="E97" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F97" s="13"/>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D98" s="15"/>
       <c r="E98" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F98" s="13"/>
     </row>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="D99" s="15"/>
       <c r="E99" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F99" s="13"/>
     </row>
@@ -3647,16 +3647,16 @@
         <v>27</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D100" s="6">
         <v>5</v>
       </c>
       <c r="E100" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="18.75">
@@ -3667,16 +3667,16 @@
         <v>28</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D101" s="6">
         <v>5</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="18.75">
@@ -3693,10 +3693,10 @@
         <v>5</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="18.75">
@@ -3713,10 +3713,10 @@
         <v>5</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F103" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="18.75">
@@ -3733,10 +3733,10 @@
         <v>1</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F104" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="18.75">
@@ -3747,21 +3747,21 @@
         <v>32</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D105" s="6">
         <v>2</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F105" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="18.75">
       <c r="A106" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>60</v>
@@ -3773,30 +3773,30 @@
         <v>8</v>
       </c>
       <c r="E106" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F106" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="18.75">
       <c r="A107" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D107" s="12">
         <v>2</v>
       </c>
       <c r="E107" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F107" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="18.75">
@@ -3807,16 +3807,16 @@
         <v>62</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D108" s="12">
         <v>3</v>
       </c>
       <c r="E108" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="18.75">
@@ -3827,16 +3827,16 @@
         <v>63</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D109" s="12">
         <v>2</v>
       </c>
       <c r="E109" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F109" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="18.75">
@@ -3847,16 +3847,16 @@
         <v>64</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D110" s="12">
         <v>2</v>
       </c>
       <c r="E110" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F110" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="18.75">
@@ -3867,16 +3867,16 @@
         <v>65</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D111" s="12">
         <v>1</v>
       </c>
       <c r="E111" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F111" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="18.75">
@@ -3887,16 +3887,16 @@
         <v>66</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D112" s="12">
         <v>3</v>
       </c>
       <c r="E112" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F112" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="18.75">
@@ -3907,16 +3907,16 @@
         <v>67</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D113" s="12">
         <v>2</v>
       </c>
       <c r="E113" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F113" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="18.75">
@@ -3927,21 +3927,21 @@
         <v>68</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D114" s="12">
         <v>4</v>
       </c>
       <c r="E114" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F114" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="18.75">
       <c r="A115" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>95</v>
@@ -3951,13 +3951,13 @@
       </c>
       <c r="D115" s="15"/>
       <c r="E115" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F115" s="13"/>
     </row>
     <row r="116" spans="1:6" ht="18.75">
       <c r="A116" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>96</v>
@@ -3967,7 +3967,7 @@
       </c>
       <c r="D116" s="15"/>
       <c r="E116" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F116" s="13"/>
     </row>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="D117" s="15"/>
       <c r="E117" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F117" s="13"/>
     </row>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="D118" s="15"/>
       <c r="E118" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F118" s="13"/>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D119" s="15"/>
       <c r="E119" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F119" s="13"/>
     </row>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="D120" s="15"/>
       <c r="E120" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F120" s="13"/>
     </row>
@@ -4047,7 +4047,7 @@
       </c>
       <c r="D121" s="15"/>
       <c r="E121" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F121" s="13"/>
     </row>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="D122" s="15"/>
       <c r="E122" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F122" s="13"/>
     </row>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="D123" s="24"/>
       <c r="E123" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F123" s="14"/>
     </row>

</xml_diff>

<commit_message>
Agrego justificacion v1 de respaldos y mer, modifico el GANTT y pongo los integradores
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73166470-4FF9-4507-8859-E50E231B23FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A52D7E7-5E45-4A71-88FA-D5953776A5A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="348">
   <si>
     <t>Nombre</t>
   </si>
@@ -1608,9 +1608,6 @@
   </si>
   <si>
     <t>Integrador 3</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t xml:space="preserve"> Tabla de actividades (Segunda entrega 4/9/2019) </t>
@@ -2210,49 +2207,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2261,16 +2234,34 @@
     <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2291,8 +2282,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2675,8 +2672,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2692,17 +2689,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="192.75" customHeight="1">
-      <c r="A1" s="48" t="s">
-        <v>348</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50"/>
+      <c r="A1" s="61" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="63"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1">
       <c r="A2" s="14" t="s">
@@ -2792,127 +2789,127 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="47" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="47">
         <v>8</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="43">
         <v>43577</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="43">
         <v>43586</v>
       </c>
       <c r="H5" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="41" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="47"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="38"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="33" t="s">
         <v>327</v>
       </c>
-      <c r="I6" s="54"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:9" ht="21.75" customHeight="1">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="47" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="47">
         <v>20</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="43">
         <v>43577</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="43">
         <v>43602</v>
       </c>
       <c r="H7" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="I7" s="53" t="s">
+      <c r="I7" s="41" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A8" s="46"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
       <c r="H8" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="I8" s="56"/>
+      <c r="I8" s="53"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A9" s="46"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="I9" s="56"/>
+      <c r="I9" s="53"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="46"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="I10" s="56"/>
+      <c r="I10" s="53"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="47"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="38"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="33" t="s">
         <v>322</v>
       </c>
-      <c r="I11" s="54"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="18.75">
       <c r="A12" s="35" t="s">
@@ -2944,46 +2941,46 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="47">
         <v>6</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F13" s="43">
         <v>43627</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G13" s="43">
         <v>43634</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>324</v>
       </c>
-      <c r="I13" s="53" t="s">
+      <c r="I13" s="41" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="47"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="38"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="33" t="s">
         <v>325</v>
       </c>
-      <c r="I14" s="54"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9" ht="18.75">
       <c r="A15" s="4" t="s">
@@ -3366,59 +3363,59 @@
       <c r="I32" s="11"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C33" s="57" t="s">
+      <c r="C33" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="60">
+      <c r="D33" s="58">
         <v>10</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F33" s="51">
+      <c r="F33" s="43">
         <v>43605</v>
       </c>
-      <c r="G33" s="51">
+      <c r="G33" s="43">
         <v>43616</v>
       </c>
       <c r="H33" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="I33" s="53" t="s">
+      <c r="I33" s="41" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A34" s="46"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
       <c r="H34" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="I34" s="56"/>
+      <c r="I34" s="53"/>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1">
-      <c r="A35" s="47"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="38"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
       <c r="H35" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="I35" s="54"/>
+      <c r="I35" s="42"/>
     </row>
     <row r="36" spans="1:9" ht="18.75">
       <c r="A36" s="4" t="s">
@@ -3828,25 +3825,25 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="18" customHeight="1">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="C53" s="47" t="s">
         <v>210</v>
       </c>
-      <c r="D53" s="39">
+      <c r="D53" s="47">
         <v>13</v>
       </c>
-      <c r="E53" s="42" t="s">
+      <c r="E53" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F53" s="51">
+      <c r="F53" s="43">
         <v>43619</v>
       </c>
-      <c r="G53" s="51">
+      <c r="G53" s="43">
         <v>43635</v>
       </c>
       <c r="H53" s="31" t="s">
@@ -3855,26 +3852,26 @@
       <c r="I53" s="11"/>
     </row>
     <row r="54" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A54" s="46"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="55"/>
+      <c r="A54" s="54"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
       <c r="H54" s="31" t="s">
         <v>332</v>
       </c>
       <c r="I54" s="11"/>
     </row>
     <row r="55" spans="1:9" ht="18" customHeight="1">
-      <c r="A55" s="47"/>
+      <c r="A55" s="40"/>
       <c r="B55" s="38"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="52"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
       <c r="H55" s="33" t="s">
         <v>325</v>
       </c>
@@ -4032,46 +4029,46 @@
       <c r="I62" s="11"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="36" t="s">
+      <c r="B63" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="39" t="s">
+      <c r="C63" s="47" t="s">
         <v>209</v>
       </c>
-      <c r="D63" s="39">
+      <c r="D63" s="47">
         <v>3</v>
       </c>
-      <c r="E63" s="42" t="s">
+      <c r="E63" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F63" s="51">
+      <c r="F63" s="43">
         <v>43586</v>
       </c>
-      <c r="G63" s="51">
+      <c r="G63" s="43">
         <v>43588</v>
       </c>
       <c r="H63" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="I63" s="53" t="s">
+      <c r="I63" s="41" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="47"/>
+      <c r="A64" s="40"/>
       <c r="B64" s="38"/>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="52"/>
-      <c r="G64" s="52"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="48"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="44"/>
       <c r="H64" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="I64" s="54"/>
+      <c r="I64" s="42"/>
     </row>
     <row r="65" spans="1:9" ht="18.75">
       <c r="A65" s="4" t="s">
@@ -4103,46 +4100,46 @@
       </c>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="45" t="s">
+      <c r="A66" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="39" t="s">
+      <c r="C66" s="47" t="s">
         <v>209</v>
       </c>
-      <c r="D66" s="39">
+      <c r="D66" s="47">
         <v>4</v>
       </c>
-      <c r="E66" s="42" t="s">
+      <c r="E66" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F66" s="51">
+      <c r="F66" s="43">
         <v>43609</v>
       </c>
-      <c r="G66" s="51">
+      <c r="G66" s="43">
         <v>43616</v>
       </c>
       <c r="H66" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="I66" s="53" t="s">
+      <c r="I66" s="41" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="47"/>
+      <c r="A67" s="40"/>
       <c r="B67" s="38"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="52"/>
-      <c r="G67" s="52"/>
+      <c r="C67" s="48"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="44"/>
       <c r="H67" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="I67" s="54"/>
+      <c r="I67" s="42"/>
     </row>
     <row r="68" spans="1:9" ht="18.75">
       <c r="A68" s="4" t="s">
@@ -4567,59 +4564,59 @@
       </c>
     </row>
     <row r="86" spans="1:9">
-      <c r="A86" s="45" t="s">
+      <c r="A86" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="B86" s="36" t="s">
+      <c r="B86" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C86" s="39" t="s">
+      <c r="C86" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="D86" s="39">
+      <c r="D86" s="47">
         <v>10</v>
       </c>
-      <c r="E86" s="42" t="s">
+      <c r="E86" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F86" s="51">
+      <c r="F86" s="43">
         <v>43613</v>
       </c>
-      <c r="G86" s="51">
+      <c r="G86" s="43">
         <v>43626</v>
       </c>
       <c r="H86" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="I86" s="53" t="s">
+      <c r="I86" s="41" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A87" s="46"/>
-      <c r="B87" s="37"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="55"/>
-      <c r="G87" s="55"/>
+      <c r="A87" s="54"/>
+      <c r="B87" s="52"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="51"/>
+      <c r="E87" s="50"/>
+      <c r="F87" s="49"/>
+      <c r="G87" s="49"/>
       <c r="H87" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="I87" s="56"/>
+      <c r="I87" s="53"/>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="47"/>
+      <c r="A88" s="40"/>
       <c r="B88" s="38"/>
-      <c r="C88" s="41"/>
-      <c r="D88" s="41"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="52"/>
-      <c r="G88" s="52"/>
+      <c r="C88" s="48"/>
+      <c r="D88" s="48"/>
+      <c r="E88" s="46"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
       <c r="H88" s="33" t="s">
         <v>326</v>
       </c>
-      <c r="I88" s="54"/>
+      <c r="I88" s="42"/>
     </row>
     <row r="89" spans="1:9" ht="18.75">
       <c r="A89" s="4" t="s">
@@ -4680,46 +4677,46 @@
       </c>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="45" t="s">
+      <c r="A91" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="B91" s="36" t="s">
+      <c r="B91" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="39" t="s">
+      <c r="C91" s="47" t="s">
         <v>209</v>
       </c>
-      <c r="D91" s="39">
+      <c r="D91" s="47">
         <v>4</v>
       </c>
-      <c r="E91" s="42" t="s">
+      <c r="E91" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F91" s="51">
+      <c r="F91" s="43">
         <v>43627</v>
       </c>
-      <c r="G91" s="51">
+      <c r="G91" s="43">
         <v>43630</v>
       </c>
       <c r="H91" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="I91" s="53" t="s">
+      <c r="I91" s="41" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="47"/>
+      <c r="A92" s="40"/>
       <c r="B92" s="38"/>
-      <c r="C92" s="41"/>
-      <c r="D92" s="41"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="52"/>
-      <c r="G92" s="52"/>
+      <c r="C92" s="48"/>
+      <c r="D92" s="48"/>
+      <c r="E92" s="46"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="44"/>
       <c r="H92" s="33" t="s">
         <v>325</v>
       </c>
-      <c r="I92" s="54"/>
+      <c r="I92" s="42"/>
     </row>
     <row r="93" spans="1:9" ht="18.75">
       <c r="A93" s="4" t="s">
@@ -5202,172 +5199,172 @@
       <c r="I114" s="11"/>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="45" t="s">
+      <c r="A115" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="B115" s="36" t="s">
+      <c r="B115" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C115" s="39" t="s">
+      <c r="C115" s="47" t="s">
         <v>209</v>
       </c>
-      <c r="D115" s="39">
+      <c r="D115" s="47">
         <v>5</v>
       </c>
-      <c r="E115" s="42" t="s">
+      <c r="E115" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F115" s="51">
+      <c r="F115" s="43">
         <v>43579</v>
       </c>
-      <c r="G115" s="51">
+      <c r="G115" s="43">
         <v>43585</v>
       </c>
       <c r="H115" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="I115" s="53" t="s">
+      <c r="I115" s="41" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="47"/>
+      <c r="A116" s="40"/>
       <c r="B116" s="38"/>
-      <c r="C116" s="41"/>
-      <c r="D116" s="41"/>
-      <c r="E116" s="44"/>
-      <c r="F116" s="52"/>
-      <c r="G116" s="52"/>
+      <c r="C116" s="48"/>
+      <c r="D116" s="48"/>
+      <c r="E116" s="46"/>
+      <c r="F116" s="44"/>
+      <c r="G116" s="44"/>
       <c r="H116" s="33" t="s">
         <v>327</v>
       </c>
-      <c r="I116" s="54"/>
+      <c r="I116" s="42"/>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="45" t="s">
+      <c r="A117" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="B117" s="36" t="s">
+      <c r="B117" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C117" s="39" t="s">
+      <c r="C117" s="47" t="s">
         <v>209</v>
       </c>
-      <c r="D117" s="39">
+      <c r="D117" s="47">
         <v>5</v>
       </c>
-      <c r="E117" s="42" t="s">
+      <c r="E117" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F117" s="51">
+      <c r="F117" s="43">
         <v>43586</v>
       </c>
-      <c r="G117" s="51">
+      <c r="G117" s="43">
         <v>43592</v>
       </c>
       <c r="H117" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="I117" s="53" t="s">
+      <c r="I117" s="41" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="47"/>
+      <c r="A118" s="40"/>
       <c r="B118" s="38"/>
-      <c r="C118" s="41"/>
-      <c r="D118" s="41"/>
-      <c r="E118" s="44"/>
-      <c r="F118" s="52"/>
-      <c r="G118" s="52"/>
+      <c r="C118" s="48"/>
+      <c r="D118" s="48"/>
+      <c r="E118" s="46"/>
+      <c r="F118" s="44"/>
+      <c r="G118" s="44"/>
       <c r="H118" s="33" t="s">
         <v>334</v>
       </c>
-      <c r="I118" s="54"/>
+      <c r="I118" s="42"/>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="45" t="s">
+      <c r="A119" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="B119" s="36" t="s">
+      <c r="B119" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C119" s="39" t="s">
+      <c r="C119" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="D119" s="39">
+      <c r="D119" s="47">
         <v>5</v>
       </c>
-      <c r="E119" s="42" t="s">
+      <c r="E119" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F119" s="51">
+      <c r="F119" s="43">
         <v>43593</v>
       </c>
-      <c r="G119" s="51">
+      <c r="G119" s="43">
         <v>43599</v>
       </c>
       <c r="H119" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="I119" s="53" t="s">
+      <c r="I119" s="41" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="47"/>
+      <c r="A120" s="40"/>
       <c r="B120" s="38"/>
-      <c r="C120" s="41"/>
-      <c r="D120" s="41"/>
-      <c r="E120" s="44"/>
-      <c r="F120" s="52"/>
-      <c r="G120" s="52"/>
+      <c r="C120" s="48"/>
+      <c r="D120" s="48"/>
+      <c r="E120" s="46"/>
+      <c r="F120" s="44"/>
+      <c r="G120" s="44"/>
       <c r="H120" s="33" t="s">
         <v>336</v>
       </c>
-      <c r="I120" s="54"/>
+      <c r="I120" s="42"/>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="45" t="s">
+      <c r="A121" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="B121" s="36" t="s">
+      <c r="B121" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C121" s="39" t="s">
+      <c r="C121" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="D121" s="39">
+      <c r="D121" s="47">
         <v>5</v>
       </c>
-      <c r="E121" s="42" t="s">
+      <c r="E121" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F121" s="51">
+      <c r="F121" s="43">
         <v>43626</v>
       </c>
-      <c r="G121" s="51">
+      <c r="G121" s="43">
         <v>43630</v>
       </c>
       <c r="H121" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="I121" s="53" t="s">
+      <c r="I121" s="41" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="122" spans="1:9">
-      <c r="A122" s="47"/>
+      <c r="A122" s="40"/>
       <c r="B122" s="38"/>
-      <c r="C122" s="41"/>
-      <c r="D122" s="41"/>
-      <c r="E122" s="44"/>
-      <c r="F122" s="52"/>
-      <c r="G122" s="52"/>
+      <c r="C122" s="48"/>
+      <c r="D122" s="48"/>
+      <c r="E122" s="46"/>
+      <c r="F122" s="44"/>
+      <c r="G122" s="44"/>
       <c r="H122" s="33" t="s">
         <v>343</v>
       </c>
-      <c r="I122" s="54"/>
+      <c r="I122" s="42"/>
     </row>
     <row r="123" spans="1:9" ht="18.75">
       <c r="A123" s="4" t="s">
@@ -5815,8 +5812,8 @@
       <c r="C143" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D143" s="63">
-        <v>4</v>
+      <c r="D143" s="36">
+        <v>3</v>
       </c>
       <c r="E143" s="9" t="s">
         <v>227</v>
@@ -5836,8 +5833,8 @@
       <c r="C144" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D144" s="63" t="s">
-        <v>347</v>
+      <c r="D144" s="36">
+        <v>2</v>
       </c>
       <c r="E144" s="20" t="s">
         <v>285</v>
@@ -5871,6 +5868,86 @@
     </row>
   </sheetData>
   <mergeCells count="104">
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="I63:I64"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="I66:I67"/>
+    <mergeCell ref="G86:G88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="D86:D88"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="I86:I88"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="I91:I92"/>
+    <mergeCell ref="G115:G116"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="F115:F116"/>
+    <mergeCell ref="I115:I116"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="C91:C92"/>
     <mergeCell ref="B121:B122"/>
     <mergeCell ref="A121:A122"/>
     <mergeCell ref="I121:I122"/>
@@ -5895,86 +5972,6 @@
     <mergeCell ref="D117:D118"/>
     <mergeCell ref="E117:E118"/>
     <mergeCell ref="C117:C118"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="I91:I92"/>
-    <mergeCell ref="G115:G116"/>
-    <mergeCell ref="E115:E116"/>
-    <mergeCell ref="F115:F116"/>
-    <mergeCell ref="I115:I116"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="C115:C116"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="I66:I67"/>
-    <mergeCell ref="G86:G88"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="E86:E88"/>
-    <mergeCell ref="D86:D88"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="I86:I88"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="I63:I64"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="I7:I11"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sigiente vez tomas te mato
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\ProyectoFinal2019-\Actividades\Proy01005\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E11AD9B-799F-4F28-BCBA-6C70CA70143E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" tabRatio="117"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -2522,7 +2523,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -3182,11 +3183,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3200,6 +3198,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3208,9 +3218,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3221,14 +3228,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3283,7 +3284,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Celda de comprobación" xfId="5" builtinId="23"/>
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
@@ -3328,7 +3329,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3405,7 +3406,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3457,7 +3458,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3651,19 +3652,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152"/>
+    <sheetView tabSelected="1" topLeftCell="B168" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3679,17 +3680,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="192.75" customHeight="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1">
       <c r="A2" s="14" t="s">
@@ -3785,19 +3786,19 @@
       <c r="B5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="55">
         <v>8</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="53">
+      <c r="F5" s="59">
         <v>43577</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="59">
         <v>43586</v>
       </c>
       <c r="H5" s="30" t="s">
@@ -3810,11 +3811,11 @@
     <row r="6" spans="1:9">
       <c r="A6" s="50"/>
       <c r="B6" s="48"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
       <c r="H6" s="32" t="s">
         <v>326</v>
       </c>
@@ -3827,19 +3828,19 @@
       <c r="B7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="55">
         <v>20</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="62" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="59">
         <v>43577</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="59">
         <v>43602</v>
       </c>
       <c r="H7" s="31" t="s">
@@ -3850,52 +3851,52 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A8" s="62"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="68"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A9" s="62"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
       <c r="H9" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="I9" s="67"/>
+      <c r="I9" s="68"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="62"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
       <c r="H10" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="I10" s="67"/>
+      <c r="I10" s="68"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="50"/>
       <c r="B11" s="48"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
       <c r="H11" s="32" t="s">
         <v>321</v>
       </c>
@@ -3937,19 +3938,19 @@
       <c r="B13" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="56">
+      <c r="D13" s="55">
         <v>6</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F13" s="53">
+      <c r="F13" s="59">
         <v>43627</v>
       </c>
-      <c r="G13" s="53">
+      <c r="G13" s="59">
         <v>43634</v>
       </c>
       <c r="H13" s="30" t="s">
@@ -3962,11 +3963,11 @@
     <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="50"/>
       <c r="B14" s="48"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
       <c r="H14" s="32" t="s">
         <v>324</v>
       </c>
@@ -4017,10 +4018,10 @@
       <c r="E16" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F16" s="53">
+      <c r="F16" s="59">
         <v>43664</v>
       </c>
-      <c r="G16" s="53">
+      <c r="G16" s="59">
         <v>43665</v>
       </c>
       <c r="H16" s="30" t="s">
@@ -4036,8 +4037,8 @@
       <c r="C17" s="46"/>
       <c r="D17" s="44"/>
       <c r="E17" s="71"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
       <c r="H17" s="32" t="s">
         <v>347</v>
       </c>
@@ -4059,10 +4060,10 @@
       <c r="E18" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F18" s="53">
+      <c r="F18" s="59">
         <v>43704</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="59">
         <v>43707</v>
       </c>
       <c r="H18" s="30" t="s">
@@ -4078,8 +4079,8 @@
       <c r="C19" s="46"/>
       <c r="D19" s="44"/>
       <c r="E19" s="42"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
       <c r="H19" s="32" t="s">
         <v>375</v>
       </c>
@@ -4130,10 +4131,10 @@
       <c r="E21" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F21" s="53">
+      <c r="F21" s="59">
         <v>43703</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="59">
         <v>43707</v>
       </c>
       <c r="H21" s="30" t="s">
@@ -4149,8 +4150,8 @@
       <c r="C22" s="46"/>
       <c r="D22" s="44"/>
       <c r="E22" s="42"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
       <c r="H22" s="32" t="s">
         <v>375</v>
       </c>
@@ -4201,10 +4202,10 @@
       <c r="E24" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F24" s="53">
+      <c r="F24" s="59">
         <v>43647</v>
       </c>
-      <c r="G24" s="53">
+      <c r="G24" s="59">
         <v>43654</v>
       </c>
       <c r="H24" s="30" t="s">
@@ -4220,8 +4221,8 @@
       <c r="C25" s="46"/>
       <c r="D25" s="44"/>
       <c r="E25" s="42"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
       <c r="H25" s="32" t="s">
         <v>371</v>
       </c>
@@ -4466,19 +4467,19 @@
       <c r="B38" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="55" t="s">
         <v>107</v>
       </c>
       <c r="D38" s="43">
         <v>10</v>
       </c>
-      <c r="E38" s="59" t="s">
+      <c r="E38" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="53">
+      <c r="F38" s="59">
         <v>43605</v>
       </c>
-      <c r="G38" s="53">
+      <c r="G38" s="59">
         <v>43616</v>
       </c>
       <c r="H38" s="30" t="s">
@@ -4489,26 +4490,26 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A39" s="62"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
       <c r="H39" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="I39" s="67"/>
+      <c r="I39" s="68"/>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1">
       <c r="A40" s="50"/>
       <c r="B40" s="48"/>
-      <c r="C40" s="58"/>
+      <c r="C40" s="57"/>
       <c r="D40" s="44"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
       <c r="H40" s="32" t="s">
         <v>329</v>
       </c>
@@ -4672,13 +4673,13 @@
       <c r="D46" s="43">
         <v>20</v>
       </c>
-      <c r="E46" s="59" t="s">
+      <c r="E46" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F46" s="53">
+      <c r="F46" s="59">
         <v>43641</v>
       </c>
-      <c r="G46" s="53">
+      <c r="G46" s="59">
         <v>43668</v>
       </c>
       <c r="H46" s="30" t="s">
@@ -4689,52 +4690,52 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="62"/>
-      <c r="B47" s="55"/>
+      <c r="A47" s="53"/>
+      <c r="B47" s="54"/>
       <c r="C47" s="72"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="66"/>
-      <c r="G47" s="66"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
       <c r="H47" s="30" t="s">
         <v>363</v>
       </c>
-      <c r="I47" s="67"/>
+      <c r="I47" s="68"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="62"/>
-      <c r="B48" s="55"/>
+      <c r="A48" s="53"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="72"/>
-      <c r="D48" s="68"/>
-      <c r="E48" s="60"/>
-      <c r="F48" s="66"/>
-      <c r="G48" s="66"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
       <c r="H48" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="I48" s="67"/>
+      <c r="I48" s="68"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="62"/>
-      <c r="B49" s="55"/>
+      <c r="A49" s="53"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="72"/>
-      <c r="D49" s="68"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="66"/>
-      <c r="G49" s="66"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
       <c r="H49" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="I49" s="67"/>
+      <c r="I49" s="68"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="50"/>
       <c r="B50" s="48"/>
       <c r="C50" s="46"/>
       <c r="D50" s="44"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="54"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
       <c r="H50" s="32" t="s">
         <v>347</v>
       </c>
@@ -4777,10 +4778,10 @@
       <c r="E52" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F52" s="53">
+      <c r="F52" s="59">
         <v>43671</v>
       </c>
-      <c r="G52" s="53">
+      <c r="G52" s="59">
         <v>43672</v>
       </c>
       <c r="H52" s="30" t="s">
@@ -4796,8 +4797,8 @@
       <c r="C53" s="46"/>
       <c r="D53" s="44"/>
       <c r="E53" s="42"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
       <c r="H53" s="32" t="s">
         <v>351</v>
       </c>
@@ -4848,10 +4849,10 @@
       <c r="E55" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F55" s="53">
+      <c r="F55" s="59">
         <v>43677</v>
       </c>
-      <c r="G55" s="53">
+      <c r="G55" s="59">
         <v>43683</v>
       </c>
       <c r="H55" s="30" t="s">
@@ -4867,8 +4868,8 @@
       <c r="C56" s="46"/>
       <c r="D56" s="44"/>
       <c r="E56" s="71"/>
-      <c r="F56" s="54"/>
-      <c r="G56" s="54"/>
+      <c r="F56" s="61"/>
+      <c r="G56" s="61"/>
       <c r="H56" s="32" t="s">
         <v>350</v>
       </c>
@@ -4911,10 +4912,10 @@
       <c r="E58" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F58" s="53">
+      <c r="F58" s="59">
         <v>43669</v>
       </c>
-      <c r="G58" s="53">
+      <c r="G58" s="59">
         <v>43675</v>
       </c>
       <c r="H58" s="30" t="s">
@@ -4930,8 +4931,8 @@
       <c r="C59" s="46"/>
       <c r="D59" s="44"/>
       <c r="E59" s="71"/>
-      <c r="F59" s="54"/>
-      <c r="G59" s="54"/>
+      <c r="F59" s="61"/>
+      <c r="G59" s="61"/>
       <c r="H59" s="32" t="s">
         <v>351</v>
       </c>
@@ -5049,19 +5050,19 @@
       <c r="B65" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="55" t="s">
         <v>210</v>
       </c>
-      <c r="D65" s="56">
+      <c r="D65" s="55">
         <v>13</v>
       </c>
-      <c r="E65" s="59" t="s">
+      <c r="E65" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F65" s="53">
+      <c r="F65" s="59">
         <v>43619</v>
       </c>
-      <c r="G65" s="53">
+      <c r="G65" s="59">
         <v>43635</v>
       </c>
       <c r="H65" s="30" t="s">
@@ -5070,13 +5071,13 @@
       <c r="I65" s="11"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A66" s="62"/>
-      <c r="B66" s="55"/>
-      <c r="C66" s="57"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="66"/>
-      <c r="G66" s="66"/>
+      <c r="A66" s="53"/>
+      <c r="B66" s="54"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="63"/>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
       <c r="H66" s="30" t="s">
         <v>331</v>
       </c>
@@ -5085,11 +5086,11 @@
     <row r="67" spans="1:9" ht="18" customHeight="1">
       <c r="A67" s="50"/>
       <c r="B67" s="48"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="61"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="54"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="61"/>
+      <c r="G67" s="61"/>
       <c r="H67" s="32" t="s">
         <v>324</v>
       </c>
@@ -5107,16 +5108,16 @@
       <c r="C68" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="56">
+      <c r="D68" s="55">
         <v>10</v>
       </c>
       <c r="E68" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F68" s="53">
+      <c r="F68" s="59">
         <v>43669</v>
       </c>
-      <c r="G68" s="53">
+      <c r="G68" s="59">
         <v>43682</v>
       </c>
       <c r="H68" s="30" t="s">
@@ -5127,26 +5128,26 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="18" customHeight="1">
-      <c r="A69" s="62"/>
-      <c r="B69" s="55"/>
+      <c r="A69" s="53"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="72"/>
-      <c r="D69" s="57"/>
+      <c r="D69" s="56"/>
       <c r="E69" s="70"/>
-      <c r="F69" s="66"/>
-      <c r="G69" s="66"/>
+      <c r="F69" s="60"/>
+      <c r="G69" s="60"/>
       <c r="H69" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="I69" s="67"/>
+      <c r="I69" s="68"/>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="50"/>
       <c r="B70" s="48"/>
       <c r="C70" s="46"/>
-      <c r="D70" s="58"/>
+      <c r="D70" s="57"/>
       <c r="E70" s="71"/>
-      <c r="F70" s="54"/>
-      <c r="G70" s="54"/>
+      <c r="F70" s="61"/>
+      <c r="G70" s="61"/>
       <c r="H70" s="32" t="s">
         <v>350</v>
       </c>
@@ -5162,16 +5163,16 @@
       <c r="C71" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="56">
+      <c r="D71" s="55">
         <v>9</v>
       </c>
       <c r="E71" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F71" s="53">
+      <c r="F71" s="59">
         <v>43683</v>
       </c>
-      <c r="G71" s="53">
+      <c r="G71" s="59">
         <v>43693</v>
       </c>
       <c r="H71" s="30" t="s">
@@ -5182,26 +5183,26 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A72" s="62"/>
-      <c r="B72" s="55"/>
+      <c r="A72" s="53"/>
+      <c r="B72" s="54"/>
       <c r="C72" s="72"/>
-      <c r="D72" s="57"/>
+      <c r="D72" s="56"/>
       <c r="E72" s="70"/>
-      <c r="F72" s="66"/>
-      <c r="G72" s="66"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="H72" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="I72" s="67"/>
+      <c r="I72" s="68"/>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="50"/>
       <c r="B73" s="48"/>
       <c r="C73" s="46"/>
-      <c r="D73" s="58"/>
+      <c r="D73" s="57"/>
       <c r="E73" s="71"/>
-      <c r="F73" s="54"/>
-      <c r="G73" s="54"/>
+      <c r="F73" s="61"/>
+      <c r="G73" s="61"/>
       <c r="H73" s="32" t="s">
         <v>358</v>
       </c>
@@ -5215,7 +5216,7 @@
         <v>46</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D74" s="10">
         <v>10</v>
@@ -5248,7 +5249,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>284</v>
+        <v>236</v>
       </c>
       <c r="F75" s="35">
         <v>43710</v>
@@ -5325,19 +5326,19 @@
       <c r="B79" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="56" t="s">
+      <c r="C79" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D79" s="56">
+      <c r="D79" s="55">
         <v>3</v>
       </c>
-      <c r="E79" s="59" t="s">
+      <c r="E79" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F79" s="53">
+      <c r="F79" s="59">
         <v>43586</v>
       </c>
-      <c r="G79" s="53">
+      <c r="G79" s="59">
         <v>43588</v>
       </c>
       <c r="H79" s="30" t="s">
@@ -5350,11 +5351,11 @@
     <row r="80" spans="1:9">
       <c r="A80" s="50"/>
       <c r="B80" s="48"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="61"/>
-      <c r="F80" s="54"/>
-      <c r="G80" s="54"/>
+      <c r="C80" s="57"/>
+      <c r="D80" s="57"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="61"/>
       <c r="H80" s="32" t="s">
         <v>333</v>
       </c>
@@ -5396,19 +5397,19 @@
       <c r="B82" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="56" t="s">
+      <c r="C82" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D82" s="56">
+      <c r="D82" s="55">
         <v>4</v>
       </c>
-      <c r="E82" s="59" t="s">
+      <c r="E82" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F82" s="53">
+      <c r="F82" s="59">
         <v>43609</v>
       </c>
-      <c r="G82" s="53">
+      <c r="G82" s="59">
         <v>43616</v>
       </c>
       <c r="H82" s="30" t="s">
@@ -5421,11 +5422,11 @@
     <row r="83" spans="1:9">
       <c r="A83" s="50"/>
       <c r="B83" s="48"/>
-      <c r="C83" s="58"/>
-      <c r="D83" s="58"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="54"/>
-      <c r="G83" s="54"/>
+      <c r="C83" s="57"/>
+      <c r="D83" s="57"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="61"/>
       <c r="H83" s="32" t="s">
         <v>329</v>
       </c>
@@ -5577,10 +5578,10 @@
       <c r="B89" s="47" t="s">
         <v>306</v>
       </c>
-      <c r="C89" s="56" t="s">
+      <c r="C89" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="56">
+      <c r="D89" s="55">
         <v>2</v>
       </c>
       <c r="E89" s="69" t="s">
@@ -5602,8 +5603,8 @@
     <row r="90" spans="1:9">
       <c r="A90" s="50"/>
       <c r="B90" s="48"/>
-      <c r="C90" s="58"/>
-      <c r="D90" s="58"/>
+      <c r="C90" s="57"/>
+      <c r="D90" s="57"/>
       <c r="E90" s="71"/>
       <c r="F90" s="40"/>
       <c r="G90" s="40"/>
@@ -5928,19 +5929,19 @@
       <c r="B104" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C104" s="56" t="s">
+      <c r="C104" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="D104" s="56">
+      <c r="D104" s="55">
         <v>10</v>
       </c>
-      <c r="E104" s="59" t="s">
+      <c r="E104" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F104" s="53">
+      <c r="F104" s="59">
         <v>43613</v>
       </c>
-      <c r="G104" s="53">
+      <c r="G104" s="59">
         <v>43626</v>
       </c>
       <c r="H104" s="30" t="s">
@@ -5951,26 +5952,26 @@
       </c>
     </row>
     <row r="105" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A105" s="62"/>
-      <c r="B105" s="55"/>
-      <c r="C105" s="57"/>
-      <c r="D105" s="57"/>
-      <c r="E105" s="60"/>
-      <c r="F105" s="66"/>
-      <c r="G105" s="66"/>
+      <c r="A105" s="53"/>
+      <c r="B105" s="54"/>
+      <c r="C105" s="56"/>
+      <c r="D105" s="56"/>
+      <c r="E105" s="63"/>
+      <c r="F105" s="60"/>
+      <c r="G105" s="60"/>
       <c r="H105" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="I105" s="67"/>
+      <c r="I105" s="68"/>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="50"/>
       <c r="B106" s="48"/>
-      <c r="C106" s="58"/>
-      <c r="D106" s="58"/>
-      <c r="E106" s="61"/>
-      <c r="F106" s="54"/>
-      <c r="G106" s="54"/>
+      <c r="C106" s="57"/>
+      <c r="D106" s="57"/>
+      <c r="E106" s="64"/>
+      <c r="F106" s="61"/>
+      <c r="G106" s="61"/>
       <c r="H106" s="32" t="s">
         <v>325</v>
       </c>
@@ -6041,19 +6042,19 @@
       <c r="B109" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="56" t="s">
+      <c r="C109" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D109" s="56">
+      <c r="D109" s="55">
         <v>4</v>
       </c>
-      <c r="E109" s="59" t="s">
+      <c r="E109" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F109" s="53">
+      <c r="F109" s="59">
         <v>43627</v>
       </c>
-      <c r="G109" s="53">
+      <c r="G109" s="59">
         <v>43630</v>
       </c>
       <c r="H109" s="30" t="s">
@@ -6066,11 +6067,11 @@
     <row r="110" spans="1:9">
       <c r="A110" s="50"/>
       <c r="B110" s="48"/>
-      <c r="C110" s="58"/>
-      <c r="D110" s="58"/>
-      <c r="E110" s="61"/>
-      <c r="F110" s="54"/>
-      <c r="G110" s="54"/>
+      <c r="C110" s="57"/>
+      <c r="D110" s="57"/>
+      <c r="E110" s="64"/>
+      <c r="F110" s="61"/>
+      <c r="G110" s="61"/>
       <c r="H110" s="32" t="s">
         <v>324</v>
       </c>
@@ -6222,17 +6223,17 @@
       </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="62"/>
-      <c r="B116" s="55"/>
+      <c r="A116" s="53"/>
+      <c r="B116" s="54"/>
       <c r="C116" s="72"/>
-      <c r="D116" s="68"/>
+      <c r="D116" s="58"/>
       <c r="E116" s="70"/>
       <c r="F116" s="77"/>
       <c r="G116" s="77"/>
       <c r="H116" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="I116" s="67"/>
+      <c r="I116" s="68"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="50"/>
@@ -6420,13 +6421,13 @@
       <c r="B126" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C126" s="56" t="s">
+      <c r="C126" s="55" t="s">
         <v>209</v>
       </c>
       <c r="D126" s="43">
         <v>5</v>
       </c>
-      <c r="E126" s="59" t="s">
+      <c r="E126" s="62" t="s">
         <v>226</v>
       </c>
       <c r="F126" s="39">
@@ -6445,9 +6446,9 @@
     <row r="127" spans="1:9">
       <c r="A127" s="50"/>
       <c r="B127" s="48"/>
-      <c r="C127" s="58"/>
+      <c r="C127" s="57"/>
       <c r="D127" s="44"/>
-      <c r="E127" s="61"/>
+      <c r="E127" s="64"/>
       <c r="F127" s="40"/>
       <c r="G127" s="40"/>
       <c r="H127" s="32" t="s">
@@ -6462,13 +6463,13 @@
       <c r="B128" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C128" s="56" t="s">
+      <c r="C128" s="55" t="s">
         <v>209</v>
       </c>
       <c r="D128" s="43">
         <v>2</v>
       </c>
-      <c r="E128" s="59" t="s">
+      <c r="E128" s="62" t="s">
         <v>226</v>
       </c>
       <c r="F128" s="39">
@@ -6487,9 +6488,9 @@
     <row r="129" spans="1:9">
       <c r="A129" s="50"/>
       <c r="B129" s="48"/>
-      <c r="C129" s="58"/>
+      <c r="C129" s="57"/>
       <c r="D129" s="44"/>
-      <c r="E129" s="61"/>
+      <c r="E129" s="64"/>
       <c r="F129" s="40"/>
       <c r="G129" s="40"/>
       <c r="H129" s="32" t="s">
@@ -6504,7 +6505,7 @@
       <c r="B130" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C130" s="56" t="s">
+      <c r="C130" s="55" t="s">
         <v>209</v>
       </c>
       <c r="D130" s="43">
@@ -6529,7 +6530,7 @@
     <row r="131" spans="1:9">
       <c r="A131" s="50"/>
       <c r="B131" s="48"/>
-      <c r="C131" s="58"/>
+      <c r="C131" s="57"/>
       <c r="D131" s="44"/>
       <c r="E131" s="42"/>
       <c r="F131" s="40"/>
@@ -6552,7 +6553,7 @@
       <c r="D132" s="43">
         <v>2</v>
       </c>
-      <c r="E132" s="59" t="s">
+      <c r="E132" s="62" t="s">
         <v>226</v>
       </c>
       <c r="F132" s="39">
@@ -6573,7 +6574,7 @@
       <c r="B133" s="48"/>
       <c r="C133" s="46"/>
       <c r="D133" s="44"/>
-      <c r="E133" s="61"/>
+      <c r="E133" s="64"/>
       <c r="F133" s="40"/>
       <c r="G133" s="40"/>
       <c r="H133" s="32" t="s">
@@ -6630,7 +6631,7 @@
       <c r="B136" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="C136" s="56" t="s">
+      <c r="C136" s="55" t="s">
         <v>168</v>
       </c>
       <c r="D136" s="43">
@@ -6655,7 +6656,7 @@
     <row r="137" spans="1:9">
       <c r="A137" s="50"/>
       <c r="B137" s="48"/>
-      <c r="C137" s="58"/>
+      <c r="C137" s="57"/>
       <c r="D137" s="44"/>
       <c r="E137" s="42"/>
       <c r="F137" s="40"/>
@@ -6672,10 +6673,10 @@
       <c r="B138" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C138" s="56" t="s">
+      <c r="C138" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="D138" s="56">
+      <c r="D138" s="55">
         <v>3</v>
       </c>
       <c r="E138" s="41" t="s">
@@ -6697,8 +6698,8 @@
     <row r="139" spans="1:9">
       <c r="A139" s="50"/>
       <c r="B139" s="48"/>
-      <c r="C139" s="58"/>
-      <c r="D139" s="58"/>
+      <c r="C139" s="57"/>
+      <c r="D139" s="57"/>
       <c r="E139" s="42"/>
       <c r="F139" s="40"/>
       <c r="G139" s="40"/>
@@ -6771,19 +6772,19 @@
       <c r="B143" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C143" s="56" t="s">
+      <c r="C143" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D143" s="56">
+      <c r="D143" s="55">
         <v>5</v>
       </c>
-      <c r="E143" s="59" t="s">
+      <c r="E143" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F143" s="53">
+      <c r="F143" s="59">
         <v>43579</v>
       </c>
-      <c r="G143" s="53">
+      <c r="G143" s="59">
         <v>43585</v>
       </c>
       <c r="H143" s="30" t="s">
@@ -6796,11 +6797,11 @@
     <row r="144" spans="1:9">
       <c r="A144" s="50"/>
       <c r="B144" s="48"/>
-      <c r="C144" s="58"/>
-      <c r="D144" s="58"/>
-      <c r="E144" s="61"/>
-      <c r="F144" s="54"/>
-      <c r="G144" s="54"/>
+      <c r="C144" s="57"/>
+      <c r="D144" s="57"/>
+      <c r="E144" s="64"/>
+      <c r="F144" s="61"/>
+      <c r="G144" s="61"/>
       <c r="H144" s="32" t="s">
         <v>326</v>
       </c>
@@ -6813,19 +6814,19 @@
       <c r="B145" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C145" s="56" t="s">
+      <c r="C145" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D145" s="56">
+      <c r="D145" s="55">
         <v>5</v>
       </c>
-      <c r="E145" s="59" t="s">
+      <c r="E145" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F145" s="53">
+      <c r="F145" s="59">
         <v>43586</v>
       </c>
-      <c r="G145" s="53">
+      <c r="G145" s="59">
         <v>43592</v>
       </c>
       <c r="H145" s="30" t="s">
@@ -6838,11 +6839,11 @@
     <row r="146" spans="1:9">
       <c r="A146" s="50"/>
       <c r="B146" s="48"/>
-      <c r="C146" s="58"/>
-      <c r="D146" s="58"/>
-      <c r="E146" s="61"/>
-      <c r="F146" s="54"/>
-      <c r="G146" s="54"/>
+      <c r="C146" s="57"/>
+      <c r="D146" s="57"/>
+      <c r="E146" s="64"/>
+      <c r="F146" s="61"/>
+      <c r="G146" s="61"/>
       <c r="H146" s="32" t="s">
         <v>333</v>
       </c>
@@ -6855,19 +6856,19 @@
       <c r="B147" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C147" s="56" t="s">
+      <c r="C147" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="D147" s="56">
+      <c r="D147" s="55">
         <v>5</v>
       </c>
-      <c r="E147" s="59" t="s">
+      <c r="E147" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F147" s="53">
+      <c r="F147" s="59">
         <v>43593</v>
       </c>
-      <c r="G147" s="53">
+      <c r="G147" s="59">
         <v>43599</v>
       </c>
       <c r="H147" s="30" t="s">
@@ -6880,11 +6881,11 @@
     <row r="148" spans="1:9">
       <c r="A148" s="50"/>
       <c r="B148" s="48"/>
-      <c r="C148" s="58"/>
-      <c r="D148" s="58"/>
-      <c r="E148" s="61"/>
-      <c r="F148" s="54"/>
-      <c r="G148" s="54"/>
+      <c r="C148" s="57"/>
+      <c r="D148" s="57"/>
+      <c r="E148" s="64"/>
+      <c r="F148" s="61"/>
+      <c r="G148" s="61"/>
       <c r="H148" s="32" t="s">
         <v>335</v>
       </c>
@@ -6897,19 +6898,19 @@
       <c r="B149" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C149" s="56" t="s">
+      <c r="C149" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="D149" s="56">
+      <c r="D149" s="55">
         <v>5</v>
       </c>
-      <c r="E149" s="59" t="s">
+      <c r="E149" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F149" s="53">
+      <c r="F149" s="59">
         <v>43626</v>
       </c>
-      <c r="G149" s="53">
+      <c r="G149" s="59">
         <v>43630</v>
       </c>
       <c r="H149" s="30" t="s">
@@ -6922,11 +6923,11 @@
     <row r="150" spans="1:9">
       <c r="A150" s="50"/>
       <c r="B150" s="48"/>
-      <c r="C150" s="58"/>
-      <c r="D150" s="58"/>
-      <c r="E150" s="61"/>
-      <c r="F150" s="54"/>
-      <c r="G150" s="54"/>
+      <c r="C150" s="57"/>
+      <c r="D150" s="57"/>
+      <c r="E150" s="64"/>
+      <c r="F150" s="61"/>
+      <c r="G150" s="61"/>
       <c r="H150" s="32" t="s">
         <v>342</v>
       </c>
@@ -7000,16 +7001,16 @@
       <c r="C153" s="45">
         <v>43641</v>
       </c>
-      <c r="D153" s="56">
+      <c r="D153" s="55">
         <v>7</v>
       </c>
       <c r="E153" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F153" s="53">
+      <c r="F153" s="59">
         <v>43647</v>
       </c>
-      <c r="G153" s="53">
+      <c r="G153" s="59">
         <v>43655</v>
       </c>
       <c r="H153" s="30" t="s">
@@ -7023,10 +7024,10 @@
       <c r="A154" s="50"/>
       <c r="B154" s="48"/>
       <c r="C154" s="46"/>
-      <c r="D154" s="58"/>
+      <c r="D154" s="57"/>
       <c r="E154" s="71"/>
-      <c r="F154" s="54"/>
-      <c r="G154" s="54"/>
+      <c r="F154" s="61"/>
+      <c r="G154" s="61"/>
       <c r="H154" s="32" t="s">
         <v>377</v>
       </c>
@@ -7106,10 +7107,10 @@
       <c r="E157" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F157" s="53">
+      <c r="F157" s="59">
         <v>43664</v>
       </c>
-      <c r="G157" s="53">
+      <c r="G157" s="59">
         <v>43665</v>
       </c>
       <c r="H157" s="30" t="s">
@@ -7123,8 +7124,8 @@
       <c r="C158" s="46"/>
       <c r="D158" s="44"/>
       <c r="E158" s="71"/>
-      <c r="F158" s="54"/>
-      <c r="G158" s="54"/>
+      <c r="F158" s="61"/>
+      <c r="G158" s="61"/>
       <c r="H158" s="32" t="s">
         <v>379</v>
       </c>
@@ -7264,10 +7265,10 @@
       <c r="E163" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F163" s="53">
+      <c r="F163" s="59">
         <v>43698</v>
       </c>
-      <c r="G163" s="53">
+      <c r="G163" s="59">
         <v>43703</v>
       </c>
       <c r="H163" s="30" t="s">
@@ -7283,8 +7284,8 @@
       <c r="C164" s="46"/>
       <c r="D164" s="44"/>
       <c r="E164" s="42"/>
-      <c r="F164" s="54"/>
-      <c r="G164" s="54"/>
+      <c r="F164" s="61"/>
+      <c r="G164" s="61"/>
       <c r="H164" s="32" t="s">
         <v>369</v>
       </c>
@@ -7493,9 +7494,9 @@
       <c r="B175" s="48"/>
       <c r="C175" s="46"/>
       <c r="D175" s="83"/>
-      <c r="E175" s="61"/>
-      <c r="F175" s="54"/>
-      <c r="G175" s="54"/>
+      <c r="E175" s="64"/>
+      <c r="F175" s="61"/>
+      <c r="G175" s="61"/>
       <c r="H175" s="32" t="s">
         <v>384</v>
       </c>
@@ -7509,7 +7510,7 @@
         <v>343</v>
       </c>
       <c r="C176" s="37" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D176" s="27">
         <v>2</v>
@@ -7676,6 +7677,12 @@
     <mergeCell ref="B109:B110"/>
     <mergeCell ref="A109:A110"/>
     <mergeCell ref="I109:I110"/>
+    <mergeCell ref="G104:G106"/>
+    <mergeCell ref="F104:F106"/>
+    <mergeCell ref="E104:E106"/>
+    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="B104:B106"/>
     <mergeCell ref="I55:I56"/>
     <mergeCell ref="G58:G59"/>
     <mergeCell ref="F58:F59"/>
@@ -7749,12 +7756,6 @@
     <mergeCell ref="I126:I127"/>
     <mergeCell ref="G126:G127"/>
     <mergeCell ref="F126:F127"/>
-    <mergeCell ref="G104:G106"/>
-    <mergeCell ref="F104:F106"/>
-    <mergeCell ref="E104:E106"/>
-    <mergeCell ref="D104:D106"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="B104:B106"/>
     <mergeCell ref="I104:I106"/>
     <mergeCell ref="A104:A106"/>
     <mergeCell ref="G89:G90"/>

</xml_diff>

<commit_message>
Pert completo, caminos incompletos
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\cosas de daniel\ProyectoFinal2019-\Actividades\Proy01005\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E11AD9B-799F-4F28-BCBA-6C70CA70143E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="117"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2508,22 +2502,22 @@
     </r>
   </si>
   <si>
-    <t>Integrador1</t>
-  </si>
-  <si>
-    <t>Integrador2</t>
-  </si>
-  <si>
-    <t>Integrador3</t>
-  </si>
-  <si>
     <t>Taller01001/Taller01002</t>
+  </si>
+  <si>
+    <t>Integ01001</t>
+  </si>
+  <si>
+    <t>Integ02002</t>
+  </si>
+  <si>
+    <t>Integ03003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -3141,10 +3135,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
@@ -3171,103 +3171,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3282,9 +3198,87 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Celda de comprobación" xfId="5" builtinId="23"/>
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
@@ -3329,7 +3323,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3406,7 +3400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3458,7 +3452,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3652,19 +3646,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B168" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3680,17 +3674,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="192.75" customHeight="1">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="83" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="85"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1">
       <c r="A2" s="14" t="s">
@@ -3780,25 +3774,25 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="62">
         <v>8</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E5" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="41">
         <v>43577</v>
       </c>
-      <c r="G5" s="59">
+      <c r="G5" s="41">
         <v>43586</v>
       </c>
       <c r="H5" s="30" t="s">
@@ -3809,38 +3803,38 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="50"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="32" t="s">
         <v>326</v>
       </c>
       <c r="I6" s="52"/>
     </row>
     <row r="7" spans="1:9" ht="21.75" customHeight="1">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="62">
         <v>20</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="64" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="59">
+      <c r="F7" s="41">
         <v>43577</v>
       </c>
-      <c r="G7" s="59">
+      <c r="G7" s="41">
         <v>43602</v>
       </c>
       <c r="H7" s="31" t="s">
@@ -3851,52 +3845,52 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A8" s="53"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
       <c r="H8" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="68"/>
+      <c r="I8" s="75"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="I9" s="68"/>
+      <c r="I9" s="75"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="I10" s="68"/>
+      <c r="I10" s="75"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="50"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="32" t="s">
         <v>321</v>
       </c>
@@ -3932,25 +3926,25 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="55">
+      <c r="D13" s="62">
         <v>6</v>
       </c>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F13" s="59">
+      <c r="F13" s="41">
         <v>43627</v>
       </c>
-      <c r="G13" s="59">
+      <c r="G13" s="41">
         <v>43634</v>
       </c>
       <c r="H13" s="30" t="s">
@@ -3961,13 +3955,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="50"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
       <c r="H14" s="32" t="s">
         <v>324</v>
       </c>
@@ -4003,25 +3997,25 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="47">
         <v>43641</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="45">
         <v>4</v>
       </c>
-      <c r="E16" s="69" t="s">
+      <c r="E16" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F16" s="59">
+      <c r="F16" s="41">
         <v>43664</v>
       </c>
-      <c r="G16" s="59">
+      <c r="G16" s="41">
         <v>43665</v>
       </c>
       <c r="H16" s="30" t="s">
@@ -4032,38 +4026,38 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="50"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="32" t="s">
         <v>347</v>
       </c>
       <c r="I17" s="52"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="47">
         <v>43641</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="45">
         <v>4</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F18" s="59">
+      <c r="F18" s="41">
         <v>43704</v>
       </c>
-      <c r="G18" s="59">
+      <c r="G18" s="41">
         <v>43707</v>
       </c>
       <c r="H18" s="30" t="s">
@@ -4074,13 +4068,13 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="50"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
       <c r="H19" s="32" t="s">
         <v>375</v>
       </c>
@@ -4116,25 +4110,25 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="47">
         <v>43641</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="45">
         <v>5</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F21" s="59">
+      <c r="F21" s="41">
         <v>43703</v>
       </c>
-      <c r="G21" s="59">
+      <c r="G21" s="41">
         <v>43707</v>
       </c>
       <c r="H21" s="30" t="s">
@@ -4145,13 +4139,13 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1">
-      <c r="A22" s="50"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="32" t="s">
         <v>375</v>
       </c>
@@ -4187,25 +4181,25 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="C24" s="45">
+      <c r="C24" s="47">
         <v>43641</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="45">
         <v>6</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F24" s="59">
+      <c r="F24" s="41">
         <v>43647</v>
       </c>
-      <c r="G24" s="59">
+      <c r="G24" s="41">
         <v>43654</v>
       </c>
       <c r="H24" s="30" t="s">
@@ -4216,38 +4210,38 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="50"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="32" t="s">
         <v>371</v>
       </c>
       <c r="I25" s="52"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="47">
         <v>43641</v>
       </c>
-      <c r="D26" s="43">
+      <c r="D26" s="45">
         <v>4</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="E26" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F26" s="39">
+      <c r="F26" s="67">
         <v>43656</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="67">
         <v>43661</v>
       </c>
       <c r="H26" s="30" t="s">
@@ -4258,13 +4252,13 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="50"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
       <c r="H27" s="32" t="s">
         <v>389</v>
       </c>
@@ -4461,25 +4455,25 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="55" t="s">
+      <c r="C38" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="43">
+      <c r="D38" s="45">
         <v>10</v>
       </c>
-      <c r="E38" s="62" t="s">
+      <c r="E38" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="59">
+      <c r="F38" s="41">
         <v>43605</v>
       </c>
-      <c r="G38" s="59">
+      <c r="G38" s="41">
         <v>43616</v>
       </c>
       <c r="H38" s="30" t="s">
@@ -4490,26 +4484,26 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A39" s="53"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
+      <c r="A39" s="74"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
       <c r="H39" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="I39" s="68"/>
+      <c r="I39" s="75"/>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1">
-      <c r="A40" s="50"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
       <c r="H40" s="32" t="s">
         <v>329</v>
       </c>
@@ -4661,25 +4655,25 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="45">
+      <c r="C46" s="47">
         <v>43641</v>
       </c>
-      <c r="D46" s="43">
+      <c r="D46" s="45">
         <v>20</v>
       </c>
-      <c r="E46" s="62" t="s">
+      <c r="E46" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F46" s="59">
+      <c r="F46" s="41">
         <v>43641</v>
       </c>
-      <c r="G46" s="59">
+      <c r="G46" s="41">
         <v>43668</v>
       </c>
       <c r="H46" s="30" t="s">
@@ -4690,52 +4684,52 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="53"/>
-      <c r="B47" s="54"/>
+      <c r="A47" s="74"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="72"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
       <c r="H47" s="30" t="s">
         <v>363</v>
       </c>
-      <c r="I47" s="68"/>
+      <c r="I47" s="75"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="53"/>
-      <c r="B48" s="54"/>
+      <c r="A48" s="74"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="72"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="60"/>
-      <c r="G48" s="60"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
       <c r="H48" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="I48" s="68"/>
+      <c r="I48" s="75"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="53"/>
-      <c r="B49" s="54"/>
+      <c r="A49" s="74"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="72"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="60"/>
-      <c r="G49" s="60"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="70"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
       <c r="H49" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="I49" s="68"/>
+      <c r="I49" s="75"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="50"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
       <c r="H50" s="32" t="s">
         <v>347</v>
       </c>
@@ -4763,25 +4757,25 @@
       <c r="I51" s="11"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="47" t="s">
+      <c r="B52" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="43">
+      <c r="D52" s="45">
         <v>2</v>
       </c>
-      <c r="E52" s="41" t="s">
+      <c r="E52" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F52" s="59">
+      <c r="F52" s="41">
         <v>43671</v>
       </c>
-      <c r="G52" s="59">
+      <c r="G52" s="41">
         <v>43672</v>
       </c>
       <c r="H52" s="30" t="s">
@@ -4792,13 +4786,13 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="50"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
       <c r="H53" s="32" t="s">
         <v>351</v>
       </c>
@@ -4834,25 +4828,25 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="47" t="s">
+      <c r="B55" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="D55" s="43">
+      <c r="D55" s="45">
         <v>5</v>
       </c>
-      <c r="E55" s="69" t="s">
+      <c r="E55" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F55" s="59">
+      <c r="F55" s="41">
         <v>43677</v>
       </c>
-      <c r="G55" s="59">
+      <c r="G55" s="41">
         <v>43683</v>
       </c>
       <c r="H55" s="30" t="s">
@@ -4863,13 +4857,13 @@
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="50"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="71"/>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="61"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
       <c r="H56" s="32" t="s">
         <v>350</v>
       </c>
@@ -4897,25 +4891,25 @@
       <c r="I57" s="11"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="B58" s="47" t="s">
+      <c r="B58" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="C58" s="45" t="s">
+      <c r="C58" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="43">
+      <c r="D58" s="45">
         <v>5</v>
       </c>
-      <c r="E58" s="69" t="s">
+      <c r="E58" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F58" s="59">
+      <c r="F58" s="41">
         <v>43669</v>
       </c>
-      <c r="G58" s="59">
+      <c r="G58" s="41">
         <v>43675</v>
       </c>
       <c r="H58" s="30" t="s">
@@ -4926,13 +4920,13 @@
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="50"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="71"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="61"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
       <c r="H59" s="32" t="s">
         <v>351</v>
       </c>
@@ -5044,25 +5038,25 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" customHeight="1">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="47" t="s">
+      <c r="B65" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="55" t="s">
+      <c r="C65" s="62" t="s">
         <v>210</v>
       </c>
-      <c r="D65" s="55">
+      <c r="D65" s="62">
         <v>13</v>
       </c>
-      <c r="E65" s="62" t="s">
+      <c r="E65" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F65" s="59">
+      <c r="F65" s="41">
         <v>43619</v>
       </c>
-      <c r="G65" s="59">
+      <c r="G65" s="41">
         <v>43635</v>
       </c>
       <c r="H65" s="30" t="s">
@@ -5071,26 +5065,26 @@
       <c r="I65" s="11"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A66" s="53"/>
-      <c r="B66" s="54"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="63"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
+      <c r="A66" s="74"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="70"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="69"/>
       <c r="H66" s="30" t="s">
         <v>331</v>
       </c>
       <c r="I66" s="11"/>
     </row>
     <row r="67" spans="1:9" ht="18" customHeight="1">
-      <c r="A67" s="50"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="57"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="64"/>
-      <c r="F67" s="61"/>
-      <c r="G67" s="61"/>
+      <c r="A67" s="40"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
       <c r="H67" s="32" t="s">
         <v>324</v>
       </c>
@@ -5099,25 +5093,25 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" customHeight="1">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="47" t="s">
+      <c r="B68" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="45" t="s">
+      <c r="C68" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="55">
+      <c r="D68" s="62">
         <v>10</v>
       </c>
-      <c r="E68" s="69" t="s">
+      <c r="E68" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F68" s="59">
+      <c r="F68" s="41">
         <v>43669</v>
       </c>
-      <c r="G68" s="59">
+      <c r="G68" s="41">
         <v>43682</v>
       </c>
       <c r="H68" s="30" t="s">
@@ -5128,51 +5122,51 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="18" customHeight="1">
-      <c r="A69" s="53"/>
-      <c r="B69" s="54"/>
+      <c r="A69" s="74"/>
+      <c r="B69" s="73"/>
       <c r="C69" s="72"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="70"/>
-      <c r="F69" s="60"/>
-      <c r="G69" s="60"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="79"/>
+      <c r="F69" s="69"/>
+      <c r="G69" s="69"/>
       <c r="H69" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="I69" s="68"/>
+      <c r="I69" s="75"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="50"/>
-      <c r="B70" s="48"/>
-      <c r="C70" s="46"/>
-      <c r="D70" s="57"/>
-      <c r="E70" s="71"/>
-      <c r="F70" s="61"/>
-      <c r="G70" s="61"/>
+      <c r="A70" s="40"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="63"/>
+      <c r="E70" s="61"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
       <c r="H70" s="32" t="s">
         <v>350</v>
       </c>
       <c r="I70" s="52"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="49" t="s">
+      <c r="A71" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="B71" s="47" t="s">
+      <c r="B71" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C71" s="45" t="s">
+      <c r="C71" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="55">
+      <c r="D71" s="62">
         <v>9</v>
       </c>
-      <c r="E71" s="69" t="s">
+      <c r="E71" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F71" s="59">
+      <c r="F71" s="41">
         <v>43683</v>
       </c>
-      <c r="G71" s="59">
+      <c r="G71" s="41">
         <v>43693</v>
       </c>
       <c r="H71" s="30" t="s">
@@ -5183,26 +5177,26 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A72" s="53"/>
-      <c r="B72" s="54"/>
+      <c r="A72" s="74"/>
+      <c r="B72" s="73"/>
       <c r="C72" s="72"/>
-      <c r="D72" s="56"/>
-      <c r="E72" s="70"/>
-      <c r="F72" s="60"/>
-      <c r="G72" s="60"/>
+      <c r="D72" s="80"/>
+      <c r="E72" s="79"/>
+      <c r="F72" s="69"/>
+      <c r="G72" s="69"/>
       <c r="H72" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="I72" s="68"/>
+      <c r="I72" s="75"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="50"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="46"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="71"/>
-      <c r="F73" s="61"/>
-      <c r="G73" s="61"/>
+      <c r="A73" s="40"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="61"/>
+      <c r="F73" s="42"/>
+      <c r="G73" s="42"/>
       <c r="H73" s="32" t="s">
         <v>358</v>
       </c>
@@ -5320,25 +5314,25 @@
       <c r="I78" s="11"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="49" t="s">
+      <c r="A79" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="B79" s="47" t="s">
+      <c r="B79" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="55" t="s">
+      <c r="C79" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D79" s="55">
+      <c r="D79" s="62">
         <v>3</v>
       </c>
-      <c r="E79" s="62" t="s">
+      <c r="E79" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F79" s="59">
+      <c r="F79" s="41">
         <v>43586</v>
       </c>
-      <c r="G79" s="59">
+      <c r="G79" s="41">
         <v>43588</v>
       </c>
       <c r="H79" s="30" t="s">
@@ -5349,13 +5343,13 @@
       </c>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="50"/>
-      <c r="B80" s="48"/>
-      <c r="C80" s="57"/>
-      <c r="D80" s="57"/>
-      <c r="E80" s="64"/>
-      <c r="F80" s="61"/>
-      <c r="G80" s="61"/>
+      <c r="A80" s="40"/>
+      <c r="B80" s="50"/>
+      <c r="C80" s="63"/>
+      <c r="D80" s="63"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="42"/>
+      <c r="G80" s="42"/>
       <c r="H80" s="32" t="s">
         <v>333</v>
       </c>
@@ -5391,25 +5385,25 @@
       </c>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="49" t="s">
+      <c r="A82" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="47" t="s">
+      <c r="B82" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="55" t="s">
+      <c r="C82" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D82" s="55">
+      <c r="D82" s="62">
         <v>4</v>
       </c>
-      <c r="E82" s="62" t="s">
+      <c r="E82" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F82" s="59">
+      <c r="F82" s="41">
         <v>43609</v>
       </c>
-      <c r="G82" s="59">
+      <c r="G82" s="41">
         <v>43616</v>
       </c>
       <c r="H82" s="30" t="s">
@@ -5420,13 +5414,13 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="50"/>
-      <c r="B83" s="48"/>
-      <c r="C83" s="57"/>
-      <c r="D83" s="57"/>
-      <c r="E83" s="64"/>
-      <c r="F83" s="61"/>
-      <c r="G83" s="61"/>
+      <c r="A83" s="40"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="63"/>
+      <c r="D83" s="63"/>
+      <c r="E83" s="55"/>
+      <c r="F83" s="42"/>
+      <c r="G83" s="42"/>
       <c r="H83" s="32" t="s">
         <v>329</v>
       </c>
@@ -5572,25 +5566,25 @@
       </c>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="49" t="s">
+      <c r="A89" s="39" t="s">
         <v>305</v>
       </c>
-      <c r="B89" s="47" t="s">
+      <c r="B89" s="49" t="s">
         <v>306</v>
       </c>
-      <c r="C89" s="55" t="s">
+      <c r="C89" s="62" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="55">
+      <c r="D89" s="62">
         <v>2</v>
       </c>
-      <c r="E89" s="69" t="s">
+      <c r="E89" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F89" s="39">
+      <c r="F89" s="67">
         <v>43671</v>
       </c>
-      <c r="G89" s="39">
+      <c r="G89" s="67">
         <v>43672</v>
       </c>
       <c r="H89" s="30" t="s">
@@ -5601,38 +5595,38 @@
       </c>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="50"/>
-      <c r="B90" s="48"/>
-      <c r="C90" s="57"/>
-      <c r="D90" s="57"/>
-      <c r="E90" s="71"/>
-      <c r="F90" s="40"/>
-      <c r="G90" s="40"/>
+      <c r="A90" s="40"/>
+      <c r="B90" s="50"/>
+      <c r="C90" s="63"/>
+      <c r="D90" s="63"/>
+      <c r="E90" s="61"/>
+      <c r="F90" s="68"/>
+      <c r="G90" s="68"/>
       <c r="H90" s="32" t="s">
         <v>351</v>
       </c>
       <c r="I90" s="52"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A91" s="49" t="s">
+      <c r="A91" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="47" t="s">
+      <c r="B91" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C91" s="45">
+      <c r="C91" s="47">
         <v>43641</v>
       </c>
-      <c r="D91" s="43">
+      <c r="D91" s="45">
         <v>3</v>
       </c>
-      <c r="E91" s="73" t="s">
+      <c r="E91" s="81" t="s">
         <v>282</v>
       </c>
-      <c r="F91" s="39">
+      <c r="F91" s="67">
         <v>43642</v>
       </c>
-      <c r="G91" s="39">
+      <c r="G91" s="67">
         <v>43644</v>
       </c>
       <c r="H91" s="30" t="s">
@@ -5641,13 +5635,13 @@
       <c r="I91" s="51"/>
     </row>
     <row r="92" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A92" s="50"/>
-      <c r="B92" s="48"/>
-      <c r="C92" s="46"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="74"/>
-      <c r="F92" s="40"/>
-      <c r="G92" s="40"/>
+      <c r="A92" s="40"/>
+      <c r="B92" s="50"/>
+      <c r="C92" s="48"/>
+      <c r="D92" s="46"/>
+      <c r="E92" s="82"/>
+      <c r="F92" s="68"/>
+      <c r="G92" s="68"/>
       <c r="H92" s="32" t="s">
         <v>362</v>
       </c>
@@ -5923,25 +5917,25 @@
       </c>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="49" t="s">
+      <c r="A104" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="B104" s="47" t="s">
+      <c r="B104" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C104" s="55" t="s">
+      <c r="C104" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="D104" s="55">
+      <c r="D104" s="62">
         <v>10</v>
       </c>
-      <c r="E104" s="62" t="s">
+      <c r="E104" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F104" s="59">
+      <c r="F104" s="41">
         <v>43613</v>
       </c>
-      <c r="G104" s="59">
+      <c r="G104" s="41">
         <v>43626</v>
       </c>
       <c r="H104" s="30" t="s">
@@ -5952,26 +5946,26 @@
       </c>
     </row>
     <row r="105" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A105" s="53"/>
-      <c r="B105" s="54"/>
-      <c r="C105" s="56"/>
-      <c r="D105" s="56"/>
-      <c r="E105" s="63"/>
-      <c r="F105" s="60"/>
-      <c r="G105" s="60"/>
+      <c r="A105" s="74"/>
+      <c r="B105" s="73"/>
+      <c r="C105" s="80"/>
+      <c r="D105" s="80"/>
+      <c r="E105" s="70"/>
+      <c r="F105" s="69"/>
+      <c r="G105" s="69"/>
       <c r="H105" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="I105" s="68"/>
+      <c r="I105" s="75"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="50"/>
-      <c r="B106" s="48"/>
-      <c r="C106" s="57"/>
-      <c r="D106" s="57"/>
-      <c r="E106" s="64"/>
-      <c r="F106" s="61"/>
-      <c r="G106" s="61"/>
+      <c r="A106" s="40"/>
+      <c r="B106" s="50"/>
+      <c r="C106" s="63"/>
+      <c r="D106" s="63"/>
+      <c r="E106" s="55"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="42"/>
       <c r="H106" s="32" t="s">
         <v>325</v>
       </c>
@@ -6036,25 +6030,25 @@
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="49" t="s">
+      <c r="A109" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="B109" s="47" t="s">
+      <c r="B109" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="55" t="s">
+      <c r="C109" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D109" s="55">
+      <c r="D109" s="62">
         <v>4</v>
       </c>
-      <c r="E109" s="62" t="s">
+      <c r="E109" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F109" s="59">
+      <c r="F109" s="41">
         <v>43627</v>
       </c>
-      <c r="G109" s="59">
+      <c r="G109" s="41">
         <v>43630</v>
       </c>
       <c r="H109" s="30" t="s">
@@ -6065,13 +6059,13 @@
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="50"/>
-      <c r="B110" s="48"/>
-      <c r="C110" s="57"/>
-      <c r="D110" s="57"/>
-      <c r="E110" s="64"/>
-      <c r="F110" s="61"/>
-      <c r="G110" s="61"/>
+      <c r="A110" s="40"/>
+      <c r="B110" s="50"/>
+      <c r="C110" s="63"/>
+      <c r="D110" s="63"/>
+      <c r="E110" s="55"/>
+      <c r="F110" s="42"/>
+      <c r="G110" s="42"/>
       <c r="H110" s="32" t="s">
         <v>324</v>
       </c>
@@ -6194,25 +6188,25 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="49" t="s">
+      <c r="A115" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="B115" s="47" t="s">
+      <c r="B115" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="C115" s="45">
+      <c r="C115" s="47">
         <v>43641</v>
       </c>
-      <c r="D115" s="43">
+      <c r="D115" s="45">
         <v>8</v>
       </c>
-      <c r="E115" s="69" t="s">
+      <c r="E115" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F115" s="75">
+      <c r="F115" s="76">
         <v>43684</v>
       </c>
-      <c r="G115" s="75">
+      <c r="G115" s="76">
         <v>43693</v>
       </c>
       <c r="H115" s="30" t="s">
@@ -6223,51 +6217,51 @@
       </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="53"/>
-      <c r="B116" s="54"/>
+      <c r="A116" s="74"/>
+      <c r="B116" s="73"/>
       <c r="C116" s="72"/>
-      <c r="D116" s="58"/>
-      <c r="E116" s="70"/>
+      <c r="D116" s="71"/>
+      <c r="E116" s="79"/>
       <c r="F116" s="77"/>
       <c r="G116" s="77"/>
       <c r="H116" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="I116" s="68"/>
+      <c r="I116" s="75"/>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="50"/>
-      <c r="B117" s="48"/>
-      <c r="C117" s="46"/>
-      <c r="D117" s="44"/>
-      <c r="E117" s="71"/>
-      <c r="F117" s="76"/>
-      <c r="G117" s="76"/>
+      <c r="A117" s="40"/>
+      <c r="B117" s="50"/>
+      <c r="C117" s="48"/>
+      <c r="D117" s="46"/>
+      <c r="E117" s="61"/>
+      <c r="F117" s="78"/>
+      <c r="G117" s="78"/>
       <c r="H117" s="32" t="s">
         <v>358</v>
       </c>
       <c r="I117" s="52"/>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="49" t="s">
+      <c r="A118" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="B118" s="47" t="s">
+      <c r="B118" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C118" s="45" t="s">
+      <c r="C118" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="D118" s="43">
+      <c r="D118" s="45">
         <v>5</v>
       </c>
-      <c r="E118" s="69" t="s">
+      <c r="E118" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F118" s="75">
+      <c r="F118" s="76">
         <v>43696</v>
       </c>
-      <c r="G118" s="75">
+      <c r="G118" s="76">
         <v>43700</v>
       </c>
       <c r="H118" s="30" t="s">
@@ -6278,13 +6272,13 @@
       </c>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="50"/>
-      <c r="B119" s="48"/>
-      <c r="C119" s="46"/>
-      <c r="D119" s="44"/>
-      <c r="E119" s="71"/>
-      <c r="F119" s="76"/>
-      <c r="G119" s="76"/>
+      <c r="A119" s="40"/>
+      <c r="B119" s="50"/>
+      <c r="C119" s="48"/>
+      <c r="D119" s="46"/>
+      <c r="E119" s="61"/>
+      <c r="F119" s="78"/>
+      <c r="G119" s="78"/>
       <c r="H119" s="32" t="s">
         <v>369</v>
       </c>
@@ -6415,25 +6409,25 @@
       </c>
     </row>
     <row r="126" spans="1:9">
-      <c r="A126" s="49" t="s">
+      <c r="A126" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="B126" s="47" t="s">
+      <c r="B126" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C126" s="55" t="s">
+      <c r="C126" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D126" s="43">
+      <c r="D126" s="45">
         <v>5</v>
       </c>
-      <c r="E126" s="62" t="s">
+      <c r="E126" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F126" s="39">
+      <c r="F126" s="67">
         <v>43643</v>
       </c>
-      <c r="G126" s="39">
+      <c r="G126" s="67">
         <v>43649</v>
       </c>
       <c r="H126" s="30" t="s">
@@ -6444,38 +6438,38 @@
       </c>
     </row>
     <row r="127" spans="1:9">
-      <c r="A127" s="50"/>
-      <c r="B127" s="48"/>
-      <c r="C127" s="57"/>
-      <c r="D127" s="44"/>
-      <c r="E127" s="64"/>
-      <c r="F127" s="40"/>
-      <c r="G127" s="40"/>
+      <c r="A127" s="40"/>
+      <c r="B127" s="50"/>
+      <c r="C127" s="63"/>
+      <c r="D127" s="46"/>
+      <c r="E127" s="55"/>
+      <c r="F127" s="68"/>
+      <c r="G127" s="68"/>
       <c r="H127" s="32" t="s">
         <v>362</v>
       </c>
       <c r="I127" s="52"/>
     </row>
     <row r="128" spans="1:9">
-      <c r="A128" s="49" t="s">
+      <c r="A128" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="B128" s="47" t="s">
+      <c r="B128" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C128" s="55" t="s">
+      <c r="C128" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D128" s="43">
+      <c r="D128" s="45">
         <v>2</v>
       </c>
-      <c r="E128" s="62" t="s">
+      <c r="E128" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F128" s="39">
+      <c r="F128" s="67">
         <v>43650</v>
       </c>
-      <c r="G128" s="39">
+      <c r="G128" s="67">
         <v>43651</v>
       </c>
       <c r="H128" s="30" t="s">
@@ -6486,38 +6480,38 @@
       </c>
     </row>
     <row r="129" spans="1:9">
-      <c r="A129" s="50"/>
-      <c r="B129" s="48"/>
-      <c r="C129" s="57"/>
-      <c r="D129" s="44"/>
-      <c r="E129" s="64"/>
-      <c r="F129" s="40"/>
-      <c r="G129" s="40"/>
+      <c r="A129" s="40"/>
+      <c r="B129" s="50"/>
+      <c r="C129" s="63"/>
+      <c r="D129" s="46"/>
+      <c r="E129" s="55"/>
+      <c r="F129" s="68"/>
+      <c r="G129" s="68"/>
       <c r="H129" s="32" t="s">
         <v>371</v>
       </c>
       <c r="I129" s="52"/>
     </row>
     <row r="130" spans="1:9">
-      <c r="A130" s="49" t="s">
+      <c r="A130" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="B130" s="47" t="s">
+      <c r="B130" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C130" s="55" t="s">
+      <c r="C130" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D130" s="43">
+      <c r="D130" s="45">
         <v>3</v>
       </c>
-      <c r="E130" s="41" t="s">
+      <c r="E130" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F130" s="39">
+      <c r="F130" s="67">
         <v>43685</v>
       </c>
-      <c r="G130" s="39">
+      <c r="G130" s="67">
         <v>43689</v>
       </c>
       <c r="H130" s="30" t="s">
@@ -6528,38 +6522,38 @@
       </c>
     </row>
     <row r="131" spans="1:9">
-      <c r="A131" s="50"/>
-      <c r="B131" s="48"/>
-      <c r="C131" s="57"/>
-      <c r="D131" s="44"/>
-      <c r="E131" s="42"/>
-      <c r="F131" s="40"/>
-      <c r="G131" s="40"/>
+      <c r="A131" s="40"/>
+      <c r="B131" s="50"/>
+      <c r="C131" s="63"/>
+      <c r="D131" s="46"/>
+      <c r="E131" s="44"/>
+      <c r="F131" s="68"/>
+      <c r="G131" s="68"/>
       <c r="H131" s="32" t="s">
         <v>355</v>
       </c>
       <c r="I131" s="52"/>
     </row>
     <row r="132" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A132" s="49" t="s">
+      <c r="A132" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="B132" s="47" t="s">
+      <c r="B132" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="C132" s="45">
+      <c r="C132" s="47">
         <v>43641</v>
       </c>
-      <c r="D132" s="43">
+      <c r="D132" s="45">
         <v>2</v>
       </c>
-      <c r="E132" s="62" t="s">
+      <c r="E132" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F132" s="39">
+      <c r="F132" s="67">
         <v>43654</v>
       </c>
-      <c r="G132" s="39">
+      <c r="G132" s="67">
         <v>43658</v>
       </c>
       <c r="H132" s="30" t="s">
@@ -6570,38 +6564,38 @@
       </c>
     </row>
     <row r="133" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A133" s="50"/>
-      <c r="B133" s="48"/>
-      <c r="C133" s="46"/>
-      <c r="D133" s="44"/>
-      <c r="E133" s="64"/>
-      <c r="F133" s="40"/>
-      <c r="G133" s="40"/>
+      <c r="A133" s="40"/>
+      <c r="B133" s="50"/>
+      <c r="C133" s="48"/>
+      <c r="D133" s="46"/>
+      <c r="E133" s="55"/>
+      <c r="F133" s="68"/>
+      <c r="G133" s="68"/>
       <c r="H133" s="32" t="s">
         <v>355</v>
       </c>
       <c r="I133" s="52"/>
     </row>
     <row r="134" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A134" s="49" t="s">
+      <c r="A134" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="B134" s="47" t="s">
+      <c r="B134" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C134" s="45">
+      <c r="C134" s="47">
         <v>43641</v>
       </c>
-      <c r="D134" s="43">
+      <c r="D134" s="45">
         <v>4</v>
       </c>
-      <c r="E134" s="41" t="s">
+      <c r="E134" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F134" s="39">
+      <c r="F134" s="67">
         <v>43690</v>
       </c>
-      <c r="G134" s="39">
+      <c r="G134" s="67">
         <v>43693</v>
       </c>
       <c r="H134" s="30" t="s">
@@ -6612,38 +6606,38 @@
       </c>
     </row>
     <row r="135" spans="1:9">
-      <c r="A135" s="50"/>
-      <c r="B135" s="48"/>
-      <c r="C135" s="46"/>
-      <c r="D135" s="44"/>
-      <c r="E135" s="42"/>
-      <c r="F135" s="40"/>
-      <c r="G135" s="40"/>
+      <c r="A135" s="40"/>
+      <c r="B135" s="50"/>
+      <c r="C135" s="48"/>
+      <c r="D135" s="46"/>
+      <c r="E135" s="44"/>
+      <c r="F135" s="68"/>
+      <c r="G135" s="68"/>
       <c r="H135" s="32" t="s">
         <v>358</v>
       </c>
       <c r="I135" s="52"/>
     </row>
     <row r="136" spans="1:9">
-      <c r="A136" s="49" t="s">
+      <c r="A136" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="B136" s="47" t="s">
+      <c r="B136" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C136" s="55" t="s">
+      <c r="C136" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="D136" s="43">
+      <c r="D136" s="45">
         <v>5</v>
       </c>
-      <c r="E136" s="41" t="s">
+      <c r="E136" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F136" s="39">
+      <c r="F136" s="67">
         <v>43698</v>
       </c>
-      <c r="G136" s="78">
+      <c r="G136" s="65">
         <v>43704</v>
       </c>
       <c r="H136" s="30" t="s">
@@ -6654,38 +6648,38 @@
       </c>
     </row>
     <row r="137" spans="1:9">
-      <c r="A137" s="50"/>
-      <c r="B137" s="48"/>
-      <c r="C137" s="57"/>
-      <c r="D137" s="44"/>
-      <c r="E137" s="42"/>
-      <c r="F137" s="40"/>
-      <c r="G137" s="79"/>
+      <c r="A137" s="40"/>
+      <c r="B137" s="50"/>
+      <c r="C137" s="63"/>
+      <c r="D137" s="46"/>
+      <c r="E137" s="44"/>
+      <c r="F137" s="68"/>
+      <c r="G137" s="66"/>
       <c r="H137" s="32" t="s">
         <v>369</v>
       </c>
       <c r="I137" s="52"/>
     </row>
     <row r="138" spans="1:9">
-      <c r="A138" s="49" t="s">
+      <c r="A138" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="B138" s="47" t="s">
+      <c r="B138" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C138" s="55" t="s">
+      <c r="C138" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="D138" s="55">
+      <c r="D138" s="62">
         <v>3</v>
       </c>
-      <c r="E138" s="41" t="s">
+      <c r="E138" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F138" s="39">
+      <c r="F138" s="67">
         <v>43705</v>
       </c>
-      <c r="G138" s="39">
+      <c r="G138" s="67">
         <v>43707</v>
       </c>
       <c r="H138" s="30" t="s">
@@ -6696,13 +6690,13 @@
       </c>
     </row>
     <row r="139" spans="1:9">
-      <c r="A139" s="50"/>
-      <c r="B139" s="48"/>
-      <c r="C139" s="57"/>
-      <c r="D139" s="57"/>
-      <c r="E139" s="42"/>
-      <c r="F139" s="40"/>
-      <c r="G139" s="40"/>
+      <c r="A139" s="40"/>
+      <c r="B139" s="50"/>
+      <c r="C139" s="63"/>
+      <c r="D139" s="63"/>
+      <c r="E139" s="44"/>
+      <c r="F139" s="68"/>
+      <c r="G139" s="68"/>
       <c r="H139" s="32" t="s">
         <v>375</v>
       </c>
@@ -6766,25 +6760,25 @@
       <c r="I142" s="11"/>
     </row>
     <row r="143" spans="1:9">
-      <c r="A143" s="49" t="s">
+      <c r="A143" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="B143" s="47" t="s">
+      <c r="B143" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C143" s="55" t="s">
+      <c r="C143" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D143" s="55">
+      <c r="D143" s="62">
         <v>5</v>
       </c>
-      <c r="E143" s="62" t="s">
+      <c r="E143" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F143" s="59">
+      <c r="F143" s="41">
         <v>43579</v>
       </c>
-      <c r="G143" s="59">
+      <c r="G143" s="41">
         <v>43585</v>
       </c>
       <c r="H143" s="30" t="s">
@@ -6795,38 +6789,38 @@
       </c>
     </row>
     <row r="144" spans="1:9">
-      <c r="A144" s="50"/>
-      <c r="B144" s="48"/>
-      <c r="C144" s="57"/>
-      <c r="D144" s="57"/>
-      <c r="E144" s="64"/>
-      <c r="F144" s="61"/>
-      <c r="G144" s="61"/>
+      <c r="A144" s="40"/>
+      <c r="B144" s="50"/>
+      <c r="C144" s="63"/>
+      <c r="D144" s="63"/>
+      <c r="E144" s="55"/>
+      <c r="F144" s="42"/>
+      <c r="G144" s="42"/>
       <c r="H144" s="32" t="s">
         <v>326</v>
       </c>
       <c r="I144" s="52"/>
     </row>
     <row r="145" spans="1:9">
-      <c r="A145" s="49" t="s">
+      <c r="A145" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="B145" s="47" t="s">
+      <c r="B145" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C145" s="55" t="s">
+      <c r="C145" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="D145" s="55">
+      <c r="D145" s="62">
         <v>5</v>
       </c>
-      <c r="E145" s="62" t="s">
+      <c r="E145" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F145" s="59">
+      <c r="F145" s="41">
         <v>43586</v>
       </c>
-      <c r="G145" s="59">
+      <c r="G145" s="41">
         <v>43592</v>
       </c>
       <c r="H145" s="30" t="s">
@@ -6837,38 +6831,38 @@
       </c>
     </row>
     <row r="146" spans="1:9">
-      <c r="A146" s="50"/>
-      <c r="B146" s="48"/>
-      <c r="C146" s="57"/>
-      <c r="D146" s="57"/>
-      <c r="E146" s="64"/>
-      <c r="F146" s="61"/>
-      <c r="G146" s="61"/>
+      <c r="A146" s="40"/>
+      <c r="B146" s="50"/>
+      <c r="C146" s="63"/>
+      <c r="D146" s="63"/>
+      <c r="E146" s="55"/>
+      <c r="F146" s="42"/>
+      <c r="G146" s="42"/>
       <c r="H146" s="32" t="s">
         <v>333</v>
       </c>
       <c r="I146" s="52"/>
     </row>
     <row r="147" spans="1:9">
-      <c r="A147" s="49" t="s">
+      <c r="A147" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="B147" s="47" t="s">
+      <c r="B147" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C147" s="55" t="s">
+      <c r="C147" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="D147" s="55">
+      <c r="D147" s="62">
         <v>5</v>
       </c>
-      <c r="E147" s="62" t="s">
+      <c r="E147" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F147" s="59">
+      <c r="F147" s="41">
         <v>43593</v>
       </c>
-      <c r="G147" s="59">
+      <c r="G147" s="41">
         <v>43599</v>
       </c>
       <c r="H147" s="30" t="s">
@@ -6879,38 +6873,38 @@
       </c>
     </row>
     <row r="148" spans="1:9">
-      <c r="A148" s="50"/>
-      <c r="B148" s="48"/>
-      <c r="C148" s="57"/>
-      <c r="D148" s="57"/>
-      <c r="E148" s="64"/>
-      <c r="F148" s="61"/>
-      <c r="G148" s="61"/>
+      <c r="A148" s="40"/>
+      <c r="B148" s="50"/>
+      <c r="C148" s="63"/>
+      <c r="D148" s="63"/>
+      <c r="E148" s="55"/>
+      <c r="F148" s="42"/>
+      <c r="G148" s="42"/>
       <c r="H148" s="32" t="s">
         <v>335</v>
       </c>
       <c r="I148" s="52"/>
     </row>
     <row r="149" spans="1:9">
-      <c r="A149" s="49" t="s">
+      <c r="A149" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="B149" s="47" t="s">
+      <c r="B149" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C149" s="55" t="s">
+      <c r="C149" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="D149" s="55">
+      <c r="D149" s="62">
         <v>5</v>
       </c>
-      <c r="E149" s="62" t="s">
+      <c r="E149" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F149" s="59">
+      <c r="F149" s="41">
         <v>43626</v>
       </c>
-      <c r="G149" s="59">
+      <c r="G149" s="41">
         <v>43630</v>
       </c>
       <c r="H149" s="30" t="s">
@@ -6921,13 +6915,13 @@
       </c>
     </row>
     <row r="150" spans="1:9">
-      <c r="A150" s="50"/>
-      <c r="B150" s="48"/>
-      <c r="C150" s="57"/>
-      <c r="D150" s="57"/>
-      <c r="E150" s="64"/>
-      <c r="F150" s="61"/>
-      <c r="G150" s="61"/>
+      <c r="A150" s="40"/>
+      <c r="B150" s="50"/>
+      <c r="C150" s="63"/>
+      <c r="D150" s="63"/>
+      <c r="E150" s="55"/>
+      <c r="F150" s="42"/>
+      <c r="G150" s="42"/>
       <c r="H150" s="32" t="s">
         <v>342</v>
       </c>
@@ -6970,7 +6964,7 @@
         <v>32</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D152" s="5">
         <v>2</v>
@@ -6992,25 +6986,25 @@
       </c>
     </row>
     <row r="153" spans="1:9">
-      <c r="A153" s="49" t="s">
+      <c r="A153" s="39" t="s">
         <v>237</v>
       </c>
-      <c r="B153" s="47" t="s">
+      <c r="B153" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C153" s="45">
+      <c r="C153" s="47">
         <v>43641</v>
       </c>
-      <c r="D153" s="55">
+      <c r="D153" s="62">
         <v>7</v>
       </c>
-      <c r="E153" s="69" t="s">
+      <c r="E153" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F153" s="59">
+      <c r="F153" s="41">
         <v>43647</v>
       </c>
-      <c r="G153" s="59">
+      <c r="G153" s="41">
         <v>43655</v>
       </c>
       <c r="H153" s="30" t="s">
@@ -7021,13 +7015,13 @@
       </c>
     </row>
     <row r="154" spans="1:9">
-      <c r="A154" s="50"/>
-      <c r="B154" s="48"/>
-      <c r="C154" s="46"/>
-      <c r="D154" s="57"/>
-      <c r="E154" s="71"/>
-      <c r="F154" s="61"/>
-      <c r="G154" s="61"/>
+      <c r="A154" s="40"/>
+      <c r="B154" s="50"/>
+      <c r="C154" s="48"/>
+      <c r="D154" s="63"/>
+      <c r="E154" s="61"/>
+      <c r="F154" s="42"/>
+      <c r="G154" s="42"/>
       <c r="H154" s="32" t="s">
         <v>377</v>
       </c>
@@ -7092,25 +7086,25 @@
       </c>
     </row>
     <row r="157" spans="1:9" ht="15.75">
-      <c r="A157" s="49" t="s">
+      <c r="A157" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="B157" s="47" t="s">
+      <c r="B157" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C157" s="45" t="s">
+      <c r="C157" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="D157" s="43">
+      <c r="D157" s="45">
         <v>2</v>
       </c>
-      <c r="E157" s="69" t="s">
+      <c r="E157" s="60" t="s">
         <v>236</v>
       </c>
-      <c r="F157" s="59">
+      <c r="F157" s="41">
         <v>43664</v>
       </c>
-      <c r="G157" s="59">
+      <c r="G157" s="41">
         <v>43665</v>
       </c>
       <c r="H157" s="30" t="s">
@@ -7119,13 +7113,13 @@
       <c r="I157" s="38"/>
     </row>
     <row r="158" spans="1:9" ht="15.75">
-      <c r="A158" s="50"/>
-      <c r="B158" s="48"/>
-      <c r="C158" s="46"/>
-      <c r="D158" s="44"/>
-      <c r="E158" s="71"/>
-      <c r="F158" s="61"/>
-      <c r="G158" s="61"/>
+      <c r="A158" s="40"/>
+      <c r="B158" s="50"/>
+      <c r="C158" s="48"/>
+      <c r="D158" s="46"/>
+      <c r="E158" s="61"/>
+      <c r="F158" s="42"/>
+      <c r="G158" s="42"/>
       <c r="H158" s="32" t="s">
         <v>379</v>
       </c>
@@ -7250,25 +7244,25 @@
       </c>
     </row>
     <row r="163" spans="1:9">
-      <c r="A163" s="49" t="s">
+      <c r="A163" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="B163" s="47" t="s">
+      <c r="B163" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="C163" s="45" t="s">
+      <c r="C163" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="D163" s="43">
+      <c r="D163" s="45">
         <v>4</v>
       </c>
-      <c r="E163" s="41" t="s">
+      <c r="E163" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="F163" s="59">
+      <c r="F163" s="41">
         <v>43698</v>
       </c>
-      <c r="G163" s="59">
+      <c r="G163" s="41">
         <v>43703</v>
       </c>
       <c r="H163" s="30" t="s">
@@ -7279,13 +7273,13 @@
       </c>
     </row>
     <row r="164" spans="1:9">
-      <c r="A164" s="50"/>
-      <c r="B164" s="48"/>
-      <c r="C164" s="46"/>
-      <c r="D164" s="44"/>
-      <c r="E164" s="42"/>
-      <c r="F164" s="61"/>
-      <c r="G164" s="61"/>
+      <c r="A164" s="40"/>
+      <c r="B164" s="50"/>
+      <c r="C164" s="48"/>
+      <c r="D164" s="46"/>
+      <c r="E164" s="44"/>
+      <c r="F164" s="42"/>
+      <c r="G164" s="42"/>
       <c r="H164" s="32" t="s">
         <v>369</v>
       </c>
@@ -7463,25 +7457,25 @@
       <c r="I173" s="12"/>
     </row>
     <row r="174" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A174" s="49" t="s">
-        <v>390</v>
-      </c>
-      <c r="B174" s="85" t="s">
+      <c r="A174" s="39" t="s">
+        <v>391</v>
+      </c>
+      <c r="B174" s="59" t="s">
         <v>383</v>
       </c>
-      <c r="C174" s="84" t="s">
+      <c r="C174" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="D174" s="82">
+      <c r="D174" s="56">
         <v>3</v>
       </c>
-      <c r="E174" s="81" t="s">
+      <c r="E174" s="54" t="s">
         <v>226</v>
       </c>
-      <c r="F174" s="80">
+      <c r="F174" s="53">
         <v>43636</v>
       </c>
-      <c r="G174" s="80">
+      <c r="G174" s="53">
         <v>43640</v>
       </c>
       <c r="H174" s="30" t="s">
@@ -7490,13 +7484,13 @@
       <c r="I174" s="11"/>
     </row>
     <row r="175" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A175" s="50"/>
-      <c r="B175" s="48"/>
-      <c r="C175" s="46"/>
-      <c r="D175" s="83"/>
-      <c r="E175" s="64"/>
-      <c r="F175" s="61"/>
-      <c r="G175" s="61"/>
+      <c r="A175" s="40"/>
+      <c r="B175" s="50"/>
+      <c r="C175" s="48"/>
+      <c r="D175" s="57"/>
+      <c r="E175" s="55"/>
+      <c r="F175" s="42"/>
+      <c r="G175" s="42"/>
       <c r="H175" s="32" t="s">
         <v>384</v>
       </c>
@@ -7504,7 +7498,7 @@
     </row>
     <row r="176" spans="1:9" ht="16.5" customHeight="1">
       <c r="A176" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>343</v>
@@ -7531,7 +7525,7 @@
     </row>
     <row r="177" spans="1:9" ht="17.25" customHeight="1" thickBot="1">
       <c r="A177" s="21" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>344</v>
@@ -7553,112 +7547,186 @@
     </row>
   </sheetData>
   <mergeCells count="310">
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="G163:G164"/>
-    <mergeCell ref="F163:F164"/>
-    <mergeCell ref="E163:E164"/>
-    <mergeCell ref="D163:D164"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="B163:B164"/>
-    <mergeCell ref="A163:A164"/>
-    <mergeCell ref="I163:I164"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="G157:G158"/>
-    <mergeCell ref="F157:F158"/>
-    <mergeCell ref="E157:E158"/>
-    <mergeCell ref="D157:D158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="G153:G154"/>
-    <mergeCell ref="F153:F154"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="I153:I154"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="I149:I150"/>
-    <mergeCell ref="G149:G150"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="I136:I137"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="I138:I139"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="I132:I133"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="I134:I135"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="I130:I131"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="G46:G50"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="I46:I50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="G71:G73"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="I89:I90"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="G143:G144"/>
+    <mergeCell ref="E143:E144"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="I143:I144"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I126:I127"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="G145:G146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="I58:I59"/>
     <mergeCell ref="C71:C73"/>
     <mergeCell ref="B71:B73"/>
     <mergeCell ref="A71:A73"/>
@@ -7683,186 +7751,112 @@
     <mergeCell ref="D104:D106"/>
     <mergeCell ref="C104:C106"/>
     <mergeCell ref="B104:B106"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="G145:G146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="G143:G144"/>
-    <mergeCell ref="E143:E144"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="I143:I144"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="C143:C144"/>
-    <mergeCell ref="D143:D144"/>
-    <mergeCell ref="G109:G110"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I126:I127"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="G71:G73"/>
-    <mergeCell ref="F71:F73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="E46:E50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="I46:I50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="I130:I131"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="I132:I133"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="I134:I135"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="I136:I137"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="I138:I139"/>
+    <mergeCell ref="G153:G154"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="I153:I154"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="I149:I150"/>
+    <mergeCell ref="G149:G150"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="G157:G158"/>
+    <mergeCell ref="F157:F158"/>
+    <mergeCell ref="E157:E158"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="C157:C158"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="G163:G164"/>
+    <mergeCell ref="F163:F164"/>
+    <mergeCell ref="E163:E164"/>
+    <mergeCell ref="D163:D164"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="B163:B164"/>
+    <mergeCell ref="A163:A164"/>
+    <mergeCell ref="I163:I164"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pert 2da Entrega finalizado con su respectiva imagen, precedencias de tabla de actividades arregladas, se agrega carpeta duraciones con las duraciones de cada entrega por separado y se agrega word con los caminos de la segunda entrega mas las primera
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D08538-BB8C-4805-A723-A1714C85CF63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" tabRatio="117"/>
+    <workbookView xWindow="0" yWindow="690" windowWidth="11535" windowHeight="14910" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2517,7 +2523,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -3135,16 +3141,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
@@ -3171,19 +3171,103 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3198,87 +3282,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Celda de comprobación" xfId="5" builtinId="23"/>
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
@@ -3323,7 +3329,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3646,19 +3652,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79:B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3674,17 +3680,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="192.75" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="65" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1">
       <c r="A2" s="14" t="s">
@@ -3774,25 +3780,25 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="55">
         <v>8</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="59">
         <v>43577</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="59">
         <v>43586</v>
       </c>
       <c r="H5" s="30" t="s">
@@ -3803,38 +3809,38 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="40"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
       <c r="H6" s="32" t="s">
         <v>326</v>
       </c>
       <c r="I6" s="52"/>
     </row>
     <row r="7" spans="1:9" ht="21.75" customHeight="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="55">
         <v>20</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="62" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7" s="59">
         <v>43577</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="59">
         <v>43602</v>
       </c>
       <c r="H7" s="31" t="s">
@@ -3845,52 +3851,52 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A8" s="74"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="75"/>
+      <c r="I8" s="68"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A9" s="74"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
       <c r="H9" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="I9" s="75"/>
+      <c r="I9" s="68"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="74"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
       <c r="H10" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="I10" s="75"/>
+      <c r="I10" s="68"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="40"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
       <c r="H11" s="32" t="s">
         <v>321</v>
       </c>
@@ -3926,25 +3932,25 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="55">
         <v>6</v>
       </c>
-      <c r="E13" s="64" t="s">
+      <c r="E13" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="59">
         <v>43627</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="59">
         <v>43634</v>
       </c>
       <c r="H13" s="30" t="s">
@@ -3955,13 +3961,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="40"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
       <c r="H14" s="32" t="s">
         <v>324</v>
       </c>
@@ -3997,25 +4003,25 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="45">
         <v>43641</v>
       </c>
-      <c r="D16" s="45">
+      <c r="D16" s="43">
         <v>4</v>
       </c>
-      <c r="E16" s="60" t="s">
+      <c r="E16" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="59">
         <v>43664</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="59">
         <v>43665</v>
       </c>
       <c r="H16" s="30" t="s">
@@ -4026,38 +4032,38 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="40"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
       <c r="H17" s="32" t="s">
         <v>347</v>
       </c>
       <c r="I17" s="52"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="45">
         <v>43641</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="43">
         <v>4</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F18" s="41">
+      <c r="F18" s="59">
         <v>43704</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="59">
         <v>43707</v>
       </c>
       <c r="H18" s="30" t="s">
@@ -4068,13 +4074,13 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="40"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
       <c r="H19" s="32" t="s">
         <v>375</v>
       </c>
@@ -4110,25 +4116,25 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="47">
+      <c r="C21" s="45">
         <v>43641</v>
       </c>
-      <c r="D21" s="45">
+      <c r="D21" s="43">
         <v>5</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="59">
         <v>43703</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="59">
         <v>43707</v>
       </c>
       <c r="H21" s="30" t="s">
@@ -4139,13 +4145,13 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1">
-      <c r="A22" s="40"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
       <c r="H22" s="32" t="s">
         <v>375</v>
       </c>
@@ -4181,25 +4187,25 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="49" t="s">
         <v>275</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="45">
         <v>43641</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="43">
         <v>6</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="59">
         <v>43647</v>
       </c>
-      <c r="G24" s="41">
+      <c r="G24" s="59">
         <v>43654</v>
       </c>
       <c r="H24" s="30" t="s">
@@ -4210,38 +4216,38 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="40"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
       <c r="H25" s="32" t="s">
         <v>371</v>
       </c>
       <c r="I25" s="52"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="49" t="s">
         <v>276</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="C26" s="47">
+      <c r="C26" s="45">
         <v>43641</v>
       </c>
-      <c r="D26" s="45">
+      <c r="D26" s="43">
         <v>4</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F26" s="67">
+      <c r="F26" s="39">
         <v>43656</v>
       </c>
-      <c r="G26" s="67">
+      <c r="G26" s="39">
         <v>43661</v>
       </c>
       <c r="H26" s="30" t="s">
@@ -4252,13 +4258,13 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="40"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
       <c r="H27" s="32" t="s">
         <v>389</v>
       </c>
@@ -4455,25 +4461,25 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="62" t="s">
+      <c r="C38" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="45">
+      <c r="D38" s="43">
         <v>10</v>
       </c>
-      <c r="E38" s="64" t="s">
+      <c r="E38" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F38" s="59">
         <v>43605</v>
       </c>
-      <c r="G38" s="41">
+      <c r="G38" s="59">
         <v>43616</v>
       </c>
       <c r="H38" s="30" t="s">
@@ -4484,26 +4490,26 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A39" s="74"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
       <c r="H39" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="I39" s="75"/>
+      <c r="I39" s="68"/>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1">
-      <c r="A40" s="40"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
+      <c r="A40" s="50"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
       <c r="H40" s="32" t="s">
         <v>329</v>
       </c>
@@ -4655,25 +4661,25 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="47">
+      <c r="C46" s="45">
         <v>43641</v>
       </c>
-      <c r="D46" s="45">
+      <c r="D46" s="43">
         <v>20</v>
       </c>
-      <c r="E46" s="64" t="s">
+      <c r="E46" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F46" s="41">
+      <c r="F46" s="59">
         <v>43641</v>
       </c>
-      <c r="G46" s="41">
+      <c r="G46" s="59">
         <v>43668</v>
       </c>
       <c r="H46" s="30" t="s">
@@ -4684,52 +4690,52 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="74"/>
-      <c r="B47" s="73"/>
+      <c r="A47" s="53"/>
+      <c r="B47" s="54"/>
       <c r="C47" s="72"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="69"/>
-      <c r="G47" s="69"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
       <c r="H47" s="30" t="s">
         <v>363</v>
       </c>
-      <c r="I47" s="75"/>
+      <c r="I47" s="68"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="74"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="53"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="72"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="69"/>
-      <c r="G48" s="69"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
       <c r="H48" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="I48" s="75"/>
+      <c r="I48" s="68"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="74"/>
-      <c r="B49" s="73"/>
+      <c r="A49" s="53"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="72"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="70"/>
-      <c r="F49" s="69"/>
-      <c r="G49" s="69"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
       <c r="H49" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="I49" s="75"/>
+      <c r="I49" s="68"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="40"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="48"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
+      <c r="A50" s="50"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
       <c r="H50" s="32" t="s">
         <v>347</v>
       </c>
@@ -4757,25 +4763,25 @@
       <c r="I51" s="11"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="39" t="s">
+      <c r="A52" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="49" t="s">
+      <c r="B52" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="47" t="s">
+      <c r="C52" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="45">
+      <c r="D52" s="43">
         <v>2</v>
       </c>
-      <c r="E52" s="43" t="s">
+      <c r="E52" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F52" s="41">
+      <c r="F52" s="59">
         <v>43671</v>
       </c>
-      <c r="G52" s="41">
+      <c r="G52" s="59">
         <v>43672</v>
       </c>
       <c r="H52" s="30" t="s">
@@ -4786,13 +4792,13 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="40"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
+      <c r="A53" s="50"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
       <c r="H53" s="32" t="s">
         <v>351</v>
       </c>
@@ -4828,25 +4834,25 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="49" t="s">
+      <c r="B55" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="47" t="s">
+      <c r="C55" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="D55" s="45">
+      <c r="D55" s="43">
         <v>5</v>
       </c>
-      <c r="E55" s="60" t="s">
+      <c r="E55" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F55" s="41">
+      <c r="F55" s="59">
         <v>43677</v>
       </c>
-      <c r="G55" s="41">
+      <c r="G55" s="59">
         <v>43683</v>
       </c>
       <c r="H55" s="30" t="s">
@@ -4857,13 +4863,13 @@
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="40"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="61"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="61"/>
+      <c r="G56" s="61"/>
       <c r="H56" s="32" t="s">
         <v>350</v>
       </c>
@@ -4891,25 +4897,25 @@
       <c r="I57" s="11"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="B58" s="49" t="s">
+      <c r="B58" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="C58" s="47" t="s">
+      <c r="C58" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="45">
+      <c r="D58" s="43">
         <v>5</v>
       </c>
-      <c r="E58" s="60" t="s">
+      <c r="E58" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F58" s="41">
+      <c r="F58" s="59">
         <v>43669</v>
       </c>
-      <c r="G58" s="41">
+      <c r="G58" s="59">
         <v>43675</v>
       </c>
       <c r="H58" s="30" t="s">
@@ -4920,13 +4926,13 @@
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="40"/>
-      <c r="B59" s="50"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="46"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
+      <c r="A59" s="50"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="71"/>
+      <c r="F59" s="61"/>
+      <c r="G59" s="61"/>
       <c r="H59" s="32" t="s">
         <v>351</v>
       </c>
@@ -5038,25 +5044,25 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" customHeight="1">
-      <c r="A65" s="39" t="s">
+      <c r="A65" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="49" t="s">
+      <c r="B65" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="62" t="s">
+      <c r="C65" s="55" t="s">
         <v>210</v>
       </c>
-      <c r="D65" s="62">
+      <c r="D65" s="55">
         <v>13</v>
       </c>
-      <c r="E65" s="64" t="s">
+      <c r="E65" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F65" s="41">
+      <c r="F65" s="59">
         <v>43619</v>
       </c>
-      <c r="G65" s="41">
+      <c r="G65" s="59">
         <v>43635</v>
       </c>
       <c r="H65" s="30" t="s">
@@ -5065,26 +5071,26 @@
       <c r="I65" s="11"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A66" s="74"/>
-      <c r="B66" s="73"/>
-      <c r="C66" s="80"/>
-      <c r="D66" s="80"/>
-      <c r="E66" s="70"/>
-      <c r="F66" s="69"/>
-      <c r="G66" s="69"/>
+      <c r="A66" s="53"/>
+      <c r="B66" s="54"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="63"/>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
       <c r="H66" s="30" t="s">
         <v>331</v>
       </c>
       <c r="I66" s="11"/>
     </row>
     <row r="67" spans="1:9" ht="18" customHeight="1">
-      <c r="A67" s="40"/>
-      <c r="B67" s="50"/>
-      <c r="C67" s="63"/>
-      <c r="D67" s="63"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
+      <c r="A67" s="50"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="61"/>
+      <c r="G67" s="61"/>
       <c r="H67" s="32" t="s">
         <v>324</v>
       </c>
@@ -5093,25 +5099,25 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" customHeight="1">
-      <c r="A68" s="39" t="s">
+      <c r="A68" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="49" t="s">
+      <c r="B68" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="47" t="s">
+      <c r="C68" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="62">
+      <c r="D68" s="55">
         <v>10</v>
       </c>
-      <c r="E68" s="60" t="s">
+      <c r="E68" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F68" s="41">
+      <c r="F68" s="59">
         <v>43669</v>
       </c>
-      <c r="G68" s="41">
+      <c r="G68" s="59">
         <v>43682</v>
       </c>
       <c r="H68" s="30" t="s">
@@ -5122,51 +5128,51 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="18" customHeight="1">
-      <c r="A69" s="74"/>
-      <c r="B69" s="73"/>
+      <c r="A69" s="53"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="72"/>
-      <c r="D69" s="80"/>
-      <c r="E69" s="79"/>
-      <c r="F69" s="69"/>
-      <c r="G69" s="69"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="70"/>
+      <c r="F69" s="60"/>
+      <c r="G69" s="60"/>
       <c r="H69" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="I69" s="75"/>
+      <c r="I69" s="68"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="40"/>
-      <c r="B70" s="50"/>
-      <c r="C70" s="48"/>
-      <c r="D70" s="63"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="42"/>
+      <c r="A70" s="50"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="57"/>
+      <c r="E70" s="71"/>
+      <c r="F70" s="61"/>
+      <c r="G70" s="61"/>
       <c r="H70" s="32" t="s">
         <v>350</v>
       </c>
       <c r="I70" s="52"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="49" t="s">
         <v>154</v>
       </c>
-      <c r="B71" s="49" t="s">
+      <c r="B71" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C71" s="47" t="s">
+      <c r="C71" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="62">
+      <c r="D71" s="55">
         <v>9</v>
       </c>
-      <c r="E71" s="60" t="s">
+      <c r="E71" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F71" s="41">
+      <c r="F71" s="59">
         <v>43683</v>
       </c>
-      <c r="G71" s="41">
+      <c r="G71" s="59">
         <v>43693</v>
       </c>
       <c r="H71" s="30" t="s">
@@ -5177,26 +5183,26 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A72" s="74"/>
-      <c r="B72" s="73"/>
+      <c r="A72" s="53"/>
+      <c r="B72" s="54"/>
       <c r="C72" s="72"/>
-      <c r="D72" s="80"/>
-      <c r="E72" s="79"/>
-      <c r="F72" s="69"/>
-      <c r="G72" s="69"/>
+      <c r="D72" s="56"/>
+      <c r="E72" s="70"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
       <c r="H72" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="I72" s="75"/>
+      <c r="I72" s="68"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="40"/>
-      <c r="B73" s="50"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="63"/>
-      <c r="E73" s="61"/>
-      <c r="F73" s="42"/>
-      <c r="G73" s="42"/>
+      <c r="A73" s="50"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="57"/>
+      <c r="E73" s="71"/>
+      <c r="F73" s="61"/>
+      <c r="G73" s="61"/>
       <c r="H73" s="32" t="s">
         <v>358</v>
       </c>
@@ -5314,25 +5320,25 @@
       <c r="I78" s="11"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="39" t="s">
+      <c r="A79" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="B79" s="49" t="s">
+      <c r="B79" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="62" t="s">
+      <c r="C79" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D79" s="62">
+      <c r="D79" s="55">
         <v>3</v>
       </c>
-      <c r="E79" s="64" t="s">
+      <c r="E79" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F79" s="41">
+      <c r="F79" s="59">
         <v>43586</v>
       </c>
-      <c r="G79" s="41">
+      <c r="G79" s="59">
         <v>43588</v>
       </c>
       <c r="H79" s="30" t="s">
@@ -5343,13 +5349,13 @@
       </c>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="40"/>
-      <c r="B80" s="50"/>
-      <c r="C80" s="63"/>
-      <c r="D80" s="63"/>
-      <c r="E80" s="55"/>
-      <c r="F80" s="42"/>
-      <c r="G80" s="42"/>
+      <c r="A80" s="50"/>
+      <c r="B80" s="48"/>
+      <c r="C80" s="57"/>
+      <c r="D80" s="57"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="61"/>
       <c r="H80" s="32" t="s">
         <v>333</v>
       </c>
@@ -5385,25 +5391,25 @@
       </c>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="39" t="s">
+      <c r="A82" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="49" t="s">
+      <c r="B82" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="62" t="s">
+      <c r="C82" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D82" s="62">
+      <c r="D82" s="55">
         <v>4</v>
       </c>
-      <c r="E82" s="64" t="s">
+      <c r="E82" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F82" s="41">
+      <c r="F82" s="59">
         <v>43609</v>
       </c>
-      <c r="G82" s="41">
+      <c r="G82" s="59">
         <v>43616</v>
       </c>
       <c r="H82" s="30" t="s">
@@ -5414,13 +5420,13 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="40"/>
-      <c r="B83" s="50"/>
-      <c r="C83" s="63"/>
-      <c r="D83" s="63"/>
-      <c r="E83" s="55"/>
-      <c r="F83" s="42"/>
-      <c r="G83" s="42"/>
+      <c r="A83" s="50"/>
+      <c r="B83" s="48"/>
+      <c r="C83" s="57"/>
+      <c r="D83" s="57"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="61"/>
       <c r="H83" s="32" t="s">
         <v>329</v>
       </c>
@@ -5566,25 +5572,25 @@
       </c>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="39" t="s">
+      <c r="A89" s="49" t="s">
         <v>305</v>
       </c>
-      <c r="B89" s="49" t="s">
+      <c r="B89" s="47" t="s">
         <v>306</v>
       </c>
-      <c r="C89" s="62" t="s">
+      <c r="C89" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="62">
+      <c r="D89" s="55">
         <v>2</v>
       </c>
-      <c r="E89" s="60" t="s">
+      <c r="E89" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F89" s="67">
+      <c r="F89" s="39">
         <v>43671</v>
       </c>
-      <c r="G89" s="67">
+      <c r="G89" s="39">
         <v>43672</v>
       </c>
       <c r="H89" s="30" t="s">
@@ -5595,38 +5601,38 @@
       </c>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="40"/>
-      <c r="B90" s="50"/>
-      <c r="C90" s="63"/>
-      <c r="D90" s="63"/>
-      <c r="E90" s="61"/>
-      <c r="F90" s="68"/>
-      <c r="G90" s="68"/>
+      <c r="A90" s="50"/>
+      <c r="B90" s="48"/>
+      <c r="C90" s="57"/>
+      <c r="D90" s="57"/>
+      <c r="E90" s="71"/>
+      <c r="F90" s="40"/>
+      <c r="G90" s="40"/>
       <c r="H90" s="32" t="s">
         <v>351</v>
       </c>
       <c r="I90" s="52"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A91" s="39" t="s">
+      <c r="A91" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="49" t="s">
+      <c r="B91" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C91" s="47">
+      <c r="C91" s="45">
         <v>43641</v>
       </c>
-      <c r="D91" s="45">
+      <c r="D91" s="43">
         <v>3</v>
       </c>
-      <c r="E91" s="81" t="s">
+      <c r="E91" s="73" t="s">
         <v>282</v>
       </c>
-      <c r="F91" s="67">
+      <c r="F91" s="39">
         <v>43642</v>
       </c>
-      <c r="G91" s="67">
+      <c r="G91" s="39">
         <v>43644</v>
       </c>
       <c r="H91" s="30" t="s">
@@ -5635,13 +5641,13 @@
       <c r="I91" s="51"/>
     </row>
     <row r="92" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A92" s="40"/>
-      <c r="B92" s="50"/>
-      <c r="C92" s="48"/>
-      <c r="D92" s="46"/>
-      <c r="E92" s="82"/>
-      <c r="F92" s="68"/>
-      <c r="G92" s="68"/>
+      <c r="A92" s="50"/>
+      <c r="B92" s="48"/>
+      <c r="C92" s="46"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="74"/>
+      <c r="F92" s="40"/>
+      <c r="G92" s="40"/>
       <c r="H92" s="32" t="s">
         <v>362</v>
       </c>
@@ -5917,25 +5923,25 @@
       </c>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="39" t="s">
+      <c r="A104" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B104" s="49" t="s">
+      <c r="B104" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C104" s="62" t="s">
+      <c r="C104" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="D104" s="62">
+      <c r="D104" s="55">
         <v>10</v>
       </c>
-      <c r="E104" s="64" t="s">
+      <c r="E104" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F104" s="41">
+      <c r="F104" s="59">
         <v>43613</v>
       </c>
-      <c r="G104" s="41">
+      <c r="G104" s="59">
         <v>43626</v>
       </c>
       <c r="H104" s="30" t="s">
@@ -5946,26 +5952,26 @@
       </c>
     </row>
     <row r="105" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A105" s="74"/>
-      <c r="B105" s="73"/>
-      <c r="C105" s="80"/>
-      <c r="D105" s="80"/>
-      <c r="E105" s="70"/>
-      <c r="F105" s="69"/>
-      <c r="G105" s="69"/>
+      <c r="A105" s="53"/>
+      <c r="B105" s="54"/>
+      <c r="C105" s="56"/>
+      <c r="D105" s="56"/>
+      <c r="E105" s="63"/>
+      <c r="F105" s="60"/>
+      <c r="G105" s="60"/>
       <c r="H105" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="I105" s="75"/>
+      <c r="I105" s="68"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="40"/>
-      <c r="B106" s="50"/>
-      <c r="C106" s="63"/>
-      <c r="D106" s="63"/>
-      <c r="E106" s="55"/>
-      <c r="F106" s="42"/>
-      <c r="G106" s="42"/>
+      <c r="A106" s="50"/>
+      <c r="B106" s="48"/>
+      <c r="C106" s="57"/>
+      <c r="D106" s="57"/>
+      <c r="E106" s="64"/>
+      <c r="F106" s="61"/>
+      <c r="G106" s="61"/>
       <c r="H106" s="32" t="s">
         <v>325</v>
       </c>
@@ -6030,25 +6036,25 @@
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="39" t="s">
+      <c r="A109" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="B109" s="49" t="s">
+      <c r="B109" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="62" t="s">
-        <v>209</v>
-      </c>
-      <c r="D109" s="62">
+      <c r="C109" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="D109" s="55">
         <v>4</v>
       </c>
-      <c r="E109" s="64" t="s">
+      <c r="E109" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F109" s="41">
+      <c r="F109" s="59">
         <v>43627</v>
       </c>
-      <c r="G109" s="41">
+      <c r="G109" s="59">
         <v>43630</v>
       </c>
       <c r="H109" s="30" t="s">
@@ -6059,13 +6065,13 @@
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="40"/>
-      <c r="B110" s="50"/>
-      <c r="C110" s="63"/>
-      <c r="D110" s="63"/>
-      <c r="E110" s="55"/>
-      <c r="F110" s="42"/>
-      <c r="G110" s="42"/>
+      <c r="A110" s="50"/>
+      <c r="B110" s="48"/>
+      <c r="C110" s="57"/>
+      <c r="D110" s="57"/>
+      <c r="E110" s="64"/>
+      <c r="F110" s="61"/>
+      <c r="G110" s="61"/>
       <c r="H110" s="32" t="s">
         <v>324</v>
       </c>
@@ -6188,25 +6194,25 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="39" t="s">
+      <c r="A115" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="B115" s="49" t="s">
+      <c r="B115" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C115" s="47">
+      <c r="C115" s="45">
         <v>43641</v>
       </c>
-      <c r="D115" s="45">
+      <c r="D115" s="43">
         <v>8</v>
       </c>
-      <c r="E115" s="60" t="s">
+      <c r="E115" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F115" s="76">
+      <c r="F115" s="75">
         <v>43684</v>
       </c>
-      <c r="G115" s="76">
+      <c r="G115" s="75">
         <v>43693</v>
       </c>
       <c r="H115" s="30" t="s">
@@ -6217,51 +6223,51 @@
       </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="74"/>
-      <c r="B116" s="73"/>
+      <c r="A116" s="53"/>
+      <c r="B116" s="54"/>
       <c r="C116" s="72"/>
-      <c r="D116" s="71"/>
-      <c r="E116" s="79"/>
+      <c r="D116" s="58"/>
+      <c r="E116" s="70"/>
       <c r="F116" s="77"/>
       <c r="G116" s="77"/>
       <c r="H116" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="I116" s="75"/>
+      <c r="I116" s="68"/>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="40"/>
-      <c r="B117" s="50"/>
-      <c r="C117" s="48"/>
-      <c r="D117" s="46"/>
-      <c r="E117" s="61"/>
-      <c r="F117" s="78"/>
-      <c r="G117" s="78"/>
+      <c r="A117" s="50"/>
+      <c r="B117" s="48"/>
+      <c r="C117" s="46"/>
+      <c r="D117" s="44"/>
+      <c r="E117" s="71"/>
+      <c r="F117" s="76"/>
+      <c r="G117" s="76"/>
       <c r="H117" s="32" t="s">
         <v>358</v>
       </c>
       <c r="I117" s="52"/>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="39" t="s">
+      <c r="A118" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="B118" s="49" t="s">
+      <c r="B118" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C118" s="47" t="s">
+      <c r="C118" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="D118" s="45">
+      <c r="D118" s="43">
         <v>5</v>
       </c>
-      <c r="E118" s="60" t="s">
+      <c r="E118" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F118" s="76">
+      <c r="F118" s="75">
         <v>43696</v>
       </c>
-      <c r="G118" s="76">
+      <c r="G118" s="75">
         <v>43700</v>
       </c>
       <c r="H118" s="30" t="s">
@@ -6272,13 +6278,13 @@
       </c>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="40"/>
-      <c r="B119" s="50"/>
-      <c r="C119" s="48"/>
-      <c r="D119" s="46"/>
-      <c r="E119" s="61"/>
-      <c r="F119" s="78"/>
-      <c r="G119" s="78"/>
+      <c r="A119" s="50"/>
+      <c r="B119" s="48"/>
+      <c r="C119" s="46"/>
+      <c r="D119" s="44"/>
+      <c r="E119" s="71"/>
+      <c r="F119" s="76"/>
+      <c r="G119" s="76"/>
       <c r="H119" s="32" t="s">
         <v>369</v>
       </c>
@@ -6409,25 +6415,25 @@
       </c>
     </row>
     <row r="126" spans="1:9">
-      <c r="A126" s="39" t="s">
+      <c r="A126" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="B126" s="49" t="s">
+      <c r="B126" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C126" s="62" t="s">
+      <c r="C126" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D126" s="45">
+      <c r="D126" s="43">
         <v>5</v>
       </c>
-      <c r="E126" s="64" t="s">
+      <c r="E126" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F126" s="67">
+      <c r="F126" s="39">
         <v>43643</v>
       </c>
-      <c r="G126" s="67">
+      <c r="G126" s="39">
         <v>43649</v>
       </c>
       <c r="H126" s="30" t="s">
@@ -6438,38 +6444,38 @@
       </c>
     </row>
     <row r="127" spans="1:9">
-      <c r="A127" s="40"/>
-      <c r="B127" s="50"/>
-      <c r="C127" s="63"/>
-      <c r="D127" s="46"/>
-      <c r="E127" s="55"/>
-      <c r="F127" s="68"/>
-      <c r="G127" s="68"/>
+      <c r="A127" s="50"/>
+      <c r="B127" s="48"/>
+      <c r="C127" s="57"/>
+      <c r="D127" s="44"/>
+      <c r="E127" s="64"/>
+      <c r="F127" s="40"/>
+      <c r="G127" s="40"/>
       <c r="H127" s="32" t="s">
         <v>362</v>
       </c>
       <c r="I127" s="52"/>
     </row>
     <row r="128" spans="1:9">
-      <c r="A128" s="39" t="s">
+      <c r="A128" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="B128" s="49" t="s">
+      <c r="B128" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C128" s="62" t="s">
+      <c r="C128" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D128" s="45">
+      <c r="D128" s="43">
         <v>2</v>
       </c>
-      <c r="E128" s="64" t="s">
+      <c r="E128" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F128" s="67">
+      <c r="F128" s="39">
         <v>43650</v>
       </c>
-      <c r="G128" s="67">
+      <c r="G128" s="39">
         <v>43651</v>
       </c>
       <c r="H128" s="30" t="s">
@@ -6480,38 +6486,38 @@
       </c>
     </row>
     <row r="129" spans="1:9">
-      <c r="A129" s="40"/>
-      <c r="B129" s="50"/>
-      <c r="C129" s="63"/>
-      <c r="D129" s="46"/>
-      <c r="E129" s="55"/>
-      <c r="F129" s="68"/>
-      <c r="G129" s="68"/>
+      <c r="A129" s="50"/>
+      <c r="B129" s="48"/>
+      <c r="C129" s="57"/>
+      <c r="D129" s="44"/>
+      <c r="E129" s="64"/>
+      <c r="F129" s="40"/>
+      <c r="G129" s="40"/>
       <c r="H129" s="32" t="s">
         <v>371</v>
       </c>
       <c r="I129" s="52"/>
     </row>
     <row r="130" spans="1:9">
-      <c r="A130" s="39" t="s">
+      <c r="A130" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="B130" s="49" t="s">
+      <c r="B130" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C130" s="62" t="s">
+      <c r="C130" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D130" s="45">
+      <c r="D130" s="43">
         <v>3</v>
       </c>
-      <c r="E130" s="43" t="s">
+      <c r="E130" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F130" s="67">
+      <c r="F130" s="39">
         <v>43685</v>
       </c>
-      <c r="G130" s="67">
+      <c r="G130" s="39">
         <v>43689</v>
       </c>
       <c r="H130" s="30" t="s">
@@ -6522,38 +6528,38 @@
       </c>
     </row>
     <row r="131" spans="1:9">
-      <c r="A131" s="40"/>
-      <c r="B131" s="50"/>
-      <c r="C131" s="63"/>
-      <c r="D131" s="46"/>
-      <c r="E131" s="44"/>
-      <c r="F131" s="68"/>
-      <c r="G131" s="68"/>
+      <c r="A131" s="50"/>
+      <c r="B131" s="48"/>
+      <c r="C131" s="57"/>
+      <c r="D131" s="44"/>
+      <c r="E131" s="42"/>
+      <c r="F131" s="40"/>
+      <c r="G131" s="40"/>
       <c r="H131" s="32" t="s">
         <v>355</v>
       </c>
       <c r="I131" s="52"/>
     </row>
     <row r="132" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A132" s="39" t="s">
+      <c r="A132" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="B132" s="49" t="s">
+      <c r="B132" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="C132" s="47">
+      <c r="C132" s="45">
         <v>43641</v>
       </c>
-      <c r="D132" s="45">
+      <c r="D132" s="43">
         <v>2</v>
       </c>
-      <c r="E132" s="64" t="s">
+      <c r="E132" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F132" s="67">
+      <c r="F132" s="39">
         <v>43654</v>
       </c>
-      <c r="G132" s="67">
+      <c r="G132" s="39">
         <v>43658</v>
       </c>
       <c r="H132" s="30" t="s">
@@ -6564,38 +6570,38 @@
       </c>
     </row>
     <row r="133" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A133" s="40"/>
-      <c r="B133" s="50"/>
-      <c r="C133" s="48"/>
-      <c r="D133" s="46"/>
-      <c r="E133" s="55"/>
-      <c r="F133" s="68"/>
-      <c r="G133" s="68"/>
+      <c r="A133" s="50"/>
+      <c r="B133" s="48"/>
+      <c r="C133" s="46"/>
+      <c r="D133" s="44"/>
+      <c r="E133" s="64"/>
+      <c r="F133" s="40"/>
+      <c r="G133" s="40"/>
       <c r="H133" s="32" t="s">
         <v>355</v>
       </c>
       <c r="I133" s="52"/>
     </row>
     <row r="134" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A134" s="39" t="s">
+      <c r="A134" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="B134" s="49" t="s">
+      <c r="B134" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="C134" s="47">
+      <c r="C134" s="45">
         <v>43641</v>
       </c>
-      <c r="D134" s="45">
+      <c r="D134" s="43">
         <v>4</v>
       </c>
-      <c r="E134" s="43" t="s">
+      <c r="E134" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F134" s="67">
+      <c r="F134" s="39">
         <v>43690</v>
       </c>
-      <c r="G134" s="67">
+      <c r="G134" s="39">
         <v>43693</v>
       </c>
       <c r="H134" s="30" t="s">
@@ -6606,38 +6612,38 @@
       </c>
     </row>
     <row r="135" spans="1:9">
-      <c r="A135" s="40"/>
-      <c r="B135" s="50"/>
-      <c r="C135" s="48"/>
-      <c r="D135" s="46"/>
-      <c r="E135" s="44"/>
-      <c r="F135" s="68"/>
-      <c r="G135" s="68"/>
+      <c r="A135" s="50"/>
+      <c r="B135" s="48"/>
+      <c r="C135" s="46"/>
+      <c r="D135" s="44"/>
+      <c r="E135" s="42"/>
+      <c r="F135" s="40"/>
+      <c r="G135" s="40"/>
       <c r="H135" s="32" t="s">
         <v>358</v>
       </c>
       <c r="I135" s="52"/>
     </row>
     <row r="136" spans="1:9">
-      <c r="A136" s="39" t="s">
+      <c r="A136" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="B136" s="49" t="s">
+      <c r="B136" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="C136" s="62" t="s">
+      <c r="C136" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="D136" s="45">
+      <c r="D136" s="43">
         <v>5</v>
       </c>
-      <c r="E136" s="43" t="s">
+      <c r="E136" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F136" s="67">
+      <c r="F136" s="39">
         <v>43698</v>
       </c>
-      <c r="G136" s="65">
+      <c r="G136" s="78">
         <v>43704</v>
       </c>
       <c r="H136" s="30" t="s">
@@ -6648,38 +6654,38 @@
       </c>
     </row>
     <row r="137" spans="1:9">
-      <c r="A137" s="40"/>
-      <c r="B137" s="50"/>
-      <c r="C137" s="63"/>
-      <c r="D137" s="46"/>
-      <c r="E137" s="44"/>
-      <c r="F137" s="68"/>
-      <c r="G137" s="66"/>
+      <c r="A137" s="50"/>
+      <c r="B137" s="48"/>
+      <c r="C137" s="57"/>
+      <c r="D137" s="44"/>
+      <c r="E137" s="42"/>
+      <c r="F137" s="40"/>
+      <c r="G137" s="79"/>
       <c r="H137" s="32" t="s">
         <v>369</v>
       </c>
       <c r="I137" s="52"/>
     </row>
     <row r="138" spans="1:9">
-      <c r="A138" s="39" t="s">
+      <c r="A138" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="B138" s="49" t="s">
+      <c r="B138" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C138" s="62" t="s">
+      <c r="C138" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="D138" s="62">
+      <c r="D138" s="55">
         <v>3</v>
       </c>
-      <c r="E138" s="43" t="s">
+      <c r="E138" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F138" s="67">
+      <c r="F138" s="39">
         <v>43705</v>
       </c>
-      <c r="G138" s="67">
+      <c r="G138" s="39">
         <v>43707</v>
       </c>
       <c r="H138" s="30" t="s">
@@ -6690,13 +6696,13 @@
       </c>
     </row>
     <row r="139" spans="1:9">
-      <c r="A139" s="40"/>
-      <c r="B139" s="50"/>
-      <c r="C139" s="63"/>
-      <c r="D139" s="63"/>
-      <c r="E139" s="44"/>
-      <c r="F139" s="68"/>
-      <c r="G139" s="68"/>
+      <c r="A139" s="50"/>
+      <c r="B139" s="48"/>
+      <c r="C139" s="57"/>
+      <c r="D139" s="57"/>
+      <c r="E139" s="42"/>
+      <c r="F139" s="40"/>
+      <c r="G139" s="40"/>
       <c r="H139" s="32" t="s">
         <v>375</v>
       </c>
@@ -6760,25 +6766,25 @@
       <c r="I142" s="11"/>
     </row>
     <row r="143" spans="1:9">
-      <c r="A143" s="39" t="s">
+      <c r="A143" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="B143" s="49" t="s">
+      <c r="B143" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C143" s="62" t="s">
+      <c r="C143" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D143" s="62">
+      <c r="D143" s="55">
         <v>5</v>
       </c>
-      <c r="E143" s="64" t="s">
+      <c r="E143" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F143" s="41">
+      <c r="F143" s="59">
         <v>43579</v>
       </c>
-      <c r="G143" s="41">
+      <c r="G143" s="59">
         <v>43585</v>
       </c>
       <c r="H143" s="30" t="s">
@@ -6789,38 +6795,38 @@
       </c>
     </row>
     <row r="144" spans="1:9">
-      <c r="A144" s="40"/>
-      <c r="B144" s="50"/>
-      <c r="C144" s="63"/>
-      <c r="D144" s="63"/>
-      <c r="E144" s="55"/>
-      <c r="F144" s="42"/>
-      <c r="G144" s="42"/>
+      <c r="A144" s="50"/>
+      <c r="B144" s="48"/>
+      <c r="C144" s="57"/>
+      <c r="D144" s="57"/>
+      <c r="E144" s="64"/>
+      <c r="F144" s="61"/>
+      <c r="G144" s="61"/>
       <c r="H144" s="32" t="s">
         <v>326</v>
       </c>
       <c r="I144" s="52"/>
     </row>
     <row r="145" spans="1:9">
-      <c r="A145" s="39" t="s">
+      <c r="A145" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="B145" s="49" t="s">
+      <c r="B145" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C145" s="62" t="s">
+      <c r="C145" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="D145" s="62">
+      <c r="D145" s="55">
         <v>5</v>
       </c>
-      <c r="E145" s="64" t="s">
+      <c r="E145" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F145" s="41">
+      <c r="F145" s="59">
         <v>43586</v>
       </c>
-      <c r="G145" s="41">
+      <c r="G145" s="59">
         <v>43592</v>
       </c>
       <c r="H145" s="30" t="s">
@@ -6831,38 +6837,38 @@
       </c>
     </row>
     <row r="146" spans="1:9">
-      <c r="A146" s="40"/>
-      <c r="B146" s="50"/>
-      <c r="C146" s="63"/>
-      <c r="D146" s="63"/>
-      <c r="E146" s="55"/>
-      <c r="F146" s="42"/>
-      <c r="G146" s="42"/>
+      <c r="A146" s="50"/>
+      <c r="B146" s="48"/>
+      <c r="C146" s="57"/>
+      <c r="D146" s="57"/>
+      <c r="E146" s="64"/>
+      <c r="F146" s="61"/>
+      <c r="G146" s="61"/>
       <c r="H146" s="32" t="s">
         <v>333</v>
       </c>
       <c r="I146" s="52"/>
     </row>
     <row r="147" spans="1:9">
-      <c r="A147" s="39" t="s">
+      <c r="A147" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="B147" s="49" t="s">
+      <c r="B147" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C147" s="62" t="s">
+      <c r="C147" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="D147" s="62">
+      <c r="D147" s="55">
         <v>5</v>
       </c>
-      <c r="E147" s="64" t="s">
+      <c r="E147" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F147" s="41">
+      <c r="F147" s="59">
         <v>43593</v>
       </c>
-      <c r="G147" s="41">
+      <c r="G147" s="59">
         <v>43599</v>
       </c>
       <c r="H147" s="30" t="s">
@@ -6873,38 +6879,38 @@
       </c>
     </row>
     <row r="148" spans="1:9">
-      <c r="A148" s="40"/>
-      <c r="B148" s="50"/>
-      <c r="C148" s="63"/>
-      <c r="D148" s="63"/>
-      <c r="E148" s="55"/>
-      <c r="F148" s="42"/>
-      <c r="G148" s="42"/>
+      <c r="A148" s="50"/>
+      <c r="B148" s="48"/>
+      <c r="C148" s="57"/>
+      <c r="D148" s="57"/>
+      <c r="E148" s="64"/>
+      <c r="F148" s="61"/>
+      <c r="G148" s="61"/>
       <c r="H148" s="32" t="s">
         <v>335</v>
       </c>
       <c r="I148" s="52"/>
     </row>
     <row r="149" spans="1:9">
-      <c r="A149" s="39" t="s">
+      <c r="A149" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="B149" s="49" t="s">
+      <c r="B149" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C149" s="62" t="s">
+      <c r="C149" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="D149" s="62">
+      <c r="D149" s="55">
         <v>5</v>
       </c>
-      <c r="E149" s="64" t="s">
+      <c r="E149" s="62" t="s">
         <v>226</v>
       </c>
-      <c r="F149" s="41">
+      <c r="F149" s="59">
         <v>43626</v>
       </c>
-      <c r="G149" s="41">
+      <c r="G149" s="59">
         <v>43630</v>
       </c>
       <c r="H149" s="30" t="s">
@@ -6915,13 +6921,13 @@
       </c>
     </row>
     <row r="150" spans="1:9">
-      <c r="A150" s="40"/>
-      <c r="B150" s="50"/>
-      <c r="C150" s="63"/>
-      <c r="D150" s="63"/>
-      <c r="E150" s="55"/>
-      <c r="F150" s="42"/>
-      <c r="G150" s="42"/>
+      <c r="A150" s="50"/>
+      <c r="B150" s="48"/>
+      <c r="C150" s="57"/>
+      <c r="D150" s="57"/>
+      <c r="E150" s="64"/>
+      <c r="F150" s="61"/>
+      <c r="G150" s="61"/>
       <c r="H150" s="32" t="s">
         <v>342</v>
       </c>
@@ -6986,25 +6992,25 @@
       </c>
     </row>
     <row r="153" spans="1:9">
-      <c r="A153" s="39" t="s">
+      <c r="A153" s="49" t="s">
         <v>237</v>
       </c>
-      <c r="B153" s="49" t="s">
+      <c r="B153" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C153" s="47">
+      <c r="C153" s="45">
         <v>43641</v>
       </c>
-      <c r="D153" s="62">
+      <c r="D153" s="55">
         <v>7</v>
       </c>
-      <c r="E153" s="60" t="s">
+      <c r="E153" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F153" s="41">
+      <c r="F153" s="59">
         <v>43647</v>
       </c>
-      <c r="G153" s="41">
+      <c r="G153" s="59">
         <v>43655</v>
       </c>
       <c r="H153" s="30" t="s">
@@ -7015,13 +7021,13 @@
       </c>
     </row>
     <row r="154" spans="1:9">
-      <c r="A154" s="40"/>
-      <c r="B154" s="50"/>
-      <c r="C154" s="48"/>
-      <c r="D154" s="63"/>
-      <c r="E154" s="61"/>
-      <c r="F154" s="42"/>
-      <c r="G154" s="42"/>
+      <c r="A154" s="50"/>
+      <c r="B154" s="48"/>
+      <c r="C154" s="46"/>
+      <c r="D154" s="57"/>
+      <c r="E154" s="71"/>
+      <c r="F154" s="61"/>
+      <c r="G154" s="61"/>
       <c r="H154" s="32" t="s">
         <v>377</v>
       </c>
@@ -7086,25 +7092,25 @@
       </c>
     </row>
     <row r="157" spans="1:9" ht="15.75">
-      <c r="A157" s="39" t="s">
+      <c r="A157" s="49" t="s">
         <v>172</v>
       </c>
-      <c r="B157" s="49" t="s">
+      <c r="B157" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C157" s="47" t="s">
+      <c r="C157" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="D157" s="45">
+      <c r="D157" s="43">
         <v>2</v>
       </c>
-      <c r="E157" s="60" t="s">
+      <c r="E157" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="F157" s="41">
+      <c r="F157" s="59">
         <v>43664</v>
       </c>
-      <c r="G157" s="41">
+      <c r="G157" s="59">
         <v>43665</v>
       </c>
       <c r="H157" s="30" t="s">
@@ -7113,13 +7119,13 @@
       <c r="I157" s="38"/>
     </row>
     <row r="158" spans="1:9" ht="15.75">
-      <c r="A158" s="40"/>
-      <c r="B158" s="50"/>
-      <c r="C158" s="48"/>
-      <c r="D158" s="46"/>
-      <c r="E158" s="61"/>
-      <c r="F158" s="42"/>
-      <c r="G158" s="42"/>
+      <c r="A158" s="50"/>
+      <c r="B158" s="48"/>
+      <c r="C158" s="46"/>
+      <c r="D158" s="44"/>
+      <c r="E158" s="71"/>
+      <c r="F158" s="61"/>
+      <c r="G158" s="61"/>
       <c r="H158" s="32" t="s">
         <v>379</v>
       </c>
@@ -7244,25 +7250,25 @@
       </c>
     </row>
     <row r="163" spans="1:9">
-      <c r="A163" s="39" t="s">
+      <c r="A163" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="B163" s="49" t="s">
+      <c r="B163" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C163" s="47" t="s">
+      <c r="C163" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="D163" s="45">
+      <c r="D163" s="43">
         <v>4</v>
       </c>
-      <c r="E163" s="43" t="s">
+      <c r="E163" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="F163" s="41">
+      <c r="F163" s="59">
         <v>43698</v>
       </c>
-      <c r="G163" s="41">
+      <c r="G163" s="59">
         <v>43703</v>
       </c>
       <c r="H163" s="30" t="s">
@@ -7273,13 +7279,13 @@
       </c>
     </row>
     <row r="164" spans="1:9">
-      <c r="A164" s="40"/>
-      <c r="B164" s="50"/>
-      <c r="C164" s="48"/>
-      <c r="D164" s="46"/>
-      <c r="E164" s="44"/>
-      <c r="F164" s="42"/>
-      <c r="G164" s="42"/>
+      <c r="A164" s="50"/>
+      <c r="B164" s="48"/>
+      <c r="C164" s="46"/>
+      <c r="D164" s="44"/>
+      <c r="E164" s="42"/>
+      <c r="F164" s="61"/>
+      <c r="G164" s="61"/>
       <c r="H164" s="32" t="s">
         <v>369</v>
       </c>
@@ -7457,25 +7463,25 @@
       <c r="I173" s="12"/>
     </row>
     <row r="174" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A174" s="39" t="s">
+      <c r="A174" s="49" t="s">
         <v>391</v>
       </c>
-      <c r="B174" s="59" t="s">
+      <c r="B174" s="85" t="s">
         <v>383</v>
       </c>
-      <c r="C174" s="58" t="s">
+      <c r="C174" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="D174" s="56">
+      <c r="D174" s="82">
         <v>3</v>
       </c>
-      <c r="E174" s="54" t="s">
+      <c r="E174" s="81" t="s">
         <v>226</v>
       </c>
-      <c r="F174" s="53">
+      <c r="F174" s="80">
         <v>43636</v>
       </c>
-      <c r="G174" s="53">
+      <c r="G174" s="80">
         <v>43640</v>
       </c>
       <c r="H174" s="30" t="s">
@@ -7484,13 +7490,13 @@
       <c r="I174" s="11"/>
     </row>
     <row r="175" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A175" s="40"/>
-      <c r="B175" s="50"/>
-      <c r="C175" s="48"/>
-      <c r="D175" s="57"/>
-      <c r="E175" s="55"/>
-      <c r="F175" s="42"/>
-      <c r="G175" s="42"/>
+      <c r="A175" s="50"/>
+      <c r="B175" s="48"/>
+      <c r="C175" s="46"/>
+      <c r="D175" s="83"/>
+      <c r="E175" s="64"/>
+      <c r="F175" s="61"/>
+      <c r="G175" s="61"/>
       <c r="H175" s="32" t="s">
         <v>384</v>
       </c>
@@ -7547,6 +7553,292 @@
     </row>
   </sheetData>
   <mergeCells count="310">
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="G163:G164"/>
+    <mergeCell ref="F163:F164"/>
+    <mergeCell ref="E163:E164"/>
+    <mergeCell ref="D163:D164"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="B163:B164"/>
+    <mergeCell ref="A163:A164"/>
+    <mergeCell ref="I163:I164"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="G157:G158"/>
+    <mergeCell ref="F157:F158"/>
+    <mergeCell ref="E157:E158"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="C157:C158"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="G153:G154"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="I153:I154"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="I149:I150"/>
+    <mergeCell ref="G149:G150"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="I136:I137"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="I138:I139"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="I132:I133"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="I134:I135"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="I130:I131"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="E46:E50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="I46:I50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="I71:I73"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="I91:I92"/>
+    <mergeCell ref="G115:G117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="C115:C117"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="I115:I117"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="I109:I110"/>
+    <mergeCell ref="G104:G106"/>
+    <mergeCell ref="F104:F106"/>
+    <mergeCell ref="E104:E106"/>
+    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="G145:G146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="G143:G144"/>
+    <mergeCell ref="E143:E144"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="I143:I144"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I126:I127"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="I89:I90"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="G71:G73"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="I24:I25"/>
     <mergeCell ref="G26:G27"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="E26:E27"/>
@@ -7571,292 +7863,6 @@
     <mergeCell ref="E65:E67"/>
     <mergeCell ref="D65:D67"/>
     <mergeCell ref="G68:G70"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="G71:G73"/>
-    <mergeCell ref="F71:F73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="G143:G144"/>
-    <mergeCell ref="E143:E144"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="I143:I144"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="C143:C144"/>
-    <mergeCell ref="D143:D144"/>
-    <mergeCell ref="G109:G110"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I126:I127"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="G145:G146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="I71:I73"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="I91:I92"/>
-    <mergeCell ref="G115:G117"/>
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="C115:C117"/>
-    <mergeCell ref="B115:B117"/>
-    <mergeCell ref="A115:A117"/>
-    <mergeCell ref="I115:I117"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="I109:I110"/>
-    <mergeCell ref="G104:G106"/>
-    <mergeCell ref="F104:F106"/>
-    <mergeCell ref="E104:E106"/>
-    <mergeCell ref="D104:D106"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="G46:G50"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="I46:I50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="I130:I131"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="I132:I133"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="I134:I135"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="I136:I137"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="I138:I139"/>
-    <mergeCell ref="G153:G154"/>
-    <mergeCell ref="F153:F154"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="I153:I154"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="I149:I150"/>
-    <mergeCell ref="G149:G150"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="G157:G158"/>
-    <mergeCell ref="F157:F158"/>
-    <mergeCell ref="E157:E158"/>
-    <mergeCell ref="D157:D158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="G163:G164"/>
-    <mergeCell ref="F163:F164"/>
-    <mergeCell ref="E163:E164"/>
-    <mergeCell ref="D163:D164"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="B163:B164"/>
-    <mergeCell ref="A163:A164"/>
-    <mergeCell ref="I163:I164"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrado caminezo y algo de taller02011
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EE9AEF-F957-42B4-BBD9-27EC7C9B1D43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFDD8D2-07C3-4E84-975D-9F5BE307C551}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3114,22 +3114,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3150,19 +3147,94 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3176,78 +3248,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3630,8 +3630,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68:E70"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3647,17 +3647,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="192.75" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="62" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="78"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="64"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1">
       <c r="A2" s="14" t="s">
@@ -3747,127 +3747,127 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="54">
         <v>8</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="58">
         <v>43577</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="58">
         <v>43586</v>
       </c>
       <c r="H5" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="I5" s="49" t="s">
+      <c r="I5" s="50" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="38"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
       <c r="H6" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="I6" s="50"/>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:9" ht="21.75" customHeight="1">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="54">
         <v>20</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="58">
         <v>43577</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="58">
         <v>43602</v>
       </c>
       <c r="H7" s="29" t="s">
         <v>317</v>
       </c>
-      <c r="I7" s="49" t="s">
+      <c r="I7" s="50" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A8" s="70"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
       <c r="H8" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="71"/>
+      <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A9" s="70"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
       <c r="H9" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="I9" s="71"/>
+      <c r="I9" s="65"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="70"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
       <c r="H10" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="I10" s="71"/>
+      <c r="I10" s="65"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="38"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
       <c r="H11" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="I11" s="50"/>
+      <c r="I11" s="51"/>
     </row>
     <row r="12" spans="1:9" ht="18.75">
       <c r="A12" s="32" t="s">
@@ -3899,46 +3899,46 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="54">
         <v>6</v>
       </c>
-      <c r="E13" s="60" t="s">
+      <c r="E13" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F13" s="39">
+      <c r="F13" s="58">
         <v>43627</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="58">
         <v>43634</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>323</v>
       </c>
-      <c r="I13" s="49" t="s">
+      <c r="I13" s="50" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="38"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="I14" s="50"/>
+      <c r="I14" s="51"/>
     </row>
     <row r="15" spans="1:9" ht="18.75">
       <c r="A15" s="4" t="s">
@@ -3970,88 +3970,88 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="44">
         <v>43641</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="42">
         <v>4</v>
       </c>
-      <c r="E16" s="60" t="s">
+      <c r="E16" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="58">
         <v>43664</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="58">
         <v>43665</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>344</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="I16" s="50" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A17" s="38"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
       <c r="H17" s="30" t="s">
         <v>345</v>
       </c>
-      <c r="I17" s="50"/>
+      <c r="I17" s="51"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="44">
         <v>43641</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="42">
         <v>4</v>
       </c>
-      <c r="E18" s="79" t="s">
+      <c r="E18" s="66" t="s">
         <v>283</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="58">
         <v>43704</v>
       </c>
-      <c r="G18" s="39">
+      <c r="G18" s="58">
         <v>43707</v>
       </c>
       <c r="H18" s="28" t="s">
         <v>384</v>
       </c>
-      <c r="I18" s="49" t="s">
+      <c r="I18" s="50" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A19" s="38"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
       <c r="H19" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="I19" s="50"/>
+      <c r="I19" s="51"/>
     </row>
     <row r="20" spans="1:9" ht="20.25" thickTop="1" thickBot="1">
       <c r="A20" s="4" t="s">
@@ -4066,7 +4066,7 @@
       <c r="D20" s="10">
         <v>2</v>
       </c>
-      <c r="E20" s="80" t="s">
+      <c r="E20" s="37" t="s">
         <v>226</v>
       </c>
       <c r="F20" s="22">
@@ -4083,46 +4083,46 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="44">
         <v>43641</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="42">
         <v>5</v>
       </c>
-      <c r="E21" s="81" t="s">
+      <c r="E21" s="67" t="s">
         <v>226</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="58">
         <v>43703</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="58">
         <v>43707</v>
       </c>
       <c r="H21" s="28" t="s">
         <v>384</v>
       </c>
-      <c r="I21" s="49" t="s">
+      <c r="I21" s="50" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A22" s="38"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
       <c r="H22" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="I22" s="50"/>
+      <c r="I22" s="51"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" thickTop="1">
       <c r="A23" s="4" t="s">
@@ -4154,88 +4154,88 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="46" t="s">
         <v>280</v>
       </c>
-      <c r="C24" s="45">
+      <c r="C24" s="44">
         <v>43641</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="42">
         <v>6</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="58">
         <v>43647</v>
       </c>
-      <c r="G24" s="39">
+      <c r="G24" s="58">
         <v>43654</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>385</v>
       </c>
-      <c r="I24" s="49" t="s">
+      <c r="I24" s="50" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="38"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
       <c r="H25" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="I25" s="50"/>
+      <c r="I25" s="51"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="46" t="s">
         <v>281</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="44">
         <v>43641</v>
       </c>
-      <c r="D26" s="43">
+      <c r="D26" s="42">
         <v>4</v>
       </c>
-      <c r="E26" s="60" t="s">
+      <c r="E26" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="38">
         <v>43656</v>
       </c>
-      <c r="G26" s="63">
+      <c r="G26" s="38">
         <v>43661</v>
       </c>
       <c r="H26" s="28" t="s">
         <v>386</v>
       </c>
-      <c r="I26" s="49" t="s">
+      <c r="I26" s="50" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="38"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="64"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
       <c r="H27" s="30" t="s">
         <v>387</v>
       </c>
-      <c r="I27" s="50"/>
+      <c r="I27" s="51"/>
     </row>
     <row r="28" spans="1:9" ht="18.75">
       <c r="A28" s="4" t="s">
@@ -4428,59 +4428,59 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="58" t="s">
+      <c r="C38" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="43">
+      <c r="D38" s="42">
         <v>10</v>
       </c>
-      <c r="E38" s="60" t="s">
+      <c r="E38" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="39">
+      <c r="F38" s="58">
         <v>43605</v>
       </c>
-      <c r="G38" s="39">
+      <c r="G38" s="58">
         <v>43616</v>
       </c>
       <c r="H38" s="28" t="s">
         <v>392</v>
       </c>
-      <c r="I38" s="49" t="s">
+      <c r="I38" s="50" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A39" s="70"/>
-      <c r="B39" s="69"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
       <c r="H39" s="28" t="s">
         <v>322</v>
       </c>
-      <c r="I39" s="71"/>
+      <c r="I39" s="65"/>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1">
-      <c r="A40" s="38"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
       <c r="H40" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="I40" s="50"/>
+      <c r="I40" s="51"/>
     </row>
     <row r="41" spans="1:9" ht="18.75">
       <c r="A41" s="4" t="s">
@@ -4628,85 +4628,85 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="45">
+      <c r="C46" s="44">
         <v>43641</v>
       </c>
-      <c r="D46" s="43">
+      <c r="D46" s="42">
         <v>20</v>
       </c>
-      <c r="E46" s="60" t="s">
+      <c r="E46" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F46" s="39">
+      <c r="F46" s="58">
         <v>43641</v>
       </c>
-      <c r="G46" s="39">
+      <c r="G46" s="58">
         <v>43668</v>
       </c>
       <c r="H46" s="28" t="s">
         <v>365</v>
       </c>
-      <c r="I46" s="49" t="s">
+      <c r="I46" s="50" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="70"/>
-      <c r="B47" s="69"/>
+      <c r="A47" s="52"/>
+      <c r="B47" s="53"/>
       <c r="C47" s="68"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="66"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="65"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="59"/>
       <c r="H47" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="I47" s="71"/>
+      <c r="I47" s="65"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="70"/>
-      <c r="B48" s="69"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="53"/>
       <c r="C48" s="68"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="65"/>
-      <c r="G48" s="65"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
       <c r="H48" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="I48" s="71"/>
+      <c r="I48" s="65"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="70"/>
-      <c r="B49" s="69"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="53"/>
       <c r="C49" s="68"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="66"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="65"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
       <c r="H49" s="28" t="s">
         <v>364</v>
       </c>
-      <c r="I49" s="71"/>
+      <c r="I49" s="65"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="38"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
+      <c r="A50" s="49"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
       <c r="H50" s="30" t="s">
         <v>345</v>
       </c>
-      <c r="I50" s="50"/>
+      <c r="I50" s="51"/>
     </row>
     <row r="51" spans="1:9" ht="18.75">
       <c r="A51" s="4" t="s">
@@ -4730,46 +4730,46 @@
       <c r="I51" s="11"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="47" t="s">
+      <c r="B52" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="43">
+      <c r="D52" s="42">
         <v>2</v>
       </c>
-      <c r="E52" s="60" t="s">
+      <c r="E52" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F52" s="39">
+      <c r="F52" s="58">
         <v>43671</v>
       </c>
-      <c r="G52" s="39">
+      <c r="G52" s="58">
         <v>43672</v>
       </c>
       <c r="H52" s="28" t="s">
         <v>366</v>
       </c>
-      <c r="I52" s="49" t="s">
+      <c r="I52" s="50" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="38"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
+      <c r="A53" s="49"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
       <c r="H53" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="I53" s="50"/>
+      <c r="I53" s="51"/>
     </row>
     <row r="54" spans="1:9" ht="18.75">
       <c r="A54" s="4" t="s">
@@ -4801,46 +4801,46 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="47" t="s">
+      <c r="B55" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D55" s="43">
+      <c r="D55" s="42">
         <v>5</v>
       </c>
-      <c r="E55" s="60" t="s">
+      <c r="E55" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F55" s="39">
+      <c r="F55" s="58">
         <v>43677</v>
       </c>
-      <c r="G55" s="39">
+      <c r="G55" s="58">
         <v>43683</v>
       </c>
       <c r="H55" s="28" t="s">
         <v>347</v>
       </c>
-      <c r="I55" s="49" t="s">
+      <c r="I55" s="50" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="38"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
+      <c r="A56" s="49"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="60"/>
       <c r="H56" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="I56" s="50"/>
+      <c r="I56" s="51"/>
     </row>
     <row r="57" spans="1:9" ht="18.75">
       <c r="A57" s="4" t="s">
@@ -4864,46 +4864,46 @@
       <c r="I57" s="11"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="B58" s="47" t="s">
+      <c r="B58" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="C58" s="45" t="s">
+      <c r="C58" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="43">
+      <c r="D58" s="42">
         <v>5</v>
       </c>
-      <c r="E58" s="60" t="s">
+      <c r="E58" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F58" s="39">
+      <c r="F58" s="58">
         <v>43669</v>
       </c>
-      <c r="G58" s="39">
+      <c r="G58" s="58">
         <v>43675</v>
       </c>
       <c r="H58" s="28" t="s">
         <v>350</v>
       </c>
-      <c r="I58" s="49" t="s">
+      <c r="I58" s="50" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="38"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
+      <c r="A59" s="49"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="60"/>
+      <c r="G59" s="60"/>
       <c r="H59" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="I59" s="50"/>
+      <c r="I59" s="51"/>
     </row>
     <row r="60" spans="1:9" ht="18.75">
       <c r="A60" s="4" t="s">
@@ -5011,25 +5011,25 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" customHeight="1">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="47" t="s">
+      <c r="B65" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="58" t="s">
+      <c r="C65" s="54" t="s">
         <v>210</v>
       </c>
-      <c r="D65" s="58">
+      <c r="D65" s="54">
         <v>13</v>
       </c>
-      <c r="E65" s="60" t="s">
+      <c r="E65" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F65" s="39">
+      <c r="F65" s="58">
         <v>43619</v>
       </c>
-      <c r="G65" s="39">
+      <c r="G65" s="58">
         <v>43635</v>
       </c>
       <c r="H65" s="28" t="s">
@@ -5038,26 +5038,26 @@
       <c r="I65" s="11"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A66" s="70"/>
-      <c r="B66" s="69"/>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="66"/>
-      <c r="F66" s="65"/>
-      <c r="G66" s="65"/>
+      <c r="A66" s="52"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="55"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="59"/>
+      <c r="G66" s="59"/>
       <c r="H66" s="28" t="s">
         <v>329</v>
       </c>
       <c r="I66" s="11"/>
     </row>
     <row r="67" spans="1:9" ht="18" customHeight="1">
-      <c r="A67" s="38"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="59"/>
-      <c r="D67" s="59"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="40"/>
-      <c r="G67" s="40"/>
+      <c r="A67" s="49"/>
+      <c r="B67" s="47"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="60"/>
+      <c r="G67" s="60"/>
       <c r="H67" s="30" t="s">
         <v>324</v>
       </c>
@@ -5066,114 +5066,114 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" customHeight="1">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="47" t="s">
+      <c r="B68" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="45" t="s">
+      <c r="C68" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="58">
+      <c r="D68" s="54">
         <v>10</v>
       </c>
-      <c r="E68" s="60" t="s">
+      <c r="E68" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F68" s="39">
+      <c r="F68" s="58">
         <v>43669</v>
       </c>
-      <c r="G68" s="39">
+      <c r="G68" s="58">
         <v>43682</v>
       </c>
       <c r="H68" s="28" t="s">
         <v>351</v>
       </c>
-      <c r="I68" s="49" t="s">
+      <c r="I68" s="50" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="18" customHeight="1">
-      <c r="A69" s="70"/>
-      <c r="B69" s="69"/>
+      <c r="A69" s="52"/>
+      <c r="B69" s="53"/>
       <c r="C69" s="68"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="66"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="61"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
       <c r="H69" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="I69" s="71"/>
+      <c r="I69" s="65"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="38"/>
-      <c r="B70" s="48"/>
-      <c r="C70" s="46"/>
-      <c r="D70" s="59"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="40"/>
-      <c r="G70" s="40"/>
+      <c r="A70" s="49"/>
+      <c r="B70" s="47"/>
+      <c r="C70" s="45"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="41"/>
+      <c r="F70" s="60"/>
+      <c r="G70" s="60"/>
       <c r="H70" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="I70" s="50"/>
+      <c r="I70" s="51"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="37" t="s">
+      <c r="A71" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="B71" s="47" t="s">
+      <c r="B71" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C71" s="45" t="s">
+      <c r="C71" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="58">
+      <c r="D71" s="54">
         <v>9</v>
       </c>
-      <c r="E71" s="60" t="s">
+      <c r="E71" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F71" s="39">
+      <c r="F71" s="58">
         <v>43683</v>
       </c>
-      <c r="G71" s="39">
+      <c r="G71" s="58">
         <v>43693</v>
       </c>
       <c r="H71" s="28" t="s">
         <v>357</v>
       </c>
-      <c r="I71" s="49" t="s">
+      <c r="I71" s="50" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A72" s="70"/>
-      <c r="B72" s="69"/>
+      <c r="A72" s="52"/>
+      <c r="B72" s="53"/>
       <c r="C72" s="68"/>
-      <c r="D72" s="75"/>
-      <c r="E72" s="66"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="65"/>
+      <c r="D72" s="55"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="59"/>
       <c r="H72" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="I72" s="71"/>
+      <c r="I72" s="65"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="38"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="46"/>
-      <c r="D73" s="59"/>
-      <c r="E73" s="53"/>
-      <c r="F73" s="40"/>
-      <c r="G73" s="40"/>
+      <c r="A73" s="49"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="45"/>
+      <c r="D73" s="56"/>
+      <c r="E73" s="41"/>
+      <c r="F73" s="60"/>
+      <c r="G73" s="60"/>
       <c r="H73" s="30" t="s">
         <v>356</v>
       </c>
-      <c r="I73" s="50"/>
+      <c r="I73" s="51"/>
     </row>
     <row r="74" spans="1:9" ht="18.75">
       <c r="A74" s="4" t="s">
@@ -5287,46 +5287,46 @@
       <c r="I78" s="11"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="37" t="s">
+      <c r="A79" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="B79" s="47" t="s">
+      <c r="B79" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="58" t="s">
+      <c r="C79" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D79" s="58">
+      <c r="D79" s="54">
         <v>3</v>
       </c>
-      <c r="E79" s="60" t="s">
+      <c r="E79" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F79" s="39">
+      <c r="F79" s="58">
         <v>43586</v>
       </c>
-      <c r="G79" s="39">
+      <c r="G79" s="58">
         <v>43588</v>
       </c>
       <c r="H79" s="28" t="s">
         <v>330</v>
       </c>
-      <c r="I79" s="49" t="s">
+      <c r="I79" s="50" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="38"/>
-      <c r="B80" s="48"/>
-      <c r="C80" s="59"/>
-      <c r="D80" s="59"/>
-      <c r="E80" s="53"/>
-      <c r="F80" s="40"/>
-      <c r="G80" s="40"/>
+      <c r="A80" s="49"/>
+      <c r="B80" s="47"/>
+      <c r="C80" s="56"/>
+      <c r="D80" s="56"/>
+      <c r="E80" s="41"/>
+      <c r="F80" s="60"/>
+      <c r="G80" s="60"/>
       <c r="H80" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="I80" s="50"/>
+      <c r="I80" s="51"/>
     </row>
     <row r="81" spans="1:9" ht="18.75">
       <c r="A81" s="4" t="s">
@@ -5358,46 +5358,46 @@
       </c>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="37" t="s">
+      <c r="A82" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="47" t="s">
+      <c r="B82" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="58" t="s">
+      <c r="C82" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D82" s="58">
+      <c r="D82" s="54">
         <v>4</v>
       </c>
-      <c r="E82" s="60" t="s">
+      <c r="E82" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F82" s="39">
+      <c r="F82" s="58">
         <v>43609</v>
       </c>
-      <c r="G82" s="39">
+      <c r="G82" s="58">
         <v>43616</v>
       </c>
       <c r="H82" s="28" t="s">
         <v>332</v>
       </c>
-      <c r="I82" s="49" t="s">
+      <c r="I82" s="50" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="38"/>
-      <c r="B83" s="48"/>
-      <c r="C83" s="59"/>
-      <c r="D83" s="59"/>
-      <c r="E83" s="53"/>
-      <c r="F83" s="40"/>
-      <c r="G83" s="40"/>
+      <c r="A83" s="49"/>
+      <c r="B83" s="47"/>
+      <c r="C83" s="56"/>
+      <c r="D83" s="56"/>
+      <c r="E83" s="41"/>
+      <c r="F83" s="60"/>
+      <c r="G83" s="60"/>
       <c r="H83" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="I83" s="50"/>
+      <c r="I83" s="51"/>
     </row>
     <row r="84" spans="1:9" ht="18.75">
       <c r="A84" s="4" t="s">
@@ -5539,86 +5539,86 @@
       </c>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="37" t="s">
+      <c r="A89" s="48" t="s">
         <v>305</v>
       </c>
-      <c r="B89" s="47" t="s">
+      <c r="B89" s="46" t="s">
         <v>306</v>
       </c>
-      <c r="C89" s="58" t="s">
+      <c r="C89" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="58">
+      <c r="D89" s="54">
         <v>2</v>
       </c>
-      <c r="E89" s="60" t="s">
+      <c r="E89" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F89" s="63">
+      <c r="F89" s="38">
         <v>43671</v>
       </c>
-      <c r="G89" s="63">
+      <c r="G89" s="38">
         <v>43672</v>
       </c>
       <c r="H89" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="I89" s="49" t="s">
+      <c r="I89" s="50" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="38"/>
-      <c r="B90" s="48"/>
-      <c r="C90" s="59"/>
-      <c r="D90" s="59"/>
-      <c r="E90" s="53"/>
-      <c r="F90" s="64"/>
-      <c r="G90" s="64"/>
+      <c r="A90" s="49"/>
+      <c r="B90" s="47"/>
+      <c r="C90" s="56"/>
+      <c r="D90" s="56"/>
+      <c r="E90" s="41"/>
+      <c r="F90" s="39"/>
+      <c r="G90" s="39"/>
       <c r="H90" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="I90" s="50"/>
+      <c r="I90" s="51"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A91" s="37" t="s">
+      <c r="A91" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="47" t="s">
+      <c r="B91" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C91" s="45">
+      <c r="C91" s="44">
         <v>43641</v>
       </c>
-      <c r="D91" s="43">
+      <c r="D91" s="42">
         <v>3</v>
       </c>
-      <c r="E91" s="60" t="s">
+      <c r="E91" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F91" s="63">
+      <c r="F91" s="38">
         <v>43642</v>
       </c>
-      <c r="G91" s="63">
+      <c r="G91" s="38">
         <v>43644</v>
       </c>
       <c r="H91" s="28" t="s">
         <v>359</v>
       </c>
-      <c r="I91" s="49"/>
+      <c r="I91" s="50"/>
     </row>
     <row r="92" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A92" s="38"/>
-      <c r="B92" s="48"/>
-      <c r="C92" s="46"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="53"/>
-      <c r="F92" s="64"/>
-      <c r="G92" s="64"/>
+      <c r="A92" s="49"/>
+      <c r="B92" s="47"/>
+      <c r="C92" s="45"/>
+      <c r="D92" s="43"/>
+      <c r="E92" s="41"/>
+      <c r="F92" s="39"/>
+      <c r="G92" s="39"/>
       <c r="H92" s="30" t="s">
         <v>360</v>
       </c>
-      <c r="I92" s="50"/>
+      <c r="I92" s="51"/>
     </row>
     <row r="93" spans="1:9" ht="18.75">
       <c r="A93" s="4" t="s">
@@ -5890,59 +5890,59 @@
       </c>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="37" t="s">
+      <c r="A104" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="B104" s="47" t="s">
+      <c r="B104" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C104" s="58" t="s">
+      <c r="C104" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="D104" s="58">
+      <c r="D104" s="54">
         <v>10</v>
       </c>
-      <c r="E104" s="60" t="s">
+      <c r="E104" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F104" s="39">
+      <c r="F104" s="58">
         <v>43613</v>
       </c>
-      <c r="G104" s="39">
+      <c r="G104" s="58">
         <v>43626</v>
       </c>
       <c r="H104" s="28" t="s">
         <v>334</v>
       </c>
-      <c r="I104" s="49" t="s">
+      <c r="I104" s="50" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A105" s="70"/>
-      <c r="B105" s="69"/>
-      <c r="C105" s="75"/>
-      <c r="D105" s="75"/>
-      <c r="E105" s="66"/>
-      <c r="F105" s="65"/>
-      <c r="G105" s="65"/>
+      <c r="A105" s="52"/>
+      <c r="B105" s="53"/>
+      <c r="C105" s="55"/>
+      <c r="D105" s="55"/>
+      <c r="E105" s="61"/>
+      <c r="F105" s="59"/>
+      <c r="G105" s="59"/>
       <c r="H105" s="28" t="s">
         <v>335</v>
       </c>
-      <c r="I105" s="71"/>
+      <c r="I105" s="65"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="38"/>
-      <c r="B106" s="48"/>
-      <c r="C106" s="59"/>
-      <c r="D106" s="59"/>
-      <c r="E106" s="53"/>
-      <c r="F106" s="40"/>
-      <c r="G106" s="40"/>
+      <c r="A106" s="49"/>
+      <c r="B106" s="47"/>
+      <c r="C106" s="56"/>
+      <c r="D106" s="56"/>
+      <c r="E106" s="41"/>
+      <c r="F106" s="60"/>
+      <c r="G106" s="60"/>
       <c r="H106" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="I106" s="50"/>
+      <c r="I106" s="51"/>
     </row>
     <row r="107" spans="1:9" ht="18.75">
       <c r="A107" s="4" t="s">
@@ -6003,46 +6003,46 @@
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="37" t="s">
+      <c r="A109" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="B109" s="47" t="s">
+      <c r="B109" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="58" t="s">
+      <c r="C109" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="D109" s="58">
+      <c r="D109" s="54">
         <v>4</v>
       </c>
-      <c r="E109" s="60" t="s">
+      <c r="E109" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F109" s="39">
+      <c r="F109" s="58">
         <v>43627</v>
       </c>
-      <c r="G109" s="39">
+      <c r="G109" s="58">
         <v>43630</v>
       </c>
       <c r="H109" s="28" t="s">
         <v>336</v>
       </c>
-      <c r="I109" s="49" t="s">
+      <c r="I109" s="50" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="38"/>
-      <c r="B110" s="48"/>
-      <c r="C110" s="59"/>
-      <c r="D110" s="59"/>
-      <c r="E110" s="53"/>
-      <c r="F110" s="40"/>
-      <c r="G110" s="40"/>
+      <c r="A110" s="49"/>
+      <c r="B110" s="47"/>
+      <c r="C110" s="56"/>
+      <c r="D110" s="56"/>
+      <c r="E110" s="41"/>
+      <c r="F110" s="60"/>
+      <c r="G110" s="60"/>
       <c r="H110" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="I110" s="50"/>
+      <c r="I110" s="51"/>
     </row>
     <row r="111" spans="1:9" ht="18.75">
       <c r="A111" s="4" t="s">
@@ -6161,101 +6161,101 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="37" t="s">
+      <c r="A115" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B115" s="47" t="s">
+      <c r="B115" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C115" s="45">
+      <c r="C115" s="44">
         <v>43641</v>
       </c>
-      <c r="D115" s="43">
+      <c r="D115" s="42">
         <v>8</v>
       </c>
-      <c r="E115" s="60" t="s">
+      <c r="E115" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F115" s="72">
+      <c r="F115" s="69">
         <v>43684</v>
       </c>
-      <c r="G115" s="72">
+      <c r="G115" s="69">
         <v>43693</v>
       </c>
       <c r="H115" s="28" t="s">
         <v>357</v>
       </c>
-      <c r="I115" s="49" t="s">
+      <c r="I115" s="50" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="70"/>
-      <c r="B116" s="69"/>
+      <c r="A116" s="52"/>
+      <c r="B116" s="53"/>
       <c r="C116" s="68"/>
-      <c r="D116" s="67"/>
-      <c r="E116" s="66"/>
-      <c r="F116" s="73"/>
-      <c r="G116" s="73"/>
+      <c r="D116" s="57"/>
+      <c r="E116" s="61"/>
+      <c r="F116" s="71"/>
+      <c r="G116" s="71"/>
       <c r="H116" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="I116" s="71"/>
+      <c r="I116" s="65"/>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="38"/>
-      <c r="B117" s="48"/>
-      <c r="C117" s="46"/>
-      <c r="D117" s="44"/>
-      <c r="E117" s="53"/>
-      <c r="F117" s="74"/>
-      <c r="G117" s="74"/>
+      <c r="A117" s="49"/>
+      <c r="B117" s="47"/>
+      <c r="C117" s="45"/>
+      <c r="D117" s="43"/>
+      <c r="E117" s="41"/>
+      <c r="F117" s="70"/>
+      <c r="G117" s="70"/>
       <c r="H117" s="30" t="s">
         <v>356</v>
       </c>
-      <c r="I117" s="50"/>
+      <c r="I117" s="51"/>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="37" t="s">
+      <c r="A118" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="B118" s="47" t="s">
+      <c r="B118" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C118" s="45" t="s">
+      <c r="C118" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="D118" s="43">
+      <c r="D118" s="42">
         <v>5</v>
       </c>
-      <c r="E118" s="60" t="s">
+      <c r="E118" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F118" s="72">
+      <c r="F118" s="69">
         <v>43696</v>
       </c>
-      <c r="G118" s="72">
+      <c r="G118" s="69">
         <v>43700</v>
       </c>
       <c r="H118" s="28" t="s">
         <v>368</v>
       </c>
-      <c r="I118" s="49" t="s">
+      <c r="I118" s="50" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="38"/>
-      <c r="B119" s="48"/>
-      <c r="C119" s="46"/>
-      <c r="D119" s="44"/>
-      <c r="E119" s="53"/>
-      <c r="F119" s="74"/>
-      <c r="G119" s="74"/>
+      <c r="A119" s="49"/>
+      <c r="B119" s="47"/>
+      <c r="C119" s="45"/>
+      <c r="D119" s="43"/>
+      <c r="E119" s="41"/>
+      <c r="F119" s="70"/>
+      <c r="G119" s="70"/>
       <c r="H119" s="30" t="s">
         <v>367</v>
       </c>
-      <c r="I119" s="50"/>
+      <c r="I119" s="51"/>
     </row>
     <row r="120" spans="1:9" ht="18.75">
       <c r="A120" s="4" t="s">
@@ -6382,298 +6382,298 @@
       </c>
     </row>
     <row r="126" spans="1:9">
-      <c r="A126" s="37" t="s">
+      <c r="A126" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="B126" s="47" t="s">
+      <c r="B126" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C126" s="58" t="s">
+      <c r="C126" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D126" s="43">
+      <c r="D126" s="42">
         <v>5</v>
       </c>
-      <c r="E126" s="60" t="s">
+      <c r="E126" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F126" s="63">
+      <c r="F126" s="38">
         <v>43643</v>
       </c>
-      <c r="G126" s="63">
+      <c r="G126" s="38">
         <v>43649</v>
       </c>
       <c r="H126" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="I126" s="49" t="s">
+      <c r="I126" s="50" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="127" spans="1:9">
-      <c r="A127" s="38"/>
-      <c r="B127" s="48"/>
-      <c r="C127" s="59"/>
-      <c r="D127" s="44"/>
-      <c r="E127" s="53"/>
-      <c r="F127" s="64"/>
-      <c r="G127" s="64"/>
+      <c r="A127" s="49"/>
+      <c r="B127" s="47"/>
+      <c r="C127" s="56"/>
+      <c r="D127" s="43"/>
+      <c r="E127" s="41"/>
+      <c r="F127" s="39"/>
+      <c r="G127" s="39"/>
       <c r="H127" s="30" t="s">
         <v>360</v>
       </c>
-      <c r="I127" s="50"/>
+      <c r="I127" s="51"/>
     </row>
     <row r="128" spans="1:9">
-      <c r="A128" s="37" t="s">
+      <c r="A128" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="B128" s="47" t="s">
+      <c r="B128" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C128" s="58" t="s">
+      <c r="C128" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D128" s="43">
+      <c r="D128" s="42">
         <v>2</v>
       </c>
-      <c r="E128" s="60" t="s">
+      <c r="E128" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F128" s="63">
+      <c r="F128" s="38">
         <v>43650</v>
       </c>
-      <c r="G128" s="63">
+      <c r="G128" s="38">
         <v>43651</v>
       </c>
       <c r="H128" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="I128" s="49" t="s">
+      <c r="I128" s="50" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="129" spans="1:9">
-      <c r="A129" s="38"/>
-      <c r="B129" s="48"/>
-      <c r="C129" s="59"/>
-      <c r="D129" s="44"/>
-      <c r="E129" s="53"/>
-      <c r="F129" s="64"/>
-      <c r="G129" s="64"/>
+      <c r="A129" s="49"/>
+      <c r="B129" s="47"/>
+      <c r="C129" s="56"/>
+      <c r="D129" s="43"/>
+      <c r="E129" s="41"/>
+      <c r="F129" s="39"/>
+      <c r="G129" s="39"/>
       <c r="H129" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="I129" s="50"/>
+      <c r="I129" s="51"/>
     </row>
     <row r="130" spans="1:9">
-      <c r="A130" s="37" t="s">
+      <c r="A130" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="B130" s="47" t="s">
+      <c r="B130" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C130" s="58" t="s">
+      <c r="C130" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D130" s="43">
+      <c r="D130" s="42">
         <v>3</v>
       </c>
-      <c r="E130" s="60" t="s">
+      <c r="E130" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F130" s="63">
+      <c r="F130" s="38">
         <v>43685</v>
       </c>
-      <c r="G130" s="63">
+      <c r="G130" s="38">
         <v>43689</v>
       </c>
       <c r="H130" s="28" t="s">
         <v>354</v>
       </c>
-      <c r="I130" s="49" t="s">
+      <c r="I130" s="50" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="131" spans="1:9">
-      <c r="A131" s="38"/>
-      <c r="B131" s="48"/>
-      <c r="C131" s="59"/>
-      <c r="D131" s="44"/>
-      <c r="E131" s="53"/>
-      <c r="F131" s="64"/>
-      <c r="G131" s="64"/>
+      <c r="A131" s="49"/>
+      <c r="B131" s="47"/>
+      <c r="C131" s="56"/>
+      <c r="D131" s="43"/>
+      <c r="E131" s="41"/>
+      <c r="F131" s="39"/>
+      <c r="G131" s="39"/>
       <c r="H131" s="30" t="s">
         <v>353</v>
       </c>
-      <c r="I131" s="50"/>
+      <c r="I131" s="51"/>
     </row>
     <row r="132" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A132" s="37" t="s">
+      <c r="A132" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="B132" s="47" t="s">
+      <c r="B132" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C132" s="45">
+      <c r="C132" s="44">
         <v>43641</v>
       </c>
-      <c r="D132" s="43">
+      <c r="D132" s="42">
         <v>2</v>
       </c>
-      <c r="E132" s="60" t="s">
+      <c r="E132" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F132" s="63">
+      <c r="F132" s="38">
         <v>43654</v>
       </c>
-      <c r="G132" s="63">
+      <c r="G132" s="38">
         <v>43658</v>
       </c>
       <c r="H132" s="28" t="s">
         <v>354</v>
       </c>
-      <c r="I132" s="49" t="s">
+      <c r="I132" s="50" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A133" s="38"/>
-      <c r="B133" s="48"/>
-      <c r="C133" s="46"/>
-      <c r="D133" s="44"/>
-      <c r="E133" s="53"/>
-      <c r="F133" s="64"/>
-      <c r="G133" s="64"/>
+      <c r="A133" s="49"/>
+      <c r="B133" s="47"/>
+      <c r="C133" s="45"/>
+      <c r="D133" s="43"/>
+      <c r="E133" s="41"/>
+      <c r="F133" s="39"/>
+      <c r="G133" s="39"/>
       <c r="H133" s="30" t="s">
         <v>353</v>
       </c>
-      <c r="I133" s="50"/>
+      <c r="I133" s="51"/>
     </row>
     <row r="134" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A134" s="37" t="s">
+      <c r="A134" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="B134" s="47" t="s">
+      <c r="B134" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C134" s="45">
+      <c r="C134" s="44">
         <v>43641</v>
       </c>
-      <c r="D134" s="43">
+      <c r="D134" s="42">
         <v>4</v>
       </c>
-      <c r="E134" s="41" t="s">
+      <c r="E134" s="72" t="s">
         <v>284</v>
       </c>
-      <c r="F134" s="63">
+      <c r="F134" s="38">
         <v>43690</v>
       </c>
-      <c r="G134" s="63">
+      <c r="G134" s="38">
         <v>43693</v>
       </c>
       <c r="H134" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="I134" s="49" t="s">
+      <c r="I134" s="50" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="135" spans="1:9">
-      <c r="A135" s="38"/>
-      <c r="B135" s="48"/>
-      <c r="C135" s="46"/>
-      <c r="D135" s="44"/>
-      <c r="E135" s="42"/>
-      <c r="F135" s="64"/>
-      <c r="G135" s="64"/>
+      <c r="A135" s="49"/>
+      <c r="B135" s="47"/>
+      <c r="C135" s="45"/>
+      <c r="D135" s="43"/>
+      <c r="E135" s="73"/>
+      <c r="F135" s="39"/>
+      <c r="G135" s="39"/>
       <c r="H135" s="30" t="s">
         <v>356</v>
       </c>
-      <c r="I135" s="50"/>
+      <c r="I135" s="51"/>
     </row>
     <row r="136" spans="1:9">
-      <c r="A136" s="37" t="s">
+      <c r="A136" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="B136" s="47" t="s">
+      <c r="B136" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C136" s="58" t="s">
+      <c r="C136" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="D136" s="43">
+      <c r="D136" s="42">
         <v>5</v>
       </c>
-      <c r="E136" s="41" t="s">
+      <c r="E136" s="72" t="s">
         <v>284</v>
       </c>
-      <c r="F136" s="63">
+      <c r="F136" s="38">
         <v>43698</v>
       </c>
-      <c r="G136" s="61">
+      <c r="G136" s="74">
         <v>43704</v>
       </c>
       <c r="H136" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="I136" s="49" t="s">
+      <c r="I136" s="50" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="137" spans="1:9">
-      <c r="A137" s="38"/>
-      <c r="B137" s="48"/>
-      <c r="C137" s="59"/>
-      <c r="D137" s="44"/>
-      <c r="E137" s="42"/>
-      <c r="F137" s="64"/>
-      <c r="G137" s="62"/>
+      <c r="A137" s="49"/>
+      <c r="B137" s="47"/>
+      <c r="C137" s="56"/>
+      <c r="D137" s="43"/>
+      <c r="E137" s="73"/>
+      <c r="F137" s="39"/>
+      <c r="G137" s="75"/>
       <c r="H137" s="30" t="s">
         <v>367</v>
       </c>
-      <c r="I137" s="50"/>
+      <c r="I137" s="51"/>
     </row>
     <row r="138" spans="1:9">
-      <c r="A138" s="37" t="s">
+      <c r="A138" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="B138" s="47" t="s">
+      <c r="B138" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C138" s="58" t="s">
+      <c r="C138" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="D138" s="58">
+      <c r="D138" s="54">
         <v>3</v>
       </c>
-      <c r="E138" s="60" t="s">
+      <c r="E138" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F138" s="63">
+      <c r="F138" s="38">
         <v>43705</v>
       </c>
-      <c r="G138" s="63">
+      <c r="G138" s="38">
         <v>43707</v>
       </c>
       <c r="H138" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="I138" s="49" t="s">
+      <c r="I138" s="50" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="139" spans="1:9">
-      <c r="A139" s="38"/>
-      <c r="B139" s="48"/>
-      <c r="C139" s="59"/>
-      <c r="D139" s="59"/>
-      <c r="E139" s="53"/>
-      <c r="F139" s="64"/>
-      <c r="G139" s="64"/>
+      <c r="A139" s="49"/>
+      <c r="B139" s="47"/>
+      <c r="C139" s="56"/>
+      <c r="D139" s="56"/>
+      <c r="E139" s="41"/>
+      <c r="F139" s="39"/>
+      <c r="G139" s="39"/>
       <c r="H139" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="I139" s="50"/>
+      <c r="I139" s="51"/>
     </row>
     <row r="140" spans="1:9" ht="18.75">
       <c r="A140" s="4" t="s">
@@ -6733,172 +6733,172 @@
       <c r="I142" s="11"/>
     </row>
     <row r="143" spans="1:9">
-      <c r="A143" s="37" t="s">
+      <c r="A143" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="B143" s="47" t="s">
+      <c r="B143" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C143" s="58" t="s">
+      <c r="C143" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D143" s="58">
+      <c r="D143" s="54">
         <v>5</v>
       </c>
-      <c r="E143" s="60" t="s">
+      <c r="E143" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F143" s="39">
+      <c r="F143" s="58">
         <v>43579</v>
       </c>
-      <c r="G143" s="39">
+      <c r="G143" s="58">
         <v>43585</v>
       </c>
       <c r="H143" s="28" t="s">
         <v>337</v>
       </c>
-      <c r="I143" s="49" t="s">
+      <c r="I143" s="50" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="144" spans="1:9">
-      <c r="A144" s="38"/>
-      <c r="B144" s="48"/>
-      <c r="C144" s="59"/>
-      <c r="D144" s="59"/>
-      <c r="E144" s="53"/>
-      <c r="F144" s="40"/>
-      <c r="G144" s="40"/>
+      <c r="A144" s="49"/>
+      <c r="B144" s="47"/>
+      <c r="C144" s="56"/>
+      <c r="D144" s="56"/>
+      <c r="E144" s="41"/>
+      <c r="F144" s="60"/>
+      <c r="G144" s="60"/>
       <c r="H144" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="I144" s="50"/>
+      <c r="I144" s="51"/>
     </row>
     <row r="145" spans="1:9">
-      <c r="A145" s="37" t="s">
+      <c r="A145" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="B145" s="47" t="s">
+      <c r="B145" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C145" s="58" t="s">
+      <c r="C145" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="D145" s="58">
+      <c r="D145" s="54">
         <v>5</v>
       </c>
-      <c r="E145" s="60" t="s">
+      <c r="E145" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F145" s="39">
+      <c r="F145" s="58">
         <v>43586</v>
       </c>
-      <c r="G145" s="39">
+      <c r="G145" s="58">
         <v>43592</v>
       </c>
       <c r="H145" s="28" t="s">
         <v>338</v>
       </c>
-      <c r="I145" s="49" t="s">
+      <c r="I145" s="50" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="146" spans="1:9">
-      <c r="A146" s="38"/>
-      <c r="B146" s="48"/>
-      <c r="C146" s="59"/>
-      <c r="D146" s="59"/>
-      <c r="E146" s="53"/>
-      <c r="F146" s="40"/>
-      <c r="G146" s="40"/>
+      <c r="A146" s="49"/>
+      <c r="B146" s="47"/>
+      <c r="C146" s="56"/>
+      <c r="D146" s="56"/>
+      <c r="E146" s="41"/>
+      <c r="F146" s="60"/>
+      <c r="G146" s="60"/>
       <c r="H146" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="I146" s="50"/>
+      <c r="I146" s="51"/>
     </row>
     <row r="147" spans="1:9">
-      <c r="A147" s="37" t="s">
+      <c r="A147" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="B147" s="47" t="s">
+      <c r="B147" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C147" s="58" t="s">
+      <c r="C147" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="D147" s="58">
+      <c r="D147" s="54">
         <v>5</v>
       </c>
-      <c r="E147" s="60" t="s">
+      <c r="E147" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F147" s="39">
+      <c r="F147" s="58">
         <v>43593</v>
       </c>
-      <c r="G147" s="39">
+      <c r="G147" s="58">
         <v>43599</v>
       </c>
       <c r="H147" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="I147" s="49" t="s">
+      <c r="I147" s="50" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="148" spans="1:9">
-      <c r="A148" s="38"/>
-      <c r="B148" s="48"/>
-      <c r="C148" s="59"/>
-      <c r="D148" s="59"/>
-      <c r="E148" s="53"/>
-      <c r="F148" s="40"/>
-      <c r="G148" s="40"/>
+      <c r="A148" s="49"/>
+      <c r="B148" s="47"/>
+      <c r="C148" s="56"/>
+      <c r="D148" s="56"/>
+      <c r="E148" s="41"/>
+      <c r="F148" s="60"/>
+      <c r="G148" s="60"/>
       <c r="H148" s="30" t="s">
         <v>333</v>
       </c>
-      <c r="I148" s="50"/>
+      <c r="I148" s="51"/>
     </row>
     <row r="149" spans="1:9">
-      <c r="A149" s="37" t="s">
+      <c r="A149" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="B149" s="47" t="s">
+      <c r="B149" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C149" s="58" t="s">
+      <c r="C149" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="D149" s="58">
+      <c r="D149" s="54">
         <v>5</v>
       </c>
-      <c r="E149" s="60" t="s">
+      <c r="E149" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F149" s="39">
+      <c r="F149" s="58">
         <v>43626</v>
       </c>
-      <c r="G149" s="39">
+      <c r="G149" s="58">
         <v>43630</v>
       </c>
       <c r="H149" s="28" t="s">
         <v>336</v>
       </c>
-      <c r="I149" s="49" t="s">
+      <c r="I149" s="50" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="150" spans="1:9">
-      <c r="A150" s="38"/>
-      <c r="B150" s="48"/>
-      <c r="C150" s="59"/>
-      <c r="D150" s="59"/>
-      <c r="E150" s="53"/>
-      <c r="F150" s="40"/>
-      <c r="G150" s="40"/>
+      <c r="A150" s="49"/>
+      <c r="B150" s="47"/>
+      <c r="C150" s="56"/>
+      <c r="D150" s="56"/>
+      <c r="E150" s="41"/>
+      <c r="F150" s="60"/>
+      <c r="G150" s="60"/>
       <c r="H150" s="30" t="s">
         <v>340</v>
       </c>
-      <c r="I150" s="50"/>
+      <c r="I150" s="51"/>
     </row>
     <row r="151" spans="1:9" ht="18.75">
       <c r="A151" s="4" t="s">
@@ -6959,46 +6959,46 @@
       </c>
     </row>
     <row r="153" spans="1:9">
-      <c r="A153" s="37" t="s">
+      <c r="A153" s="48" t="s">
         <v>237</v>
       </c>
-      <c r="B153" s="47" t="s">
+      <c r="B153" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C153" s="45">
+      <c r="C153" s="44">
         <v>43641</v>
       </c>
-      <c r="D153" s="58">
+      <c r="D153" s="54">
         <v>7</v>
       </c>
-      <c r="E153" s="60" t="s">
+      <c r="E153" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F153" s="39">
+      <c r="F153" s="58">
         <v>43647</v>
       </c>
-      <c r="G153" s="39">
+      <c r="G153" s="58">
         <v>43655</v>
       </c>
       <c r="H153" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="I153" s="49" t="s">
+      <c r="I153" s="50" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="154" spans="1:9">
-      <c r="A154" s="38"/>
-      <c r="B154" s="48"/>
-      <c r="C154" s="46"/>
-      <c r="D154" s="59"/>
-      <c r="E154" s="53"/>
-      <c r="F154" s="40"/>
-      <c r="G154" s="40"/>
+      <c r="A154" s="49"/>
+      <c r="B154" s="47"/>
+      <c r="C154" s="45"/>
+      <c r="D154" s="56"/>
+      <c r="E154" s="41"/>
+      <c r="F154" s="60"/>
+      <c r="G154" s="60"/>
       <c r="H154" s="30" t="s">
         <v>375</v>
       </c>
-      <c r="I154" s="50"/>
+      <c r="I154" s="51"/>
     </row>
     <row r="155" spans="1:9" ht="18.75">
       <c r="A155" s="4" t="s">
@@ -7059,25 +7059,25 @@
       </c>
     </row>
     <row r="157" spans="1:9" ht="15.75">
-      <c r="A157" s="37" t="s">
+      <c r="A157" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="B157" s="47" t="s">
+      <c r="B157" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C157" s="45" t="s">
+      <c r="C157" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="D157" s="43">
+      <c r="D157" s="42">
         <v>2</v>
       </c>
-      <c r="E157" s="60" t="s">
+      <c r="E157" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F157" s="39">
+      <c r="F157" s="58">
         <v>43664</v>
       </c>
-      <c r="G157" s="39">
+      <c r="G157" s="58">
         <v>43665</v>
       </c>
       <c r="H157" s="28" t="s">
@@ -7086,13 +7086,13 @@
       <c r="I157" s="36"/>
     </row>
     <row r="158" spans="1:9" ht="15.75">
-      <c r="A158" s="38"/>
-      <c r="B158" s="48"/>
-      <c r="C158" s="46"/>
-      <c r="D158" s="44"/>
-      <c r="E158" s="53"/>
-      <c r="F158" s="40"/>
-      <c r="G158" s="40"/>
+      <c r="A158" s="49"/>
+      <c r="B158" s="47"/>
+      <c r="C158" s="45"/>
+      <c r="D158" s="43"/>
+      <c r="E158" s="41"/>
+      <c r="F158" s="60"/>
+      <c r="G158" s="60"/>
       <c r="H158" s="30" t="s">
         <v>377</v>
       </c>
@@ -7217,46 +7217,46 @@
       </c>
     </row>
     <row r="163" spans="1:9">
-      <c r="A163" s="37" t="s">
+      <c r="A163" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="B163" s="47" t="s">
+      <c r="B163" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C163" s="45" t="s">
+      <c r="C163" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="D163" s="43">
+      <c r="D163" s="42">
         <v>4</v>
       </c>
-      <c r="E163" s="60" t="s">
+      <c r="E163" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="F163" s="39">
+      <c r="F163" s="58">
         <v>43698</v>
       </c>
-      <c r="G163" s="39">
+      <c r="G163" s="58">
         <v>43703</v>
       </c>
       <c r="H163" s="28" t="s">
         <v>380</v>
       </c>
-      <c r="I163" s="49" t="s">
+      <c r="I163" s="50" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="164" spans="1:9">
-      <c r="A164" s="38"/>
-      <c r="B164" s="48"/>
-      <c r="C164" s="46"/>
-      <c r="D164" s="44"/>
-      <c r="E164" s="53"/>
-      <c r="F164" s="40"/>
-      <c r="G164" s="40"/>
+      <c r="A164" s="49"/>
+      <c r="B164" s="47"/>
+      <c r="C164" s="45"/>
+      <c r="D164" s="43"/>
+      <c r="E164" s="41"/>
+      <c r="F164" s="60"/>
+      <c r="G164" s="60"/>
       <c r="H164" s="30" t="s">
         <v>367</v>
       </c>
-      <c r="I164" s="50"/>
+      <c r="I164" s="51"/>
     </row>
     <row r="165" spans="1:9" ht="18.75">
       <c r="A165" s="4" t="s">
@@ -7430,25 +7430,25 @@
       <c r="I173" s="12"/>
     </row>
     <row r="174" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A174" s="37" t="s">
+      <c r="A174" s="48" t="s">
         <v>389</v>
       </c>
-      <c r="B174" s="57" t="s">
+      <c r="B174" s="81" t="s">
         <v>381</v>
       </c>
-      <c r="C174" s="56" t="s">
+      <c r="C174" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="D174" s="54">
+      <c r="D174" s="78">
         <v>3</v>
       </c>
-      <c r="E174" s="52" t="s">
+      <c r="E174" s="77" t="s">
         <v>226</v>
       </c>
-      <c r="F174" s="51">
+      <c r="F174" s="76">
         <v>43636</v>
       </c>
-      <c r="G174" s="51">
+      <c r="G174" s="76">
         <v>43640</v>
       </c>
       <c r="H174" s="28" t="s">
@@ -7457,13 +7457,13 @@
       <c r="I174" s="11"/>
     </row>
     <row r="175" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A175" s="38"/>
-      <c r="B175" s="48"/>
-      <c r="C175" s="46"/>
-      <c r="D175" s="55"/>
-      <c r="E175" s="53"/>
-      <c r="F175" s="40"/>
-      <c r="G175" s="40"/>
+      <c r="A175" s="49"/>
+      <c r="B175" s="47"/>
+      <c r="C175" s="45"/>
+      <c r="D175" s="79"/>
+      <c r="E175" s="41"/>
+      <c r="F175" s="60"/>
+      <c r="G175" s="60"/>
       <c r="H175" s="30" t="s">
         <v>382</v>
       </c>
@@ -7520,6 +7520,292 @@
     </row>
   </sheetData>
   <mergeCells count="310">
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="G163:G164"/>
+    <mergeCell ref="F163:F164"/>
+    <mergeCell ref="E163:E164"/>
+    <mergeCell ref="D163:D164"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="B163:B164"/>
+    <mergeCell ref="A163:A164"/>
+    <mergeCell ref="I163:I164"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="G157:G158"/>
+    <mergeCell ref="F157:F158"/>
+    <mergeCell ref="E157:E158"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="C157:C158"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="G153:G154"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="I153:I154"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="I149:I150"/>
+    <mergeCell ref="G149:G150"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="I136:I137"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="I138:I139"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="I132:I133"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="I134:I135"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="I130:I131"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="E46:E50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="I46:I50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="I71:I73"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="I91:I92"/>
+    <mergeCell ref="G115:G117"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="E115:E117"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="C115:C117"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="I115:I117"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="I109:I110"/>
+    <mergeCell ref="G104:G106"/>
+    <mergeCell ref="F104:F106"/>
+    <mergeCell ref="E104:E106"/>
+    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="G145:G146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="G143:G144"/>
+    <mergeCell ref="E143:E144"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="I143:I144"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I126:I127"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="I89:I90"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="G71:G73"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="I24:I25"/>
     <mergeCell ref="G26:G27"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="E26:E27"/>
@@ -7544,292 +7830,6 @@
     <mergeCell ref="E65:E67"/>
     <mergeCell ref="D65:D67"/>
     <mergeCell ref="G68:G70"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="G71:G73"/>
-    <mergeCell ref="F71:F73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="G143:G144"/>
-    <mergeCell ref="E143:E144"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="I143:I144"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="C143:C144"/>
-    <mergeCell ref="D143:D144"/>
-    <mergeCell ref="G109:G110"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I126:I127"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="G145:G146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="I71:I73"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="I91:I92"/>
-    <mergeCell ref="G115:G117"/>
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="C115:C117"/>
-    <mergeCell ref="B115:B117"/>
-    <mergeCell ref="A115:A117"/>
-    <mergeCell ref="I115:I117"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="I109:I110"/>
-    <mergeCell ref="G104:G106"/>
-    <mergeCell ref="F104:F106"/>
-    <mergeCell ref="E104:E106"/>
-    <mergeCell ref="D104:D106"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="G46:G50"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="I46:I50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="I130:I131"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="I132:I133"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="I134:I135"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="I136:I137"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="I138:I139"/>
-    <mergeCell ref="G153:G154"/>
-    <mergeCell ref="F153:F154"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="I153:I154"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="I149:I150"/>
-    <mergeCell ref="G149:G150"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="G157:G158"/>
-    <mergeCell ref="F157:F158"/>
-    <mergeCell ref="E157:E158"/>
-    <mergeCell ref="D157:D158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="G163:G164"/>
-    <mergeCell ref="F163:F164"/>
-    <mergeCell ref="E163:E164"/>
-    <mergeCell ref="D163:D164"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="B163:B164"/>
-    <mergeCell ref="A163:A164"/>
-    <mergeCell ref="I163:I164"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tabla de recursos actualizada, asignacion de recusos a la tabla de actividades 35%
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFDD8D2-07C3-4E84-975D-9F5BE307C551}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="20730" windowHeight="11700" tabRatio="117"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="393">
   <si>
     <t>Nombre</t>
   </si>
@@ -888,9 +882,6 @@
     <t xml:space="preserve">Salvador </t>
   </si>
   <si>
-    <t>Daniel y salvador</t>
-  </si>
-  <si>
     <t>Couto y salvador</t>
   </si>
   <si>
@@ -946,12 +937,6 @@
   </si>
   <si>
     <t>GANTT V2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salvador, tomas </t>
-  </si>
-  <si>
-    <t>Salvador , tomas</t>
   </si>
   <si>
     <t xml:space="preserve">Daniel, tomas  </t>
@@ -2498,12 +2483,21 @@
       <t xml:space="preserve"> 40%</t>
     </r>
   </si>
+  <si>
+    <t>P[01],S[02],T[02]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P[02],P[03], </t>
+  </si>
+  <si>
+    <t>P[03],P[04],</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3117,10 +3111,16 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
@@ -3147,89 +3147,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3249,9 +3171,81 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Celda de comprobación" xfId="5" builtinId="23"/>
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
@@ -3296,7 +3290,7 @@
         <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FBBEC53F-606B-49AB-BB7B-0121B51735D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3373,7 +3367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3425,7 +3419,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3619,47 +3613,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="101.28515625" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="8" max="8" width="53" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="192.75" customHeight="1">
-      <c r="A1" s="62" t="s">
-        <v>343</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="64"/>
-    </row>
-    <row r="2" spans="1:9" ht="24.75" customHeight="1">
+    <row r="1" spans="1:9" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
+        <v>340</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
+    </row>
+    <row r="2" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>124</v>
       </c>
@@ -3676,19 +3671,19 @@
         <v>222</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>104</v>
       </c>
@@ -3711,13 +3706,13 @@
         <v>43621</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I3" s="31" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>105</v>
       </c>
@@ -3740,136 +3735,136 @@
         <v>43580</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I4" s="31" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A5" s="48" t="s">
+    <row r="5" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="58">
         <v>8</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="40">
         <v>43577</v>
       </c>
-      <c r="G5" s="58">
+      <c r="G5" s="40">
         <v>43586</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I5" s="50" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="49"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="30" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I6" s="51"/>
     </row>
-    <row r="7" spans="1:9" ht="21.75" customHeight="1">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="58">
         <v>20</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="58">
+      <c r="F7" s="40">
         <v>43577</v>
       </c>
-      <c r="G7" s="58">
+      <c r="G7" s="40">
         <v>43602</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="I7" s="50" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
+    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="71"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
       <c r="H8" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="I8" s="72"/>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="71"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="28" t="s">
+        <v>316</v>
+      </c>
+      <c r="I9" s="72"/>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="71"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="I10" s="72"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="65"/>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="28" t="s">
-        <v>319</v>
-      </c>
-      <c r="I9" s="65"/>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="28" t="s">
-        <v>320</v>
-      </c>
-      <c r="I10" s="65"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="49"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="30" t="s">
-        <v>321</v>
-      </c>
       <c r="I11" s="51"/>
     </row>
-    <row r="12" spans="1:9" ht="18.75">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>108</v>
       </c>
@@ -3892,55 +3887,55 @@
         <v>43612</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="48" t="s">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="58">
         <v>6</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="40">
         <v>43627</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="40">
         <v>43634</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="I13" s="50" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="49"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I14" s="51"/>
     </row>
-    <row r="15" spans="1:9" ht="18.75">
+    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>227</v>
       </c>
@@ -3963,97 +3958,91 @@
         <v>43623</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="48" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="46">
         <v>43641</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="44">
         <v>4</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F16" s="58">
+      <c r="F16" s="40">
         <v>43664</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="40">
         <v>43665</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="I16" s="50" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="30" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I17" s="51"/>
     </row>
-    <row r="18" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A18" s="48" t="s">
+    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="46">
         <v>43641</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="44">
         <v>4</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="E18" s="80" t="s">
         <v>283</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="40">
         <v>43704</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="40">
         <v>43707</v>
       </c>
-      <c r="H18" s="28" t="s">
-        <v>384</v>
-      </c>
-      <c r="I18" s="50" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="30" t="s">
-        <v>373</v>
-      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="50"/>
+    </row>
+    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="51"/>
     </row>
-    <row r="20" spans="1:9" ht="20.25" thickTop="1" thickBot="1">
+    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>144</v>
       </c>
@@ -4076,55 +4065,55 @@
         <v>43697</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A21" s="48" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="44">
+      <c r="C21" s="46">
         <v>43641</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="44">
         <v>5</v>
       </c>
-      <c r="E21" s="67" t="s">
+      <c r="E21" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F21" s="58">
+      <c r="F21" s="40">
         <v>43703</v>
       </c>
-      <c r="G21" s="58">
+      <c r="G21" s="40">
         <v>43707</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I21" s="50" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A22" s="49"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="39"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I22" s="51"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" thickTop="1">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>228</v>
       </c>
@@ -4147,97 +4136,97 @@
         <v>43643</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="48" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="38" t="s">
         <v>275</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="48" t="s">
         <v>280</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="46">
         <v>43641</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="44">
         <v>6</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F24" s="58">
+      <c r="F24" s="40">
         <v>43647</v>
       </c>
-      <c r="G24" s="58">
+      <c r="G24" s="40">
         <v>43654</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="I24" s="50" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="49"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
       <c r="H25" s="30" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I25" s="51"/>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="48" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
         <v>276</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="48" t="s">
         <v>281</v>
       </c>
-      <c r="C26" s="44">
+      <c r="C26" s="46">
         <v>43641</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="44">
         <v>4</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F26" s="38">
+      <c r="F26" s="62">
         <v>43656</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="62">
         <v>43661</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I26" s="50" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="49"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="39"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
       <c r="H27" s="30" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I27" s="51"/>
     </row>
-    <row r="28" spans="1:9" ht="18.75">
+    <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>178</v>
       </c>
@@ -4256,7 +4245,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" ht="18.75">
+    <row r="29" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>179</v>
       </c>
@@ -4275,7 +4264,7 @@
       <c r="H29" s="25"/>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" ht="18.75">
+    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>180</v>
       </c>
@@ -4294,7 +4283,7 @@
       <c r="H30" s="25"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" ht="18.75">
+    <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>181</v>
       </c>
@@ -4313,7 +4302,7 @@
       <c r="H31" s="25"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" ht="18.75">
+    <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>182</v>
       </c>
@@ -4332,7 +4321,7 @@
       <c r="H32" s="25"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" ht="18.75">
+    <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>183</v>
       </c>
@@ -4351,7 +4340,7 @@
       <c r="H33" s="25"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:9" ht="18.75">
+    <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>229</v>
       </c>
@@ -4370,7 +4359,7 @@
       <c r="H34" s="25"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9" ht="18.75">
+    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>230</v>
       </c>
@@ -4389,7 +4378,7 @@
       <c r="H35" s="25"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="1:9" ht="18.75">
+    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>277</v>
       </c>
@@ -4408,7 +4397,7 @@
       <c r="H36" s="25"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9" ht="18.75">
+    <row r="37" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>278</v>
       </c>
@@ -4427,62 +4416,62 @@
       <c r="H37" s="25"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="1:9" ht="15" customHeight="1">
-      <c r="A38" s="48" t="s">
+    <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="48" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="54" t="s">
+      <c r="C38" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="42">
+      <c r="D38" s="44">
         <v>10</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="58">
+      <c r="F38" s="40">
         <v>43605</v>
       </c>
-      <c r="G38" s="58">
+      <c r="G38" s="40">
         <v>43616</v>
       </c>
       <c r="H38" s="28" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I38" s="50" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A39" s="52"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="71"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
       <c r="H39" s="28" t="s">
-        <v>322</v>
-      </c>
-      <c r="I39" s="65"/>
-    </row>
-    <row r="40" spans="1:9" ht="15" customHeight="1">
-      <c r="A40" s="49"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
+        <v>319</v>
+      </c>
+      <c r="I39" s="72"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="39"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
       <c r="H40" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I40" s="51"/>
     </row>
-    <row r="41" spans="1:9" ht="18.75">
+    <row r="41" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>109</v>
       </c>
@@ -4505,13 +4494,13 @@
         <v>43621</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I41" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="18.75">
+    <row r="42" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>110</v>
       </c>
@@ -4534,13 +4523,13 @@
         <v>43622</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I42" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="18.75">
+    <row r="43" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>111</v>
       </c>
@@ -4563,13 +4552,13 @@
         <v>43622</v>
       </c>
       <c r="H43" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I43" s="11" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="18.75">
+    <row r="44" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>112</v>
       </c>
@@ -4592,13 +4581,13 @@
         <v>43626</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I44" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18.75">
+    <row r="45" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>113</v>
       </c>
@@ -4621,94 +4610,94 @@
         <v>43635</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I45" s="11" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="48" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="44">
+      <c r="C46" s="46">
         <v>43641</v>
       </c>
-      <c r="D46" s="42">
+      <c r="D46" s="44">
         <v>20</v>
       </c>
-      <c r="E46" s="40" t="s">
+      <c r="E46" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F46" s="58">
+      <c r="F46" s="40">
         <v>43641</v>
       </c>
-      <c r="G46" s="58">
+      <c r="G46" s="40">
         <v>43668</v>
       </c>
       <c r="H46" s="28" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="I46" s="50" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="52"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="68"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="71"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="66"/>
       <c r="H47" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="I47" s="72"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="71"/>
+      <c r="B48" s="70"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="I48" s="72"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="71"/>
+      <c r="B49" s="70"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="I47" s="65"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="52"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="28" t="s">
-        <v>363</v>
-      </c>
-      <c r="I48" s="65"/>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="52"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="28" t="s">
-        <v>364</v>
-      </c>
-      <c r="I49" s="65"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="49"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="60"/>
+      <c r="I49" s="72"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="39"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="30" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I50" s="51"/>
     </row>
-    <row r="51" spans="1:9" ht="18.75">
+    <row r="51" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>147</v>
       </c>
@@ -4719,7 +4708,7 @@
         <v>146</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>283</v>
@@ -4729,49 +4718,49 @@
       <c r="H51" s="26"/>
       <c r="I51" s="11"/>
     </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="48" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B52" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="42">
+      <c r="D52" s="44">
         <v>2</v>
       </c>
-      <c r="E52" s="40" t="s">
+      <c r="E52" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F52" s="58">
+      <c r="F52" s="40">
         <v>43671</v>
       </c>
-      <c r="G52" s="58">
+      <c r="G52" s="40">
         <v>43672</v>
       </c>
       <c r="H52" s="28" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="I52" s="50" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="49"/>
-      <c r="B53" s="47"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="39"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="30" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I53" s="51"/>
     </row>
-    <row r="54" spans="1:9" ht="18.75">
+    <row r="54" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>149</v>
       </c>
@@ -4794,55 +4783,55 @@
         <v>43675</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="48" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="44" t="s">
+      <c r="C55" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D55" s="42">
+      <c r="D55" s="44">
         <v>5</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="E55" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F55" s="58">
+      <c r="F55" s="40">
         <v>43677</v>
       </c>
-      <c r="G55" s="58">
+      <c r="G55" s="40">
         <v>43683</v>
       </c>
       <c r="H55" s="28" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I55" s="50" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="49"/>
-      <c r="B56" s="47"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="60"/>
-      <c r="G56" s="60"/>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="39"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="30" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I56" s="51"/>
     </row>
-    <row r="57" spans="1:9" ht="18.75">
+    <row r="57" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>151</v>
       </c>
@@ -4853,7 +4842,7 @@
         <v>146</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E57" s="18" t="s">
         <v>283</v>
@@ -4863,49 +4852,49 @@
       <c r="H57" s="26"/>
       <c r="I57" s="11"/>
     </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="48" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="C58" s="44" t="s">
+      <c r="C58" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="42">
+      <c r="D58" s="44">
         <v>5</v>
       </c>
-      <c r="E58" s="40" t="s">
+      <c r="E58" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F58" s="58">
+      <c r="F58" s="40">
         <v>43669</v>
       </c>
-      <c r="G58" s="58">
+      <c r="G58" s="40">
         <v>43675</v>
       </c>
       <c r="H58" s="28" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="I58" s="50" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="49"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="39"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="30" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I59" s="51"/>
     </row>
-    <row r="60" spans="1:9" ht="18.75">
+    <row r="60" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>184</v>
       </c>
@@ -4924,7 +4913,7 @@
       <c r="H60" s="25"/>
       <c r="I60" s="11"/>
     </row>
-    <row r="61" spans="1:9" ht="18.75">
+    <row r="61" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>185</v>
       </c>
@@ -4943,7 +4932,7 @@
       <c r="H61" s="25"/>
       <c r="I61" s="11"/>
     </row>
-    <row r="62" spans="1:9" ht="18.75">
+    <row r="62" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>186</v>
       </c>
@@ -4962,7 +4951,7 @@
       <c r="H62" s="25"/>
       <c r="I62" s="11"/>
     </row>
-    <row r="63" spans="1:9" ht="18.75">
+    <row r="63" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>218</v>
       </c>
@@ -4981,7 +4970,7 @@
       <c r="H63" s="25"/>
       <c r="I63" s="11"/>
     </row>
-    <row r="64" spans="1:9" ht="18.75">
+    <row r="64" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>114</v>
       </c>
@@ -5004,178 +4993,178 @@
         <v>43577</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I64" s="11" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="18" customHeight="1">
-      <c r="A65" s="48" t="s">
+    <row r="65" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="54" t="s">
+      <c r="C65" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="D65" s="54">
+      <c r="D65" s="58">
         <v>13</v>
       </c>
-      <c r="E65" s="40" t="s">
+      <c r="E65" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F65" s="58">
+      <c r="F65" s="40">
         <v>43619</v>
       </c>
-      <c r="G65" s="58">
+      <c r="G65" s="40">
         <v>43635</v>
       </c>
       <c r="H65" s="28" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="I65" s="11"/>
     </row>
-    <row r="66" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A66" s="52"/>
-      <c r="B66" s="53"/>
-      <c r="C66" s="55"/>
-      <c r="D66" s="55"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="59"/>
-      <c r="G66" s="59"/>
+    <row r="66" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="71"/>
+      <c r="B66" s="70"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="67"/>
+      <c r="F66" s="66"/>
+      <c r="G66" s="66"/>
       <c r="H66" s="28" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I66" s="11"/>
     </row>
-    <row r="67" spans="1:9" ht="18" customHeight="1">
-      <c r="A67" s="49"/>
-      <c r="B67" s="47"/>
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="60"/>
-      <c r="G67" s="60"/>
+    <row r="67" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="39"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="41"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I67" s="11" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="18" customHeight="1">
-      <c r="A68" s="48" t="s">
+    <row r="68" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="44" t="s">
+      <c r="C68" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="54">
+      <c r="D68" s="58">
         <v>10</v>
       </c>
-      <c r="E68" s="40" t="s">
+      <c r="E68" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F68" s="58">
+      <c r="F68" s="40">
         <v>43669</v>
       </c>
-      <c r="G68" s="58">
+      <c r="G68" s="40">
         <v>43682</v>
       </c>
       <c r="H68" s="28" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="I68" s="50" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="71"/>
+      <c r="B69" s="70"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="67"/>
+      <c r="F69" s="66"/>
+      <c r="G69" s="66"/>
+      <c r="H69" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="I69" s="72"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="39"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="47"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="41"/>
+      <c r="G70" s="41"/>
+      <c r="H70" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="I70" s="51"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D71" s="58">
+        <v>9</v>
+      </c>
+      <c r="E71" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="F71" s="40">
+        <v>43683</v>
+      </c>
+      <c r="G71" s="40">
+        <v>43693</v>
+      </c>
+      <c r="H71" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="I71" s="50" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="18" customHeight="1">
-      <c r="A69" s="52"/>
-      <c r="B69" s="53"/>
-      <c r="C69" s="68"/>
-      <c r="D69" s="55"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="59"/>
-      <c r="G69" s="59"/>
-      <c r="H69" s="28" t="s">
+    <row r="72" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="71"/>
+      <c r="B72" s="70"/>
+      <c r="C72" s="69"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="67"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="I69" s="65"/>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="49"/>
-      <c r="B70" s="47"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="60"/>
-      <c r="G70" s="60"/>
-      <c r="H70" s="30" t="s">
-        <v>348</v>
-      </c>
-      <c r="I70" s="51"/>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="B71" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="C71" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="D71" s="54">
-        <v>9</v>
-      </c>
-      <c r="E71" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="F71" s="58">
-        <v>43683</v>
-      </c>
-      <c r="G71" s="58">
-        <v>43693</v>
-      </c>
-      <c r="H71" s="28" t="s">
-        <v>357</v>
-      </c>
-      <c r="I71" s="50" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A72" s="52"/>
-      <c r="B72" s="53"/>
-      <c r="C72" s="68"/>
-      <c r="D72" s="55"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="I72" s="65"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="49"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="56"/>
-      <c r="E73" s="41"/>
-      <c r="F73" s="60"/>
-      <c r="G73" s="60"/>
+      <c r="I72" s="72"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="39"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="41"/>
+      <c r="G73" s="41"/>
       <c r="H73" s="30" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I73" s="51"/>
     </row>
-    <row r="74" spans="1:9" ht="18.75">
+    <row r="74" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>155</v>
       </c>
@@ -5199,10 +5188,10 @@
       </c>
       <c r="H74" s="24"/>
       <c r="I74" s="11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="18.75">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>156</v>
       </c>
@@ -5210,7 +5199,7 @@
         <v>47</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D75" s="10">
         <v>2</v>
@@ -5226,10 +5215,10 @@
       </c>
       <c r="H75" s="24"/>
       <c r="I75" s="11" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="18.75">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>187</v>
       </c>
@@ -5248,7 +5237,7 @@
       <c r="H76" s="25"/>
       <c r="I76" s="11"/>
     </row>
-    <row r="77" spans="1:9" ht="18.75">
+    <row r="77" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>188</v>
       </c>
@@ -5267,7 +5256,7 @@
       <c r="H77" s="25"/>
       <c r="I77" s="11"/>
     </row>
-    <row r="78" spans="1:9" ht="18.75">
+    <row r="78" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>189</v>
       </c>
@@ -5286,49 +5275,49 @@
       <c r="H78" s="25"/>
       <c r="I78" s="11"/>
     </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="48" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="B79" s="46" t="s">
+      <c r="B79" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="54" t="s">
+      <c r="C79" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D79" s="54">
+      <c r="D79" s="58">
         <v>3</v>
       </c>
-      <c r="E79" s="40" t="s">
+      <c r="E79" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F79" s="58">
+      <c r="F79" s="40">
         <v>43586</v>
       </c>
-      <c r="G79" s="58">
+      <c r="G79" s="40">
         <v>43588</v>
       </c>
       <c r="H79" s="28" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="I79" s="50" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="49"/>
-      <c r="B80" s="47"/>
-      <c r="C80" s="56"/>
-      <c r="D80" s="56"/>
-      <c r="E80" s="41"/>
-      <c r="F80" s="60"/>
-      <c r="G80" s="60"/>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="39"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="59"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="41"/>
+      <c r="G80" s="41"/>
       <c r="H80" s="30" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I80" s="51"/>
     </row>
-    <row r="81" spans="1:9" ht="18.75">
+    <row r="81" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>117</v>
       </c>
@@ -5351,55 +5340,55 @@
         <v>43579</v>
       </c>
       <c r="H81" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I81" s="11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="48" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="46" t="s">
+      <c r="B82" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="54" t="s">
+      <c r="C82" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D82" s="54">
+      <c r="D82" s="58">
         <v>4</v>
       </c>
-      <c r="E82" s="40" t="s">
+      <c r="E82" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F82" s="58">
+      <c r="F82" s="40">
         <v>43609</v>
       </c>
-      <c r="G82" s="58">
+      <c r="G82" s="40">
         <v>43616</v>
       </c>
       <c r="H82" s="28" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="I82" s="50" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="49"/>
-      <c r="B83" s="47"/>
-      <c r="C83" s="56"/>
-      <c r="D83" s="56"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="60"/>
-      <c r="G83" s="60"/>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="39"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="59"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="43"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="41"/>
       <c r="H83" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I83" s="51"/>
     </row>
-    <row r="84" spans="1:9" ht="18.75">
+    <row r="84" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>119</v>
       </c>
@@ -5422,7 +5411,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="18.75">
+    <row r="85" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>120</v>
       </c>
@@ -5445,13 +5434,13 @@
         <v>43577</v>
       </c>
       <c r="H85" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I85" s="11" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="18.75">
+    <row r="86" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>121</v>
       </c>
@@ -5474,13 +5463,13 @@
         <v>43577</v>
       </c>
       <c r="H86" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I86" s="11" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="18.75">
+    <row r="87" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>122</v>
       </c>
@@ -5503,13 +5492,13 @@
         <v>43578</v>
       </c>
       <c r="H87" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I87" s="11" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="18.75">
+    <row r="88" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>123</v>
       </c>
@@ -5532,95 +5521,95 @@
         <v>43592</v>
       </c>
       <c r="H88" s="30" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I88" s="11" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="48" t="s">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="B89" s="48" t="s">
         <v>305</v>
       </c>
-      <c r="B89" s="46" t="s">
+      <c r="C89" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="D89" s="58">
+        <v>2</v>
+      </c>
+      <c r="E89" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="F89" s="62">
+        <v>43671</v>
+      </c>
+      <c r="G89" s="62">
+        <v>43672</v>
+      </c>
+      <c r="H89" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="I89" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="C89" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="D89" s="54">
-        <v>2</v>
-      </c>
-      <c r="E89" s="40" t="s">
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="39"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="59"/>
+      <c r="E90" s="43"/>
+      <c r="F90" s="63"/>
+      <c r="G90" s="63"/>
+      <c r="H90" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="I90" s="51"/>
+    </row>
+    <row r="91" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="B91" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C91" s="46">
+        <v>43641</v>
+      </c>
+      <c r="D91" s="44">
+        <v>3</v>
+      </c>
+      <c r="E91" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F89" s="38">
-        <v>43671</v>
-      </c>
-      <c r="G89" s="38">
-        <v>43672</v>
-      </c>
-      <c r="H89" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="I89" s="50" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="49"/>
-      <c r="B90" s="47"/>
-      <c r="C90" s="56"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="41"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="30" t="s">
-        <v>349</v>
-      </c>
-      <c r="I90" s="51"/>
-    </row>
-    <row r="91" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A91" s="48" t="s">
-        <v>157</v>
-      </c>
-      <c r="B91" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C91" s="44">
-        <v>43641</v>
-      </c>
-      <c r="D91" s="42">
-        <v>3</v>
-      </c>
-      <c r="E91" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="F91" s="38">
+      <c r="F91" s="62">
         <v>43642</v>
       </c>
-      <c r="G91" s="38">
+      <c r="G91" s="62">
         <v>43644</v>
       </c>
       <c r="H91" s="28" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="I91" s="50"/>
     </row>
-    <row r="92" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A92" s="49"/>
-      <c r="B92" s="47"/>
-      <c r="C92" s="45"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="41"/>
-      <c r="F92" s="39"/>
-      <c r="G92" s="39"/>
+    <row r="92" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="39"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="47"/>
+      <c r="D92" s="45"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="63"/>
+      <c r="G92" s="63"/>
       <c r="H92" s="30" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="I92" s="51"/>
     </row>
-    <row r="93" spans="1:9" ht="18.75">
+    <row r="93" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>158</v>
       </c>
@@ -5643,13 +5632,13 @@
         <v>43683</v>
       </c>
       <c r="H93" s="30" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I93" s="11" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="18.75">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>159</v>
       </c>
@@ -5672,13 +5661,13 @@
         <v>43678</v>
       </c>
       <c r="H94" s="30" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="18.75">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>160</v>
       </c>
@@ -5701,13 +5690,13 @@
         <v>43668</v>
       </c>
       <c r="H95" s="30" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I95" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="18.75">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>161</v>
       </c>
@@ -5730,13 +5719,13 @@
         <v>43669</v>
       </c>
       <c r="H96" s="30" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I96" s="11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="18.75">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>162</v>
       </c>
@@ -5759,13 +5748,13 @@
         <v>43641</v>
       </c>
       <c r="H97" s="30" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I97" s="11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="18.75">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>214</v>
       </c>
@@ -5784,7 +5773,7 @@
       <c r="H98" s="25"/>
       <c r="I98" s="11"/>
     </row>
-    <row r="99" spans="1:9" ht="18.75">
+    <row r="99" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>213</v>
       </c>
@@ -5803,7 +5792,7 @@
       <c r="H99" s="25"/>
       <c r="I99" s="11"/>
     </row>
-    <row r="100" spans="1:9" ht="18.75">
+    <row r="100" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>190</v>
       </c>
@@ -5822,7 +5811,7 @@
       <c r="H100" s="25"/>
       <c r="I100" s="11"/>
     </row>
-    <row r="101" spans="1:9" ht="18.75">
+    <row r="101" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>191</v>
       </c>
@@ -5841,7 +5830,7 @@
       <c r="H101" s="25"/>
       <c r="I101" s="11"/>
     </row>
-    <row r="102" spans="1:9" ht="18.75">
+    <row r="102" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>192</v>
       </c>
@@ -5860,7 +5849,7 @@
       <c r="H102" s="25"/>
       <c r="I102" s="11"/>
     </row>
-    <row r="103" spans="1:9" ht="18.75">
+    <row r="103" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>125</v>
       </c>
@@ -5883,68 +5872,68 @@
         <v>43601</v>
       </c>
       <c r="H103" s="30" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="I103" s="11" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="48" t="s">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B104" s="46" t="s">
+      <c r="B104" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C104" s="54" t="s">
+      <c r="C104" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="D104" s="54">
+      <c r="D104" s="58">
         <v>10</v>
       </c>
-      <c r="E104" s="40" t="s">
+      <c r="E104" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F104" s="58">
+      <c r="F104" s="40">
         <v>43613</v>
       </c>
-      <c r="G104" s="58">
+      <c r="G104" s="40">
         <v>43626</v>
       </c>
       <c r="H104" s="28" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I104" s="50" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A105" s="52"/>
-      <c r="B105" s="53"/>
-      <c r="C105" s="55"/>
-      <c r="D105" s="55"/>
-      <c r="E105" s="61"/>
-      <c r="F105" s="59"/>
-      <c r="G105" s="59"/>
+    <row r="105" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="71"/>
+      <c r="B105" s="70"/>
+      <c r="C105" s="76"/>
+      <c r="D105" s="76"/>
+      <c r="E105" s="67"/>
+      <c r="F105" s="66"/>
+      <c r="G105" s="66"/>
       <c r="H105" s="28" t="s">
-        <v>335</v>
-      </c>
-      <c r="I105" s="65"/>
-    </row>
-    <row r="106" spans="1:9">
-      <c r="A106" s="49"/>
-      <c r="B106" s="47"/>
-      <c r="C106" s="56"/>
-      <c r="D106" s="56"/>
-      <c r="E106" s="41"/>
-      <c r="F106" s="60"/>
-      <c r="G106" s="60"/>
+        <v>332</v>
+      </c>
+      <c r="I105" s="72"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="39"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="59"/>
+      <c r="D106" s="59"/>
+      <c r="E106" s="43"/>
+      <c r="F106" s="41"/>
+      <c r="G106" s="41"/>
       <c r="H106" s="30" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I106" s="51"/>
     </row>
-    <row r="107" spans="1:9" ht="18.75">
+    <row r="107" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>127</v>
       </c>
@@ -5967,13 +5956,13 @@
         <v>43580</v>
       </c>
       <c r="H107" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I107" s="11" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="18.75">
+    <row r="108" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>128</v>
       </c>
@@ -5996,55 +5985,55 @@
         <v>43585</v>
       </c>
       <c r="H108" s="30" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I108" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
-      <c r="A109" s="48" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="B109" s="46" t="s">
+      <c r="B109" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="54" t="s">
+      <c r="C109" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="D109" s="54">
+      <c r="D109" s="58">
         <v>4</v>
       </c>
-      <c r="E109" s="40" t="s">
+      <c r="E109" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F109" s="58">
+      <c r="F109" s="40">
         <v>43627</v>
       </c>
-      <c r="G109" s="58">
+      <c r="G109" s="40">
         <v>43630</v>
       </c>
       <c r="H109" s="28" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="I109" s="50" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
-      <c r="A110" s="49"/>
-      <c r="B110" s="47"/>
-      <c r="C110" s="56"/>
-      <c r="D110" s="56"/>
-      <c r="E110" s="41"/>
-      <c r="F110" s="60"/>
-      <c r="G110" s="60"/>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="39"/>
+      <c r="B110" s="49"/>
+      <c r="C110" s="59"/>
+      <c r="D110" s="59"/>
+      <c r="E110" s="43"/>
+      <c r="F110" s="41"/>
+      <c r="G110" s="41"/>
       <c r="H110" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I110" s="51"/>
     </row>
-    <row r="111" spans="1:9" ht="18.75">
+    <row r="111" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>130</v>
       </c>
@@ -6067,13 +6056,13 @@
         <v>43633</v>
       </c>
       <c r="H111" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I111" s="11" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="18.75">
+    <row r="112" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>215</v>
       </c>
@@ -6096,13 +6085,13 @@
         <v>43683</v>
       </c>
       <c r="H112" s="30" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I112" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="18.75">
+    <row r="113" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>163</v>
       </c>
@@ -6125,13 +6114,13 @@
         <v>43678</v>
       </c>
       <c r="H113" s="30" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I113" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="18.75">
+    <row r="114" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>164</v>
       </c>
@@ -6154,110 +6143,110 @@
         <v>43684</v>
       </c>
       <c r="H114" s="30" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I114" s="11" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
-      <c r="A115" s="48" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="B115" s="46" t="s">
+      <c r="B115" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C115" s="44">
+      <c r="C115" s="46">
         <v>43641</v>
       </c>
-      <c r="D115" s="42">
+      <c r="D115" s="44">
         <v>8</v>
       </c>
-      <c r="E115" s="40" t="s">
+      <c r="E115" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F115" s="69">
+      <c r="F115" s="73">
         <v>43684</v>
       </c>
-      <c r="G115" s="69">
+      <c r="G115" s="73">
         <v>43693</v>
       </c>
       <c r="H115" s="28" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="I115" s="50" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
-      <c r="A116" s="52"/>
-      <c r="B116" s="53"/>
-      <c r="C116" s="68"/>
-      <c r="D116" s="57"/>
-      <c r="E116" s="61"/>
-      <c r="F116" s="71"/>
-      <c r="G116" s="71"/>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="71"/>
+      <c r="B116" s="70"/>
+      <c r="C116" s="69"/>
+      <c r="D116" s="68"/>
+      <c r="E116" s="67"/>
+      <c r="F116" s="74"/>
+      <c r="G116" s="74"/>
       <c r="H116" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="I116" s="65"/>
-    </row>
-    <row r="117" spans="1:9">
-      <c r="A117" s="49"/>
-      <c r="B117" s="47"/>
-      <c r="C117" s="45"/>
-      <c r="D117" s="43"/>
-      <c r="E117" s="41"/>
-      <c r="F117" s="70"/>
-      <c r="G117" s="70"/>
+        <v>352</v>
+      </c>
+      <c r="I116" s="72"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="39"/>
+      <c r="B117" s="49"/>
+      <c r="C117" s="47"/>
+      <c r="D117" s="45"/>
+      <c r="E117" s="43"/>
+      <c r="F117" s="75"/>
+      <c r="G117" s="75"/>
       <c r="H117" s="30" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I117" s="51"/>
     </row>
-    <row r="118" spans="1:9">
-      <c r="A118" s="48" t="s">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B118" s="46" t="s">
+      <c r="B118" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C118" s="44" t="s">
+      <c r="C118" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="D118" s="42">
+      <c r="D118" s="44">
         <v>5</v>
       </c>
-      <c r="E118" s="40" t="s">
+      <c r="E118" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F118" s="69">
+      <c r="F118" s="73">
         <v>43696</v>
       </c>
-      <c r="G118" s="69">
+      <c r="G118" s="73">
         <v>43700</v>
       </c>
       <c r="H118" s="28" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="I118" s="50" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
-      <c r="A119" s="49"/>
-      <c r="B119" s="47"/>
-      <c r="C119" s="45"/>
-      <c r="D119" s="43"/>
-      <c r="E119" s="41"/>
-      <c r="F119" s="70"/>
-      <c r="G119" s="70"/>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="39"/>
+      <c r="B119" s="49"/>
+      <c r="C119" s="47"/>
+      <c r="D119" s="45"/>
+      <c r="E119" s="43"/>
+      <c r="F119" s="75"/>
+      <c r="G119" s="75"/>
       <c r="H119" s="30" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="I119" s="51"/>
     </row>
-    <row r="120" spans="1:9" ht="18.75">
+    <row r="120" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>217</v>
       </c>
@@ -6276,7 +6265,7 @@
       <c r="H120" s="25"/>
       <c r="I120" s="11"/>
     </row>
-    <row r="121" spans="1:9" ht="18.75">
+    <row r="121" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>216</v>
       </c>
@@ -6295,7 +6284,7 @@
       <c r="H121" s="25"/>
       <c r="I121" s="11"/>
     </row>
-    <row r="122" spans="1:9" ht="18.75">
+    <row r="122" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>193</v>
       </c>
@@ -6314,7 +6303,7 @@
       <c r="H122" s="25"/>
       <c r="I122" s="11"/>
     </row>
-    <row r="123" spans="1:9" ht="18.75">
+    <row r="123" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>194</v>
       </c>
@@ -6333,7 +6322,7 @@
       <c r="H123" s="25"/>
       <c r="I123" s="11"/>
     </row>
-    <row r="124" spans="1:9" ht="18.75">
+    <row r="124" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>195</v>
       </c>
@@ -6352,7 +6341,7 @@
       <c r="H124" s="25"/>
       <c r="I124" s="11"/>
     </row>
-    <row r="125" spans="1:9" ht="18.75">
+    <row r="125" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>131</v>
       </c>
@@ -6375,307 +6364,307 @@
         <v>43642</v>
       </c>
       <c r="H125" s="30" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I125" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
-      <c r="A126" s="48" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="B126" s="46" t="s">
+      <c r="B126" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C126" s="54" t="s">
+      <c r="C126" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D126" s="42">
+      <c r="D126" s="44">
         <v>5</v>
       </c>
-      <c r="E126" s="40" t="s">
+      <c r="E126" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F126" s="38">
+      <c r="F126" s="62">
         <v>43643</v>
       </c>
-      <c r="G126" s="38">
+      <c r="G126" s="62">
         <v>43649</v>
       </c>
       <c r="H126" s="28" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="I126" s="50" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
-      <c r="A127" s="49"/>
-      <c r="B127" s="47"/>
-      <c r="C127" s="56"/>
-      <c r="D127" s="43"/>
-      <c r="E127" s="41"/>
-      <c r="F127" s="39"/>
-      <c r="G127" s="39"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="39"/>
+      <c r="B127" s="49"/>
+      <c r="C127" s="59"/>
+      <c r="D127" s="45"/>
+      <c r="E127" s="43"/>
+      <c r="F127" s="63"/>
+      <c r="G127" s="63"/>
       <c r="H127" s="30" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="I127" s="51"/>
     </row>
-    <row r="128" spans="1:9">
-      <c r="A128" s="48" t="s">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="B128" s="46" t="s">
+      <c r="B128" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C128" s="54" t="s">
+      <c r="C128" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D128" s="42">
+      <c r="D128" s="44">
         <v>2</v>
       </c>
-      <c r="E128" s="40" t="s">
+      <c r="E128" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F128" s="38">
+      <c r="F128" s="62">
         <v>43650</v>
       </c>
-      <c r="G128" s="38">
+      <c r="G128" s="62">
         <v>43651</v>
       </c>
       <c r="H128" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="I128" s="50" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="39"/>
+      <c r="B129" s="49"/>
+      <c r="C129" s="59"/>
+      <c r="D129" s="45"/>
+      <c r="E129" s="43"/>
+      <c r="F129" s="63"/>
+      <c r="G129" s="63"/>
+      <c r="H129" s="30" t="s">
+        <v>366</v>
+      </c>
+      <c r="I129" s="51"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B130" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C130" s="58" t="s">
+        <v>209</v>
+      </c>
+      <c r="D130" s="44">
+        <v>3</v>
+      </c>
+      <c r="E130" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="F130" s="62">
+        <v>43685</v>
+      </c>
+      <c r="G130" s="62">
+        <v>43689</v>
+      </c>
+      <c r="H130" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="I130" s="50" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="39"/>
+      <c r="B131" s="49"/>
+      <c r="C131" s="59"/>
+      <c r="D131" s="45"/>
+      <c r="E131" s="43"/>
+      <c r="F131" s="63"/>
+      <c r="G131" s="63"/>
+      <c r="H131" s="30" t="s">
+        <v>350</v>
+      </c>
+      <c r="I131" s="51"/>
+    </row>
+    <row r="132" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B132" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C132" s="46">
+        <v>43641</v>
+      </c>
+      <c r="D132" s="44">
+        <v>2</v>
+      </c>
+      <c r="E132" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="F132" s="62">
+        <v>43654</v>
+      </c>
+      <c r="G132" s="62">
+        <v>43658</v>
+      </c>
+      <c r="H132" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="I132" s="50" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="39"/>
+      <c r="B133" s="49"/>
+      <c r="C133" s="47"/>
+      <c r="D133" s="45"/>
+      <c r="E133" s="43"/>
+      <c r="F133" s="63"/>
+      <c r="G133" s="63"/>
+      <c r="H133" s="30" t="s">
+        <v>350</v>
+      </c>
+      <c r="I133" s="51"/>
+    </row>
+    <row r="134" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B134" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C134" s="46">
+        <v>43641</v>
+      </c>
+      <c r="D134" s="44">
+        <v>4</v>
+      </c>
+      <c r="E134" s="64" t="s">
+        <v>284</v>
+      </c>
+      <c r="F134" s="62">
+        <v>43690</v>
+      </c>
+      <c r="G134" s="62">
+        <v>43693</v>
+      </c>
+      <c r="H134" s="28" t="s">
+        <v>352</v>
+      </c>
+      <c r="I134" s="50" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="39"/>
+      <c r="B135" s="49"/>
+      <c r="C135" s="47"/>
+      <c r="D135" s="45"/>
+      <c r="E135" s="65"/>
+      <c r="F135" s="63"/>
+      <c r="G135" s="63"/>
+      <c r="H135" s="30" t="s">
+        <v>353</v>
+      </c>
+      <c r="I135" s="51"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="B136" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="C136" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D136" s="44">
+        <v>5</v>
+      </c>
+      <c r="E136" s="64" t="s">
+        <v>284</v>
+      </c>
+      <c r="F136" s="62">
+        <v>43698</v>
+      </c>
+      <c r="G136" s="60">
+        <v>43704</v>
+      </c>
+      <c r="H136" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="I136" s="50" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="39"/>
+      <c r="B137" s="49"/>
+      <c r="C137" s="59"/>
+      <c r="D137" s="45"/>
+      <c r="E137" s="65"/>
+      <c r="F137" s="63"/>
+      <c r="G137" s="61"/>
+      <c r="H137" s="30" t="s">
+        <v>364</v>
+      </c>
+      <c r="I137" s="51"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="B138" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="C138" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D138" s="58">
+        <v>3</v>
+      </c>
+      <c r="E138" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="F138" s="62">
+        <v>43705</v>
+      </c>
+      <c r="G138" s="62">
+        <v>43707</v>
+      </c>
+      <c r="H138" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="I138" s="50" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="39"/>
+      <c r="B139" s="49"/>
+      <c r="C139" s="59"/>
+      <c r="D139" s="59"/>
+      <c r="E139" s="43"/>
+      <c r="F139" s="63"/>
+      <c r="G139" s="63"/>
+      <c r="H139" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="I128" s="50" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9">
-      <c r="A129" s="49"/>
-      <c r="B129" s="47"/>
-      <c r="C129" s="56"/>
-      <c r="D129" s="43"/>
-      <c r="E129" s="41"/>
-      <c r="F129" s="39"/>
-      <c r="G129" s="39"/>
-      <c r="H129" s="30" t="s">
-        <v>369</v>
-      </c>
-      <c r="I129" s="51"/>
-    </row>
-    <row r="130" spans="1:9">
-      <c r="A130" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="B130" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="C130" s="54" t="s">
-        <v>209</v>
-      </c>
-      <c r="D130" s="42">
-        <v>3</v>
-      </c>
-      <c r="E130" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="F130" s="38">
-        <v>43685</v>
-      </c>
-      <c r="G130" s="38">
-        <v>43689</v>
-      </c>
-      <c r="H130" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="I130" s="50" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
-      <c r="A131" s="49"/>
-      <c r="B131" s="47"/>
-      <c r="C131" s="56"/>
-      <c r="D131" s="43"/>
-      <c r="E131" s="41"/>
-      <c r="F131" s="39"/>
-      <c r="G131" s="39"/>
-      <c r="H131" s="30" t="s">
-        <v>353</v>
-      </c>
-      <c r="I131" s="51"/>
-    </row>
-    <row r="132" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A132" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="B132" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="C132" s="44">
-        <v>43641</v>
-      </c>
-      <c r="D132" s="42">
-        <v>2</v>
-      </c>
-      <c r="E132" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="F132" s="38">
-        <v>43654</v>
-      </c>
-      <c r="G132" s="38">
-        <v>43658</v>
-      </c>
-      <c r="H132" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="I132" s="50" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A133" s="49"/>
-      <c r="B133" s="47"/>
-      <c r="C133" s="45"/>
-      <c r="D133" s="43"/>
-      <c r="E133" s="41"/>
-      <c r="F133" s="39"/>
-      <c r="G133" s="39"/>
-      <c r="H133" s="30" t="s">
-        <v>353</v>
-      </c>
-      <c r="I133" s="51"/>
-    </row>
-    <row r="134" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A134" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B134" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C134" s="44">
-        <v>43641</v>
-      </c>
-      <c r="D134" s="42">
-        <v>4</v>
-      </c>
-      <c r="E134" s="72" t="s">
-        <v>284</v>
-      </c>
-      <c r="F134" s="38">
-        <v>43690</v>
-      </c>
-      <c r="G134" s="38">
-        <v>43693</v>
-      </c>
-      <c r="H134" s="28" t="s">
-        <v>355</v>
-      </c>
-      <c r="I134" s="50" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9">
-      <c r="A135" s="49"/>
-      <c r="B135" s="47"/>
-      <c r="C135" s="45"/>
-      <c r="D135" s="43"/>
-      <c r="E135" s="73"/>
-      <c r="F135" s="39"/>
-      <c r="G135" s="39"/>
-      <c r="H135" s="30" t="s">
-        <v>356</v>
-      </c>
-      <c r="I135" s="51"/>
-    </row>
-    <row r="136" spans="1:9">
-      <c r="A136" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="B136" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="C136" s="54" t="s">
-        <v>168</v>
-      </c>
-      <c r="D136" s="42">
-        <v>5</v>
-      </c>
-      <c r="E136" s="72" t="s">
-        <v>284</v>
-      </c>
-      <c r="F136" s="38">
-        <v>43698</v>
-      </c>
-      <c r="G136" s="74">
-        <v>43704</v>
-      </c>
-      <c r="H136" s="28" t="s">
-        <v>371</v>
-      </c>
-      <c r="I136" s="50" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9">
-      <c r="A137" s="49"/>
-      <c r="B137" s="47"/>
-      <c r="C137" s="56"/>
-      <c r="D137" s="43"/>
-      <c r="E137" s="73"/>
-      <c r="F137" s="39"/>
-      <c r="G137" s="75"/>
-      <c r="H137" s="30" t="s">
-        <v>367</v>
-      </c>
-      <c r="I137" s="51"/>
-    </row>
-    <row r="138" spans="1:9">
-      <c r="A138" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="B138" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C138" s="54" t="s">
-        <v>168</v>
-      </c>
-      <c r="D138" s="54">
-        <v>3</v>
-      </c>
-      <c r="E138" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="F138" s="38">
-        <v>43705</v>
-      </c>
-      <c r="G138" s="38">
-        <v>43707</v>
-      </c>
-      <c r="H138" s="28" t="s">
-        <v>372</v>
-      </c>
-      <c r="I138" s="50" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9">
-      <c r="A139" s="49"/>
-      <c r="B139" s="47"/>
-      <c r="C139" s="56"/>
-      <c r="D139" s="56"/>
-      <c r="E139" s="41"/>
-      <c r="F139" s="39"/>
-      <c r="G139" s="39"/>
-      <c r="H139" s="30" t="s">
-        <v>373</v>
-      </c>
       <c r="I139" s="51"/>
     </row>
-    <row r="140" spans="1:9" ht="18.75">
+    <row r="140" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>196</v>
       </c>
@@ -6694,7 +6683,7 @@
       <c r="H140" s="25"/>
       <c r="I140" s="11"/>
     </row>
-    <row r="141" spans="1:9" ht="18.75">
+    <row r="141" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>197</v>
       </c>
@@ -6713,7 +6702,7 @@
       <c r="H141" s="25"/>
       <c r="I141" s="11"/>
     </row>
-    <row r="142" spans="1:9" ht="18.75">
+    <row r="142" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>198</v>
       </c>
@@ -6732,175 +6721,175 @@
       <c r="H142" s="25"/>
       <c r="I142" s="11"/>
     </row>
-    <row r="143" spans="1:9">
-      <c r="A143" s="48" t="s">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B143" s="46" t="s">
+      <c r="B143" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C143" s="54" t="s">
+      <c r="C143" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D143" s="54">
+      <c r="D143" s="58">
         <v>5</v>
       </c>
-      <c r="E143" s="40" t="s">
+      <c r="E143" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F143" s="58">
+      <c r="F143" s="40">
         <v>43579</v>
       </c>
-      <c r="G143" s="58">
+      <c r="G143" s="40">
         <v>43585</v>
       </c>
       <c r="H143" s="28" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I143" s="50" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
-      <c r="A144" s="49"/>
-      <c r="B144" s="47"/>
-      <c r="C144" s="56"/>
-      <c r="D144" s="56"/>
-      <c r="E144" s="41"/>
-      <c r="F144" s="60"/>
-      <c r="G144" s="60"/>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="39"/>
+      <c r="B144" s="49"/>
+      <c r="C144" s="59"/>
+      <c r="D144" s="59"/>
+      <c r="E144" s="43"/>
+      <c r="F144" s="41"/>
+      <c r="G144" s="41"/>
       <c r="H144" s="30" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I144" s="51"/>
     </row>
-    <row r="145" spans="1:9">
-      <c r="A145" s="48" t="s">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="B145" s="46" t="s">
+      <c r="B145" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C145" s="54" t="s">
+      <c r="C145" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D145" s="54">
+      <c r="D145" s="58">
         <v>5</v>
       </c>
-      <c r="E145" s="40" t="s">
+      <c r="E145" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F145" s="58">
+      <c r="F145" s="40">
         <v>43586</v>
       </c>
-      <c r="G145" s="58">
+      <c r="G145" s="40">
         <v>43592</v>
       </c>
       <c r="H145" s="28" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I145" s="50" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
-      <c r="A146" s="49"/>
-      <c r="B146" s="47"/>
-      <c r="C146" s="56"/>
-      <c r="D146" s="56"/>
-      <c r="E146" s="41"/>
-      <c r="F146" s="60"/>
-      <c r="G146" s="60"/>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="39"/>
+      <c r="B146" s="49"/>
+      <c r="C146" s="59"/>
+      <c r="D146" s="59"/>
+      <c r="E146" s="43"/>
+      <c r="F146" s="41"/>
+      <c r="G146" s="41"/>
       <c r="H146" s="30" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I146" s="51"/>
     </row>
-    <row r="147" spans="1:9">
-      <c r="A147" s="48" t="s">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="B147" s="46" t="s">
+      <c r="B147" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C147" s="54" t="s">
+      <c r="C147" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="D147" s="54">
+      <c r="D147" s="58">
         <v>5</v>
       </c>
-      <c r="E147" s="40" t="s">
+      <c r="E147" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F147" s="58">
+      <c r="F147" s="40">
         <v>43593</v>
       </c>
-      <c r="G147" s="58">
+      <c r="G147" s="40">
         <v>43599</v>
       </c>
       <c r="H147" s="28" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="I147" s="50" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
-      <c r="A148" s="49"/>
-      <c r="B148" s="47"/>
-      <c r="C148" s="56"/>
-      <c r="D148" s="56"/>
-      <c r="E148" s="41"/>
-      <c r="F148" s="60"/>
-      <c r="G148" s="60"/>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="39"/>
+      <c r="B148" s="49"/>
+      <c r="C148" s="59"/>
+      <c r="D148" s="59"/>
+      <c r="E148" s="43"/>
+      <c r="F148" s="41"/>
+      <c r="G148" s="41"/>
       <c r="H148" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="I148" s="51"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="B149" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C149" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="D149" s="58">
+        <v>5</v>
+      </c>
+      <c r="E149" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="F149" s="40">
+        <v>43626</v>
+      </c>
+      <c r="G149" s="40">
+        <v>43630</v>
+      </c>
+      <c r="H149" s="28" t="s">
         <v>333</v>
-      </c>
-      <c r="I148" s="51"/>
-    </row>
-    <row r="149" spans="1:9">
-      <c r="A149" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="B149" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C149" s="54" t="s">
-        <v>138</v>
-      </c>
-      <c r="D149" s="54">
-        <v>5</v>
-      </c>
-      <c r="E149" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="F149" s="58">
-        <v>43626</v>
-      </c>
-      <c r="G149" s="58">
-        <v>43630</v>
-      </c>
-      <c r="H149" s="28" t="s">
-        <v>336</v>
       </c>
       <c r="I149" s="50" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
-      <c r="A150" s="49"/>
-      <c r="B150" s="47"/>
-      <c r="C150" s="56"/>
-      <c r="D150" s="56"/>
-      <c r="E150" s="41"/>
-      <c r="F150" s="60"/>
-      <c r="G150" s="60"/>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="39"/>
+      <c r="B150" s="49"/>
+      <c r="C150" s="59"/>
+      <c r="D150" s="59"/>
+      <c r="E150" s="43"/>
+      <c r="F150" s="41"/>
+      <c r="G150" s="41"/>
       <c r="H150" s="30" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I150" s="51"/>
     </row>
-    <row r="151" spans="1:9" ht="18.75">
+    <row r="151" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>140</v>
       </c>
@@ -6923,13 +6912,13 @@
         <v>43633</v>
       </c>
       <c r="H151" s="30" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I151" s="11" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="18.75">
+    <row r="152" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>141</v>
       </c>
@@ -6937,7 +6926,7 @@
         <v>32</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D152" s="5">
         <v>2</v>
@@ -6952,55 +6941,55 @@
         <v>43635</v>
       </c>
       <c r="H152" s="30" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I152" s="11" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
-      <c r="A153" s="48" t="s">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="B153" s="46" t="s">
+      <c r="B153" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C153" s="44">
+      <c r="C153" s="46">
         <v>43641</v>
       </c>
-      <c r="D153" s="54">
+      <c r="D153" s="58">
         <v>7</v>
       </c>
-      <c r="E153" s="40" t="s">
+      <c r="E153" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F153" s="58">
+      <c r="F153" s="40">
         <v>43647</v>
       </c>
-      <c r="G153" s="58">
+      <c r="G153" s="40">
         <v>43655</v>
       </c>
       <c r="H153" s="28" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="I153" s="50" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9">
-      <c r="A154" s="49"/>
-      <c r="B154" s="47"/>
-      <c r="C154" s="45"/>
-      <c r="D154" s="56"/>
-      <c r="E154" s="41"/>
-      <c r="F154" s="60"/>
-      <c r="G154" s="60"/>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="39"/>
+      <c r="B154" s="49"/>
+      <c r="C154" s="47"/>
+      <c r="D154" s="59"/>
+      <c r="E154" s="43"/>
+      <c r="F154" s="41"/>
+      <c r="G154" s="41"/>
       <c r="H154" s="30" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I154" s="51"/>
     </row>
-    <row r="155" spans="1:9" ht="18.75">
+    <row r="155" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>238</v>
       </c>
@@ -7023,13 +7012,13 @@
         <v>43663</v>
       </c>
       <c r="H155" s="30" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="I155" s="11" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" ht="18.75">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>171</v>
       </c>
@@ -7052,55 +7041,55 @@
         <v>43670</v>
       </c>
       <c r="H156" s="30" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="I156" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="15.75">
-      <c r="A157" s="48" t="s">
+    <row r="157" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A157" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B157" s="46" t="s">
+      <c r="B157" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C157" s="44" t="s">
+      <c r="C157" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="D157" s="42">
+      <c r="D157" s="44">
         <v>2</v>
       </c>
-      <c r="E157" s="40" t="s">
+      <c r="E157" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F157" s="58">
+      <c r="F157" s="40">
         <v>43664</v>
       </c>
-      <c r="G157" s="58">
+      <c r="G157" s="40">
         <v>43665</v>
       </c>
       <c r="H157" s="28" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="I157" s="36"/>
     </row>
-    <row r="158" spans="1:9" ht="15.75">
-      <c r="A158" s="49"/>
-      <c r="B158" s="47"/>
-      <c r="C158" s="45"/>
-      <c r="D158" s="43"/>
-      <c r="E158" s="41"/>
-      <c r="F158" s="60"/>
-      <c r="G158" s="60"/>
+    <row r="158" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A158" s="39"/>
+      <c r="B158" s="49"/>
+      <c r="C158" s="47"/>
+      <c r="D158" s="45"/>
+      <c r="E158" s="43"/>
+      <c r="F158" s="41"/>
+      <c r="G158" s="41"/>
       <c r="H158" s="30" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="I158" s="36" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" ht="18.75">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>173</v>
       </c>
@@ -7123,13 +7112,13 @@
         <v>43685</v>
       </c>
       <c r="H159" s="30" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="I159" s="11" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" ht="18.75">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>174</v>
       </c>
@@ -7152,13 +7141,13 @@
         <v>43693</v>
       </c>
       <c r="H160" s="30" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="I160" s="11" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" ht="18.75">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>175</v>
       </c>
@@ -7181,13 +7170,13 @@
         <v>43692</v>
       </c>
       <c r="H161" s="30" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="I161" s="11" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" ht="18.75">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>176</v>
       </c>
@@ -7210,55 +7199,55 @@
         <v>43689</v>
       </c>
       <c r="H162" s="30" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="I162" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
-      <c r="A163" s="48" t="s">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="B163" s="46" t="s">
+      <c r="B163" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C163" s="44" t="s">
+      <c r="C163" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="D163" s="42">
+      <c r="D163" s="44">
         <v>4</v>
       </c>
-      <c r="E163" s="40" t="s">
+      <c r="E163" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F163" s="58">
+      <c r="F163" s="40">
         <v>43698</v>
       </c>
-      <c r="G163" s="58">
+      <c r="G163" s="40">
         <v>43703</v>
       </c>
       <c r="H163" s="28" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I163" s="50" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9">
-      <c r="A164" s="49"/>
-      <c r="B164" s="47"/>
-      <c r="C164" s="45"/>
-      <c r="D164" s="43"/>
-      <c r="E164" s="41"/>
-      <c r="F164" s="60"/>
-      <c r="G164" s="60"/>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" s="39"/>
+      <c r="B164" s="49"/>
+      <c r="C164" s="47"/>
+      <c r="D164" s="45"/>
+      <c r="E164" s="43"/>
+      <c r="F164" s="41"/>
+      <c r="G164" s="41"/>
       <c r="H164" s="30" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="I164" s="51"/>
     </row>
-    <row r="165" spans="1:9" ht="18.75">
+    <row r="165" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>239</v>
       </c>
@@ -7277,7 +7266,7 @@
       <c r="H165" s="24"/>
       <c r="I165" s="11"/>
     </row>
-    <row r="166" spans="1:9" ht="18.75">
+    <row r="166" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>240</v>
       </c>
@@ -7296,7 +7285,7 @@
       <c r="H166" s="25"/>
       <c r="I166" s="11"/>
     </row>
-    <row r="167" spans="1:9" ht="18.75">
+    <row r="167" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>199</v>
       </c>
@@ -7315,7 +7304,7 @@
       <c r="H167" s="25"/>
       <c r="I167" s="11"/>
     </row>
-    <row r="168" spans="1:9" ht="18.75">
+    <row r="168" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>200</v>
       </c>
@@ -7334,7 +7323,7 @@
       <c r="H168" s="25"/>
       <c r="I168" s="11"/>
     </row>
-    <row r="169" spans="1:9" ht="18.75">
+    <row r="169" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>201</v>
       </c>
@@ -7353,7 +7342,7 @@
       <c r="H169" s="25"/>
       <c r="I169" s="11"/>
     </row>
-    <row r="170" spans="1:9" ht="18.75">
+    <row r="170" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>202</v>
       </c>
@@ -7372,7 +7361,7 @@
       <c r="H170" s="25"/>
       <c r="I170" s="11"/>
     </row>
-    <row r="171" spans="1:9" ht="18.75">
+    <row r="171" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>203</v>
       </c>
@@ -7391,7 +7380,7 @@
       <c r="H171" s="25"/>
       <c r="I171" s="11"/>
     </row>
-    <row r="172" spans="1:9" ht="18.75">
+    <row r="172" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>204</v>
       </c>
@@ -7410,7 +7399,7 @@
       <c r="H172" s="25"/>
       <c r="I172" s="11"/>
     </row>
-    <row r="173" spans="1:9" ht="19.5" thickBot="1">
+    <row r="173" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="19" t="s">
         <v>205</v>
       </c>
@@ -7429,52 +7418,52 @@
       <c r="H173" s="27"/>
       <c r="I173" s="12"/>
     </row>
-    <row r="174" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A174" s="48" t="s">
-        <v>389</v>
-      </c>
-      <c r="B174" s="81" t="s">
-        <v>381</v>
-      </c>
-      <c r="C174" s="80" t="s">
+    <row r="174" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="B174" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="C174" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="D174" s="78">
+      <c r="D174" s="54">
         <v>3</v>
       </c>
-      <c r="E174" s="77" t="s">
+      <c r="E174" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="F174" s="76">
+      <c r="F174" s="52">
         <v>43636</v>
       </c>
-      <c r="G174" s="76">
+      <c r="G174" s="52">
         <v>43640</v>
       </c>
       <c r="H174" s="28" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="I174" s="11"/>
     </row>
-    <row r="175" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A175" s="49"/>
-      <c r="B175" s="47"/>
-      <c r="C175" s="45"/>
-      <c r="D175" s="79"/>
-      <c r="E175" s="41"/>
-      <c r="F175" s="60"/>
-      <c r="G175" s="60"/>
+    <row r="175" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="39"/>
+      <c r="B175" s="49"/>
+      <c r="C175" s="47"/>
+      <c r="D175" s="55"/>
+      <c r="E175" s="43"/>
+      <c r="F175" s="41"/>
+      <c r="G175" s="41"/>
       <c r="H175" s="30" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I175" s="11"/>
     </row>
-    <row r="176" spans="1:9" ht="16.5" customHeight="1">
+    <row r="176" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C176" s="35" t="s">
         <v>155</v>
@@ -7492,16 +7481,16 @@
         <v>43711</v>
       </c>
       <c r="H176" s="30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I176" s="11"/>
     </row>
-    <row r="177" spans="1:9" ht="17.25" customHeight="1" thickBot="1">
+    <row r="177" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="19" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C177" s="8">
         <v>43712</v>
@@ -7515,117 +7504,191 @@
       <c r="H177" s="27"/>
       <c r="I177" s="12"/>
     </row>
-    <row r="178" spans="1:9" ht="15.75" customHeight="1">
+    <row r="178" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="310">
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="G163:G164"/>
-    <mergeCell ref="F163:F164"/>
-    <mergeCell ref="E163:E164"/>
-    <mergeCell ref="D163:D164"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="B163:B164"/>
-    <mergeCell ref="A163:A164"/>
-    <mergeCell ref="I163:I164"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="G157:G158"/>
-    <mergeCell ref="F157:F158"/>
-    <mergeCell ref="E157:E158"/>
-    <mergeCell ref="D157:D158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="G153:G154"/>
-    <mergeCell ref="F153:F154"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="I153:I154"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="I149:I150"/>
-    <mergeCell ref="G149:G150"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="I136:I137"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="I138:I139"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="I132:I133"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="I134:I135"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="I130:I131"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="G46:G50"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="I46:I50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="G71:G73"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="I89:I90"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="G143:G144"/>
+    <mergeCell ref="E143:E144"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="I143:I144"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I126:I127"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="G145:G146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="I58:I59"/>
     <mergeCell ref="C71:C73"/>
     <mergeCell ref="B71:B73"/>
     <mergeCell ref="A71:A73"/>
@@ -7650,186 +7713,112 @@
     <mergeCell ref="D104:D106"/>
     <mergeCell ref="C104:C106"/>
     <mergeCell ref="B104:B106"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="G145:G146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="G143:G144"/>
-    <mergeCell ref="E143:E144"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="I143:I144"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="C143:C144"/>
-    <mergeCell ref="D143:D144"/>
-    <mergeCell ref="G109:G110"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I126:I127"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="G71:G73"/>
-    <mergeCell ref="F71:F73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="E46:E50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="I46:I50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="I130:I131"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="I132:I133"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="I134:I135"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="I136:I137"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="I138:I139"/>
+    <mergeCell ref="G153:G154"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="I153:I154"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="I149:I150"/>
+    <mergeCell ref="G149:G150"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="G157:G158"/>
+    <mergeCell ref="F157:F158"/>
+    <mergeCell ref="E157:E158"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="C157:C158"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="G163:G164"/>
+    <mergeCell ref="F163:F164"/>
+    <mergeCell ref="E163:E164"/>
+    <mergeCell ref="D163:D164"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="B163:B164"/>
+    <mergeCell ref="A163:A164"/>
+    <mergeCell ref="I163:I164"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrador listo sin anexos cargados
</commit_message>
<xml_diff>
--- a/Actividades/Proy01005/Tabla de actividades.xlsx
+++ b/Actividades/Proy01005/Tabla de actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Proy01005\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFDD8D2-07C3-4E84-975D-9F5BE307C551}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42771FE-C0EC-403C-83FE-CCEF35AF9364}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3117,10 +3117,16 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
@@ -3147,89 +3153,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3247,6 +3175,78 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3630,8 +3630,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3647,17 +3647,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="192.75" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="79" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="64"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="81"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1">
       <c r="A2" s="14" t="s">
@@ -3747,25 +3747,25 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" customHeight="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="58">
         <v>8</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="40">
         <v>43577</v>
       </c>
-      <c r="G5" s="58">
+      <c r="G5" s="40">
         <v>43586</v>
       </c>
       <c r="H5" s="28" t="s">
@@ -3776,38 +3776,38 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="49"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="30" t="s">
         <v>326</v>
       </c>
       <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:9" ht="21.75" customHeight="1">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="58">
         <v>20</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="F7" s="58">
+      <c r="F7" s="40">
         <v>43577</v>
       </c>
-      <c r="G7" s="58">
+      <c r="G7" s="40">
         <v>43602</v>
       </c>
       <c r="H7" s="29" t="s">
@@ -3818,52 +3818,52 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
       <c r="H8" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="I8" s="65"/>
+      <c r="I8" s="72"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A9" s="52"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
       <c r="H9" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="I9" s="65"/>
+      <c r="I9" s="72"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
       <c r="H10" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="I10" s="65"/>
+      <c r="I10" s="72"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="49"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="30" t="s">
         <v>321</v>
       </c>
@@ -3899,25 +3899,25 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="58">
         <v>6</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="40">
         <v>43627</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="40">
         <v>43634</v>
       </c>
       <c r="H13" s="28" t="s">
@@ -3928,13 +3928,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="49"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="30" t="s">
         <v>324</v>
       </c>
@@ -3970,25 +3970,25 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="46">
         <v>43641</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="44">
         <v>4</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F16" s="58">
+      <c r="F16" s="40">
         <v>43664</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="40">
         <v>43665</v>
       </c>
       <c r="H16" s="28" t="s">
@@ -3999,38 +3999,38 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="30" t="s">
         <v>345</v>
       </c>
       <c r="I17" s="51"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="46">
         <v>43641</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="44">
         <v>4</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="E18" s="77" t="s">
         <v>283</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="40">
         <v>43704</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="40">
         <v>43707</v>
       </c>
       <c r="H18" s="28" t="s">
@@ -4041,13 +4041,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
       <c r="H19" s="30" t="s">
         <v>373</v>
       </c>
@@ -4083,25 +4083,25 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="44">
+      <c r="C21" s="46">
         <v>43641</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="44">
         <v>5</v>
       </c>
-      <c r="E21" s="67" t="s">
+      <c r="E21" s="78" t="s">
         <v>226</v>
       </c>
-      <c r="F21" s="58">
+      <c r="F21" s="40">
         <v>43703</v>
       </c>
-      <c r="G21" s="58">
+      <c r="G21" s="40">
         <v>43707</v>
       </c>
       <c r="H21" s="28" t="s">
@@ -4112,13 +4112,13 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A22" s="49"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="30" t="s">
         <v>373</v>
       </c>
@@ -4154,25 +4154,25 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="38" t="s">
         <v>275</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="48" t="s">
         <v>280</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="46">
         <v>43641</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="44">
         <v>6</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F24" s="58">
+      <c r="F24" s="40">
         <v>43647</v>
       </c>
-      <c r="G24" s="58">
+      <c r="G24" s="40">
         <v>43654</v>
       </c>
       <c r="H24" s="28" t="s">
@@ -4183,38 +4183,38 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="49"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
       <c r="H25" s="30" t="s">
         <v>369</v>
       </c>
       <c r="I25" s="51"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="38" t="s">
         <v>276</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="48" t="s">
         <v>281</v>
       </c>
-      <c r="C26" s="44">
+      <c r="C26" s="46">
         <v>43641</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="44">
         <v>4</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F26" s="38">
+      <c r="F26" s="62">
         <v>43656</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="62">
         <v>43661</v>
       </c>
       <c r="H26" s="28" t="s">
@@ -4225,13 +4225,13 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="49"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
       <c r="H27" s="30" t="s">
         <v>387</v>
       </c>
@@ -4428,25 +4428,25 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="48" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="54" t="s">
+      <c r="C38" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="42">
+      <c r="D38" s="44">
         <v>10</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="58">
+      <c r="F38" s="40">
         <v>43605</v>
       </c>
-      <c r="G38" s="58">
+      <c r="G38" s="40">
         <v>43616</v>
       </c>
       <c r="H38" s="28" t="s">
@@ -4457,26 +4457,26 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A39" s="52"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
+      <c r="A39" s="71"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
       <c r="H39" s="28" t="s">
         <v>322</v>
       </c>
-      <c r="I39" s="65"/>
+      <c r="I39" s="72"/>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1">
-      <c r="A40" s="49"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
       <c r="H40" s="30" t="s">
         <v>327</v>
       </c>
@@ -4628,25 +4628,25 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="48" t="s">
+      <c r="A46" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="44">
+      <c r="C46" s="46">
         <v>43641</v>
       </c>
-      <c r="D46" s="42">
+      <c r="D46" s="44">
         <v>20</v>
       </c>
-      <c r="E46" s="40" t="s">
+      <c r="E46" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F46" s="58">
+      <c r="F46" s="40">
         <v>43641</v>
       </c>
-      <c r="G46" s="58">
+      <c r="G46" s="40">
         <v>43668</v>
       </c>
       <c r="H46" s="28" t="s">
@@ -4657,52 +4657,52 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="52"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="68"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
+      <c r="A47" s="71"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="66"/>
       <c r="H47" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="I47" s="65"/>
+      <c r="I47" s="72"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="52"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
+      <c r="A48" s="71"/>
+      <c r="B48" s="70"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
       <c r="H48" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="I48" s="65"/>
+      <c r="I48" s="72"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="52"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="70"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
       <c r="H49" s="28" t="s">
         <v>364</v>
       </c>
-      <c r="I49" s="65"/>
+      <c r="I49" s="72"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="49"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="60"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="30" t="s">
         <v>345</v>
       </c>
@@ -4730,25 +4730,25 @@
       <c r="I51" s="11"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="48" t="s">
+      <c r="A52" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B52" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="42">
+      <c r="D52" s="44">
         <v>2</v>
       </c>
-      <c r="E52" s="40" t="s">
+      <c r="E52" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F52" s="58">
+      <c r="F52" s="40">
         <v>43671</v>
       </c>
-      <c r="G52" s="58">
+      <c r="G52" s="40">
         <v>43672</v>
       </c>
       <c r="H52" s="28" t="s">
@@ -4759,13 +4759,13 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="49"/>
-      <c r="B53" s="47"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="30" t="s">
         <v>349</v>
       </c>
@@ -4801,25 +4801,25 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="48" t="s">
+      <c r="A55" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="44" t="s">
+      <c r="C55" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D55" s="42">
+      <c r="D55" s="44">
         <v>5</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="E55" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F55" s="58">
+      <c r="F55" s="40">
         <v>43677</v>
       </c>
-      <c r="G55" s="58">
+      <c r="G55" s="40">
         <v>43683</v>
       </c>
       <c r="H55" s="28" t="s">
@@ -4830,13 +4830,13 @@
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="49"/>
-      <c r="B56" s="47"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="60"/>
-      <c r="G56" s="60"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="30" t="s">
         <v>348</v>
       </c>
@@ -4864,25 +4864,25 @@
       <c r="I57" s="11"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="48" t="s">
+      <c r="A58" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="C58" s="44" t="s">
+      <c r="C58" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="42">
+      <c r="D58" s="44">
         <v>5</v>
       </c>
-      <c r="E58" s="40" t="s">
+      <c r="E58" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F58" s="58">
+      <c r="F58" s="40">
         <v>43669</v>
       </c>
-      <c r="G58" s="58">
+      <c r="G58" s="40">
         <v>43675</v>
       </c>
       <c r="H58" s="28" t="s">
@@ -4893,13 +4893,13 @@
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="49"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
+      <c r="A59" s="39"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="30" t="s">
         <v>349</v>
       </c>
@@ -5011,25 +5011,25 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" customHeight="1">
-      <c r="A65" s="48" t="s">
+      <c r="A65" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="54" t="s">
+      <c r="C65" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="D65" s="54">
+      <c r="D65" s="58">
         <v>13</v>
       </c>
-      <c r="E65" s="40" t="s">
+      <c r="E65" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F65" s="58">
+      <c r="F65" s="40">
         <v>43619</v>
       </c>
-      <c r="G65" s="58">
+      <c r="G65" s="40">
         <v>43635</v>
       </c>
       <c r="H65" s="28" t="s">
@@ -5038,26 +5038,26 @@
       <c r="I65" s="11"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A66" s="52"/>
-      <c r="B66" s="53"/>
-      <c r="C66" s="55"/>
-      <c r="D66" s="55"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="59"/>
-      <c r="G66" s="59"/>
+      <c r="A66" s="71"/>
+      <c r="B66" s="70"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="67"/>
+      <c r="F66" s="66"/>
+      <c r="G66" s="66"/>
       <c r="H66" s="28" t="s">
         <v>329</v>
       </c>
       <c r="I66" s="11"/>
     </row>
     <row r="67" spans="1:9" ht="18" customHeight="1">
-      <c r="A67" s="49"/>
-      <c r="B67" s="47"/>
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="60"/>
-      <c r="G67" s="60"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="41"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="30" t="s">
         <v>324</v>
       </c>
@@ -5066,25 +5066,25 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" customHeight="1">
-      <c r="A68" s="48" t="s">
+      <c r="A68" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="44" t="s">
+      <c r="C68" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="54">
+      <c r="D68" s="58">
         <v>10</v>
       </c>
-      <c r="E68" s="40" t="s">
+      <c r="E68" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F68" s="58">
+      <c r="F68" s="40">
         <v>43669</v>
       </c>
-      <c r="G68" s="58">
+      <c r="G68" s="40">
         <v>43682</v>
       </c>
       <c r="H68" s="28" t="s">
@@ -5095,51 +5095,51 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="18" customHeight="1">
-      <c r="A69" s="52"/>
-      <c r="B69" s="53"/>
-      <c r="C69" s="68"/>
-      <c r="D69" s="55"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="59"/>
-      <c r="G69" s="59"/>
+      <c r="A69" s="71"/>
+      <c r="B69" s="70"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="67"/>
+      <c r="F69" s="66"/>
+      <c r="G69" s="66"/>
       <c r="H69" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="I69" s="65"/>
+      <c r="I69" s="72"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="49"/>
-      <c r="B70" s="47"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="60"/>
-      <c r="G70" s="60"/>
+      <c r="A70" s="39"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="47"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="41"/>
+      <c r="G70" s="41"/>
       <c r="H70" s="30" t="s">
         <v>348</v>
       </c>
       <c r="I70" s="51"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="48" t="s">
+      <c r="A71" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="B71" s="46" t="s">
+      <c r="B71" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="C71" s="44" t="s">
+      <c r="C71" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="54">
+      <c r="D71" s="58">
         <v>9</v>
       </c>
-      <c r="E71" s="40" t="s">
+      <c r="E71" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F71" s="58">
+      <c r="F71" s="40">
         <v>43683</v>
       </c>
-      <c r="G71" s="58">
+      <c r="G71" s="40">
         <v>43693</v>
       </c>
       <c r="H71" s="28" t="s">
@@ -5150,26 +5150,26 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A72" s="52"/>
-      <c r="B72" s="53"/>
-      <c r="C72" s="68"/>
-      <c r="D72" s="55"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="59"/>
+      <c r="A72" s="71"/>
+      <c r="B72" s="70"/>
+      <c r="C72" s="69"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="67"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
       <c r="H72" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="I72" s="65"/>
+      <c r="I72" s="72"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="49"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="56"/>
-      <c r="E73" s="41"/>
-      <c r="F73" s="60"/>
-      <c r="G73" s="60"/>
+      <c r="A73" s="39"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="41"/>
+      <c r="G73" s="41"/>
       <c r="H73" s="30" t="s">
         <v>356</v>
       </c>
@@ -5287,25 +5287,25 @@
       <c r="I78" s="11"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="48" t="s">
+      <c r="A79" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="B79" s="46" t="s">
+      <c r="B79" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="54" t="s">
+      <c r="C79" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D79" s="54">
+      <c r="D79" s="58">
         <v>3</v>
       </c>
-      <c r="E79" s="40" t="s">
+      <c r="E79" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F79" s="58">
+      <c r="F79" s="40">
         <v>43586</v>
       </c>
-      <c r="G79" s="58">
+      <c r="G79" s="40">
         <v>43588</v>
       </c>
       <c r="H79" s="28" t="s">
@@ -5316,13 +5316,13 @@
       </c>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="49"/>
-      <c r="B80" s="47"/>
-      <c r="C80" s="56"/>
-      <c r="D80" s="56"/>
-      <c r="E80" s="41"/>
-      <c r="F80" s="60"/>
-      <c r="G80" s="60"/>
+      <c r="A80" s="39"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="59"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="41"/>
+      <c r="G80" s="41"/>
       <c r="H80" s="30" t="s">
         <v>331</v>
       </c>
@@ -5358,25 +5358,25 @@
       </c>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="48" t="s">
+      <c r="A82" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="46" t="s">
+      <c r="B82" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="54" t="s">
+      <c r="C82" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D82" s="54">
+      <c r="D82" s="58">
         <v>4</v>
       </c>
-      <c r="E82" s="40" t="s">
+      <c r="E82" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F82" s="58">
+      <c r="F82" s="40">
         <v>43609</v>
       </c>
-      <c r="G82" s="58">
+      <c r="G82" s="40">
         <v>43616</v>
       </c>
       <c r="H82" s="28" t="s">
@@ -5387,13 +5387,13 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="49"/>
-      <c r="B83" s="47"/>
-      <c r="C83" s="56"/>
-      <c r="D83" s="56"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="60"/>
-      <c r="G83" s="60"/>
+      <c r="A83" s="39"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="59"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="43"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="41"/>
       <c r="H83" s="30" t="s">
         <v>327</v>
       </c>
@@ -5539,25 +5539,25 @@
       </c>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="48" t="s">
+      <c r="A89" s="38" t="s">
         <v>305</v>
       </c>
-      <c r="B89" s="46" t="s">
+      <c r="B89" s="48" t="s">
         <v>306</v>
       </c>
-      <c r="C89" s="54" t="s">
+      <c r="C89" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="54">
+      <c r="D89" s="58">
         <v>2</v>
       </c>
-      <c r="E89" s="40" t="s">
+      <c r="E89" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F89" s="38">
+      <c r="F89" s="62">
         <v>43671</v>
       </c>
-      <c r="G89" s="38">
+      <c r="G89" s="62">
         <v>43672</v>
       </c>
       <c r="H89" s="28" t="s">
@@ -5568,38 +5568,38 @@
       </c>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="49"/>
-      <c r="B90" s="47"/>
-      <c r="C90" s="56"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="41"/>
-      <c r="F90" s="39"/>
-      <c r="G90" s="39"/>
+      <c r="A90" s="39"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="59"/>
+      <c r="E90" s="43"/>
+      <c r="F90" s="63"/>
+      <c r="G90" s="63"/>
       <c r="H90" s="30" t="s">
         <v>349</v>
       </c>
       <c r="I90" s="51"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A91" s="48" t="s">
+      <c r="A91" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="46" t="s">
+      <c r="B91" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C91" s="44">
+      <c r="C91" s="46">
         <v>43641</v>
       </c>
-      <c r="D91" s="42">
+      <c r="D91" s="44">
         <v>3</v>
       </c>
-      <c r="E91" s="40" t="s">
+      <c r="E91" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F91" s="38">
+      <c r="F91" s="62">
         <v>43642</v>
       </c>
-      <c r="G91" s="38">
+      <c r="G91" s="62">
         <v>43644</v>
       </c>
       <c r="H91" s="28" t="s">
@@ -5608,13 +5608,13 @@
       <c r="I91" s="50"/>
     </row>
     <row r="92" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A92" s="49"/>
-      <c r="B92" s="47"/>
-      <c r="C92" s="45"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="41"/>
-      <c r="F92" s="39"/>
-      <c r="G92" s="39"/>
+      <c r="A92" s="39"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="47"/>
+      <c r="D92" s="45"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="63"/>
+      <c r="G92" s="63"/>
       <c r="H92" s="30" t="s">
         <v>360</v>
       </c>
@@ -5890,25 +5890,25 @@
       </c>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="48" t="s">
+      <c r="A104" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B104" s="46" t="s">
+      <c r="B104" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C104" s="54" t="s">
+      <c r="C104" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="D104" s="54">
+      <c r="D104" s="58">
         <v>10</v>
       </c>
-      <c r="E104" s="40" t="s">
+      <c r="E104" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F104" s="58">
+      <c r="F104" s="40">
         <v>43613</v>
       </c>
-      <c r="G104" s="58">
+      <c r="G104" s="40">
         <v>43626</v>
       </c>
       <c r="H104" s="28" t="s">
@@ -5919,26 +5919,26 @@
       </c>
     </row>
     <row r="105" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A105" s="52"/>
-      <c r="B105" s="53"/>
-      <c r="C105" s="55"/>
-      <c r="D105" s="55"/>
-      <c r="E105" s="61"/>
-      <c r="F105" s="59"/>
-      <c r="G105" s="59"/>
+      <c r="A105" s="71"/>
+      <c r="B105" s="70"/>
+      <c r="C105" s="76"/>
+      <c r="D105" s="76"/>
+      <c r="E105" s="67"/>
+      <c r="F105" s="66"/>
+      <c r="G105" s="66"/>
       <c r="H105" s="28" t="s">
         <v>335</v>
       </c>
-      <c r="I105" s="65"/>
+      <c r="I105" s="72"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="49"/>
-      <c r="B106" s="47"/>
-      <c r="C106" s="56"/>
-      <c r="D106" s="56"/>
-      <c r="E106" s="41"/>
-      <c r="F106" s="60"/>
-      <c r="G106" s="60"/>
+      <c r="A106" s="39"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="59"/>
+      <c r="D106" s="59"/>
+      <c r="E106" s="43"/>
+      <c r="F106" s="41"/>
+      <c r="G106" s="41"/>
       <c r="H106" s="30" t="s">
         <v>325</v>
       </c>
@@ -6003,25 +6003,25 @@
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="48" t="s">
+      <c r="A109" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="B109" s="46" t="s">
+      <c r="B109" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="54" t="s">
+      <c r="C109" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="D109" s="54">
+      <c r="D109" s="58">
         <v>4</v>
       </c>
-      <c r="E109" s="40" t="s">
+      <c r="E109" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F109" s="58">
+      <c r="F109" s="40">
         <v>43627</v>
       </c>
-      <c r="G109" s="58">
+      <c r="G109" s="40">
         <v>43630</v>
       </c>
       <c r="H109" s="28" t="s">
@@ -6032,13 +6032,13 @@
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="49"/>
-      <c r="B110" s="47"/>
-      <c r="C110" s="56"/>
-      <c r="D110" s="56"/>
-      <c r="E110" s="41"/>
-      <c r="F110" s="60"/>
-      <c r="G110" s="60"/>
+      <c r="A110" s="39"/>
+      <c r="B110" s="49"/>
+      <c r="C110" s="59"/>
+      <c r="D110" s="59"/>
+      <c r="E110" s="43"/>
+      <c r="F110" s="41"/>
+      <c r="G110" s="41"/>
       <c r="H110" s="30" t="s">
         <v>324</v>
       </c>
@@ -6161,25 +6161,25 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="48" t="s">
+      <c r="A115" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="B115" s="46" t="s">
+      <c r="B115" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C115" s="44">
+      <c r="C115" s="46">
         <v>43641</v>
       </c>
-      <c r="D115" s="42">
+      <c r="D115" s="44">
         <v>8</v>
       </c>
-      <c r="E115" s="40" t="s">
+      <c r="E115" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F115" s="69">
+      <c r="F115" s="73">
         <v>43684</v>
       </c>
-      <c r="G115" s="69">
+      <c r="G115" s="73">
         <v>43693</v>
       </c>
       <c r="H115" s="28" t="s">
@@ -6190,51 +6190,51 @@
       </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="52"/>
-      <c r="B116" s="53"/>
-      <c r="C116" s="68"/>
-      <c r="D116" s="57"/>
-      <c r="E116" s="61"/>
-      <c r="F116" s="71"/>
-      <c r="G116" s="71"/>
+      <c r="A116" s="71"/>
+      <c r="B116" s="70"/>
+      <c r="C116" s="69"/>
+      <c r="D116" s="68"/>
+      <c r="E116" s="67"/>
+      <c r="F116" s="74"/>
+      <c r="G116" s="74"/>
       <c r="H116" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="I116" s="65"/>
+      <c r="I116" s="72"/>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="49"/>
-      <c r="B117" s="47"/>
-      <c r="C117" s="45"/>
-      <c r="D117" s="43"/>
-      <c r="E117" s="41"/>
-      <c r="F117" s="70"/>
-      <c r="G117" s="70"/>
+      <c r="A117" s="39"/>
+      <c r="B117" s="49"/>
+      <c r="C117" s="47"/>
+      <c r="D117" s="45"/>
+      <c r="E117" s="43"/>
+      <c r="F117" s="75"/>
+      <c r="G117" s="75"/>
       <c r="H117" s="30" t="s">
         <v>356</v>
       </c>
       <c r="I117" s="51"/>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="48" t="s">
+      <c r="A118" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="B118" s="46" t="s">
+      <c r="B118" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C118" s="44" t="s">
+      <c r="C118" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="D118" s="42">
+      <c r="D118" s="44">
         <v>5</v>
       </c>
-      <c r="E118" s="40" t="s">
+      <c r="E118" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F118" s="69">
+      <c r="F118" s="73">
         <v>43696</v>
       </c>
-      <c r="G118" s="69">
+      <c r="G118" s="73">
         <v>43700</v>
       </c>
       <c r="H118" s="28" t="s">
@@ -6245,13 +6245,13 @@
       </c>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="49"/>
-      <c r="B119" s="47"/>
-      <c r="C119" s="45"/>
-      <c r="D119" s="43"/>
-      <c r="E119" s="41"/>
-      <c r="F119" s="70"/>
-      <c r="G119" s="70"/>
+      <c r="A119" s="39"/>
+      <c r="B119" s="49"/>
+      <c r="C119" s="47"/>
+      <c r="D119" s="45"/>
+      <c r="E119" s="43"/>
+      <c r="F119" s="75"/>
+      <c r="G119" s="75"/>
       <c r="H119" s="30" t="s">
         <v>367</v>
       </c>
@@ -6382,25 +6382,25 @@
       </c>
     </row>
     <row r="126" spans="1:9">
-      <c r="A126" s="48" t="s">
+      <c r="A126" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="B126" s="46" t="s">
+      <c r="B126" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C126" s="54" t="s">
+      <c r="C126" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D126" s="42">
+      <c r="D126" s="44">
         <v>5</v>
       </c>
-      <c r="E126" s="40" t="s">
+      <c r="E126" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F126" s="38">
+      <c r="F126" s="62">
         <v>43643</v>
       </c>
-      <c r="G126" s="38">
+      <c r="G126" s="62">
         <v>43649</v>
       </c>
       <c r="H126" s="28" t="s">
@@ -6411,38 +6411,38 @@
       </c>
     </row>
     <row r="127" spans="1:9">
-      <c r="A127" s="49"/>
-      <c r="B127" s="47"/>
-      <c r="C127" s="56"/>
-      <c r="D127" s="43"/>
-      <c r="E127" s="41"/>
-      <c r="F127" s="39"/>
-      <c r="G127" s="39"/>
+      <c r="A127" s="39"/>
+      <c r="B127" s="49"/>
+      <c r="C127" s="59"/>
+      <c r="D127" s="45"/>
+      <c r="E127" s="43"/>
+      <c r="F127" s="63"/>
+      <c r="G127" s="63"/>
       <c r="H127" s="30" t="s">
         <v>360</v>
       </c>
       <c r="I127" s="51"/>
     </row>
     <row r="128" spans="1:9">
-      <c r="A128" s="48" t="s">
+      <c r="A128" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="B128" s="46" t="s">
+      <c r="B128" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C128" s="54" t="s">
+      <c r="C128" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D128" s="42">
+      <c r="D128" s="44">
         <v>2</v>
       </c>
-      <c r="E128" s="40" t="s">
+      <c r="E128" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F128" s="38">
+      <c r="F128" s="62">
         <v>43650</v>
       </c>
-      <c r="G128" s="38">
+      <c r="G128" s="62">
         <v>43651</v>
       </c>
       <c r="H128" s="28" t="s">
@@ -6453,38 +6453,38 @@
       </c>
     </row>
     <row r="129" spans="1:9">
-      <c r="A129" s="49"/>
-      <c r="B129" s="47"/>
-      <c r="C129" s="56"/>
-      <c r="D129" s="43"/>
-      <c r="E129" s="41"/>
-      <c r="F129" s="39"/>
-      <c r="G129" s="39"/>
+      <c r="A129" s="39"/>
+      <c r="B129" s="49"/>
+      <c r="C129" s="59"/>
+      <c r="D129" s="45"/>
+      <c r="E129" s="43"/>
+      <c r="F129" s="63"/>
+      <c r="G129" s="63"/>
       <c r="H129" s="30" t="s">
         <v>369</v>
       </c>
       <c r="I129" s="51"/>
     </row>
     <row r="130" spans="1:9">
-      <c r="A130" s="48" t="s">
+      <c r="A130" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="B130" s="46" t="s">
+      <c r="B130" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C130" s="54" t="s">
+      <c r="C130" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D130" s="42">
+      <c r="D130" s="44">
         <v>3</v>
       </c>
-      <c r="E130" s="40" t="s">
+      <c r="E130" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F130" s="38">
+      <c r="F130" s="62">
         <v>43685</v>
       </c>
-      <c r="G130" s="38">
+      <c r="G130" s="62">
         <v>43689</v>
       </c>
       <c r="H130" s="28" t="s">
@@ -6495,38 +6495,38 @@
       </c>
     </row>
     <row r="131" spans="1:9">
-      <c r="A131" s="49"/>
-      <c r="B131" s="47"/>
-      <c r="C131" s="56"/>
-      <c r="D131" s="43"/>
-      <c r="E131" s="41"/>
-      <c r="F131" s="39"/>
-      <c r="G131" s="39"/>
+      <c r="A131" s="39"/>
+      <c r="B131" s="49"/>
+      <c r="C131" s="59"/>
+      <c r="D131" s="45"/>
+      <c r="E131" s="43"/>
+      <c r="F131" s="63"/>
+      <c r="G131" s="63"/>
       <c r="H131" s="30" t="s">
         <v>353</v>
       </c>
       <c r="I131" s="51"/>
     </row>
     <row r="132" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A132" s="48" t="s">
+      <c r="A132" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="B132" s="46" t="s">
+      <c r="B132" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C132" s="44">
+      <c r="C132" s="46">
         <v>43641</v>
       </c>
-      <c r="D132" s="42">
+      <c r="D132" s="44">
         <v>2</v>
       </c>
-      <c r="E132" s="40" t="s">
+      <c r="E132" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F132" s="38">
+      <c r="F132" s="62">
         <v>43654</v>
       </c>
-      <c r="G132" s="38">
+      <c r="G132" s="62">
         <v>43658</v>
       </c>
       <c r="H132" s="28" t="s">
@@ -6537,38 +6537,38 @@
       </c>
     </row>
     <row r="133" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A133" s="49"/>
-      <c r="B133" s="47"/>
-      <c r="C133" s="45"/>
-      <c r="D133" s="43"/>
-      <c r="E133" s="41"/>
-      <c r="F133" s="39"/>
-      <c r="G133" s="39"/>
+      <c r="A133" s="39"/>
+      <c r="B133" s="49"/>
+      <c r="C133" s="47"/>
+      <c r="D133" s="45"/>
+      <c r="E133" s="43"/>
+      <c r="F133" s="63"/>
+      <c r="G133" s="63"/>
       <c r="H133" s="30" t="s">
         <v>353</v>
       </c>
       <c r="I133" s="51"/>
     </row>
     <row r="134" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A134" s="48" t="s">
+      <c r="A134" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B134" s="46" t="s">
+      <c r="B134" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C134" s="44">
+      <c r="C134" s="46">
         <v>43641</v>
       </c>
-      <c r="D134" s="42">
+      <c r="D134" s="44">
         <v>4</v>
       </c>
-      <c r="E134" s="72" t="s">
+      <c r="E134" s="64" t="s">
         <v>284</v>
       </c>
-      <c r="F134" s="38">
+      <c r="F134" s="62">
         <v>43690</v>
       </c>
-      <c r="G134" s="38">
+      <c r="G134" s="62">
         <v>43693</v>
       </c>
       <c r="H134" s="28" t="s">
@@ -6579,38 +6579,38 @@
       </c>
     </row>
     <row r="135" spans="1:9">
-      <c r="A135" s="49"/>
-      <c r="B135" s="47"/>
-      <c r="C135" s="45"/>
-      <c r="D135" s="43"/>
-      <c r="E135" s="73"/>
-      <c r="F135" s="39"/>
-      <c r="G135" s="39"/>
+      <c r="A135" s="39"/>
+      <c r="B135" s="49"/>
+      <c r="C135" s="47"/>
+      <c r="D135" s="45"/>
+      <c r="E135" s="65"/>
+      <c r="F135" s="63"/>
+      <c r="G135" s="63"/>
       <c r="H135" s="30" t="s">
         <v>356</v>
       </c>
       <c r="I135" s="51"/>
     </row>
     <row r="136" spans="1:9">
-      <c r="A136" s="48" t="s">
+      <c r="A136" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B136" s="46" t="s">
+      <c r="B136" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C136" s="54" t="s">
+      <c r="C136" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="D136" s="42">
+      <c r="D136" s="44">
         <v>5</v>
       </c>
-      <c r="E136" s="72" t="s">
+      <c r="E136" s="64" t="s">
         <v>284</v>
       </c>
-      <c r="F136" s="38">
+      <c r="F136" s="62">
         <v>43698</v>
       </c>
-      <c r="G136" s="74">
+      <c r="G136" s="60">
         <v>43704</v>
       </c>
       <c r="H136" s="28" t="s">
@@ -6621,38 +6621,38 @@
       </c>
     </row>
     <row r="137" spans="1:9">
-      <c r="A137" s="49"/>
-      <c r="B137" s="47"/>
-      <c r="C137" s="56"/>
-      <c r="D137" s="43"/>
-      <c r="E137" s="73"/>
-      <c r="F137" s="39"/>
-      <c r="G137" s="75"/>
+      <c r="A137" s="39"/>
+      <c r="B137" s="49"/>
+      <c r="C137" s="59"/>
+      <c r="D137" s="45"/>
+      <c r="E137" s="65"/>
+      <c r="F137" s="63"/>
+      <c r="G137" s="61"/>
       <c r="H137" s="30" t="s">
         <v>367</v>
       </c>
       <c r="I137" s="51"/>
     </row>
     <row r="138" spans="1:9">
-      <c r="A138" s="48" t="s">
+      <c r="A138" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B138" s="46" t="s">
+      <c r="B138" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C138" s="54" t="s">
+      <c r="C138" s="58" t="s">
         <v>168</v>
       </c>
-      <c r="D138" s="54">
+      <c r="D138" s="58">
         <v>3</v>
       </c>
-      <c r="E138" s="40" t="s">
+      <c r="E138" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F138" s="38">
+      <c r="F138" s="62">
         <v>43705</v>
       </c>
-      <c r="G138" s="38">
+      <c r="G138" s="62">
         <v>43707</v>
       </c>
       <c r="H138" s="28" t="s">
@@ -6663,13 +6663,13 @@
       </c>
     </row>
     <row r="139" spans="1:9">
-      <c r="A139" s="49"/>
-      <c r="B139" s="47"/>
-      <c r="C139" s="56"/>
-      <c r="D139" s="56"/>
-      <c r="E139" s="41"/>
-      <c r="F139" s="39"/>
-      <c r="G139" s="39"/>
+      <c r="A139" s="39"/>
+      <c r="B139" s="49"/>
+      <c r="C139" s="59"/>
+      <c r="D139" s="59"/>
+      <c r="E139" s="43"/>
+      <c r="F139" s="63"/>
+      <c r="G139" s="63"/>
       <c r="H139" s="30" t="s">
         <v>373</v>
       </c>
@@ -6733,25 +6733,25 @@
       <c r="I142" s="11"/>
     </row>
     <row r="143" spans="1:9">
-      <c r="A143" s="48" t="s">
+      <c r="A143" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B143" s="46" t="s">
+      <c r="B143" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C143" s="54" t="s">
+      <c r="C143" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D143" s="54">
+      <c r="D143" s="58">
         <v>5</v>
       </c>
-      <c r="E143" s="40" t="s">
+      <c r="E143" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F143" s="58">
+      <c r="F143" s="40">
         <v>43579</v>
       </c>
-      <c r="G143" s="58">
+      <c r="G143" s="40">
         <v>43585</v>
       </c>
       <c r="H143" s="28" t="s">
@@ -6762,38 +6762,38 @@
       </c>
     </row>
     <row r="144" spans="1:9">
-      <c r="A144" s="49"/>
-      <c r="B144" s="47"/>
-      <c r="C144" s="56"/>
-      <c r="D144" s="56"/>
-      <c r="E144" s="41"/>
-      <c r="F144" s="60"/>
-      <c r="G144" s="60"/>
+      <c r="A144" s="39"/>
+      <c r="B144" s="49"/>
+      <c r="C144" s="59"/>
+      <c r="D144" s="59"/>
+      <c r="E144" s="43"/>
+      <c r="F144" s="41"/>
+      <c r="G144" s="41"/>
       <c r="H144" s="30" t="s">
         <v>326</v>
       </c>
       <c r="I144" s="51"/>
     </row>
     <row r="145" spans="1:9">
-      <c r="A145" s="48" t="s">
+      <c r="A145" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="B145" s="46" t="s">
+      <c r="B145" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C145" s="54" t="s">
+      <c r="C145" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="D145" s="54">
+      <c r="D145" s="58">
         <v>5</v>
       </c>
-      <c r="E145" s="40" t="s">
+      <c r="E145" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F145" s="58">
+      <c r="F145" s="40">
         <v>43586</v>
       </c>
-      <c r="G145" s="58">
+      <c r="G145" s="40">
         <v>43592</v>
       </c>
       <c r="H145" s="28" t="s">
@@ -6804,38 +6804,38 @@
       </c>
     </row>
     <row r="146" spans="1:9">
-      <c r="A146" s="49"/>
-      <c r="B146" s="47"/>
-      <c r="C146" s="56"/>
-      <c r="D146" s="56"/>
-      <c r="E146" s="41"/>
-      <c r="F146" s="60"/>
-      <c r="G146" s="60"/>
+      <c r="A146" s="39"/>
+      <c r="B146" s="49"/>
+      <c r="C146" s="59"/>
+      <c r="D146" s="59"/>
+      <c r="E146" s="43"/>
+      <c r="F146" s="41"/>
+      <c r="G146" s="41"/>
       <c r="H146" s="30" t="s">
         <v>331</v>
       </c>
       <c r="I146" s="51"/>
     </row>
     <row r="147" spans="1:9">
-      <c r="A147" s="48" t="s">
+      <c r="A147" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="B147" s="46" t="s">
+      <c r="B147" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C147" s="54" t="s">
+      <c r="C147" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="D147" s="54">
+      <c r="D147" s="58">
         <v>5</v>
       </c>
-      <c r="E147" s="40" t="s">
+      <c r="E147" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F147" s="58">
+      <c r="F147" s="40">
         <v>43593</v>
       </c>
-      <c r="G147" s="58">
+      <c r="G147" s="40">
         <v>43599</v>
       </c>
       <c r="H147" s="28" t="s">
@@ -6846,38 +6846,38 @@
       </c>
     </row>
     <row r="148" spans="1:9">
-      <c r="A148" s="49"/>
-      <c r="B148" s="47"/>
-      <c r="C148" s="56"/>
-      <c r="D148" s="56"/>
-      <c r="E148" s="41"/>
-      <c r="F148" s="60"/>
-      <c r="G148" s="60"/>
+      <c r="A148" s="39"/>
+      <c r="B148" s="49"/>
+      <c r="C148" s="59"/>
+      <c r="D148" s="59"/>
+      <c r="E148" s="43"/>
+      <c r="F148" s="41"/>
+      <c r="G148" s="41"/>
       <c r="H148" s="30" t="s">
         <v>333</v>
       </c>
       <c r="I148" s="51"/>
     </row>
     <row r="149" spans="1:9">
-      <c r="A149" s="48" t="s">
+      <c r="A149" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="B149" s="46" t="s">
+      <c r="B149" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C149" s="54" t="s">
+      <c r="C149" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="D149" s="54">
+      <c r="D149" s="58">
         <v>5</v>
       </c>
-      <c r="E149" s="40" t="s">
+      <c r="E149" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F149" s="58">
+      <c r="F149" s="40">
         <v>43626</v>
       </c>
-      <c r="G149" s="58">
+      <c r="G149" s="40">
         <v>43630</v>
       </c>
       <c r="H149" s="28" t="s">
@@ -6888,13 +6888,13 @@
       </c>
     </row>
     <row r="150" spans="1:9">
-      <c r="A150" s="49"/>
-      <c r="B150" s="47"/>
-      <c r="C150" s="56"/>
-      <c r="D150" s="56"/>
-      <c r="E150" s="41"/>
-      <c r="F150" s="60"/>
-      <c r="G150" s="60"/>
+      <c r="A150" s="39"/>
+      <c r="B150" s="49"/>
+      <c r="C150" s="59"/>
+      <c r="D150" s="59"/>
+      <c r="E150" s="43"/>
+      <c r="F150" s="41"/>
+      <c r="G150" s="41"/>
       <c r="H150" s="30" t="s">
         <v>340</v>
       </c>
@@ -6959,25 +6959,25 @@
       </c>
     </row>
     <row r="153" spans="1:9">
-      <c r="A153" s="48" t="s">
+      <c r="A153" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="B153" s="46" t="s">
+      <c r="B153" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C153" s="44">
+      <c r="C153" s="46">
         <v>43641</v>
       </c>
-      <c r="D153" s="54">
+      <c r="D153" s="58">
         <v>7</v>
       </c>
-      <c r="E153" s="40" t="s">
+      <c r="E153" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F153" s="58">
+      <c r="F153" s="40">
         <v>43647</v>
       </c>
-      <c r="G153" s="58">
+      <c r="G153" s="40">
         <v>43655</v>
       </c>
       <c r="H153" s="28" t="s">
@@ -6988,13 +6988,13 @@
       </c>
     </row>
     <row r="154" spans="1:9">
-      <c r="A154" s="49"/>
-      <c r="B154" s="47"/>
-      <c r="C154" s="45"/>
-      <c r="D154" s="56"/>
-      <c r="E154" s="41"/>
-      <c r="F154" s="60"/>
-      <c r="G154" s="60"/>
+      <c r="A154" s="39"/>
+      <c r="B154" s="49"/>
+      <c r="C154" s="47"/>
+      <c r="D154" s="59"/>
+      <c r="E154" s="43"/>
+      <c r="F154" s="41"/>
+      <c r="G154" s="41"/>
       <c r="H154" s="30" t="s">
         <v>375</v>
       </c>
@@ -7059,25 +7059,25 @@
       </c>
     </row>
     <row r="157" spans="1:9" ht="15.75">
-      <c r="A157" s="48" t="s">
+      <c r="A157" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B157" s="46" t="s">
+      <c r="B157" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C157" s="44" t="s">
+      <c r="C157" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="D157" s="42">
+      <c r="D157" s="44">
         <v>2</v>
       </c>
-      <c r="E157" s="40" t="s">
+      <c r="E157" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F157" s="58">
+      <c r="F157" s="40">
         <v>43664</v>
       </c>
-      <c r="G157" s="58">
+      <c r="G157" s="40">
         <v>43665</v>
       </c>
       <c r="H157" s="28" t="s">
@@ -7086,13 +7086,13 @@
       <c r="I157" s="36"/>
     </row>
     <row r="158" spans="1:9" ht="15.75">
-      <c r="A158" s="49"/>
-      <c r="B158" s="47"/>
-      <c r="C158" s="45"/>
-      <c r="D158" s="43"/>
-      <c r="E158" s="41"/>
-      <c r="F158" s="60"/>
-      <c r="G158" s="60"/>
+      <c r="A158" s="39"/>
+      <c r="B158" s="49"/>
+      <c r="C158" s="47"/>
+      <c r="D158" s="45"/>
+      <c r="E158" s="43"/>
+      <c r="F158" s="41"/>
+      <c r="G158" s="41"/>
       <c r="H158" s="30" t="s">
         <v>377</v>
       </c>
@@ -7217,25 +7217,25 @@
       </c>
     </row>
     <row r="163" spans="1:9">
-      <c r="A163" s="48" t="s">
+      <c r="A163" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="B163" s="46" t="s">
+      <c r="B163" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C163" s="44" t="s">
+      <c r="C163" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="D163" s="42">
+      <c r="D163" s="44">
         <v>4</v>
       </c>
-      <c r="E163" s="40" t="s">
+      <c r="E163" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="F163" s="58">
+      <c r="F163" s="40">
         <v>43698</v>
       </c>
-      <c r="G163" s="58">
+      <c r="G163" s="40">
         <v>43703</v>
       </c>
       <c r="H163" s="28" t="s">
@@ -7246,13 +7246,13 @@
       </c>
     </row>
     <row r="164" spans="1:9">
-      <c r="A164" s="49"/>
-      <c r="B164" s="47"/>
-      <c r="C164" s="45"/>
-      <c r="D164" s="43"/>
-      <c r="E164" s="41"/>
-      <c r="F164" s="60"/>
-      <c r="G164" s="60"/>
+      <c r="A164" s="39"/>
+      <c r="B164" s="49"/>
+      <c r="C164" s="47"/>
+      <c r="D164" s="45"/>
+      <c r="E164" s="43"/>
+      <c r="F164" s="41"/>
+      <c r="G164" s="41"/>
       <c r="H164" s="30" t="s">
         <v>367</v>
       </c>
@@ -7430,25 +7430,25 @@
       <c r="I173" s="12"/>
     </row>
     <row r="174" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A174" s="48" t="s">
+      <c r="A174" s="38" t="s">
         <v>389</v>
       </c>
-      <c r="B174" s="81" t="s">
+      <c r="B174" s="57" t="s">
         <v>381</v>
       </c>
-      <c r="C174" s="80" t="s">
+      <c r="C174" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="D174" s="78">
+      <c r="D174" s="54">
         <v>3</v>
       </c>
-      <c r="E174" s="77" t="s">
+      <c r="E174" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="F174" s="76">
+      <c r="F174" s="52">
         <v>43636</v>
       </c>
-      <c r="G174" s="76">
+      <c r="G174" s="52">
         <v>43640</v>
       </c>
       <c r="H174" s="28" t="s">
@@ -7457,13 +7457,13 @@
       <c r="I174" s="11"/>
     </row>
     <row r="175" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A175" s="49"/>
-      <c r="B175" s="47"/>
-      <c r="C175" s="45"/>
-      <c r="D175" s="79"/>
-      <c r="E175" s="41"/>
-      <c r="F175" s="60"/>
-      <c r="G175" s="60"/>
+      <c r="A175" s="39"/>
+      <c r="B175" s="49"/>
+      <c r="C175" s="47"/>
+      <c r="D175" s="55"/>
+      <c r="E175" s="43"/>
+      <c r="F175" s="41"/>
+      <c r="G175" s="41"/>
       <c r="H175" s="30" t="s">
         <v>382</v>
       </c>
@@ -7520,112 +7520,186 @@
     </row>
   </sheetData>
   <mergeCells count="310">
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="G163:G164"/>
-    <mergeCell ref="F163:F164"/>
-    <mergeCell ref="E163:E164"/>
-    <mergeCell ref="D163:D164"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="B163:B164"/>
-    <mergeCell ref="A163:A164"/>
-    <mergeCell ref="I163:I164"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="G157:G158"/>
-    <mergeCell ref="F157:F158"/>
-    <mergeCell ref="E157:E158"/>
-    <mergeCell ref="D157:D158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="G153:G154"/>
-    <mergeCell ref="F153:F154"/>
-    <mergeCell ref="E153:E154"/>
-    <mergeCell ref="D153:D154"/>
-    <mergeCell ref="C153:C154"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="I153:I154"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="I149:I150"/>
-    <mergeCell ref="G149:G150"/>
-    <mergeCell ref="F149:F150"/>
-    <mergeCell ref="E149:E150"/>
-    <mergeCell ref="D149:D150"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="I136:I137"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="I138:I139"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="I132:I133"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="I134:I135"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="I130:I131"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="G46:G50"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="I46:I50"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="G71:G73"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="I89:I90"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="G143:G144"/>
+    <mergeCell ref="E143:E144"/>
+    <mergeCell ref="F143:F144"/>
+    <mergeCell ref="I143:I144"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="F109:F110"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="D109:D110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I126:I127"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="I145:I146"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="I147:I148"/>
+    <mergeCell ref="F147:F148"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="G145:G146"/>
+    <mergeCell ref="F145:F146"/>
+    <mergeCell ref="D145:D146"/>
+    <mergeCell ref="E145:E146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="I58:I59"/>
     <mergeCell ref="C71:C73"/>
     <mergeCell ref="B71:B73"/>
     <mergeCell ref="A71:A73"/>
@@ -7650,186 +7724,112 @@
     <mergeCell ref="D104:D106"/>
     <mergeCell ref="C104:C106"/>
     <mergeCell ref="B104:B106"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="I145:I146"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="I147:I148"/>
-    <mergeCell ref="F147:F148"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="D147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="G145:G146"/>
-    <mergeCell ref="F145:F146"/>
-    <mergeCell ref="D145:D146"/>
-    <mergeCell ref="E145:E146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="G143:G144"/>
-    <mergeCell ref="E143:E144"/>
-    <mergeCell ref="F143:F144"/>
-    <mergeCell ref="I143:I144"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="C143:C144"/>
-    <mergeCell ref="D143:D144"/>
-    <mergeCell ref="G109:G110"/>
-    <mergeCell ref="F109:F110"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="D109:D110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I126:I127"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="G71:G73"/>
-    <mergeCell ref="F71:F73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="G46:G50"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="E46:E50"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="I46:I50"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="I130:I131"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="I132:I133"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="I134:I135"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="C136:C137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="I136:I137"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="I138:I139"/>
+    <mergeCell ref="G153:G154"/>
+    <mergeCell ref="F153:F154"/>
+    <mergeCell ref="E153:E154"/>
+    <mergeCell ref="D153:D154"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="I153:I154"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="I149:I150"/>
+    <mergeCell ref="G149:G150"/>
+    <mergeCell ref="F149:F150"/>
+    <mergeCell ref="E149:E150"/>
+    <mergeCell ref="D149:D150"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="G157:G158"/>
+    <mergeCell ref="F157:F158"/>
+    <mergeCell ref="E157:E158"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="C157:C158"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="G163:G164"/>
+    <mergeCell ref="F163:F164"/>
+    <mergeCell ref="E163:E164"/>
+    <mergeCell ref="D163:D164"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="B163:B164"/>
+    <mergeCell ref="A163:A164"/>
+    <mergeCell ref="I163:I164"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>